<commit_message>
báo cáo ngày 21
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemva\Downloads\Microsoft.SkypeApp_kzf8qxf38zg5c!App\All\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PCA_Report\DailyReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>No.</t>
   </si>
@@ -88,6 +88,33 @@
   </si>
   <si>
     <t>15/11/2018</t>
+  </si>
+  <si>
+    <t>16/11/2018</t>
+  </si>
+  <si>
+    <t>Tạm dừng phát triển</t>
+  </si>
+  <si>
+    <t>Nghiên cứu tìm hiểu CronTrigger</t>
+  </si>
+  <si>
+    <t>17/11/2018</t>
+  </si>
+  <si>
+    <t>Nghiên cứu tìm hiểu Hangfire</t>
+  </si>
+  <si>
+    <t>Xây dựng chức năng quản lý job</t>
+  </si>
+  <si>
+    <t>Xây dựng trang tạo mới</t>
+  </si>
+  <si>
+    <t>19/11/2018</t>
+  </si>
+  <si>
+    <t>20/11/2018</t>
   </si>
 </sst>
 </file>
@@ -867,7 +894,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS4" sqref="AS4:BF4"/>
+      <selection pane="bottomLeft" activeCell="BG11" sqref="BG11:CA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1288,9 @@
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="19"/>
+      <c r="D5" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -1289,20 +1318,28 @@
       <c r="AC5" s="19"/>
       <c r="AD5" s="19"/>
       <c r="AE5" s="19"/>
-      <c r="AF5" s="20"/>
+      <c r="AF5" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="AG5" s="20"/>
       <c r="AH5" s="20"/>
       <c r="AI5" s="20"/>
       <c r="AJ5" s="20"/>
-      <c r="AK5" s="19"/>
+      <c r="AK5" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="AL5" s="19"/>
       <c r="AM5" s="19"/>
       <c r="AN5" s="19"/>
       <c r="AO5" s="19"/>
-      <c r="AP5" s="21"/>
+      <c r="AP5" s="21">
+        <v>0.75</v>
+      </c>
       <c r="AQ5" s="21"/>
       <c r="AR5" s="21"/>
-      <c r="AS5" s="19"/>
+      <c r="AS5" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="AT5" s="19"/>
       <c r="AU5" s="19"/>
       <c r="AV5" s="19"/>
@@ -1316,7 +1353,9 @@
       <c r="BD5" s="19"/>
       <c r="BE5" s="19"/>
       <c r="BF5" s="19"/>
-      <c r="BG5" s="22"/>
+      <c r="BG5" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="BH5" s="22"/>
       <c r="BI5" s="22"/>
       <c r="BJ5" s="22"/>
@@ -1344,7 +1383,9 @@
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -1372,20 +1413,28 @@
       <c r="AC6" s="19"/>
       <c r="AD6" s="19"/>
       <c r="AE6" s="19"/>
-      <c r="AF6" s="20"/>
+      <c r="AF6" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="AG6" s="20"/>
       <c r="AH6" s="20"/>
       <c r="AI6" s="20"/>
       <c r="AJ6" s="20"/>
-      <c r="AK6" s="19"/>
+      <c r="AK6" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="AL6" s="19"/>
       <c r="AM6" s="19"/>
       <c r="AN6" s="19"/>
       <c r="AO6" s="19"/>
-      <c r="AP6" s="21"/>
+      <c r="AP6" s="21">
+        <v>0.5</v>
+      </c>
       <c r="AQ6" s="21"/>
       <c r="AR6" s="21"/>
-      <c r="AS6" s="19"/>
+      <c r="AS6" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="AT6" s="19"/>
       <c r="AU6" s="19"/>
       <c r="AV6" s="19"/>
@@ -1427,7 +1476,9 @@
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -1455,20 +1506,28 @@
       <c r="AC7" s="19"/>
       <c r="AD7" s="19"/>
       <c r="AE7" s="19"/>
-      <c r="AF7" s="20"/>
+      <c r="AF7" s="20" t="s">
+        <v>24</v>
+      </c>
       <c r="AG7" s="20"/>
       <c r="AH7" s="20"/>
       <c r="AI7" s="20"/>
       <c r="AJ7" s="20"/>
-      <c r="AK7" s="19"/>
+      <c r="AK7" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="AL7" s="19"/>
       <c r="AM7" s="19"/>
       <c r="AN7" s="19"/>
       <c r="AO7" s="19"/>
-      <c r="AP7" s="21"/>
+      <c r="AP7" s="21">
+        <v>0.8</v>
+      </c>
       <c r="AQ7" s="21"/>
       <c r="AR7" s="21"/>
-      <c r="AS7" s="19"/>
+      <c r="AS7" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="AT7" s="19"/>
       <c r="AU7" s="19"/>
       <c r="AV7" s="19"/>
@@ -1510,7 +1569,9 @@
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
@@ -1538,20 +1599,28 @@
       <c r="AC8" s="19"/>
       <c r="AD8" s="19"/>
       <c r="AE8" s="19"/>
-      <c r="AF8" s="20"/>
+      <c r="AF8" s="20" t="s">
+        <v>24</v>
+      </c>
       <c r="AG8" s="20"/>
       <c r="AH8" s="20"/>
       <c r="AI8" s="20"/>
       <c r="AJ8" s="20"/>
-      <c r="AK8" s="19"/>
+      <c r="AK8" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="AL8" s="19"/>
       <c r="AM8" s="19"/>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
-      <c r="AP8" s="21"/>
+      <c r="AP8" s="21">
+        <v>0.4</v>
+      </c>
       <c r="AQ8" s="21"/>
       <c r="AR8" s="21"/>
-      <c r="AS8" s="19"/>
+      <c r="AS8" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="AT8" s="19"/>
       <c r="AU8" s="19"/>
       <c r="AV8" s="19"/>
@@ -1593,7 +1662,9 @@
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="19"/>
+      <c r="D9" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -1621,20 +1692,28 @@
       <c r="AC9" s="19"/>
       <c r="AD9" s="19"/>
       <c r="AE9" s="19"/>
-      <c r="AF9" s="20"/>
+      <c r="AF9" s="20" t="s">
+        <v>24</v>
+      </c>
       <c r="AG9" s="20"/>
       <c r="AH9" s="20"/>
       <c r="AI9" s="20"/>
       <c r="AJ9" s="20"/>
-      <c r="AK9" s="19"/>
+      <c r="AK9" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="AL9" s="19"/>
       <c r="AM9" s="19"/>
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
-      <c r="AP9" s="21"/>
+      <c r="AP9" s="21">
+        <v>0.1</v>
+      </c>
       <c r="AQ9" s="21"/>
       <c r="AR9" s="21"/>
-      <c r="AS9" s="19"/>
+      <c r="AS9" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="AT9" s="19"/>
       <c r="AU9" s="19"/>
       <c r="AV9" s="19"/>
@@ -1648,7 +1727,9 @@
       <c r="BD9" s="19"/>
       <c r="BE9" s="19"/>
       <c r="BF9" s="19"/>
-      <c r="BG9" s="22"/>
+      <c r="BG9" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="BH9" s="22"/>
       <c r="BI9" s="22"/>
       <c r="BJ9" s="22"/>
@@ -1676,7 +1757,9 @@
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -1704,20 +1787,28 @@
       <c r="AC10" s="19"/>
       <c r="AD10" s="19"/>
       <c r="AE10" s="19"/>
-      <c r="AF10" s="20"/>
+      <c r="AF10" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="AG10" s="20"/>
       <c r="AH10" s="20"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="20"/>
-      <c r="AK10" s="19"/>
+      <c r="AK10" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="AL10" s="19"/>
       <c r="AM10" s="19"/>
       <c r="AN10" s="19"/>
       <c r="AO10" s="19"/>
-      <c r="AP10" s="21"/>
+      <c r="AP10" s="21">
+        <v>0.3</v>
+      </c>
       <c r="AQ10" s="21"/>
       <c r="AR10" s="21"/>
-      <c r="AS10" s="19"/>
+      <c r="AS10" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="AT10" s="19"/>
       <c r="AU10" s="19"/>
       <c r="AV10" s="19"/>
@@ -1759,7 +1850,9 @@
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
@@ -1787,20 +1880,28 @@
       <c r="AC11" s="19"/>
       <c r="AD11" s="19"/>
       <c r="AE11" s="19"/>
-      <c r="AF11" s="20"/>
+      <c r="AF11" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="AG11" s="20"/>
       <c r="AH11" s="20"/>
       <c r="AI11" s="20"/>
       <c r="AJ11" s="20"/>
-      <c r="AK11" s="19"/>
+      <c r="AK11" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="AL11" s="19"/>
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
-      <c r="AP11" s="21"/>
+      <c r="AP11" s="21">
+        <v>0.6</v>
+      </c>
       <c r="AQ11" s="21"/>
       <c r="AR11" s="21"/>
-      <c r="AS11" s="19"/>
+      <c r="AS11" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="AT11" s="19"/>
       <c r="AU11" s="19"/>
       <c r="AV11" s="19"/>
@@ -6447,7 +6548,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>AS2:BF31 AS33:BF61</xm:sqref>
+          <xm:sqref>AS33:BF61 AS2:BF31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Báo cáo ngày 21/12/2018
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="73">
   <si>
     <t>No.</t>
   </si>
@@ -221,6 +221,24 @@
   </si>
   <si>
     <t>Trang tạo mới Job - code step 5 - tạo giao diện thân thiện người dùng</t>
+  </si>
+  <si>
+    <t>20/12/2018</t>
+  </si>
+  <si>
+    <t>Trang tạo mới Job - code step 5 - nội dung hiển thị</t>
+  </si>
+  <si>
+    <t>Trang tạo mới Job - hoàn thành thêm dữ liệu vào database</t>
+  </si>
+  <si>
+    <t>21/12/2018</t>
+  </si>
+  <si>
+    <t>Trang tạo mới Job - Thay đổi giao diện</t>
+  </si>
+  <si>
+    <t>Trang tạo mới Job - Test</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1041,8 @@
   <dimension ref="A1:CA61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS51" sqref="AS51:BF51"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AS56" sqref="AS56:BF56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5805,7 +5823,9 @@
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="5"/>
-      <c r="D52" s="9"/>
+      <c r="D52" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
@@ -5833,20 +5853,28 @@
       <c r="AC52" s="9"/>
       <c r="AD52" s="9"/>
       <c r="AE52" s="9"/>
-      <c r="AF52" s="10"/>
+      <c r="AF52" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="AG52" s="10"/>
       <c r="AH52" s="10"/>
       <c r="AI52" s="10"/>
       <c r="AJ52" s="10"/>
-      <c r="AK52" s="9"/>
+      <c r="AK52" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL52" s="9"/>
       <c r="AM52" s="9"/>
       <c r="AN52" s="9"/>
       <c r="AO52" s="9"/>
-      <c r="AP52" s="11"/>
+      <c r="AP52" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ52" s="11"/>
       <c r="AR52" s="11"/>
-      <c r="AS52" s="9"/>
+      <c r="AS52" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT52" s="9"/>
       <c r="AU52" s="9"/>
       <c r="AV52" s="9"/>
@@ -5888,7 +5916,9 @@
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="5"/>
-      <c r="D53" s="9"/>
+      <c r="D53" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
@@ -5916,20 +5946,28 @@
       <c r="AC53" s="9"/>
       <c r="AD53" s="9"/>
       <c r="AE53" s="9"/>
-      <c r="AF53" s="10"/>
+      <c r="AF53" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="AG53" s="10"/>
       <c r="AH53" s="10"/>
       <c r="AI53" s="10"/>
       <c r="AJ53" s="10"/>
-      <c r="AK53" s="9"/>
+      <c r="AK53" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL53" s="9"/>
       <c r="AM53" s="9"/>
       <c r="AN53" s="9"/>
       <c r="AO53" s="9"/>
-      <c r="AP53" s="11"/>
+      <c r="AP53" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ53" s="11"/>
       <c r="AR53" s="11"/>
-      <c r="AS53" s="9"/>
+      <c r="AS53" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT53" s="9"/>
       <c r="AU53" s="9"/>
       <c r="AV53" s="9"/>
@@ -5971,7 +6009,9 @@
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="5"/>
-      <c r="D54" s="9"/>
+      <c r="D54" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
@@ -5999,20 +6039,28 @@
       <c r="AC54" s="9"/>
       <c r="AD54" s="9"/>
       <c r="AE54" s="9"/>
-      <c r="AF54" s="10"/>
+      <c r="AF54" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="AG54" s="10"/>
       <c r="AH54" s="10"/>
       <c r="AI54" s="10"/>
       <c r="AJ54" s="10"/>
-      <c r="AK54" s="9"/>
+      <c r="AK54" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL54" s="9"/>
       <c r="AM54" s="9"/>
       <c r="AN54" s="9"/>
       <c r="AO54" s="9"/>
-      <c r="AP54" s="11"/>
+      <c r="AP54" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ54" s="11"/>
       <c r="AR54" s="11"/>
-      <c r="AS54" s="9"/>
+      <c r="AS54" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT54" s="9"/>
       <c r="AU54" s="9"/>
       <c r="AV54" s="9"/>
@@ -6054,7 +6102,9 @@
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="5"/>
-      <c r="D55" s="9"/>
+      <c r="D55" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
@@ -6082,20 +6132,28 @@
       <c r="AC55" s="9"/>
       <c r="AD55" s="9"/>
       <c r="AE55" s="9"/>
-      <c r="AF55" s="10"/>
+      <c r="AF55" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="AG55" s="10"/>
       <c r="AH55" s="10"/>
       <c r="AI55" s="10"/>
       <c r="AJ55" s="10"/>
-      <c r="AK55" s="9"/>
+      <c r="AK55" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL55" s="9"/>
       <c r="AM55" s="9"/>
       <c r="AN55" s="9"/>
       <c r="AO55" s="9"/>
-      <c r="AP55" s="11"/>
+      <c r="AP55" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ55" s="11"/>
       <c r="AR55" s="11"/>
-      <c r="AS55" s="9"/>
+      <c r="AS55" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT55" s="9"/>
       <c r="AU55" s="9"/>
       <c r="AV55" s="9"/>
@@ -6137,7 +6195,9 @@
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="5"/>
-      <c r="D56" s="9"/>
+      <c r="D56" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -6165,20 +6225,28 @@
       <c r="AC56" s="9"/>
       <c r="AD56" s="9"/>
       <c r="AE56" s="9"/>
-      <c r="AF56" s="10"/>
+      <c r="AF56" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="AG56" s="10"/>
       <c r="AH56" s="10"/>
       <c r="AI56" s="10"/>
       <c r="AJ56" s="10"/>
-      <c r="AK56" s="9"/>
+      <c r="AK56" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL56" s="9"/>
       <c r="AM56" s="9"/>
       <c r="AN56" s="9"/>
       <c r="AO56" s="9"/>
-      <c r="AP56" s="11"/>
+      <c r="AP56" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ56" s="11"/>
       <c r="AR56" s="11"/>
-      <c r="AS56" s="9"/>
+      <c r="AS56" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT56" s="9"/>
       <c r="AU56" s="9"/>
       <c r="AV56" s="9"/>

</xml_diff>

<commit_message>
báo cáo ngày 22/12/2018
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="76">
   <si>
     <t>No.</t>
   </si>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>Trang tạo mới Job - Test</t>
+  </si>
+  <si>
+    <t>22/12/2018</t>
+  </si>
+  <si>
+    <t>Trang tạo mới Job - Test (hoàn thiện giao diện thân thiện - không bị thay đổi các ô input nếu không cần thiết)</t>
+  </si>
+  <si>
+    <t>Cập nhật thay đổi của database</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1051,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS56" sqref="AS56:BF56"/>
+      <selection pane="bottomLeft" activeCell="AS58" sqref="AS58:BF58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6288,7 +6297,9 @@
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="5"/>
-      <c r="D57" s="9"/>
+      <c r="D57" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
@@ -6316,20 +6327,28 @@
       <c r="AC57" s="9"/>
       <c r="AD57" s="9"/>
       <c r="AE57" s="9"/>
-      <c r="AF57" s="10"/>
+      <c r="AF57" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="AG57" s="10"/>
       <c r="AH57" s="10"/>
       <c r="AI57" s="10"/>
       <c r="AJ57" s="10"/>
-      <c r="AK57" s="9"/>
+      <c r="AK57" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL57" s="9"/>
       <c r="AM57" s="9"/>
       <c r="AN57" s="9"/>
       <c r="AO57" s="9"/>
-      <c r="AP57" s="11"/>
+      <c r="AP57" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ57" s="11"/>
       <c r="AR57" s="11"/>
-      <c r="AS57" s="9"/>
+      <c r="AS57" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT57" s="9"/>
       <c r="AU57" s="9"/>
       <c r="AV57" s="9"/>
@@ -6371,7 +6390,9 @@
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="9"/>
+      <c r="D58" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -6399,20 +6420,28 @@
       <c r="AC58" s="9"/>
       <c r="AD58" s="9"/>
       <c r="AE58" s="9"/>
-      <c r="AF58" s="10"/>
+      <c r="AF58" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="AG58" s="10"/>
       <c r="AH58" s="10"/>
       <c r="AI58" s="10"/>
       <c r="AJ58" s="10"/>
-      <c r="AK58" s="9"/>
+      <c r="AK58" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL58" s="9"/>
       <c r="AM58" s="9"/>
       <c r="AN58" s="9"/>
       <c r="AO58" s="9"/>
-      <c r="AP58" s="11"/>
+      <c r="AP58" s="11">
+        <v>0.6</v>
+      </c>
       <c r="AQ58" s="11"/>
       <c r="AR58" s="11"/>
-      <c r="AS58" s="9"/>
+      <c r="AS58" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT58" s="9"/>
       <c r="AU58" s="9"/>
       <c r="AV58" s="9"/>

</xml_diff>

<commit_message>
Báo cáo ngày 24/12/2018
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="78">
   <si>
     <t>No.</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>Cập nhật thay đổi của database</t>
+  </si>
+  <si>
+    <t>24/12/2018</t>
+  </si>
+  <si>
+    <t>Trang tạo mới Job - Step1 - Thay đổi giao diện theo database mới</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1056,8 @@
   <dimension ref="A1:CA61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS58" sqref="AS58:BF58"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6483,7 +6489,9 @@
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="5"/>
-      <c r="D59" s="9"/>
+      <c r="D59" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -6511,20 +6519,28 @@
       <c r="AC59" s="9"/>
       <c r="AD59" s="9"/>
       <c r="AE59" s="9"/>
-      <c r="AF59" s="10"/>
+      <c r="AF59" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="AG59" s="10"/>
       <c r="AH59" s="10"/>
       <c r="AI59" s="10"/>
       <c r="AJ59" s="10"/>
-      <c r="AK59" s="9"/>
+      <c r="AK59" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL59" s="9"/>
       <c r="AM59" s="9"/>
       <c r="AN59" s="9"/>
       <c r="AO59" s="9"/>
-      <c r="AP59" s="11"/>
+      <c r="AP59" s="11">
+        <v>0.8</v>
+      </c>
       <c r="AQ59" s="11"/>
       <c r="AR59" s="11"/>
-      <c r="AS59" s="9"/>
+      <c r="AS59" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT59" s="9"/>
       <c r="AU59" s="9"/>
       <c r="AV59" s="9"/>
@@ -6566,7 +6582,9 @@
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="5"/>
-      <c r="D60" s="9"/>
+      <c r="D60" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
@@ -6594,20 +6612,28 @@
       <c r="AC60" s="9"/>
       <c r="AD60" s="9"/>
       <c r="AE60" s="9"/>
-      <c r="AF60" s="10"/>
+      <c r="AF60" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="AG60" s="10"/>
       <c r="AH60" s="10"/>
       <c r="AI60" s="10"/>
       <c r="AJ60" s="10"/>
-      <c r="AK60" s="9"/>
+      <c r="AK60" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL60" s="9"/>
       <c r="AM60" s="9"/>
       <c r="AN60" s="9"/>
       <c r="AO60" s="9"/>
-      <c r="AP60" s="11"/>
+      <c r="AP60" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ60" s="11"/>
       <c r="AR60" s="11"/>
-      <c r="AS60" s="9"/>
+      <c r="AS60" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT60" s="9"/>
       <c r="AU60" s="9"/>
       <c r="AV60" s="9"/>

</xml_diff>

<commit_message>
báo cáo ngày 3/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="93">
   <si>
     <t>No.</t>
   </si>
@@ -293,6 +293,12 @@
   </si>
   <si>
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 trang tạo mới - Collapse - Thay đổi từ đơn giao diện (db cũ) sang đa giao diện (db mới)</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 trang tạo mới - đổ dữ liệu vào session</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 trang tạo mới - Test</t>
   </si>
 </sst>
 </file>
@@ -560,14 +566,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,6 +586,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +699,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1084,7 +1090,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1092,11 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA70"/>
+  <dimension ref="A1:CA73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AV73" sqref="AV73"/>
+      <selection pane="bottomLeft" activeCell="AH75" sqref="AH75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,192 +1117,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="23" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="24" t="s">
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="22" t="s">
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="25" t="s">
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="25"/>
-      <c r="BJ1" s="25"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="25"/>
-      <c r="BO1" s="25"/>
-      <c r="BP1" s="25"/>
-      <c r="BQ1" s="25"/>
-      <c r="BR1" s="25"/>
-      <c r="BS1" s="25"/>
-      <c r="BT1" s="25"/>
-      <c r="BU1" s="25"/>
-      <c r="BV1" s="25"/>
-      <c r="BW1" s="25"/>
-      <c r="BX1" s="25"/>
-      <c r="BY1" s="25"/>
-      <c r="BZ1" s="25"/>
-      <c r="CA1" s="25"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="21">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4017,43 +4023,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="18"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
-      <c r="AD32" s="18"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="19">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="24">
         <v>43293</v>
       </c>
-      <c r="AG32" s="19"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="19"/>
-      <c r="AJ32" s="19"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4082,27 +4088,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="20"/>
-      <c r="BH32" s="20"/>
-      <c r="BI32" s="20"/>
-      <c r="BJ32" s="20"/>
-      <c r="BK32" s="20"/>
-      <c r="BL32" s="20"/>
-      <c r="BM32" s="20"/>
-      <c r="BN32" s="20"/>
-      <c r="BO32" s="20"/>
-      <c r="BP32" s="20"/>
-      <c r="BQ32" s="20"/>
-      <c r="BR32" s="20"/>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="BV32" s="20"/>
-      <c r="BW32" s="20"/>
-      <c r="BX32" s="20"/>
-      <c r="BY32" s="20"/>
-      <c r="BZ32" s="20"/>
-      <c r="CA32" s="20"/>
+      <c r="BG32" s="25"/>
+      <c r="BH32" s="25"/>
+      <c r="BI32" s="25"/>
+      <c r="BJ32" s="25"/>
+      <c r="BK32" s="25"/>
+      <c r="BL32" s="25"/>
+      <c r="BM32" s="25"/>
+      <c r="BN32" s="25"/>
+      <c r="BO32" s="25"/>
+      <c r="BP32" s="25"/>
+      <c r="BQ32" s="25"/>
+      <c r="BR32" s="25"/>
+      <c r="BS32" s="25"/>
+      <c r="BT32" s="25"/>
+      <c r="BU32" s="25"/>
+      <c r="BV32" s="25"/>
+      <c r="BW32" s="25"/>
+      <c r="BX32" s="25"/>
+      <c r="BY32" s="25"/>
+      <c r="BZ32" s="25"/>
+      <c r="CA32" s="25"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4154,27 +4160,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="16">
+      <c r="AP33" s="26">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="16"/>
-      <c r="AR33" s="16"/>
-      <c r="AS33" s="17" t="s">
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="17"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="17"/>
-      <c r="BB33" s="17"/>
-      <c r="BC33" s="17"/>
-      <c r="BD33" s="17"/>
-      <c r="BE33" s="17"/>
-      <c r="BF33" s="17"/>
+      <c r="AT33" s="27"/>
+      <c r="AU33" s="27"/>
+      <c r="AV33" s="27"/>
+      <c r="AW33" s="27"/>
+      <c r="AX33" s="27"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
+      <c r="BA33" s="27"/>
+      <c r="BB33" s="27"/>
+      <c r="BC33" s="27"/>
+      <c r="BD33" s="27"/>
+      <c r="BE33" s="27"/>
+      <c r="BF33" s="27"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4482,36 +4488,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-      <c r="V37" s="14"/>
-      <c r="W37" s="14"/>
-      <c r="X37" s="14"/>
-      <c r="Y37" s="14"/>
-      <c r="Z37" s="14"/>
-      <c r="AA37" s="14"/>
-      <c r="AB37" s="14"/>
-      <c r="AC37" s="14"/>
-      <c r="AD37" s="14"/>
-      <c r="AE37" s="15"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="30"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4575,36 +4581,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-      <c r="V38" s="14"/>
-      <c r="W38" s="14"/>
-      <c r="X38" s="14"/>
-      <c r="Y38" s="14"/>
-      <c r="Z38" s="14"/>
-      <c r="AA38" s="14"/>
-      <c r="AB38" s="14"/>
-      <c r="AC38" s="14"/>
-      <c r="AD38" s="14"/>
-      <c r="AE38" s="15"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="30"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4761,36 +4767,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14"/>
-      <c r="Y40" s="14"/>
-      <c r="Z40" s="14"/>
-      <c r="AA40" s="14"/>
-      <c r="AB40" s="14"/>
-      <c r="AC40" s="14"/>
-      <c r="AD40" s="14"/>
-      <c r="AE40" s="15"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="30"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4947,36 +4953,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="14"/>
-      <c r="Y42" s="14"/>
-      <c r="Z42" s="14"/>
-      <c r="AA42" s="14"/>
-      <c r="AB42" s="14"/>
-      <c r="AC42" s="14"/>
-      <c r="AD42" s="14"/>
-      <c r="AE42" s="15"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="30"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5040,36 +5046,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="15"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="30"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5133,36 +5139,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="14"/>
-      <c r="Y44" s="14"/>
-      <c r="Z44" s="14"/>
-      <c r="AA44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AC44" s="14"/>
-      <c r="AD44" s="14"/>
-      <c r="AE44" s="15"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="30"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -7636,8 +7642,774 @@
       <c r="BZ70" s="12"/>
       <c r="CA70" s="12"/>
     </row>
+    <row r="71" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A71" s="8">
+        <v>60</v>
+      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+      <c r="O71" s="9"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="9"/>
+      <c r="R71" s="9"/>
+      <c r="S71" s="9"/>
+      <c r="T71" s="9"/>
+      <c r="U71" s="9"/>
+      <c r="V71" s="9"/>
+      <c r="W71" s="9"/>
+      <c r="X71" s="9"/>
+      <c r="Y71" s="9"/>
+      <c r="Z71" s="9"/>
+      <c r="AA71" s="9"/>
+      <c r="AB71" s="9"/>
+      <c r="AC71" s="9"/>
+      <c r="AD71" s="9"/>
+      <c r="AE71" s="9"/>
+      <c r="AF71" s="10">
+        <v>43525</v>
+      </c>
+      <c r="AG71" s="10"/>
+      <c r="AH71" s="10"/>
+      <c r="AI71" s="10"/>
+      <c r="AJ71" s="10"/>
+      <c r="AK71" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL71" s="9"/>
+      <c r="AM71" s="9"/>
+      <c r="AN71" s="9"/>
+      <c r="AO71" s="9"/>
+      <c r="AP71" s="11">
+        <v>1</v>
+      </c>
+      <c r="AQ71" s="11"/>
+      <c r="AR71" s="11"/>
+      <c r="AS71" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT71" s="9"/>
+      <c r="AU71" s="9"/>
+      <c r="AV71" s="9"/>
+      <c r="AW71" s="9"/>
+      <c r="AX71" s="9"/>
+      <c r="AY71" s="9"/>
+      <c r="AZ71" s="9"/>
+      <c r="BA71" s="9"/>
+      <c r="BB71" s="9"/>
+      <c r="BC71" s="9"/>
+      <c r="BD71" s="9"/>
+      <c r="BE71" s="9"/>
+      <c r="BF71" s="9"/>
+      <c r="BG71" s="12"/>
+      <c r="BH71" s="12"/>
+      <c r="BI71" s="12"/>
+      <c r="BJ71" s="12"/>
+      <c r="BK71" s="12"/>
+      <c r="BL71" s="12"/>
+      <c r="BM71" s="12"/>
+      <c r="BN71" s="12"/>
+      <c r="BO71" s="12"/>
+      <c r="BP71" s="12"/>
+      <c r="BQ71" s="12"/>
+      <c r="BR71" s="12"/>
+      <c r="BS71" s="12"/>
+      <c r="BT71" s="12"/>
+      <c r="BU71" s="12"/>
+      <c r="BV71" s="12"/>
+      <c r="BW71" s="12"/>
+      <c r="BX71" s="12"/>
+      <c r="BY71" s="12"/>
+      <c r="BZ71" s="12"/>
+      <c r="CA71" s="12"/>
+    </row>
+    <row r="72" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A72" s="8">
+        <v>60</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+      <c r="O72" s="9"/>
+      <c r="P72" s="9"/>
+      <c r="Q72" s="9"/>
+      <c r="R72" s="9"/>
+      <c r="S72" s="9"/>
+      <c r="T72" s="9"/>
+      <c r="U72" s="9"/>
+      <c r="V72" s="9"/>
+      <c r="W72" s="9"/>
+      <c r="X72" s="9"/>
+      <c r="Y72" s="9"/>
+      <c r="Z72" s="9"/>
+      <c r="AA72" s="9"/>
+      <c r="AB72" s="9"/>
+      <c r="AC72" s="9"/>
+      <c r="AD72" s="9"/>
+      <c r="AE72" s="9"/>
+      <c r="AF72" s="10">
+        <v>43525</v>
+      </c>
+      <c r="AG72" s="10"/>
+      <c r="AH72" s="10"/>
+      <c r="AI72" s="10"/>
+      <c r="AJ72" s="10"/>
+      <c r="AK72" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL72" s="9"/>
+      <c r="AM72" s="9"/>
+      <c r="AN72" s="9"/>
+      <c r="AO72" s="9"/>
+      <c r="AP72" s="11">
+        <v>1</v>
+      </c>
+      <c r="AQ72" s="11"/>
+      <c r="AR72" s="11"/>
+      <c r="AS72" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT72" s="9"/>
+      <c r="AU72" s="9"/>
+      <c r="AV72" s="9"/>
+      <c r="AW72" s="9"/>
+      <c r="AX72" s="9"/>
+      <c r="AY72" s="9"/>
+      <c r="AZ72" s="9"/>
+      <c r="BA72" s="9"/>
+      <c r="BB72" s="9"/>
+      <c r="BC72" s="9"/>
+      <c r="BD72" s="9"/>
+      <c r="BE72" s="9"/>
+      <c r="BF72" s="9"/>
+      <c r="BG72" s="12"/>
+      <c r="BH72" s="12"/>
+      <c r="BI72" s="12"/>
+      <c r="BJ72" s="12"/>
+      <c r="BK72" s="12"/>
+      <c r="BL72" s="12"/>
+      <c r="BM72" s="12"/>
+      <c r="BN72" s="12"/>
+      <c r="BO72" s="12"/>
+      <c r="BP72" s="12"/>
+      <c r="BQ72" s="12"/>
+      <c r="BR72" s="12"/>
+      <c r="BS72" s="12"/>
+      <c r="BT72" s="12"/>
+      <c r="BU72" s="12"/>
+      <c r="BV72" s="12"/>
+      <c r="BW72" s="12"/>
+      <c r="BX72" s="12"/>
+      <c r="BY72" s="12"/>
+      <c r="BZ72" s="12"/>
+      <c r="CA72" s="12"/>
+    </row>
+    <row r="73" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A73" s="8">
+        <v>60</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="9"/>
+      <c r="R73" s="9"/>
+      <c r="S73" s="9"/>
+      <c r="T73" s="9"/>
+      <c r="U73" s="9"/>
+      <c r="V73" s="9"/>
+      <c r="W73" s="9"/>
+      <c r="X73" s="9"/>
+      <c r="Y73" s="9"/>
+      <c r="Z73" s="9"/>
+      <c r="AA73" s="9"/>
+      <c r="AB73" s="9"/>
+      <c r="AC73" s="9"/>
+      <c r="AD73" s="9"/>
+      <c r="AE73" s="9"/>
+      <c r="AF73" s="10">
+        <v>43525</v>
+      </c>
+      <c r="AG73" s="10"/>
+      <c r="AH73" s="10"/>
+      <c r="AI73" s="10"/>
+      <c r="AJ73" s="10"/>
+      <c r="AK73" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL73" s="9"/>
+      <c r="AM73" s="9"/>
+      <c r="AN73" s="9"/>
+      <c r="AO73" s="9"/>
+      <c r="AP73" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="AQ73" s="11"/>
+      <c r="AR73" s="11"/>
+      <c r="AS73" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT73" s="9"/>
+      <c r="AU73" s="9"/>
+      <c r="AV73" s="9"/>
+      <c r="AW73" s="9"/>
+      <c r="AX73" s="9"/>
+      <c r="AY73" s="9"/>
+      <c r="AZ73" s="9"/>
+      <c r="BA73" s="9"/>
+      <c r="BB73" s="9"/>
+      <c r="BC73" s="9"/>
+      <c r="BD73" s="9"/>
+      <c r="BE73" s="9"/>
+      <c r="BF73" s="9"/>
+      <c r="BG73" s="12"/>
+      <c r="BH73" s="12"/>
+      <c r="BI73" s="12"/>
+      <c r="BJ73" s="12"/>
+      <c r="BK73" s="12"/>
+      <c r="BL73" s="12"/>
+      <c r="BM73" s="12"/>
+      <c r="BN73" s="12"/>
+      <c r="BO73" s="12"/>
+      <c r="BP73" s="12"/>
+      <c r="BQ73" s="12"/>
+      <c r="BR73" s="12"/>
+      <c r="BS73" s="12"/>
+      <c r="BT73" s="12"/>
+      <c r="BU73" s="12"/>
+      <c r="BV73" s="12"/>
+      <c r="BW73" s="12"/>
+      <c r="BX73" s="12"/>
+      <c r="BY73" s="12"/>
+      <c r="BZ73" s="12"/>
+      <c r="CA73" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="490">
+  <mergeCells count="511">
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -7662,475 +8434,9 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C73">
       <formula1>"!,?"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8149,7 +8455,7 @@
           <x14:formula1>
             <xm:f>Info!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>AK3:AO70</xm:sqref>
+          <xm:sqref>AK3:AO73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -8158,7 +8464,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>AS2:BF70</xm:sqref>
+          <xm:sqref>AS2:BF73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Báo cáo ngày 5/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="96">
   <si>
     <t>No.</t>
   </si>
@@ -306,6 +306,9 @@
   <si>
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Gộp bước 3 (mapping column) vào bước 2 (detail job)</t>
   </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Tạo thêm trường khớp trường ở phần mapping</t>
+  </si>
 </sst>
 </file>
 
@@ -572,14 +575,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,6 +595,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +708,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1096,7 +1099,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1108,7 +1111,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121:CA123"/>
+      <selection pane="bottomLeft" activeCell="AS79" sqref="AS79:BF79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,192 +1126,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="23" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="24" t="s">
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="22" t="s">
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="25" t="s">
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="25"/>
-      <c r="BJ1" s="25"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="25"/>
-      <c r="BO1" s="25"/>
-      <c r="BP1" s="25"/>
-      <c r="BQ1" s="25"/>
-      <c r="BR1" s="25"/>
-      <c r="BS1" s="25"/>
-      <c r="BT1" s="25"/>
-      <c r="BU1" s="25"/>
-      <c r="BV1" s="25"/>
-      <c r="BW1" s="25"/>
-      <c r="BX1" s="25"/>
-      <c r="BY1" s="25"/>
-      <c r="BZ1" s="25"/>
-      <c r="CA1" s="25"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="21">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4029,43 +4032,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="18"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
-      <c r="AD32" s="18"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="19">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="24">
         <v>43293</v>
       </c>
-      <c r="AG32" s="19"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="19"/>
-      <c r="AJ32" s="19"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4094,27 +4097,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="20"/>
-      <c r="BH32" s="20"/>
-      <c r="BI32" s="20"/>
-      <c r="BJ32" s="20"/>
-      <c r="BK32" s="20"/>
-      <c r="BL32" s="20"/>
-      <c r="BM32" s="20"/>
-      <c r="BN32" s="20"/>
-      <c r="BO32" s="20"/>
-      <c r="BP32" s="20"/>
-      <c r="BQ32" s="20"/>
-      <c r="BR32" s="20"/>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="BV32" s="20"/>
-      <c r="BW32" s="20"/>
-      <c r="BX32" s="20"/>
-      <c r="BY32" s="20"/>
-      <c r="BZ32" s="20"/>
-      <c r="CA32" s="20"/>
+      <c r="BG32" s="25"/>
+      <c r="BH32" s="25"/>
+      <c r="BI32" s="25"/>
+      <c r="BJ32" s="25"/>
+      <c r="BK32" s="25"/>
+      <c r="BL32" s="25"/>
+      <c r="BM32" s="25"/>
+      <c r="BN32" s="25"/>
+      <c r="BO32" s="25"/>
+      <c r="BP32" s="25"/>
+      <c r="BQ32" s="25"/>
+      <c r="BR32" s="25"/>
+      <c r="BS32" s="25"/>
+      <c r="BT32" s="25"/>
+      <c r="BU32" s="25"/>
+      <c r="BV32" s="25"/>
+      <c r="BW32" s="25"/>
+      <c r="BX32" s="25"/>
+      <c r="BY32" s="25"/>
+      <c r="BZ32" s="25"/>
+      <c r="CA32" s="25"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4166,27 +4169,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="16">
+      <c r="AP33" s="26">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="16"/>
-      <c r="AR33" s="16"/>
-      <c r="AS33" s="17" t="s">
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="17"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="17"/>
-      <c r="BB33" s="17"/>
-      <c r="BC33" s="17"/>
-      <c r="BD33" s="17"/>
-      <c r="BE33" s="17"/>
-      <c r="BF33" s="17"/>
+      <c r="AT33" s="27"/>
+      <c r="AU33" s="27"/>
+      <c r="AV33" s="27"/>
+      <c r="AW33" s="27"/>
+      <c r="AX33" s="27"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
+      <c r="BA33" s="27"/>
+      <c r="BB33" s="27"/>
+      <c r="BC33" s="27"/>
+      <c r="BD33" s="27"/>
+      <c r="BE33" s="27"/>
+      <c r="BF33" s="27"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4494,36 +4497,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-      <c r="V37" s="14"/>
-      <c r="W37" s="14"/>
-      <c r="X37" s="14"/>
-      <c r="Y37" s="14"/>
-      <c r="Z37" s="14"/>
-      <c r="AA37" s="14"/>
-      <c r="AB37" s="14"/>
-      <c r="AC37" s="14"/>
-      <c r="AD37" s="14"/>
-      <c r="AE37" s="15"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="30"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4587,36 +4590,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-      <c r="V38" s="14"/>
-      <c r="W38" s="14"/>
-      <c r="X38" s="14"/>
-      <c r="Y38" s="14"/>
-      <c r="Z38" s="14"/>
-      <c r="AA38" s="14"/>
-      <c r="AB38" s="14"/>
-      <c r="AC38" s="14"/>
-      <c r="AD38" s="14"/>
-      <c r="AE38" s="15"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="30"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4773,36 +4776,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14"/>
-      <c r="Y40" s="14"/>
-      <c r="Z40" s="14"/>
-      <c r="AA40" s="14"/>
-      <c r="AB40" s="14"/>
-      <c r="AC40" s="14"/>
-      <c r="AD40" s="14"/>
-      <c r="AE40" s="15"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="30"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4959,36 +4962,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="14"/>
-      <c r="Y42" s="14"/>
-      <c r="Z42" s="14"/>
-      <c r="AA42" s="14"/>
-      <c r="AB42" s="14"/>
-      <c r="AC42" s="14"/>
-      <c r="AD42" s="14"/>
-      <c r="AE42" s="15"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="30"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5052,36 +5055,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="15"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="30"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5145,36 +5148,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="14"/>
-      <c r="Y44" s="14"/>
-      <c r="Z44" s="14"/>
-      <c r="AA44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AC44" s="14"/>
-      <c r="AD44" s="14"/>
-      <c r="AE44" s="15"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="30"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -8119,7 +8122,9 @@
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="5"/>
-      <c r="D76" s="9"/>
+      <c r="D76" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
@@ -8147,20 +8152,28 @@
       <c r="AC76" s="9"/>
       <c r="AD76" s="9"/>
       <c r="AE76" s="9"/>
-      <c r="AF76" s="10"/>
+      <c r="AF76" s="10">
+        <v>43586</v>
+      </c>
       <c r="AG76" s="10"/>
       <c r="AH76" s="10"/>
       <c r="AI76" s="10"/>
       <c r="AJ76" s="10"/>
-      <c r="AK76" s="9"/>
+      <c r="AK76" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL76" s="9"/>
       <c r="AM76" s="9"/>
       <c r="AN76" s="9"/>
       <c r="AO76" s="9"/>
-      <c r="AP76" s="11"/>
+      <c r="AP76" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ76" s="11"/>
       <c r="AR76" s="11"/>
-      <c r="AS76" s="9"/>
+      <c r="AS76" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT76" s="9"/>
       <c r="AU76" s="9"/>
       <c r="AV76" s="9"/>
@@ -8202,7 +8215,9 @@
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="5"/>
-      <c r="D77" s="9"/>
+      <c r="D77" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
@@ -8230,20 +8245,28 @@
       <c r="AC77" s="9"/>
       <c r="AD77" s="9"/>
       <c r="AE77" s="9"/>
-      <c r="AF77" s="10"/>
+      <c r="AF77" s="10">
+        <v>43586</v>
+      </c>
       <c r="AG77" s="10"/>
       <c r="AH77" s="10"/>
       <c r="AI77" s="10"/>
       <c r="AJ77" s="10"/>
-      <c r="AK77" s="9"/>
+      <c r="AK77" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL77" s="9"/>
       <c r="AM77" s="9"/>
       <c r="AN77" s="9"/>
       <c r="AO77" s="9"/>
-      <c r="AP77" s="11"/>
+      <c r="AP77" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ77" s="11"/>
       <c r="AR77" s="11"/>
-      <c r="AS77" s="9"/>
+      <c r="AS77" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT77" s="9"/>
       <c r="AU77" s="9"/>
       <c r="AV77" s="9"/>
@@ -12099,356 +12122,493 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12473,493 +12633,356 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Báo cáo ngày 7/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="98">
   <si>
     <t>No.</t>
   </si>
@@ -309,6 +309,12 @@
   <si>
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Tạo thêm trường khớp trường ở phần mapping</t>
   </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Tạo mới điều kiện có mapping table</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Thêm mới dòng trong table mapping - Xử lý select2</t>
+  </si>
 </sst>
 </file>
 
@@ -575,6 +581,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -595,14 +609,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +714,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1099,7 +1105,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1111,7 +1117,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS79" sqref="AS79:BF79"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79:AE79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,192 +1132,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="15" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="14" t="s">
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="16" t="s">
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="14" t="s">
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
-      <c r="BC1" s="14"/>
-      <c r="BD1" s="14"/>
-      <c r="BE1" s="14"/>
-      <c r="BF1" s="14"/>
-      <c r="BG1" s="17" t="s">
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="17"/>
-      <c r="BP1" s="17"/>
-      <c r="BQ1" s="17"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="17"/>
-      <c r="BT1" s="17"/>
-      <c r="BU1" s="17"/>
-      <c r="BV1" s="17"/>
-      <c r="BW1" s="17"/>
-      <c r="BX1" s="17"/>
-      <c r="BY1" s="17"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="20" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="19" t="s">
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="21">
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="29">
         <v>1</v>
       </c>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="19" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
-      <c r="BN2" s="22"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2" s="22"/>
-      <c r="BQ2" s="22"/>
-      <c r="BR2" s="22"/>
-      <c r="BS2" s="22"/>
-      <c r="BT2" s="22"/>
-      <c r="BU2" s="22"/>
-      <c r="BV2" s="22"/>
-      <c r="BW2" s="22"/>
-      <c r="BX2" s="22"/>
-      <c r="BY2" s="22"/>
-      <c r="BZ2" s="22"/>
-      <c r="CA2" s="22"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="30"/>
+      <c r="BJ2" s="30"/>
+      <c r="BK2" s="30"/>
+      <c r="BL2" s="30"/>
+      <c r="BM2" s="30"/>
+      <c r="BN2" s="30"/>
+      <c r="BO2" s="30"/>
+      <c r="BP2" s="30"/>
+      <c r="BQ2" s="30"/>
+      <c r="BR2" s="30"/>
+      <c r="BS2" s="30"/>
+      <c r="BT2" s="30"/>
+      <c r="BU2" s="30"/>
+      <c r="BV2" s="30"/>
+      <c r="BW2" s="30"/>
+      <c r="BX2" s="30"/>
+      <c r="BY2" s="30"/>
+      <c r="BZ2" s="30"/>
+      <c r="CA2" s="30"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4032,43 +4038,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="23"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="23"/>
-      <c r="AD32" s="23"/>
-      <c r="AE32" s="23"/>
-      <c r="AF32" s="24">
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+      <c r="V32" s="18"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
+      <c r="AA32" s="18"/>
+      <c r="AB32" s="18"/>
+      <c r="AC32" s="18"/>
+      <c r="AD32" s="18"/>
+      <c r="AE32" s="18"/>
+      <c r="AF32" s="19">
         <v>43293</v>
       </c>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="24"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="24"/>
+      <c r="AG32" s="19"/>
+      <c r="AH32" s="19"/>
+      <c r="AI32" s="19"/>
+      <c r="AJ32" s="19"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4097,27 +4103,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="25"/>
-      <c r="BH32" s="25"/>
-      <c r="BI32" s="25"/>
-      <c r="BJ32" s="25"/>
-      <c r="BK32" s="25"/>
-      <c r="BL32" s="25"/>
-      <c r="BM32" s="25"/>
-      <c r="BN32" s="25"/>
-      <c r="BO32" s="25"/>
-      <c r="BP32" s="25"/>
-      <c r="BQ32" s="25"/>
-      <c r="BR32" s="25"/>
-      <c r="BS32" s="25"/>
-      <c r="BT32" s="25"/>
-      <c r="BU32" s="25"/>
-      <c r="BV32" s="25"/>
-      <c r="BW32" s="25"/>
-      <c r="BX32" s="25"/>
-      <c r="BY32" s="25"/>
-      <c r="BZ32" s="25"/>
-      <c r="CA32" s="25"/>
+      <c r="BG32" s="20"/>
+      <c r="BH32" s="20"/>
+      <c r="BI32" s="20"/>
+      <c r="BJ32" s="20"/>
+      <c r="BK32" s="20"/>
+      <c r="BL32" s="20"/>
+      <c r="BM32" s="20"/>
+      <c r="BN32" s="20"/>
+      <c r="BO32" s="20"/>
+      <c r="BP32" s="20"/>
+      <c r="BQ32" s="20"/>
+      <c r="BR32" s="20"/>
+      <c r="BS32" s="20"/>
+      <c r="BT32" s="20"/>
+      <c r="BU32" s="20"/>
+      <c r="BV32" s="20"/>
+      <c r="BW32" s="20"/>
+      <c r="BX32" s="20"/>
+      <c r="BY32" s="20"/>
+      <c r="BZ32" s="20"/>
+      <c r="CA32" s="20"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4169,27 +4175,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="26">
+      <c r="AP33" s="16">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="27" t="s">
+      <c r="AQ33" s="16"/>
+      <c r="AR33" s="16"/>
+      <c r="AS33" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="27"/>
-      <c r="AU33" s="27"/>
-      <c r="AV33" s="27"/>
-      <c r="AW33" s="27"/>
-      <c r="AX33" s="27"/>
-      <c r="AY33" s="27"/>
-      <c r="AZ33" s="27"/>
-      <c r="BA33" s="27"/>
-      <c r="BB33" s="27"/>
-      <c r="BC33" s="27"/>
-      <c r="BD33" s="27"/>
-      <c r="BE33" s="27"/>
-      <c r="BF33" s="27"/>
+      <c r="AT33" s="17"/>
+      <c r="AU33" s="17"/>
+      <c r="AV33" s="17"/>
+      <c r="AW33" s="17"/>
+      <c r="AX33" s="17"/>
+      <c r="AY33" s="17"/>
+      <c r="AZ33" s="17"/>
+      <c r="BA33" s="17"/>
+      <c r="BB33" s="17"/>
+      <c r="BC33" s="17"/>
+      <c r="BD33" s="17"/>
+      <c r="BE33" s="17"/>
+      <c r="BF33" s="17"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4497,36 +4503,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="29"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="30"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="15"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4590,36 +4596,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="30"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="14"/>
+      <c r="AA38" s="14"/>
+      <c r="AB38" s="14"/>
+      <c r="AC38" s="14"/>
+      <c r="AD38" s="14"/>
+      <c r="AE38" s="15"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4776,36 +4782,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="30"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="14"/>
+      <c r="AA40" s="14"/>
+      <c r="AB40" s="14"/>
+      <c r="AC40" s="14"/>
+      <c r="AD40" s="14"/>
+      <c r="AE40" s="15"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4962,36 +4968,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="30"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14"/>
+      <c r="AB42" s="14"/>
+      <c r="AC42" s="14"/>
+      <c r="AD42" s="14"/>
+      <c r="AE42" s="15"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5055,36 +5061,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="30"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="15"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5148,36 +5154,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="30"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="14"/>
+      <c r="Z44" s="14"/>
+      <c r="AA44" s="14"/>
+      <c r="AB44" s="14"/>
+      <c r="AC44" s="14"/>
+      <c r="AD44" s="14"/>
+      <c r="AE44" s="15"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -8308,7 +8314,9 @@
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="5"/>
-      <c r="D78" s="9"/>
+      <c r="D78" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
@@ -8336,20 +8344,28 @@
       <c r="AC78" s="9"/>
       <c r="AD78" s="9"/>
       <c r="AE78" s="9"/>
-      <c r="AF78" s="10"/>
+      <c r="AF78" s="10">
+        <v>43647</v>
+      </c>
       <c r="AG78" s="10"/>
       <c r="AH78" s="10"/>
       <c r="AI78" s="10"/>
       <c r="AJ78" s="10"/>
-      <c r="AK78" s="9"/>
+      <c r="AK78" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL78" s="9"/>
       <c r="AM78" s="9"/>
       <c r="AN78" s="9"/>
       <c r="AO78" s="9"/>
-      <c r="AP78" s="11"/>
+      <c r="AP78" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ78" s="11"/>
       <c r="AR78" s="11"/>
-      <c r="AS78" s="9"/>
+      <c r="AS78" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT78" s="9"/>
       <c r="AU78" s="9"/>
       <c r="AV78" s="9"/>
@@ -8391,7 +8407,9 @@
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="5"/>
-      <c r="D79" s="9"/>
+      <c r="D79" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
@@ -8419,20 +8437,28 @@
       <c r="AC79" s="9"/>
       <c r="AD79" s="9"/>
       <c r="AE79" s="9"/>
-      <c r="AF79" s="10"/>
+      <c r="AF79" s="10">
+        <v>43647</v>
+      </c>
       <c r="AG79" s="10"/>
       <c r="AH79" s="10"/>
       <c r="AI79" s="10"/>
       <c r="AJ79" s="10"/>
-      <c r="AK79" s="9"/>
+      <c r="AK79" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL79" s="9"/>
       <c r="AM79" s="9"/>
       <c r="AN79" s="9"/>
       <c r="AO79" s="9"/>
-      <c r="AP79" s="11"/>
+      <c r="AP79" s="11">
+        <v>0.3</v>
+      </c>
       <c r="AQ79" s="11"/>
       <c r="AR79" s="11"/>
-      <c r="AS79" s="9"/>
+      <c r="AS79" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT79" s="9"/>
       <c r="AU79" s="9"/>
       <c r="AV79" s="9"/>
@@ -12122,493 +12148,356 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12633,356 +12522,493 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Báo cáo ngày 8/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="102">
   <si>
     <t>No.</t>
   </si>
@@ -315,6 +315,18 @@
   <si>
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Thêm mới dòng trong table mapping - Xử lý select2</t>
   </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Tạo mới điều kiện có mapping table - Thêm,sửa select2 vào các select đã clone</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Test</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Lưu vào session</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Thêm việc kiểm tra kết nối quan hệ (referent)</t>
+  </si>
 </sst>
 </file>
 
@@ -581,14 +593,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,6 +613,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,7 +726,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1105,7 +1117,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1116,8 +1128,8 @@
   <dimension ref="A1:CA123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79:AE79"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D85" sqref="D85:AE85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,192 +1144,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="23" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="24" t="s">
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="22" t="s">
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="25" t="s">
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="25"/>
-      <c r="BJ1" s="25"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="25"/>
-      <c r="BO1" s="25"/>
-      <c r="BP1" s="25"/>
-      <c r="BQ1" s="25"/>
-      <c r="BR1" s="25"/>
-      <c r="BS1" s="25"/>
-      <c r="BT1" s="25"/>
-      <c r="BU1" s="25"/>
-      <c r="BV1" s="25"/>
-      <c r="BW1" s="25"/>
-      <c r="BX1" s="25"/>
-      <c r="BY1" s="25"/>
-      <c r="BZ1" s="25"/>
-      <c r="CA1" s="25"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="21">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4038,43 +4050,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="18"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
-      <c r="AD32" s="18"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="19">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="24">
         <v>43293</v>
       </c>
-      <c r="AG32" s="19"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="19"/>
-      <c r="AJ32" s="19"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4103,27 +4115,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="20"/>
-      <c r="BH32" s="20"/>
-      <c r="BI32" s="20"/>
-      <c r="BJ32" s="20"/>
-      <c r="BK32" s="20"/>
-      <c r="BL32" s="20"/>
-      <c r="BM32" s="20"/>
-      <c r="BN32" s="20"/>
-      <c r="BO32" s="20"/>
-      <c r="BP32" s="20"/>
-      <c r="BQ32" s="20"/>
-      <c r="BR32" s="20"/>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="BV32" s="20"/>
-      <c r="BW32" s="20"/>
-      <c r="BX32" s="20"/>
-      <c r="BY32" s="20"/>
-      <c r="BZ32" s="20"/>
-      <c r="CA32" s="20"/>
+      <c r="BG32" s="25"/>
+      <c r="BH32" s="25"/>
+      <c r="BI32" s="25"/>
+      <c r="BJ32" s="25"/>
+      <c r="BK32" s="25"/>
+      <c r="BL32" s="25"/>
+      <c r="BM32" s="25"/>
+      <c r="BN32" s="25"/>
+      <c r="BO32" s="25"/>
+      <c r="BP32" s="25"/>
+      <c r="BQ32" s="25"/>
+      <c r="BR32" s="25"/>
+      <c r="BS32" s="25"/>
+      <c r="BT32" s="25"/>
+      <c r="BU32" s="25"/>
+      <c r="BV32" s="25"/>
+      <c r="BW32" s="25"/>
+      <c r="BX32" s="25"/>
+      <c r="BY32" s="25"/>
+      <c r="BZ32" s="25"/>
+      <c r="CA32" s="25"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4175,27 +4187,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="16">
+      <c r="AP33" s="26">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="16"/>
-      <c r="AR33" s="16"/>
-      <c r="AS33" s="17" t="s">
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="17"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="17"/>
-      <c r="BB33" s="17"/>
-      <c r="BC33" s="17"/>
-      <c r="BD33" s="17"/>
-      <c r="BE33" s="17"/>
-      <c r="BF33" s="17"/>
+      <c r="AT33" s="27"/>
+      <c r="AU33" s="27"/>
+      <c r="AV33" s="27"/>
+      <c r="AW33" s="27"/>
+      <c r="AX33" s="27"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
+      <c r="BA33" s="27"/>
+      <c r="BB33" s="27"/>
+      <c r="BC33" s="27"/>
+      <c r="BD33" s="27"/>
+      <c r="BE33" s="27"/>
+      <c r="BF33" s="27"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4503,36 +4515,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-      <c r="V37" s="14"/>
-      <c r="W37" s="14"/>
-      <c r="X37" s="14"/>
-      <c r="Y37" s="14"/>
-      <c r="Z37" s="14"/>
-      <c r="AA37" s="14"/>
-      <c r="AB37" s="14"/>
-      <c r="AC37" s="14"/>
-      <c r="AD37" s="14"/>
-      <c r="AE37" s="15"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="30"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4596,36 +4608,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-      <c r="V38" s="14"/>
-      <c r="W38" s="14"/>
-      <c r="X38" s="14"/>
-      <c r="Y38" s="14"/>
-      <c r="Z38" s="14"/>
-      <c r="AA38" s="14"/>
-      <c r="AB38" s="14"/>
-      <c r="AC38" s="14"/>
-      <c r="AD38" s="14"/>
-      <c r="AE38" s="15"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="30"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4782,36 +4794,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14"/>
-      <c r="Y40" s="14"/>
-      <c r="Z40" s="14"/>
-      <c r="AA40" s="14"/>
-      <c r="AB40" s="14"/>
-      <c r="AC40" s="14"/>
-      <c r="AD40" s="14"/>
-      <c r="AE40" s="15"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="30"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4968,36 +4980,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="14"/>
-      <c r="Y42" s="14"/>
-      <c r="Z42" s="14"/>
-      <c r="AA42" s="14"/>
-      <c r="AB42" s="14"/>
-      <c r="AC42" s="14"/>
-      <c r="AD42" s="14"/>
-      <c r="AE42" s="15"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="30"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5061,36 +5073,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="15"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="30"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5154,36 +5166,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="14"/>
-      <c r="Y44" s="14"/>
-      <c r="Z44" s="14"/>
-      <c r="AA44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AC44" s="14"/>
-      <c r="AD44" s="14"/>
-      <c r="AE44" s="15"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="30"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -8500,7 +8512,9 @@
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="5"/>
-      <c r="D80" s="9"/>
+      <c r="D80" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
@@ -8528,20 +8542,28 @@
       <c r="AC80" s="9"/>
       <c r="AD80" s="9"/>
       <c r="AE80" s="9"/>
-      <c r="AF80" s="10"/>
+      <c r="AF80" s="10">
+        <v>43678</v>
+      </c>
       <c r="AG80" s="10"/>
       <c r="AH80" s="10"/>
       <c r="AI80" s="10"/>
       <c r="AJ80" s="10"/>
-      <c r="AK80" s="9"/>
+      <c r="AK80" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL80" s="9"/>
       <c r="AM80" s="9"/>
       <c r="AN80" s="9"/>
       <c r="AO80" s="9"/>
-      <c r="AP80" s="11"/>
+      <c r="AP80" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ80" s="11"/>
       <c r="AR80" s="11"/>
-      <c r="AS80" s="9"/>
+      <c r="AS80" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT80" s="9"/>
       <c r="AU80" s="9"/>
       <c r="AV80" s="9"/>
@@ -8583,7 +8605,9 @@
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="5"/>
-      <c r="D81" s="9"/>
+      <c r="D81" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
@@ -8611,20 +8635,28 @@
       <c r="AC81" s="9"/>
       <c r="AD81" s="9"/>
       <c r="AE81" s="9"/>
-      <c r="AF81" s="10"/>
+      <c r="AF81" s="10">
+        <v>43678</v>
+      </c>
       <c r="AG81" s="10"/>
       <c r="AH81" s="10"/>
       <c r="AI81" s="10"/>
       <c r="AJ81" s="10"/>
-      <c r="AK81" s="9"/>
+      <c r="AK81" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL81" s="9"/>
       <c r="AM81" s="9"/>
       <c r="AN81" s="9"/>
       <c r="AO81" s="9"/>
-      <c r="AP81" s="11"/>
+      <c r="AP81" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ81" s="11"/>
       <c r="AR81" s="11"/>
-      <c r="AS81" s="9"/>
+      <c r="AS81" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT81" s="9"/>
       <c r="AU81" s="9"/>
       <c r="AV81" s="9"/>
@@ -8666,7 +8698,9 @@
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="5"/>
-      <c r="D82" s="9"/>
+      <c r="D82" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
@@ -8694,20 +8728,28 @@
       <c r="AC82" s="9"/>
       <c r="AD82" s="9"/>
       <c r="AE82" s="9"/>
-      <c r="AF82" s="10"/>
+      <c r="AF82" s="10">
+        <v>43678</v>
+      </c>
       <c r="AG82" s="10"/>
       <c r="AH82" s="10"/>
       <c r="AI82" s="10"/>
       <c r="AJ82" s="10"/>
-      <c r="AK82" s="9"/>
+      <c r="AK82" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL82" s="9"/>
       <c r="AM82" s="9"/>
       <c r="AN82" s="9"/>
       <c r="AO82" s="9"/>
-      <c r="AP82" s="11"/>
+      <c r="AP82" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ82" s="11"/>
       <c r="AR82" s="11"/>
-      <c r="AS82" s="9"/>
+      <c r="AS82" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT82" s="9"/>
       <c r="AU82" s="9"/>
       <c r="AV82" s="9"/>
@@ -8749,7 +8791,9 @@
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="5"/>
-      <c r="D83" s="9"/>
+      <c r="D83" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
@@ -8777,20 +8821,28 @@
       <c r="AC83" s="9"/>
       <c r="AD83" s="9"/>
       <c r="AE83" s="9"/>
-      <c r="AF83" s="10"/>
+      <c r="AF83" s="10">
+        <v>43678</v>
+      </c>
       <c r="AG83" s="10"/>
       <c r="AH83" s="10"/>
       <c r="AI83" s="10"/>
       <c r="AJ83" s="10"/>
-      <c r="AK83" s="9"/>
+      <c r="AK83" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL83" s="9"/>
       <c r="AM83" s="9"/>
       <c r="AN83" s="9"/>
       <c r="AO83" s="9"/>
-      <c r="AP83" s="11"/>
+      <c r="AP83" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ83" s="11"/>
       <c r="AR83" s="11"/>
-      <c r="AS83" s="9"/>
+      <c r="AS83" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT83" s="9"/>
       <c r="AU83" s="9"/>
       <c r="AV83" s="9"/>
@@ -8832,7 +8884,9 @@
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="5"/>
-      <c r="D84" s="9"/>
+      <c r="D84" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
@@ -8860,20 +8914,28 @@
       <c r="AC84" s="9"/>
       <c r="AD84" s="9"/>
       <c r="AE84" s="9"/>
-      <c r="AF84" s="10"/>
+      <c r="AF84" s="10">
+        <v>43678</v>
+      </c>
       <c r="AG84" s="10"/>
       <c r="AH84" s="10"/>
       <c r="AI84" s="10"/>
       <c r="AJ84" s="10"/>
-      <c r="AK84" s="9"/>
+      <c r="AK84" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL84" s="9"/>
       <c r="AM84" s="9"/>
       <c r="AN84" s="9"/>
       <c r="AO84" s="9"/>
-      <c r="AP84" s="11"/>
+      <c r="AP84" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ84" s="11"/>
       <c r="AR84" s="11"/>
-      <c r="AS84" s="9"/>
+      <c r="AS84" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT84" s="9"/>
       <c r="AU84" s="9"/>
       <c r="AV84" s="9"/>
@@ -12148,356 +12210,493 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12522,493 +12721,356 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Báo cáo ngày 9/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="104">
   <si>
     <t>No.</t>
   </si>
@@ -322,10 +322,16 @@
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Test</t>
   </si>
   <si>
-    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Lưu vào session</t>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Thêm việc kiểm tra kết nối quan hệ (referent)</t>
   </si>
   <si>
-    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Thêm việc kiểm tra kết nối quan hệ (referent)</t>
+    <t xml:space="preserve">Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Lưu vào session </t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Chỉnh sửa giao diện</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Đổ dữ liệu  mapping vào session</t>
   </si>
 </sst>
 </file>
@@ -593,6 +599,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -613,14 +627,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +732,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1117,7 +1123,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1128,8 +1134,8 @@
   <dimension ref="A1:CA123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D85" sqref="D85:AE85"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D87" sqref="D87:AE87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,192 +1150,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="15" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="14" t="s">
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="16" t="s">
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="14" t="s">
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
-      <c r="BC1" s="14"/>
-      <c r="BD1" s="14"/>
-      <c r="BE1" s="14"/>
-      <c r="BF1" s="14"/>
-      <c r="BG1" s="17" t="s">
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="17"/>
-      <c r="BP1" s="17"/>
-      <c r="BQ1" s="17"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="17"/>
-      <c r="BT1" s="17"/>
-      <c r="BU1" s="17"/>
-      <c r="BV1" s="17"/>
-      <c r="BW1" s="17"/>
-      <c r="BX1" s="17"/>
-      <c r="BY1" s="17"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="20" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="19" t="s">
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="21">
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="29">
         <v>1</v>
       </c>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="19" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
-      <c r="BN2" s="22"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2" s="22"/>
-      <c r="BQ2" s="22"/>
-      <c r="BR2" s="22"/>
-      <c r="BS2" s="22"/>
-      <c r="BT2" s="22"/>
-      <c r="BU2" s="22"/>
-      <c r="BV2" s="22"/>
-      <c r="BW2" s="22"/>
-      <c r="BX2" s="22"/>
-      <c r="BY2" s="22"/>
-      <c r="BZ2" s="22"/>
-      <c r="CA2" s="22"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="30"/>
+      <c r="BJ2" s="30"/>
+      <c r="BK2" s="30"/>
+      <c r="BL2" s="30"/>
+      <c r="BM2" s="30"/>
+      <c r="BN2" s="30"/>
+      <c r="BO2" s="30"/>
+      <c r="BP2" s="30"/>
+      <c r="BQ2" s="30"/>
+      <c r="BR2" s="30"/>
+      <c r="BS2" s="30"/>
+      <c r="BT2" s="30"/>
+      <c r="BU2" s="30"/>
+      <c r="BV2" s="30"/>
+      <c r="BW2" s="30"/>
+      <c r="BX2" s="30"/>
+      <c r="BY2" s="30"/>
+      <c r="BZ2" s="30"/>
+      <c r="CA2" s="30"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4050,43 +4056,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="23"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="23"/>
-      <c r="AD32" s="23"/>
-      <c r="AE32" s="23"/>
-      <c r="AF32" s="24">
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+      <c r="V32" s="18"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
+      <c r="AA32" s="18"/>
+      <c r="AB32" s="18"/>
+      <c r="AC32" s="18"/>
+      <c r="AD32" s="18"/>
+      <c r="AE32" s="18"/>
+      <c r="AF32" s="19">
         <v>43293</v>
       </c>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="24"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="24"/>
+      <c r="AG32" s="19"/>
+      <c r="AH32" s="19"/>
+      <c r="AI32" s="19"/>
+      <c r="AJ32" s="19"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4115,27 +4121,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="25"/>
-      <c r="BH32" s="25"/>
-      <c r="BI32" s="25"/>
-      <c r="BJ32" s="25"/>
-      <c r="BK32" s="25"/>
-      <c r="BL32" s="25"/>
-      <c r="BM32" s="25"/>
-      <c r="BN32" s="25"/>
-      <c r="BO32" s="25"/>
-      <c r="BP32" s="25"/>
-      <c r="BQ32" s="25"/>
-      <c r="BR32" s="25"/>
-      <c r="BS32" s="25"/>
-      <c r="BT32" s="25"/>
-      <c r="BU32" s="25"/>
-      <c r="BV32" s="25"/>
-      <c r="BW32" s="25"/>
-      <c r="BX32" s="25"/>
-      <c r="BY32" s="25"/>
-      <c r="BZ32" s="25"/>
-      <c r="CA32" s="25"/>
+      <c r="BG32" s="20"/>
+      <c r="BH32" s="20"/>
+      <c r="BI32" s="20"/>
+      <c r="BJ32" s="20"/>
+      <c r="BK32" s="20"/>
+      <c r="BL32" s="20"/>
+      <c r="BM32" s="20"/>
+      <c r="BN32" s="20"/>
+      <c r="BO32" s="20"/>
+      <c r="BP32" s="20"/>
+      <c r="BQ32" s="20"/>
+      <c r="BR32" s="20"/>
+      <c r="BS32" s="20"/>
+      <c r="BT32" s="20"/>
+      <c r="BU32" s="20"/>
+      <c r="BV32" s="20"/>
+      <c r="BW32" s="20"/>
+      <c r="BX32" s="20"/>
+      <c r="BY32" s="20"/>
+      <c r="BZ32" s="20"/>
+      <c r="CA32" s="20"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4187,27 +4193,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="26">
+      <c r="AP33" s="16">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="27" t="s">
+      <c r="AQ33" s="16"/>
+      <c r="AR33" s="16"/>
+      <c r="AS33" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="27"/>
-      <c r="AU33" s="27"/>
-      <c r="AV33" s="27"/>
-      <c r="AW33" s="27"/>
-      <c r="AX33" s="27"/>
-      <c r="AY33" s="27"/>
-      <c r="AZ33" s="27"/>
-      <c r="BA33" s="27"/>
-      <c r="BB33" s="27"/>
-      <c r="BC33" s="27"/>
-      <c r="BD33" s="27"/>
-      <c r="BE33" s="27"/>
-      <c r="BF33" s="27"/>
+      <c r="AT33" s="17"/>
+      <c r="AU33" s="17"/>
+      <c r="AV33" s="17"/>
+      <c r="AW33" s="17"/>
+      <c r="AX33" s="17"/>
+      <c r="AY33" s="17"/>
+      <c r="AZ33" s="17"/>
+      <c r="BA33" s="17"/>
+      <c r="BB33" s="17"/>
+      <c r="BC33" s="17"/>
+      <c r="BD33" s="17"/>
+      <c r="BE33" s="17"/>
+      <c r="BF33" s="17"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4515,36 +4521,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="29"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="30"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="15"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4608,36 +4614,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="30"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="14"/>
+      <c r="AA38" s="14"/>
+      <c r="AB38" s="14"/>
+      <c r="AC38" s="14"/>
+      <c r="AD38" s="14"/>
+      <c r="AE38" s="15"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4794,36 +4800,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="30"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="14"/>
+      <c r="AA40" s="14"/>
+      <c r="AB40" s="14"/>
+      <c r="AC40" s="14"/>
+      <c r="AD40" s="14"/>
+      <c r="AE40" s="15"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4980,36 +4986,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="30"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14"/>
+      <c r="AB42" s="14"/>
+      <c r="AC42" s="14"/>
+      <c r="AD42" s="14"/>
+      <c r="AE42" s="15"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5073,36 +5079,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="30"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="15"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5166,36 +5172,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="30"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="14"/>
+      <c r="Z44" s="14"/>
+      <c r="AA44" s="14"/>
+      <c r="AB44" s="14"/>
+      <c r="AC44" s="14"/>
+      <c r="AD44" s="14"/>
+      <c r="AE44" s="15"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -8792,7 +8798,7 @@
       <c r="B83" s="8"/>
       <c r="C83" s="5"/>
       <c r="D83" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
@@ -8885,7 +8891,7 @@
       <c r="B84" s="8"/>
       <c r="C84" s="5"/>
       <c r="D84" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
@@ -8977,7 +8983,9 @@
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="5"/>
-      <c r="D85" s="9"/>
+      <c r="D85" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
@@ -9005,20 +9013,28 @@
       <c r="AC85" s="9"/>
       <c r="AD85" s="9"/>
       <c r="AE85" s="9"/>
-      <c r="AF85" s="10"/>
+      <c r="AF85" s="10">
+        <v>43709</v>
+      </c>
       <c r="AG85" s="10"/>
       <c r="AH85" s="10"/>
       <c r="AI85" s="10"/>
       <c r="AJ85" s="10"/>
-      <c r="AK85" s="9"/>
+      <c r="AK85" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL85" s="9"/>
       <c r="AM85" s="9"/>
       <c r="AN85" s="9"/>
       <c r="AO85" s="9"/>
-      <c r="AP85" s="11"/>
+      <c r="AP85" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ85" s="11"/>
       <c r="AR85" s="11"/>
-      <c r="AS85" s="9"/>
+      <c r="AS85" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT85" s="9"/>
       <c r="AU85" s="9"/>
       <c r="AV85" s="9"/>
@@ -9060,7 +9076,9 @@
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="5"/>
-      <c r="D86" s="9"/>
+      <c r="D86" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
@@ -9088,20 +9106,28 @@
       <c r="AC86" s="9"/>
       <c r="AD86" s="9"/>
       <c r="AE86" s="9"/>
-      <c r="AF86" s="10"/>
+      <c r="AF86" s="10">
+        <v>43709</v>
+      </c>
       <c r="AG86" s="10"/>
       <c r="AH86" s="10"/>
       <c r="AI86" s="10"/>
       <c r="AJ86" s="10"/>
-      <c r="AK86" s="9"/>
+      <c r="AK86" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL86" s="9"/>
       <c r="AM86" s="9"/>
       <c r="AN86" s="9"/>
       <c r="AO86" s="9"/>
-      <c r="AP86" s="11"/>
+      <c r="AP86" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ86" s="11"/>
       <c r="AR86" s="11"/>
-      <c r="AS86" s="9"/>
+      <c r="AS86" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT86" s="9"/>
       <c r="AU86" s="9"/>
       <c r="AV86" s="9"/>
@@ -9143,7 +9169,9 @@
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="5"/>
-      <c r="D87" s="9"/>
+      <c r="D87" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
       <c r="G87" s="9"/>
@@ -9171,20 +9199,28 @@
       <c r="AC87" s="9"/>
       <c r="AD87" s="9"/>
       <c r="AE87" s="9"/>
-      <c r="AF87" s="10"/>
+      <c r="AF87" s="10">
+        <v>43709</v>
+      </c>
       <c r="AG87" s="10"/>
       <c r="AH87" s="10"/>
       <c r="AI87" s="10"/>
       <c r="AJ87" s="10"/>
-      <c r="AK87" s="9"/>
+      <c r="AK87" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL87" s="9"/>
       <c r="AM87" s="9"/>
       <c r="AN87" s="9"/>
       <c r="AO87" s="9"/>
-      <c r="AP87" s="11"/>
+      <c r="AP87" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ87" s="11"/>
       <c r="AR87" s="11"/>
-      <c r="AS87" s="9"/>
+      <c r="AS87" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT87" s="9"/>
       <c r="AU87" s="9"/>
       <c r="AV87" s="9"/>
@@ -12210,493 +12246,356 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12721,356 +12620,493 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Tìm hiểu về lazy load và reference entity ngày 10/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="106">
   <si>
     <t>No.</t>
   </si>
@@ -333,6 +333,12 @@
   <si>
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Đổ dữ liệu  mapping vào session</t>
   </si>
+  <si>
+    <t xml:space="preserve">Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Tìm hiểu về lazy load entity </t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Tìm hiểu về reference entity</t>
+  </si>
 </sst>
 </file>
 
@@ -599,14 +605,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,6 +625,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,7 +738,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,7 +1129,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1135,7 +1141,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D87" sqref="D87:AE87"/>
+      <selection pane="bottomLeft" activeCell="D89" sqref="D89:AE89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,192 +1156,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="23" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="24" t="s">
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="22" t="s">
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="25" t="s">
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="25"/>
-      <c r="BJ1" s="25"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="25"/>
-      <c r="BO1" s="25"/>
-      <c r="BP1" s="25"/>
-      <c r="BQ1" s="25"/>
-      <c r="BR1" s="25"/>
-      <c r="BS1" s="25"/>
-      <c r="BT1" s="25"/>
-      <c r="BU1" s="25"/>
-      <c r="BV1" s="25"/>
-      <c r="BW1" s="25"/>
-      <c r="BX1" s="25"/>
-      <c r="BY1" s="25"/>
-      <c r="BZ1" s="25"/>
-      <c r="CA1" s="25"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="21">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4056,43 +4062,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="18"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
-      <c r="AD32" s="18"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="19">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="24">
         <v>43293</v>
       </c>
-      <c r="AG32" s="19"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="19"/>
-      <c r="AJ32" s="19"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4121,27 +4127,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="20"/>
-      <c r="BH32" s="20"/>
-      <c r="BI32" s="20"/>
-      <c r="BJ32" s="20"/>
-      <c r="BK32" s="20"/>
-      <c r="BL32" s="20"/>
-      <c r="BM32" s="20"/>
-      <c r="BN32" s="20"/>
-      <c r="BO32" s="20"/>
-      <c r="BP32" s="20"/>
-      <c r="BQ32" s="20"/>
-      <c r="BR32" s="20"/>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="BV32" s="20"/>
-      <c r="BW32" s="20"/>
-      <c r="BX32" s="20"/>
-      <c r="BY32" s="20"/>
-      <c r="BZ32" s="20"/>
-      <c r="CA32" s="20"/>
+      <c r="BG32" s="25"/>
+      <c r="BH32" s="25"/>
+      <c r="BI32" s="25"/>
+      <c r="BJ32" s="25"/>
+      <c r="BK32" s="25"/>
+      <c r="BL32" s="25"/>
+      <c r="BM32" s="25"/>
+      <c r="BN32" s="25"/>
+      <c r="BO32" s="25"/>
+      <c r="BP32" s="25"/>
+      <c r="BQ32" s="25"/>
+      <c r="BR32" s="25"/>
+      <c r="BS32" s="25"/>
+      <c r="BT32" s="25"/>
+      <c r="BU32" s="25"/>
+      <c r="BV32" s="25"/>
+      <c r="BW32" s="25"/>
+      <c r="BX32" s="25"/>
+      <c r="BY32" s="25"/>
+      <c r="BZ32" s="25"/>
+      <c r="CA32" s="25"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4193,27 +4199,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="16">
+      <c r="AP33" s="26">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="16"/>
-      <c r="AR33" s="16"/>
-      <c r="AS33" s="17" t="s">
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="17"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="17"/>
-      <c r="BB33" s="17"/>
-      <c r="BC33" s="17"/>
-      <c r="BD33" s="17"/>
-      <c r="BE33" s="17"/>
-      <c r="BF33" s="17"/>
+      <c r="AT33" s="27"/>
+      <c r="AU33" s="27"/>
+      <c r="AV33" s="27"/>
+      <c r="AW33" s="27"/>
+      <c r="AX33" s="27"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
+      <c r="BA33" s="27"/>
+      <c r="BB33" s="27"/>
+      <c r="BC33" s="27"/>
+      <c r="BD33" s="27"/>
+      <c r="BE33" s="27"/>
+      <c r="BF33" s="27"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4521,36 +4527,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-      <c r="V37" s="14"/>
-      <c r="W37" s="14"/>
-      <c r="X37" s="14"/>
-      <c r="Y37" s="14"/>
-      <c r="Z37" s="14"/>
-      <c r="AA37" s="14"/>
-      <c r="AB37" s="14"/>
-      <c r="AC37" s="14"/>
-      <c r="AD37" s="14"/>
-      <c r="AE37" s="15"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="30"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4614,36 +4620,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-      <c r="V38" s="14"/>
-      <c r="W38" s="14"/>
-      <c r="X38" s="14"/>
-      <c r="Y38" s="14"/>
-      <c r="Z38" s="14"/>
-      <c r="AA38" s="14"/>
-      <c r="AB38" s="14"/>
-      <c r="AC38" s="14"/>
-      <c r="AD38" s="14"/>
-      <c r="AE38" s="15"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="30"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4800,36 +4806,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14"/>
-      <c r="Y40" s="14"/>
-      <c r="Z40" s="14"/>
-      <c r="AA40" s="14"/>
-      <c r="AB40" s="14"/>
-      <c r="AC40" s="14"/>
-      <c r="AD40" s="14"/>
-      <c r="AE40" s="15"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="30"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4986,36 +4992,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="14"/>
-      <c r="Y42" s="14"/>
-      <c r="Z42" s="14"/>
-      <c r="AA42" s="14"/>
-      <c r="AB42" s="14"/>
-      <c r="AC42" s="14"/>
-      <c r="AD42" s="14"/>
-      <c r="AE42" s="15"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="30"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5079,36 +5085,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="15"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="30"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5172,36 +5178,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="14"/>
-      <c r="Y44" s="14"/>
-      <c r="Z44" s="14"/>
-      <c r="AA44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AC44" s="14"/>
-      <c r="AD44" s="14"/>
-      <c r="AE44" s="15"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="30"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -9262,7 +9268,9 @@
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="5"/>
-      <c r="D88" s="9"/>
+      <c r="D88" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="E88" s="9"/>
       <c r="F88" s="9"/>
       <c r="G88" s="9"/>
@@ -9290,12 +9298,16 @@
       <c r="AC88" s="9"/>
       <c r="AD88" s="9"/>
       <c r="AE88" s="9"/>
-      <c r="AF88" s="10"/>
+      <c r="AF88" s="10">
+        <v>43739</v>
+      </c>
       <c r="AG88" s="10"/>
       <c r="AH88" s="10"/>
       <c r="AI88" s="10"/>
       <c r="AJ88" s="10"/>
-      <c r="AK88" s="9"/>
+      <c r="AK88" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL88" s="9"/>
       <c r="AM88" s="9"/>
       <c r="AN88" s="9"/>
@@ -9303,7 +9315,9 @@
       <c r="AP88" s="11"/>
       <c r="AQ88" s="11"/>
       <c r="AR88" s="11"/>
-      <c r="AS88" s="9"/>
+      <c r="AS88" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT88" s="9"/>
       <c r="AU88" s="9"/>
       <c r="AV88" s="9"/>
@@ -9345,7 +9359,9 @@
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="5"/>
-      <c r="D89" s="9"/>
+      <c r="D89" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
       <c r="G89" s="9"/>
@@ -9373,12 +9389,16 @@
       <c r="AC89" s="9"/>
       <c r="AD89" s="9"/>
       <c r="AE89" s="9"/>
-      <c r="AF89" s="10"/>
+      <c r="AF89" s="10">
+        <v>43739</v>
+      </c>
       <c r="AG89" s="10"/>
       <c r="AH89" s="10"/>
       <c r="AI89" s="10"/>
       <c r="AJ89" s="10"/>
-      <c r="AK89" s="9"/>
+      <c r="AK89" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL89" s="9"/>
       <c r="AM89" s="9"/>
       <c r="AN89" s="9"/>
@@ -9386,7 +9406,9 @@
       <c r="AP89" s="11"/>
       <c r="AQ89" s="11"/>
       <c r="AR89" s="11"/>
-      <c r="AS89" s="9"/>
+      <c r="AS89" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT89" s="9"/>
       <c r="AU89" s="9"/>
       <c r="AV89" s="9"/>
@@ -12246,356 +12268,493 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12620,493 +12779,356 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Tìm hiểu về lazy load và reference entity ngày 11/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="106">
   <si>
     <t>No.</t>
   </si>
@@ -605,6 +605,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -625,14 +633,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,7 +738,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1129,7 +1129,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1141,7 +1141,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D89" sqref="D89:AE89"/>
+      <selection pane="bottomLeft" activeCell="AK92" sqref="AK92:AO92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,192 +1156,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="15" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="14" t="s">
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="16" t="s">
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="14" t="s">
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
-      <c r="BC1" s="14"/>
-      <c r="BD1" s="14"/>
-      <c r="BE1" s="14"/>
-      <c r="BF1" s="14"/>
-      <c r="BG1" s="17" t="s">
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="17"/>
-      <c r="BP1" s="17"/>
-      <c r="BQ1" s="17"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="17"/>
-      <c r="BT1" s="17"/>
-      <c r="BU1" s="17"/>
-      <c r="BV1" s="17"/>
-      <c r="BW1" s="17"/>
-      <c r="BX1" s="17"/>
-      <c r="BY1" s="17"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="20" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="19" t="s">
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="21">
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="29">
         <v>1</v>
       </c>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="19" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
-      <c r="BN2" s="22"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2" s="22"/>
-      <c r="BQ2" s="22"/>
-      <c r="BR2" s="22"/>
-      <c r="BS2" s="22"/>
-      <c r="BT2" s="22"/>
-      <c r="BU2" s="22"/>
-      <c r="BV2" s="22"/>
-      <c r="BW2" s="22"/>
-      <c r="BX2" s="22"/>
-      <c r="BY2" s="22"/>
-      <c r="BZ2" s="22"/>
-      <c r="CA2" s="22"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="30"/>
+      <c r="BJ2" s="30"/>
+      <c r="BK2" s="30"/>
+      <c r="BL2" s="30"/>
+      <c r="BM2" s="30"/>
+      <c r="BN2" s="30"/>
+      <c r="BO2" s="30"/>
+      <c r="BP2" s="30"/>
+      <c r="BQ2" s="30"/>
+      <c r="BR2" s="30"/>
+      <c r="BS2" s="30"/>
+      <c r="BT2" s="30"/>
+      <c r="BU2" s="30"/>
+      <c r="BV2" s="30"/>
+      <c r="BW2" s="30"/>
+      <c r="BX2" s="30"/>
+      <c r="BY2" s="30"/>
+      <c r="BZ2" s="30"/>
+      <c r="CA2" s="30"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4062,43 +4062,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="23"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="23"/>
-      <c r="AD32" s="23"/>
-      <c r="AE32" s="23"/>
-      <c r="AF32" s="24">
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+      <c r="V32" s="18"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
+      <c r="AA32" s="18"/>
+      <c r="AB32" s="18"/>
+      <c r="AC32" s="18"/>
+      <c r="AD32" s="18"/>
+      <c r="AE32" s="18"/>
+      <c r="AF32" s="19">
         <v>43293</v>
       </c>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="24"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="24"/>
+      <c r="AG32" s="19"/>
+      <c r="AH32" s="19"/>
+      <c r="AI32" s="19"/>
+      <c r="AJ32" s="19"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4127,27 +4127,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="25"/>
-      <c r="BH32" s="25"/>
-      <c r="BI32" s="25"/>
-      <c r="BJ32" s="25"/>
-      <c r="BK32" s="25"/>
-      <c r="BL32" s="25"/>
-      <c r="BM32" s="25"/>
-      <c r="BN32" s="25"/>
-      <c r="BO32" s="25"/>
-      <c r="BP32" s="25"/>
-      <c r="BQ32" s="25"/>
-      <c r="BR32" s="25"/>
-      <c r="BS32" s="25"/>
-      <c r="BT32" s="25"/>
-      <c r="BU32" s="25"/>
-      <c r="BV32" s="25"/>
-      <c r="BW32" s="25"/>
-      <c r="BX32" s="25"/>
-      <c r="BY32" s="25"/>
-      <c r="BZ32" s="25"/>
-      <c r="CA32" s="25"/>
+      <c r="BG32" s="20"/>
+      <c r="BH32" s="20"/>
+      <c r="BI32" s="20"/>
+      <c r="BJ32" s="20"/>
+      <c r="BK32" s="20"/>
+      <c r="BL32" s="20"/>
+      <c r="BM32" s="20"/>
+      <c r="BN32" s="20"/>
+      <c r="BO32" s="20"/>
+      <c r="BP32" s="20"/>
+      <c r="BQ32" s="20"/>
+      <c r="BR32" s="20"/>
+      <c r="BS32" s="20"/>
+      <c r="BT32" s="20"/>
+      <c r="BU32" s="20"/>
+      <c r="BV32" s="20"/>
+      <c r="BW32" s="20"/>
+      <c r="BX32" s="20"/>
+      <c r="BY32" s="20"/>
+      <c r="BZ32" s="20"/>
+      <c r="CA32" s="20"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4199,27 +4199,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="26">
+      <c r="AP33" s="16">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="27" t="s">
+      <c r="AQ33" s="16"/>
+      <c r="AR33" s="16"/>
+      <c r="AS33" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="27"/>
-      <c r="AU33" s="27"/>
-      <c r="AV33" s="27"/>
-      <c r="AW33" s="27"/>
-      <c r="AX33" s="27"/>
-      <c r="AY33" s="27"/>
-      <c r="AZ33" s="27"/>
-      <c r="BA33" s="27"/>
-      <c r="BB33" s="27"/>
-      <c r="BC33" s="27"/>
-      <c r="BD33" s="27"/>
-      <c r="BE33" s="27"/>
-      <c r="BF33" s="27"/>
+      <c r="AT33" s="17"/>
+      <c r="AU33" s="17"/>
+      <c r="AV33" s="17"/>
+      <c r="AW33" s="17"/>
+      <c r="AX33" s="17"/>
+      <c r="AY33" s="17"/>
+      <c r="AZ33" s="17"/>
+      <c r="BA33" s="17"/>
+      <c r="BB33" s="17"/>
+      <c r="BC33" s="17"/>
+      <c r="BD33" s="17"/>
+      <c r="BE33" s="17"/>
+      <c r="BF33" s="17"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4527,36 +4527,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="29"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="30"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="15"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4620,36 +4620,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="30"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="14"/>
+      <c r="AA38" s="14"/>
+      <c r="AB38" s="14"/>
+      <c r="AC38" s="14"/>
+      <c r="AD38" s="14"/>
+      <c r="AE38" s="15"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4806,36 +4806,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="30"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="14"/>
+      <c r="AA40" s="14"/>
+      <c r="AB40" s="14"/>
+      <c r="AC40" s="14"/>
+      <c r="AD40" s="14"/>
+      <c r="AE40" s="15"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4992,36 +4992,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="30"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14"/>
+      <c r="AB42" s="14"/>
+      <c r="AC42" s="14"/>
+      <c r="AD42" s="14"/>
+      <c r="AE42" s="15"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5085,36 +5085,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="30"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="15"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5178,36 +5178,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="30"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="14"/>
+      <c r="Z44" s="14"/>
+      <c r="AA44" s="14"/>
+      <c r="AB44" s="14"/>
+      <c r="AC44" s="14"/>
+      <c r="AD44" s="14"/>
+      <c r="AE44" s="15"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -9450,7 +9450,9 @@
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="5"/>
-      <c r="D90" s="9"/>
+      <c r="D90" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
@@ -9478,12 +9480,16 @@
       <c r="AC90" s="9"/>
       <c r="AD90" s="9"/>
       <c r="AE90" s="9"/>
-      <c r="AF90" s="10"/>
+      <c r="AF90" s="10">
+        <v>43770</v>
+      </c>
       <c r="AG90" s="10"/>
       <c r="AH90" s="10"/>
       <c r="AI90" s="10"/>
       <c r="AJ90" s="10"/>
-      <c r="AK90" s="9"/>
+      <c r="AK90" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL90" s="9"/>
       <c r="AM90" s="9"/>
       <c r="AN90" s="9"/>
@@ -9491,7 +9497,9 @@
       <c r="AP90" s="11"/>
       <c r="AQ90" s="11"/>
       <c r="AR90" s="11"/>
-      <c r="AS90" s="9"/>
+      <c r="AS90" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT90" s="9"/>
       <c r="AU90" s="9"/>
       <c r="AV90" s="9"/>
@@ -12268,493 +12276,356 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12779,356 +12650,493 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Báo cáo ngày 14/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="108">
   <si>
     <t>No.</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Tìm hiểu về reference entity</t>
+  </si>
+  <si>
+    <t>14/1/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Làm giao diện xác nhận</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1147,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK92" sqref="AK92:AO92"/>
+      <selection pane="bottomLeft" activeCell="AP94" sqref="AP94:AR94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9541,7 +9547,9 @@
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="5"/>
-      <c r="D91" s="9"/>
+      <c r="D91" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
@@ -9569,12 +9577,16 @@
       <c r="AC91" s="9"/>
       <c r="AD91" s="9"/>
       <c r="AE91" s="9"/>
-      <c r="AF91" s="10"/>
+      <c r="AF91" s="10">
+        <v>43800</v>
+      </c>
       <c r="AG91" s="10"/>
       <c r="AH91" s="10"/>
       <c r="AI91" s="10"/>
       <c r="AJ91" s="10"/>
-      <c r="AK91" s="9"/>
+      <c r="AK91" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL91" s="9"/>
       <c r="AM91" s="9"/>
       <c r="AN91" s="9"/>
@@ -9582,7 +9594,9 @@
       <c r="AP91" s="11"/>
       <c r="AQ91" s="11"/>
       <c r="AR91" s="11"/>
-      <c r="AS91" s="9"/>
+      <c r="AS91" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT91" s="9"/>
       <c r="AU91" s="9"/>
       <c r="AV91" s="9"/>
@@ -9624,7 +9638,9 @@
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="5"/>
-      <c r="D92" s="9"/>
+      <c r="D92" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
       <c r="G92" s="9"/>
@@ -9652,20 +9668,28 @@
       <c r="AC92" s="9"/>
       <c r="AD92" s="9"/>
       <c r="AE92" s="9"/>
-      <c r="AF92" s="10"/>
+      <c r="AF92" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="AG92" s="10"/>
       <c r="AH92" s="10"/>
       <c r="AI92" s="10"/>
       <c r="AJ92" s="10"/>
-      <c r="AK92" s="9"/>
+      <c r="AK92" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL92" s="9"/>
       <c r="AM92" s="9"/>
       <c r="AN92" s="9"/>
       <c r="AO92" s="9"/>
-      <c r="AP92" s="11"/>
+      <c r="AP92" s="11">
+        <v>0.5</v>
+      </c>
       <c r="AQ92" s="11"/>
       <c r="AR92" s="11"/>
-      <c r="AS92" s="9"/>
+      <c r="AS92" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT92" s="9"/>
       <c r="AU92" s="9"/>
       <c r="AV92" s="9"/>

</xml_diff>

<commit_message>
Báo cáo ngày 16/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="111">
   <si>
     <t>No.</t>
   </si>
@@ -345,6 +345,15 @@
   <si>
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Làm giao diện xác nhận</t>
   </si>
+  <si>
+    <t>15/1/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 2 - Lưu thông tin JOB, JOBDetail, Mapping, Ref vào database</t>
+  </si>
+  <si>
+    <t>16/1/2019</t>
+  </si>
 </sst>
 </file>
 
@@ -611,14 +620,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -639,6 +640,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,7 +753,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1135,7 +1144,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1147,7 +1156,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP94" sqref="AP94:AR94"/>
+      <selection pane="bottomLeft" activeCell="AS95" sqref="AS95:BF95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,192 +1171,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="23" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="24" t="s">
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="22" t="s">
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="25" t="s">
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="25"/>
-      <c r="BJ1" s="25"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="25"/>
-      <c r="BO1" s="25"/>
-      <c r="BP1" s="25"/>
-      <c r="BQ1" s="25"/>
-      <c r="BR1" s="25"/>
-      <c r="BS1" s="25"/>
-      <c r="BT1" s="25"/>
-      <c r="BU1" s="25"/>
-      <c r="BV1" s="25"/>
-      <c r="BW1" s="25"/>
-      <c r="BX1" s="25"/>
-      <c r="BY1" s="25"/>
-      <c r="BZ1" s="25"/>
-      <c r="CA1" s="25"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="21">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4068,43 +4077,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="18"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
-      <c r="AD32" s="18"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="19">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="24">
         <v>43293</v>
       </c>
-      <c r="AG32" s="19"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="19"/>
-      <c r="AJ32" s="19"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4133,27 +4142,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="20"/>
-      <c r="BH32" s="20"/>
-      <c r="BI32" s="20"/>
-      <c r="BJ32" s="20"/>
-      <c r="BK32" s="20"/>
-      <c r="BL32" s="20"/>
-      <c r="BM32" s="20"/>
-      <c r="BN32" s="20"/>
-      <c r="BO32" s="20"/>
-      <c r="BP32" s="20"/>
-      <c r="BQ32" s="20"/>
-      <c r="BR32" s="20"/>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="BV32" s="20"/>
-      <c r="BW32" s="20"/>
-      <c r="BX32" s="20"/>
-      <c r="BY32" s="20"/>
-      <c r="BZ32" s="20"/>
-      <c r="CA32" s="20"/>
+      <c r="BG32" s="25"/>
+      <c r="BH32" s="25"/>
+      <c r="BI32" s="25"/>
+      <c r="BJ32" s="25"/>
+      <c r="BK32" s="25"/>
+      <c r="BL32" s="25"/>
+      <c r="BM32" s="25"/>
+      <c r="BN32" s="25"/>
+      <c r="BO32" s="25"/>
+      <c r="BP32" s="25"/>
+      <c r="BQ32" s="25"/>
+      <c r="BR32" s="25"/>
+      <c r="BS32" s="25"/>
+      <c r="BT32" s="25"/>
+      <c r="BU32" s="25"/>
+      <c r="BV32" s="25"/>
+      <c r="BW32" s="25"/>
+      <c r="BX32" s="25"/>
+      <c r="BY32" s="25"/>
+      <c r="BZ32" s="25"/>
+      <c r="CA32" s="25"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4205,27 +4214,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="16">
+      <c r="AP33" s="26">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="16"/>
-      <c r="AR33" s="16"/>
-      <c r="AS33" s="17" t="s">
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="17"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="17"/>
-      <c r="BB33" s="17"/>
-      <c r="BC33" s="17"/>
-      <c r="BD33" s="17"/>
-      <c r="BE33" s="17"/>
-      <c r="BF33" s="17"/>
+      <c r="AT33" s="27"/>
+      <c r="AU33" s="27"/>
+      <c r="AV33" s="27"/>
+      <c r="AW33" s="27"/>
+      <c r="AX33" s="27"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
+      <c r="BA33" s="27"/>
+      <c r="BB33" s="27"/>
+      <c r="BC33" s="27"/>
+      <c r="BD33" s="27"/>
+      <c r="BE33" s="27"/>
+      <c r="BF33" s="27"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4533,36 +4542,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-      <c r="V37" s="14"/>
-      <c r="W37" s="14"/>
-      <c r="X37" s="14"/>
-      <c r="Y37" s="14"/>
-      <c r="Z37" s="14"/>
-      <c r="AA37" s="14"/>
-      <c r="AB37" s="14"/>
-      <c r="AC37" s="14"/>
-      <c r="AD37" s="14"/>
-      <c r="AE37" s="15"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="30"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4626,36 +4635,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-      <c r="V38" s="14"/>
-      <c r="W38" s="14"/>
-      <c r="X38" s="14"/>
-      <c r="Y38" s="14"/>
-      <c r="Z38" s="14"/>
-      <c r="AA38" s="14"/>
-      <c r="AB38" s="14"/>
-      <c r="AC38" s="14"/>
-      <c r="AD38" s="14"/>
-      <c r="AE38" s="15"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="30"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4812,36 +4821,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14"/>
-      <c r="Y40" s="14"/>
-      <c r="Z40" s="14"/>
-      <c r="AA40" s="14"/>
-      <c r="AB40" s="14"/>
-      <c r="AC40" s="14"/>
-      <c r="AD40" s="14"/>
-      <c r="AE40" s="15"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="30"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4998,36 +5007,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="14"/>
-      <c r="Y42" s="14"/>
-      <c r="Z42" s="14"/>
-      <c r="AA42" s="14"/>
-      <c r="AB42" s="14"/>
-      <c r="AC42" s="14"/>
-      <c r="AD42" s="14"/>
-      <c r="AE42" s="15"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="30"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5091,36 +5100,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="15"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="30"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5184,36 +5193,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="14"/>
-      <c r="Y44" s="14"/>
-      <c r="Z44" s="14"/>
-      <c r="AA44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AC44" s="14"/>
-      <c r="AD44" s="14"/>
-      <c r="AE44" s="15"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="30"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -9731,7 +9740,9 @@
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="5"/>
-      <c r="D93" s="9"/>
+      <c r="D93" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
       <c r="G93" s="9"/>
@@ -9759,20 +9770,28 @@
       <c r="AC93" s="9"/>
       <c r="AD93" s="9"/>
       <c r="AE93" s="9"/>
-      <c r="AF93" s="10"/>
+      <c r="AF93" s="10" t="s">
+        <v>108</v>
+      </c>
       <c r="AG93" s="10"/>
       <c r="AH93" s="10"/>
       <c r="AI93" s="10"/>
       <c r="AJ93" s="10"/>
-      <c r="AK93" s="9"/>
+      <c r="AK93" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL93" s="9"/>
       <c r="AM93" s="9"/>
       <c r="AN93" s="9"/>
       <c r="AO93" s="9"/>
-      <c r="AP93" s="11"/>
+      <c r="AP93" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ93" s="11"/>
       <c r="AR93" s="11"/>
-      <c r="AS93" s="9"/>
+      <c r="AS93" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT93" s="9"/>
       <c r="AU93" s="9"/>
       <c r="AV93" s="9"/>
@@ -9814,7 +9833,9 @@
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="5"/>
-      <c r="D94" s="9"/>
+      <c r="D94" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
@@ -9842,20 +9863,28 @@
       <c r="AC94" s="9"/>
       <c r="AD94" s="9"/>
       <c r="AE94" s="9"/>
-      <c r="AF94" s="10"/>
+      <c r="AF94" s="10" t="s">
+        <v>110</v>
+      </c>
       <c r="AG94" s="10"/>
       <c r="AH94" s="10"/>
       <c r="AI94" s="10"/>
       <c r="AJ94" s="10"/>
-      <c r="AK94" s="9"/>
+      <c r="AK94" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL94" s="9"/>
       <c r="AM94" s="9"/>
       <c r="AN94" s="9"/>
       <c r="AO94" s="9"/>
-      <c r="AP94" s="11"/>
+      <c r="AP94" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ94" s="11"/>
       <c r="AR94" s="11"/>
-      <c r="AS94" s="9"/>
+      <c r="AS94" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT94" s="9"/>
       <c r="AU94" s="9"/>
       <c r="AV94" s="9"/>
@@ -12300,356 +12329,493 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12674,493 +12840,356 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Xử lý giao diện xác nhận trong trang tạo mới syncdata
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="113">
   <si>
     <t>No.</t>
   </si>
@@ -354,6 +354,12 @@
   <si>
     <t>16/1/2019</t>
   </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 3 - Sử xý giao diện xác nhận</t>
+  </si>
+  <si>
+    <t>18/1/2019</t>
+  </si>
 </sst>
 </file>
 
@@ -620,6 +626,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -640,14 +654,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,7 +759,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1144,7 +1150,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1156,7 +1162,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS95" sqref="AS95:BF95"/>
+      <selection pane="bottomLeft" activeCell="AP95" sqref="AP95:AR95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,192 +1177,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="15" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="14" t="s">
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="16" t="s">
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="14" t="s">
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
-      <c r="BC1" s="14"/>
-      <c r="BD1" s="14"/>
-      <c r="BE1" s="14"/>
-      <c r="BF1" s="14"/>
-      <c r="BG1" s="17" t="s">
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="17"/>
-      <c r="BP1" s="17"/>
-      <c r="BQ1" s="17"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="17"/>
-      <c r="BT1" s="17"/>
-      <c r="BU1" s="17"/>
-      <c r="BV1" s="17"/>
-      <c r="BW1" s="17"/>
-      <c r="BX1" s="17"/>
-      <c r="BY1" s="17"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="20" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="19" t="s">
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="21">
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="29">
         <v>1</v>
       </c>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="19" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
-      <c r="BN2" s="22"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2" s="22"/>
-      <c r="BQ2" s="22"/>
-      <c r="BR2" s="22"/>
-      <c r="BS2" s="22"/>
-      <c r="BT2" s="22"/>
-      <c r="BU2" s="22"/>
-      <c r="BV2" s="22"/>
-      <c r="BW2" s="22"/>
-      <c r="BX2" s="22"/>
-      <c r="BY2" s="22"/>
-      <c r="BZ2" s="22"/>
-      <c r="CA2" s="22"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="30"/>
+      <c r="BJ2" s="30"/>
+      <c r="BK2" s="30"/>
+      <c r="BL2" s="30"/>
+      <c r="BM2" s="30"/>
+      <c r="BN2" s="30"/>
+      <c r="BO2" s="30"/>
+      <c r="BP2" s="30"/>
+      <c r="BQ2" s="30"/>
+      <c r="BR2" s="30"/>
+      <c r="BS2" s="30"/>
+      <c r="BT2" s="30"/>
+      <c r="BU2" s="30"/>
+      <c r="BV2" s="30"/>
+      <c r="BW2" s="30"/>
+      <c r="BX2" s="30"/>
+      <c r="BY2" s="30"/>
+      <c r="BZ2" s="30"/>
+      <c r="CA2" s="30"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4077,43 +4083,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="23"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="23"/>
-      <c r="AD32" s="23"/>
-      <c r="AE32" s="23"/>
-      <c r="AF32" s="24">
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+      <c r="V32" s="18"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
+      <c r="AA32" s="18"/>
+      <c r="AB32" s="18"/>
+      <c r="AC32" s="18"/>
+      <c r="AD32" s="18"/>
+      <c r="AE32" s="18"/>
+      <c r="AF32" s="19">
         <v>43293</v>
       </c>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="24"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="24"/>
+      <c r="AG32" s="19"/>
+      <c r="AH32" s="19"/>
+      <c r="AI32" s="19"/>
+      <c r="AJ32" s="19"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4142,27 +4148,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="25"/>
-      <c r="BH32" s="25"/>
-      <c r="BI32" s="25"/>
-      <c r="BJ32" s="25"/>
-      <c r="BK32" s="25"/>
-      <c r="BL32" s="25"/>
-      <c r="BM32" s="25"/>
-      <c r="BN32" s="25"/>
-      <c r="BO32" s="25"/>
-      <c r="BP32" s="25"/>
-      <c r="BQ32" s="25"/>
-      <c r="BR32" s="25"/>
-      <c r="BS32" s="25"/>
-      <c r="BT32" s="25"/>
-      <c r="BU32" s="25"/>
-      <c r="BV32" s="25"/>
-      <c r="BW32" s="25"/>
-      <c r="BX32" s="25"/>
-      <c r="BY32" s="25"/>
-      <c r="BZ32" s="25"/>
-      <c r="CA32" s="25"/>
+      <c r="BG32" s="20"/>
+      <c r="BH32" s="20"/>
+      <c r="BI32" s="20"/>
+      <c r="BJ32" s="20"/>
+      <c r="BK32" s="20"/>
+      <c r="BL32" s="20"/>
+      <c r="BM32" s="20"/>
+      <c r="BN32" s="20"/>
+      <c r="BO32" s="20"/>
+      <c r="BP32" s="20"/>
+      <c r="BQ32" s="20"/>
+      <c r="BR32" s="20"/>
+      <c r="BS32" s="20"/>
+      <c r="BT32" s="20"/>
+      <c r="BU32" s="20"/>
+      <c r="BV32" s="20"/>
+      <c r="BW32" s="20"/>
+      <c r="BX32" s="20"/>
+      <c r="BY32" s="20"/>
+      <c r="BZ32" s="20"/>
+      <c r="CA32" s="20"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -4214,27 +4220,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="26">
+      <c r="AP33" s="16">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="27" t="s">
+      <c r="AQ33" s="16"/>
+      <c r="AR33" s="16"/>
+      <c r="AS33" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="27"/>
-      <c r="AU33" s="27"/>
-      <c r="AV33" s="27"/>
-      <c r="AW33" s="27"/>
-      <c r="AX33" s="27"/>
-      <c r="AY33" s="27"/>
-      <c r="AZ33" s="27"/>
-      <c r="BA33" s="27"/>
-      <c r="BB33" s="27"/>
-      <c r="BC33" s="27"/>
-      <c r="BD33" s="27"/>
-      <c r="BE33" s="27"/>
-      <c r="BF33" s="27"/>
+      <c r="AT33" s="17"/>
+      <c r="AU33" s="17"/>
+      <c r="AV33" s="17"/>
+      <c r="AW33" s="17"/>
+      <c r="AX33" s="17"/>
+      <c r="AY33" s="17"/>
+      <c r="AZ33" s="17"/>
+      <c r="BA33" s="17"/>
+      <c r="BB33" s="17"/>
+      <c r="BC33" s="17"/>
+      <c r="BD33" s="17"/>
+      <c r="BE33" s="17"/>
+      <c r="BF33" s="17"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4542,36 +4548,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="29"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="30"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="15"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4635,36 +4641,36 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="30"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="14"/>
+      <c r="AA38" s="14"/>
+      <c r="AB38" s="14"/>
+      <c r="AC38" s="14"/>
+      <c r="AD38" s="14"/>
+      <c r="AE38" s="15"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4821,36 +4827,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="30"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="14"/>
+      <c r="AA40" s="14"/>
+      <c r="AB40" s="14"/>
+      <c r="AC40" s="14"/>
+      <c r="AD40" s="14"/>
+      <c r="AE40" s="15"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -5007,36 +5013,36 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="30"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14"/>
+      <c r="AB42" s="14"/>
+      <c r="AC42" s="14"/>
+      <c r="AD42" s="14"/>
+      <c r="AE42" s="15"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5100,36 +5106,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="30"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="15"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5193,36 +5199,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="30"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="14"/>
+      <c r="Z44" s="14"/>
+      <c r="AA44" s="14"/>
+      <c r="AB44" s="14"/>
+      <c r="AC44" s="14"/>
+      <c r="AD44" s="14"/>
+      <c r="AE44" s="15"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -9926,7 +9932,9 @@
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="5"/>
-      <c r="D95" s="9"/>
+      <c r="D95" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
       <c r="G95" s="9"/>
@@ -9954,20 +9962,28 @@
       <c r="AC95" s="9"/>
       <c r="AD95" s="9"/>
       <c r="AE95" s="9"/>
-      <c r="AF95" s="10"/>
+      <c r="AF95" s="10" t="s">
+        <v>112</v>
+      </c>
       <c r="AG95" s="10"/>
       <c r="AH95" s="10"/>
       <c r="AI95" s="10"/>
       <c r="AJ95" s="10"/>
-      <c r="AK95" s="9"/>
+      <c r="AK95" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL95" s="9"/>
       <c r="AM95" s="9"/>
       <c r="AN95" s="9"/>
       <c r="AO95" s="9"/>
-      <c r="AP95" s="11"/>
+      <c r="AP95" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ95" s="11"/>
       <c r="AR95" s="11"/>
-      <c r="AS95" s="9"/>
+      <c r="AS95" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT95" s="9"/>
       <c r="AU95" s="9"/>
       <c r="AV95" s="9"/>
@@ -12329,493 +12345,356 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12840,356 +12719,493 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Báo cáo ngày 22/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="118">
   <si>
     <t>No.</t>
   </si>
@@ -359,6 +359,21 @@
   </si>
   <si>
     <t>18/1/2019</t>
+  </si>
+  <si>
+    <t>22/1/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 3 - Sử xý giao diện xác nhận (chỉnh sửa)</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 3 - Xóa thiết lập và điều kiện</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 3 - Sao chép câu lệnh đồng bộ ở bước xác nhận</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  - Chỉnh sửa giao diện bước 3 - Lỗi khi ở clone thiết lập thứ 2 nếu để bảng nguồn là bảng KhachHang thì có lỗi</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1177,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP95" sqref="AP95:AR95"/>
+      <selection pane="bottomLeft" activeCell="AP100" sqref="AP100:AR100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10025,7 +10040,9 @@
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="5"/>
-      <c r="D96" s="9"/>
+      <c r="D96" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
@@ -10053,20 +10070,28 @@
       <c r="AC96" s="9"/>
       <c r="AD96" s="9"/>
       <c r="AE96" s="9"/>
-      <c r="AF96" s="10"/>
+      <c r="AF96" s="10" t="s">
+        <v>113</v>
+      </c>
       <c r="AG96" s="10"/>
       <c r="AH96" s="10"/>
       <c r="AI96" s="10"/>
       <c r="AJ96" s="10"/>
-      <c r="AK96" s="9"/>
+      <c r="AK96" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL96" s="9"/>
       <c r="AM96" s="9"/>
       <c r="AN96" s="9"/>
       <c r="AO96" s="9"/>
-      <c r="AP96" s="11"/>
+      <c r="AP96" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ96" s="11"/>
       <c r="AR96" s="11"/>
-      <c r="AS96" s="9"/>
+      <c r="AS96" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT96" s="9"/>
       <c r="AU96" s="9"/>
       <c r="AV96" s="9"/>
@@ -10108,7 +10133,9 @@
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="5"/>
-      <c r="D97" s="9"/>
+      <c r="D97" s="9" t="s">
+        <v>115</v>
+      </c>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
       <c r="G97" s="9"/>
@@ -10136,20 +10163,28 @@
       <c r="AC97" s="9"/>
       <c r="AD97" s="9"/>
       <c r="AE97" s="9"/>
-      <c r="AF97" s="10"/>
+      <c r="AF97" s="10" t="s">
+        <v>113</v>
+      </c>
       <c r="AG97" s="10"/>
       <c r="AH97" s="10"/>
       <c r="AI97" s="10"/>
       <c r="AJ97" s="10"/>
-      <c r="AK97" s="9"/>
+      <c r="AK97" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL97" s="9"/>
       <c r="AM97" s="9"/>
       <c r="AN97" s="9"/>
       <c r="AO97" s="9"/>
-      <c r="AP97" s="11"/>
+      <c r="AP97" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ97" s="11"/>
       <c r="AR97" s="11"/>
-      <c r="AS97" s="9"/>
+      <c r="AS97" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT97" s="9"/>
       <c r="AU97" s="9"/>
       <c r="AV97" s="9"/>
@@ -10191,7 +10226,9 @@
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="5"/>
-      <c r="D98" s="9"/>
+      <c r="D98" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
@@ -10219,20 +10256,28 @@
       <c r="AC98" s="9"/>
       <c r="AD98" s="9"/>
       <c r="AE98" s="9"/>
-      <c r="AF98" s="10"/>
+      <c r="AF98" s="10" t="s">
+        <v>113</v>
+      </c>
       <c r="AG98" s="10"/>
       <c r="AH98" s="10"/>
       <c r="AI98" s="10"/>
       <c r="AJ98" s="10"/>
-      <c r="AK98" s="9"/>
+      <c r="AK98" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL98" s="9"/>
       <c r="AM98" s="9"/>
       <c r="AN98" s="9"/>
       <c r="AO98" s="9"/>
-      <c r="AP98" s="11"/>
+      <c r="AP98" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ98" s="11"/>
       <c r="AR98" s="11"/>
-      <c r="AS98" s="9"/>
+      <c r="AS98" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT98" s="9"/>
       <c r="AU98" s="9"/>
       <c r="AV98" s="9"/>
@@ -10274,7 +10319,9 @@
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="5"/>
-      <c r="D99" s="9"/>
+      <c r="D99" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
       <c r="G99" s="9"/>
@@ -10302,20 +10349,28 @@
       <c r="AC99" s="9"/>
       <c r="AD99" s="9"/>
       <c r="AE99" s="9"/>
-      <c r="AF99" s="10"/>
+      <c r="AF99" s="10" t="s">
+        <v>113</v>
+      </c>
       <c r="AG99" s="10"/>
       <c r="AH99" s="10"/>
       <c r="AI99" s="10"/>
       <c r="AJ99" s="10"/>
-      <c r="AK99" s="9"/>
+      <c r="AK99" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL99" s="9"/>
       <c r="AM99" s="9"/>
       <c r="AN99" s="9"/>
       <c r="AO99" s="9"/>
-      <c r="AP99" s="11"/>
+      <c r="AP99" s="11">
+        <v>0</v>
+      </c>
       <c r="AQ99" s="11"/>
       <c r="AR99" s="11"/>
-      <c r="AS99" s="9"/>
+      <c r="AS99" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT99" s="9"/>
       <c r="AU99" s="9"/>
       <c r="AV99" s="9"/>

</xml_diff>

<commit_message>
TÌm hiểu về cron expression
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="123">
   <si>
     <t>No.</t>
   </si>
@@ -375,6 +375,21 @@
   <si>
     <t>Trang tạo mới  - Chỉnh sửa giao diện bước 3 - Lỗi khi ở clone thiết lập thứ 2 nếu để bảng nguồn là bảng KhachHang thì có lỗi</t>
   </si>
+  <si>
+    <t>23/1/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Test</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Tìm hiểu về cron expression hangfire</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thay đổi giao diện step 1</t>
+  </si>
+  <si>
+    <t>24/1/2019</t>
+  </si>
 </sst>
 </file>
 
@@ -641,14 +656,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -669,6 +676,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,14 +782,14 @@
       <xdr:col>96</xdr:col>
       <xdr:colOff>55080</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>111825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1165,7 +1180,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1177,7 +1192,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP100" sqref="AP100:AR100"/>
+      <selection pane="bottomLeft" activeCell="D116" sqref="D116:AE116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,192 +1207,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="23" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="24" t="s">
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="22" t="s">
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="25" t="s">
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="25"/>
-      <c r="BJ1" s="25"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="25"/>
-      <c r="BO1" s="25"/>
-      <c r="BP1" s="25"/>
-      <c r="BQ1" s="25"/>
-      <c r="BR1" s="25"/>
-      <c r="BS1" s="25"/>
-      <c r="BT1" s="25"/>
-      <c r="BU1" s="25"/>
-      <c r="BV1" s="25"/>
-      <c r="BW1" s="25"/>
-      <c r="BX1" s="25"/>
-      <c r="BY1" s="25"/>
-      <c r="BZ1" s="25"/>
-      <c r="CA1" s="25"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="21">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -1565,7 +1580,7 @@
       <c r="BZ4" s="12"/>
       <c r="CA4" s="12"/>
     </row>
-    <row r="5" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1661,10 +1676,10 @@
       <c r="CA5" s="12"/>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -1939,7 +1954,7 @@
       <c r="BZ8" s="12"/>
       <c r="CA8" s="12"/>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -2035,10 +2050,10 @@
       <c r="CA9" s="12"/>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
         <v>33</v>
@@ -2313,7 +2328,7 @@
       <c r="BZ12" s="12"/>
       <c r="CA12" s="12"/>
     </row>
-    <row r="13" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -2409,10 +2424,10 @@
       <c r="CA13" s="12"/>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="18">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5"/>
       <c r="D14" s="9" t="s">
         <v>33</v>
@@ -2689,7 +2704,7 @@
       <c r="BZ16" s="12"/>
       <c r="CA16" s="12"/>
     </row>
-    <row r="17" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -2785,10 +2800,10 @@
       <c r="CA17" s="12"/>
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="18">
         <v>17</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
         <v>38</v>
@@ -3063,7 +3078,7 @@
       <c r="BZ20" s="12"/>
       <c r="CA20" s="12"/>
     </row>
-    <row r="21" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -3157,10 +3172,10 @@
       <c r="CA21" s="12"/>
     </row>
     <row r="22" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="18">
         <v>21</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="5"/>
       <c r="D22" s="9" t="s">
         <v>44</v>
@@ -3439,7 +3454,7 @@
       <c r="BZ24" s="12"/>
       <c r="CA24" s="12"/>
     </row>
-    <row r="25" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -3533,10 +3548,10 @@
       <c r="CA25" s="12"/>
     </row>
     <row r="26" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="18">
         <v>25</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
         <v>38</v>
@@ -3811,7 +3826,7 @@
       <c r="BZ28" s="12"/>
       <c r="CA28" s="12"/>
     </row>
-    <row r="29" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -3907,10 +3922,10 @@
       <c r="CA29" s="12"/>
     </row>
     <row r="30" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="18">
         <v>29</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="5"/>
       <c r="D30" s="9" t="s">
         <v>48</v>
@@ -4098,43 +4113,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="18"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
-      <c r="AD32" s="18"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="19">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="24">
         <v>43293</v>
       </c>
-      <c r="AG32" s="19"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="19"/>
-      <c r="AJ32" s="19"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4163,29 +4178,29 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="20"/>
-      <c r="BH32" s="20"/>
-      <c r="BI32" s="20"/>
-      <c r="BJ32" s="20"/>
-      <c r="BK32" s="20"/>
-      <c r="BL32" s="20"/>
-      <c r="BM32" s="20"/>
-      <c r="BN32" s="20"/>
-      <c r="BO32" s="20"/>
-      <c r="BP32" s="20"/>
-      <c r="BQ32" s="20"/>
-      <c r="BR32" s="20"/>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="BV32" s="20"/>
-      <c r="BW32" s="20"/>
-      <c r="BX32" s="20"/>
-      <c r="BY32" s="20"/>
-      <c r="BZ32" s="20"/>
-      <c r="CA32" s="20"/>
+      <c r="BG32" s="25"/>
+      <c r="BH32" s="25"/>
+      <c r="BI32" s="25"/>
+      <c r="BJ32" s="25"/>
+      <c r="BK32" s="25"/>
+      <c r="BL32" s="25"/>
+      <c r="BM32" s="25"/>
+      <c r="BN32" s="25"/>
+      <c r="BO32" s="25"/>
+      <c r="BP32" s="25"/>
+      <c r="BQ32" s="25"/>
+      <c r="BR32" s="25"/>
+      <c r="BS32" s="25"/>
+      <c r="BT32" s="25"/>
+      <c r="BU32" s="25"/>
+      <c r="BV32" s="25"/>
+      <c r="BW32" s="25"/>
+      <c r="BX32" s="25"/>
+      <c r="BY32" s="25"/>
+      <c r="BZ32" s="25"/>
+      <c r="CA32" s="25"/>
     </row>
-    <row r="33" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>32</v>
       </c>
@@ -4235,27 +4250,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="16">
+      <c r="AP33" s="26">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="16"/>
-      <c r="AR33" s="16"/>
-      <c r="AS33" s="17" t="s">
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="17"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="17"/>
-      <c r="BB33" s="17"/>
-      <c r="BC33" s="17"/>
-      <c r="BD33" s="17"/>
-      <c r="BE33" s="17"/>
-      <c r="BF33" s="17"/>
+      <c r="AT33" s="27"/>
+      <c r="AU33" s="27"/>
+      <c r="AV33" s="27"/>
+      <c r="AW33" s="27"/>
+      <c r="AX33" s="27"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
+      <c r="BA33" s="27"/>
+      <c r="BB33" s="27"/>
+      <c r="BC33" s="27"/>
+      <c r="BD33" s="27"/>
+      <c r="BE33" s="27"/>
+      <c r="BF33" s="27"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4279,10 +4294,10 @@
       <c r="CA33" s="12"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+      <c r="A34" s="18">
         <v>33</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="18"/>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>50</v>
@@ -4557,42 +4572,42 @@
       <c r="BZ36" s="12"/>
       <c r="CA36" s="12"/>
     </row>
-    <row r="37" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>36</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-      <c r="V37" s="14"/>
-      <c r="W37" s="14"/>
-      <c r="X37" s="14"/>
-      <c r="Y37" s="14"/>
-      <c r="Z37" s="14"/>
-      <c r="AA37" s="14"/>
-      <c r="AB37" s="14"/>
-      <c r="AC37" s="14"/>
-      <c r="AD37" s="14"/>
-      <c r="AE37" s="15"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="30"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4651,41 +4666,41 @@
       <c r="CA37" s="12"/>
     </row>
     <row r="38" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="A38" s="18">
         <v>37</v>
       </c>
-      <c r="B38" s="8"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-      <c r="V38" s="14"/>
-      <c r="W38" s="14"/>
-      <c r="X38" s="14"/>
-      <c r="Y38" s="14"/>
-      <c r="Z38" s="14"/>
-      <c r="AA38" s="14"/>
-      <c r="AB38" s="14"/>
-      <c r="AC38" s="14"/>
-      <c r="AD38" s="14"/>
-      <c r="AE38" s="15"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="30"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4842,36 +4857,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14"/>
-      <c r="Y40" s="14"/>
-      <c r="Z40" s="14"/>
-      <c r="AA40" s="14"/>
-      <c r="AB40" s="14"/>
-      <c r="AC40" s="14"/>
-      <c r="AD40" s="14"/>
-      <c r="AE40" s="15"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="30"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4929,7 +4944,7 @@
       <c r="BZ40" s="12"/>
       <c r="CA40" s="12"/>
     </row>
-    <row r="41" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>40</v>
       </c>
@@ -5023,41 +5038,41 @@
       <c r="CA41" s="12"/>
     </row>
     <row r="42" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
+      <c r="A42" s="18">
         <v>41</v>
       </c>
-      <c r="B42" s="8"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="14"/>
-      <c r="Y42" s="14"/>
-      <c r="Z42" s="14"/>
-      <c r="AA42" s="14"/>
-      <c r="AB42" s="14"/>
-      <c r="AC42" s="14"/>
-      <c r="AD42" s="14"/>
-      <c r="AE42" s="15"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="30"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5121,36 +5136,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="15"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="30"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5214,36 +5229,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="14"/>
-      <c r="Y44" s="14"/>
-      <c r="Z44" s="14"/>
-      <c r="AA44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AC44" s="14"/>
-      <c r="AD44" s="14"/>
-      <c r="AE44" s="15"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="30"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -5301,7 +5316,7 @@
       <c r="BZ44" s="12"/>
       <c r="CA44" s="12"/>
     </row>
-    <row r="45" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>44</v>
       </c>
@@ -5395,10 +5410,10 @@
       <c r="CA45" s="12"/>
     </row>
     <row r="46" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
+      <c r="A46" s="18">
         <v>45</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="5"/>
       <c r="D46" s="9" t="s">
         <v>60</v>
@@ -5673,7 +5688,7 @@
       <c r="BZ48" s="12"/>
       <c r="CA48" s="12"/>
     </row>
-    <row r="49" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>48</v>
       </c>
@@ -5767,10 +5782,10 @@
       <c r="CA49" s="12"/>
     </row>
     <row r="50" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
+      <c r="A50" s="18">
         <v>49</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="18"/>
       <c r="C50" s="5"/>
       <c r="D50" s="9" t="s">
         <v>65</v>
@@ -6045,7 +6060,7 @@
       <c r="BZ52" s="12"/>
       <c r="CA52" s="12"/>
     </row>
-    <row r="53" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>52</v>
       </c>
@@ -6139,10 +6154,10 @@
       <c r="CA53" s="12"/>
     </row>
     <row r="54" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
+      <c r="A54" s="18">
         <v>53</v>
       </c>
-      <c r="B54" s="8"/>
+      <c r="B54" s="18"/>
       <c r="C54" s="5"/>
       <c r="D54" s="9" t="s">
         <v>69</v>
@@ -6417,7 +6432,7 @@
       <c r="BZ56" s="12"/>
       <c r="CA56" s="12"/>
     </row>
-    <row r="57" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>56</v>
       </c>
@@ -6511,10 +6526,10 @@
       <c r="CA57" s="12"/>
     </row>
     <row r="58" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
+      <c r="A58" s="18">
         <v>57</v>
       </c>
-      <c r="B58" s="8"/>
+      <c r="B58" s="18"/>
       <c r="C58" s="5"/>
       <c r="D58" s="9" t="s">
         <v>75</v>
@@ -6789,7 +6804,7 @@
       <c r="BZ60" s="12"/>
       <c r="CA60" s="12"/>
     </row>
-    <row r="61" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>60</v>
       </c>
@@ -6883,10 +6898,10 @@
       <c r="CA61" s="12"/>
     </row>
     <row r="62" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A62" s="8">
-        <v>60</v>
-      </c>
-      <c r="B62" s="8"/>
+      <c r="A62" s="18">
+        <v>61</v>
+      </c>
+      <c r="B62" s="18"/>
       <c r="C62" s="5"/>
       <c r="D62" s="9" t="s">
         <v>78</v>
@@ -6977,7 +6992,7 @@
     </row>
     <row r="63" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="5"/>
@@ -7070,7 +7085,7 @@
     </row>
     <row r="64" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="5"/>
@@ -7161,9 +7176,9 @@
       <c r="BZ64" s="12"/>
       <c r="CA64" s="12"/>
     </row>
-    <row r="65" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="5"/>
@@ -7253,10 +7268,10 @@
       <c r="CA65" s="12"/>
     </row>
     <row r="66" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A66" s="8">
-        <v>60</v>
-      </c>
-      <c r="B66" s="8"/>
+      <c r="A66" s="18">
+        <v>65</v>
+      </c>
+      <c r="B66" s="18"/>
       <c r="C66" s="5"/>
       <c r="D66" s="9" t="s">
         <v>85</v>
@@ -7347,7 +7362,7 @@
     </row>
     <row r="67" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="5"/>
@@ -7440,7 +7455,7 @@
     </row>
     <row r="68" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="5"/>
@@ -7531,9 +7546,9 @@
       <c r="BZ68" s="12"/>
       <c r="CA68" s="12"/>
     </row>
-    <row r="69" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="5"/>
@@ -7625,10 +7640,10 @@
       <c r="CA69" s="12"/>
     </row>
     <row r="70" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A70" s="8">
-        <v>60</v>
-      </c>
-      <c r="B70" s="8"/>
+      <c r="A70" s="18">
+        <v>69</v>
+      </c>
+      <c r="B70" s="18"/>
       <c r="C70" s="5"/>
       <c r="D70" s="9" t="s">
         <v>90</v>
@@ -7719,7 +7734,7 @@
     </row>
     <row r="71" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B71" s="8"/>
       <c r="C71" s="5"/>
@@ -7812,7 +7827,7 @@
     </row>
     <row r="72" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="5"/>
@@ -7903,9 +7918,9 @@
       <c r="BZ72" s="12"/>
       <c r="CA72" s="12"/>
     </row>
-    <row r="73" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="5"/>
@@ -7997,10 +8012,10 @@
       <c r="CA73" s="12"/>
     </row>
     <row r="74" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
-        <v>60</v>
-      </c>
-      <c r="B74" s="8"/>
+      <c r="A74" s="18">
+        <v>73</v>
+      </c>
+      <c r="B74" s="18"/>
       <c r="C74" s="5"/>
       <c r="D74" s="9" t="s">
         <v>93</v>
@@ -8091,7 +8106,7 @@
     </row>
     <row r="75" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="5"/>
@@ -8184,7 +8199,7 @@
     </row>
     <row r="76" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="5"/>
@@ -8275,9 +8290,9 @@
       <c r="BZ76" s="12"/>
       <c r="CA76" s="12"/>
     </row>
-    <row r="77" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="8">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="5"/>
@@ -8369,10 +8384,10 @@
       <c r="CA77" s="12"/>
     </row>
     <row r="78" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
-        <v>60</v>
-      </c>
-      <c r="B78" s="8"/>
+      <c r="A78" s="18">
+        <v>77</v>
+      </c>
+      <c r="B78" s="18"/>
       <c r="C78" s="5"/>
       <c r="D78" s="9" t="s">
         <v>97</v>
@@ -8463,7 +8478,7 @@
     </row>
     <row r="79" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="5"/>
@@ -8556,7 +8571,7 @@
     </row>
     <row r="80" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="5"/>
@@ -8647,9 +8662,9 @@
       <c r="BZ80" s="12"/>
       <c r="CA80" s="12"/>
     </row>
-    <row r="81" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="5"/>
@@ -8741,10 +8756,10 @@
       <c r="CA81" s="12"/>
     </row>
     <row r="82" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A82" s="8">
-        <v>60</v>
-      </c>
-      <c r="B82" s="8"/>
+      <c r="A82" s="18">
+        <v>81</v>
+      </c>
+      <c r="B82" s="18"/>
       <c r="C82" s="5"/>
       <c r="D82" s="9" t="s">
         <v>99</v>
@@ -8835,7 +8850,7 @@
     </row>
     <row r="83" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="5"/>
@@ -8928,7 +8943,7 @@
     </row>
     <row r="84" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="5"/>
@@ -9019,9 +9034,9 @@
       <c r="BZ84" s="12"/>
       <c r="CA84" s="12"/>
     </row>
-    <row r="85" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="5"/>
@@ -9113,10 +9128,10 @@
       <c r="CA85" s="12"/>
     </row>
     <row r="86" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A86" s="8">
-        <v>60</v>
-      </c>
-      <c r="B86" s="8"/>
+      <c r="A86" s="18">
+        <v>85</v>
+      </c>
+      <c r="B86" s="18"/>
       <c r="C86" s="5"/>
       <c r="D86" s="9" t="s">
         <v>99</v>
@@ -9207,7 +9222,7 @@
     </row>
     <row r="87" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="5"/>
@@ -9300,7 +9315,7 @@
     </row>
     <row r="88" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="5"/>
@@ -9389,9 +9404,9 @@
       <c r="BZ88" s="12"/>
       <c r="CA88" s="12"/>
     </row>
-    <row r="89" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="5"/>
@@ -9481,10 +9496,10 @@
       <c r="CA89" s="12"/>
     </row>
     <row r="90" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A90" s="8">
-        <v>60</v>
-      </c>
-      <c r="B90" s="8"/>
+      <c r="A90" s="18">
+        <v>89</v>
+      </c>
+      <c r="B90" s="18"/>
       <c r="C90" s="5"/>
       <c r="D90" s="9" t="s">
         <v>105</v>
@@ -9573,7 +9588,7 @@
     </row>
     <row r="91" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="5"/>
@@ -9664,7 +9679,7 @@
     </row>
     <row r="92" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="5"/>
@@ -9755,9 +9770,9 @@
       <c r="BZ92" s="12"/>
       <c r="CA92" s="12"/>
     </row>
-    <row r="93" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="8">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="5"/>
@@ -9849,10 +9864,10 @@
       <c r="CA93" s="12"/>
     </row>
     <row r="94" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A94" s="8">
-        <v>60</v>
-      </c>
-      <c r="B94" s="8"/>
+      <c r="A94" s="18">
+        <v>93</v>
+      </c>
+      <c r="B94" s="18"/>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
         <v>109</v>
@@ -9943,7 +9958,7 @@
     </row>
     <row r="95" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="5"/>
@@ -10036,7 +10051,7 @@
     </row>
     <row r="96" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="5"/>
@@ -10127,9 +10142,9 @@
       <c r="BZ96" s="12"/>
       <c r="CA96" s="12"/>
     </row>
-    <row r="97" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="8">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="5"/>
@@ -10221,10 +10236,10 @@
       <c r="CA97" s="12"/>
     </row>
     <row r="98" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A98" s="8">
-        <v>60</v>
-      </c>
-      <c r="B98" s="8"/>
+      <c r="A98" s="18">
+        <v>97</v>
+      </c>
+      <c r="B98" s="18"/>
       <c r="C98" s="5"/>
       <c r="D98" s="9" t="s">
         <v>116</v>
@@ -10315,7 +10330,7 @@
     </row>
     <row r="99" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="5"/>
@@ -10408,11 +10423,13 @@
     </row>
     <row r="100" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="5"/>
-      <c r="D100" s="9"/>
+      <c r="D100" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
@@ -10440,20 +10457,28 @@
       <c r="AC100" s="9"/>
       <c r="AD100" s="9"/>
       <c r="AE100" s="9"/>
-      <c r="AF100" s="10"/>
+      <c r="AF100" s="10" t="s">
+        <v>118</v>
+      </c>
       <c r="AG100" s="10"/>
       <c r="AH100" s="10"/>
       <c r="AI100" s="10"/>
       <c r="AJ100" s="10"/>
-      <c r="AK100" s="9"/>
+      <c r="AK100" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL100" s="9"/>
       <c r="AM100" s="9"/>
       <c r="AN100" s="9"/>
       <c r="AO100" s="9"/>
-      <c r="AP100" s="11"/>
+      <c r="AP100" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ100" s="11"/>
       <c r="AR100" s="11"/>
-      <c r="AS100" s="9"/>
+      <c r="AS100" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT100" s="9"/>
       <c r="AU100" s="9"/>
       <c r="AV100" s="9"/>
@@ -10489,13 +10514,15 @@
       <c r="BZ100" s="12"/>
       <c r="CA100" s="12"/>
     </row>
-    <row r="101" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="8">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="5"/>
-      <c r="D101" s="9"/>
+      <c r="D101" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
       <c r="G101" s="9"/>
@@ -10523,20 +10550,28 @@
       <c r="AC101" s="9"/>
       <c r="AD101" s="9"/>
       <c r="AE101" s="9"/>
-      <c r="AF101" s="10"/>
+      <c r="AF101" s="10" t="s">
+        <v>118</v>
+      </c>
       <c r="AG101" s="10"/>
       <c r="AH101" s="10"/>
       <c r="AI101" s="10"/>
       <c r="AJ101" s="10"/>
-      <c r="AK101" s="9"/>
+      <c r="AK101" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL101" s="9"/>
       <c r="AM101" s="9"/>
       <c r="AN101" s="9"/>
       <c r="AO101" s="9"/>
-      <c r="AP101" s="11"/>
+      <c r="AP101" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ101" s="11"/>
       <c r="AR101" s="11"/>
-      <c r="AS101" s="9"/>
+      <c r="AS101" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT101" s="9"/>
       <c r="AU101" s="9"/>
       <c r="AV101" s="9"/>
@@ -10573,12 +10608,14 @@
       <c r="CA101" s="12"/>
     </row>
     <row r="102" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A102" s="8">
-        <v>60</v>
-      </c>
-      <c r="B102" s="8"/>
+      <c r="A102" s="18">
+        <v>101</v>
+      </c>
+      <c r="B102" s="18"/>
       <c r="C102" s="5"/>
-      <c r="D102" s="9"/>
+      <c r="D102" s="9" t="s">
+        <v>120</v>
+      </c>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
       <c r="G102" s="9"/>
@@ -10606,20 +10643,28 @@
       <c r="AC102" s="9"/>
       <c r="AD102" s="9"/>
       <c r="AE102" s="9"/>
-      <c r="AF102" s="10"/>
+      <c r="AF102" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="AG102" s="10"/>
       <c r="AH102" s="10"/>
       <c r="AI102" s="10"/>
       <c r="AJ102" s="10"/>
-      <c r="AK102" s="9"/>
+      <c r="AK102" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL102" s="9"/>
       <c r="AM102" s="9"/>
       <c r="AN102" s="9"/>
       <c r="AO102" s="9"/>
-      <c r="AP102" s="11"/>
+      <c r="AP102" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ102" s="11"/>
       <c r="AR102" s="11"/>
-      <c r="AS102" s="9"/>
+      <c r="AS102" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT102" s="9"/>
       <c r="AU102" s="9"/>
       <c r="AV102" s="9"/>
@@ -10657,11 +10702,13 @@
     </row>
     <row r="103" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="5"/>
-      <c r="D103" s="9"/>
+      <c r="D103" s="9" t="s">
+        <v>121</v>
+      </c>
       <c r="E103" s="9"/>
       <c r="F103" s="9"/>
       <c r="G103" s="9"/>
@@ -10689,20 +10736,28 @@
       <c r="AC103" s="9"/>
       <c r="AD103" s="9"/>
       <c r="AE103" s="9"/>
-      <c r="AF103" s="10"/>
+      <c r="AF103" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="AG103" s="10"/>
       <c r="AH103" s="10"/>
       <c r="AI103" s="10"/>
       <c r="AJ103" s="10"/>
-      <c r="AK103" s="9"/>
+      <c r="AK103" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL103" s="9"/>
       <c r="AM103" s="9"/>
       <c r="AN103" s="9"/>
       <c r="AO103" s="9"/>
-      <c r="AP103" s="11"/>
+      <c r="AP103" s="11">
+        <v>0.1</v>
+      </c>
       <c r="AQ103" s="11"/>
       <c r="AR103" s="11"/>
-      <c r="AS103" s="9"/>
+      <c r="AS103" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT103" s="9"/>
       <c r="AU103" s="9"/>
       <c r="AV103" s="9"/>
@@ -10740,7 +10795,7 @@
     </row>
     <row r="104" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="5"/>
@@ -10821,9 +10876,9 @@
       <c r="BZ104" s="12"/>
       <c r="CA104" s="12"/>
     </row>
-    <row r="105" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="8">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="B105" s="8"/>
       <c r="C105" s="5"/>
@@ -10905,10 +10960,10 @@
       <c r="CA105" s="12"/>
     </row>
     <row r="106" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A106" s="8">
-        <v>60</v>
-      </c>
-      <c r="B106" s="8"/>
+      <c r="A106" s="18">
+        <v>105</v>
+      </c>
+      <c r="B106" s="18"/>
       <c r="C106" s="5"/>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
@@ -10989,7 +11044,7 @@
     </row>
     <row r="107" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="5"/>
@@ -11072,7 +11127,7 @@
     </row>
     <row r="108" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="5"/>
@@ -11153,9 +11208,9 @@
       <c r="BZ108" s="12"/>
       <c r="CA108" s="12"/>
     </row>
-    <row r="109" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="8">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B109" s="8"/>
       <c r="C109" s="5"/>
@@ -11237,10 +11292,10 @@
       <c r="CA109" s="12"/>
     </row>
     <row r="110" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A110" s="8">
-        <v>60</v>
-      </c>
-      <c r="B110" s="8"/>
+      <c r="A110" s="18">
+        <v>109</v>
+      </c>
+      <c r="B110" s="18"/>
       <c r="C110" s="5"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
@@ -11321,7 +11376,7 @@
     </row>
     <row r="111" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="5"/>
@@ -11404,7 +11459,7 @@
     </row>
     <row r="112" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="5"/>
@@ -11485,9 +11540,9 @@
       <c r="BZ112" s="12"/>
       <c r="CA112" s="12"/>
     </row>
-    <row r="113" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="8">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="B113" s="8"/>
       <c r="C113" s="5"/>
@@ -11569,10 +11624,10 @@
       <c r="CA113" s="12"/>
     </row>
     <row r="114" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A114" s="8">
-        <v>60</v>
-      </c>
-      <c r="B114" s="8"/>
+      <c r="A114" s="18">
+        <v>113</v>
+      </c>
+      <c r="B114" s="18"/>
       <c r="C114" s="5"/>
       <c r="D114" s="9"/>
       <c r="E114" s="9"/>
@@ -11653,7 +11708,7 @@
     </row>
     <row r="115" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A115" s="8">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="B115" s="8"/>
       <c r="C115" s="5"/>
@@ -11736,7 +11791,7 @@
     </row>
     <row r="116" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A116" s="8">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B116" s="8"/>
       <c r="C116" s="5"/>
@@ -11817,9 +11872,9 @@
       <c r="BZ116" s="12"/>
       <c r="CA116" s="12"/>
     </row>
-    <row r="117" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="8">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="5"/>
@@ -11901,10 +11956,10 @@
       <c r="CA117" s="12"/>
     </row>
     <row r="118" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A118" s="8">
-        <v>60</v>
-      </c>
-      <c r="B118" s="8"/>
+      <c r="A118" s="18">
+        <v>117</v>
+      </c>
+      <c r="B118" s="18"/>
       <c r="C118" s="5"/>
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
@@ -11985,7 +12040,7 @@
     </row>
     <row r="119" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A119" s="8">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="B119" s="8"/>
       <c r="C119" s="5"/>
@@ -12068,7 +12123,7 @@
     </row>
     <row r="120" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A120" s="8">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="5"/>
@@ -12149,9 +12204,9 @@
       <c r="BZ120" s="12"/>
       <c r="CA120" s="12"/>
     </row>
-    <row r="121" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="8">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="5"/>
@@ -12233,10 +12288,10 @@
       <c r="CA121" s="12"/>
     </row>
     <row r="122" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A122" s="8">
-        <v>60</v>
-      </c>
-      <c r="B122" s="8"/>
+      <c r="A122" s="18">
+        <v>121</v>
+      </c>
+      <c r="B122" s="18"/>
       <c r="C122" s="5"/>
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
@@ -12317,7 +12372,7 @@
     </row>
     <row r="123" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A123" s="8">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="B123" s="8"/>
       <c r="C123" s="5"/>
@@ -12400,356 +12455,493 @@
     </row>
   </sheetData>
   <mergeCells count="861">
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12774,493 +12966,356 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="BG123:CA123"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Báo cáo ngày 25/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="124">
   <si>
     <t>No.</t>
   </si>
@@ -382,13 +382,16 @@
     <t>Trang tạo mới  -Test</t>
   </si>
   <si>
-    <t>Trang tạo mới  -Tìm hiểu về cron expression hangfire</t>
-  </si>
-  <si>
     <t>Trang tạo mới  -Thay đổi giao diện step 1</t>
   </si>
   <si>
     <t>24/1/2019</t>
+  </si>
+  <si>
+    <t>25/1/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trang tạo mới  -Thực hiện đồng bộ </t>
   </si>
 </sst>
 </file>
@@ -656,6 +659,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -671,19 +683,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,7 +792,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1180,7 +1183,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1191,8 +1194,8 @@
   <dimension ref="A1:CA123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D116" sqref="D116:AE116"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP104" sqref="AP104:AR104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,192 +1210,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="15" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="14" t="s">
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="16" t="s">
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="14" t="s">
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
-      <c r="BC1" s="14"/>
-      <c r="BD1" s="14"/>
-      <c r="BE1" s="14"/>
-      <c r="BF1" s="14"/>
-      <c r="BG1" s="17" t="s">
+      <c r="AT1" s="23"/>
+      <c r="AU1" s="23"/>
+      <c r="AV1" s="23"/>
+      <c r="AW1" s="23"/>
+      <c r="AX1" s="23"/>
+      <c r="AY1" s="23"/>
+      <c r="AZ1" s="23"/>
+      <c r="BA1" s="23"/>
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23"/>
+      <c r="BG1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="17"/>
-      <c r="BP1" s="17"/>
-      <c r="BQ1" s="17"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="17"/>
-      <c r="BT1" s="17"/>
-      <c r="BU1" s="17"/>
-      <c r="BV1" s="17"/>
-      <c r="BW1" s="17"/>
-      <c r="BX1" s="17"/>
-      <c r="BY1" s="17"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
+      <c r="BH1" s="26"/>
+      <c r="BI1" s="26"/>
+      <c r="BJ1" s="26"/>
+      <c r="BK1" s="26"/>
+      <c r="BL1" s="26"/>
+      <c r="BM1" s="26"/>
+      <c r="BN1" s="26"/>
+      <c r="BO1" s="26"/>
+      <c r="BP1" s="26"/>
+      <c r="BQ1" s="26"/>
+      <c r="BR1" s="26"/>
+      <c r="BS1" s="26"/>
+      <c r="BT1" s="26"/>
+      <c r="BU1" s="26"/>
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26"/>
+      <c r="CA1" s="26"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="20" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="19" t="s">
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="21">
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="29">
         <v>1</v>
       </c>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="19" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
-      <c r="BN2" s="22"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2" s="22"/>
-      <c r="BQ2" s="22"/>
-      <c r="BR2" s="22"/>
-      <c r="BS2" s="22"/>
-      <c r="BT2" s="22"/>
-      <c r="BU2" s="22"/>
-      <c r="BV2" s="22"/>
-      <c r="BW2" s="22"/>
-      <c r="BX2" s="22"/>
-      <c r="BY2" s="22"/>
-      <c r="BZ2" s="22"/>
-      <c r="CA2" s="22"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="30"/>
+      <c r="BJ2" s="30"/>
+      <c r="BK2" s="30"/>
+      <c r="BL2" s="30"/>
+      <c r="BM2" s="30"/>
+      <c r="BN2" s="30"/>
+      <c r="BO2" s="30"/>
+      <c r="BP2" s="30"/>
+      <c r="BQ2" s="30"/>
+      <c r="BR2" s="30"/>
+      <c r="BS2" s="30"/>
+      <c r="BT2" s="30"/>
+      <c r="BU2" s="30"/>
+      <c r="BV2" s="30"/>
+      <c r="BW2" s="30"/>
+      <c r="BX2" s="30"/>
+      <c r="BY2" s="30"/>
+      <c r="BZ2" s="30"/>
+      <c r="CA2" s="30"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -1676,10 +1679,10 @@
       <c r="CA5" s="12"/>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -2050,10 +2053,10 @@
       <c r="CA9" s="12"/>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
         <v>33</v>
@@ -2424,10 +2427,10 @@
       <c r="CA13" s="12"/>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="9" t="s">
         <v>33</v>
@@ -2800,10 +2803,10 @@
       <c r="CA17" s="12"/>
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="18"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
         <v>38</v>
@@ -3172,10 +3175,10 @@
       <c r="CA21" s="12"/>
     </row>
     <row r="22" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
+      <c r="A22" s="13">
         <v>21</v>
       </c>
-      <c r="B22" s="18"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="9" t="s">
         <v>44</v>
@@ -3548,10 +3551,10 @@
       <c r="CA25" s="12"/>
     </row>
     <row r="26" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A26" s="18">
+      <c r="A26" s="13">
         <v>25</v>
       </c>
-      <c r="B26" s="18"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
         <v>38</v>
@@ -3922,10 +3925,10 @@
       <c r="CA29" s="12"/>
     </row>
     <row r="30" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A30" s="18">
+      <c r="A30" s="13">
         <v>29</v>
       </c>
-      <c r="B30" s="18"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="5"/>
       <c r="D30" s="9" t="s">
         <v>48</v>
@@ -4113,43 +4116,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="23"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="23"/>
-      <c r="AD32" s="23"/>
-      <c r="AE32" s="23"/>
-      <c r="AF32" s="24">
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="19"/>
+      <c r="AC32" s="19"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="19"/>
+      <c r="AF32" s="20">
         <v>43293</v>
       </c>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="24"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="24"/>
+      <c r="AG32" s="20"/>
+      <c r="AH32" s="20"/>
+      <c r="AI32" s="20"/>
+      <c r="AJ32" s="20"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4178,27 +4181,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="25"/>
-      <c r="BH32" s="25"/>
-      <c r="BI32" s="25"/>
-      <c r="BJ32" s="25"/>
-      <c r="BK32" s="25"/>
-      <c r="BL32" s="25"/>
-      <c r="BM32" s="25"/>
-      <c r="BN32" s="25"/>
-      <c r="BO32" s="25"/>
-      <c r="BP32" s="25"/>
-      <c r="BQ32" s="25"/>
-      <c r="BR32" s="25"/>
-      <c r="BS32" s="25"/>
-      <c r="BT32" s="25"/>
-      <c r="BU32" s="25"/>
-      <c r="BV32" s="25"/>
-      <c r="BW32" s="25"/>
-      <c r="BX32" s="25"/>
-      <c r="BY32" s="25"/>
-      <c r="BZ32" s="25"/>
-      <c r="CA32" s="25"/>
+      <c r="BG32" s="21"/>
+      <c r="BH32" s="21"/>
+      <c r="BI32" s="21"/>
+      <c r="BJ32" s="21"/>
+      <c r="BK32" s="21"/>
+      <c r="BL32" s="21"/>
+      <c r="BM32" s="21"/>
+      <c r="BN32" s="21"/>
+      <c r="BO32" s="21"/>
+      <c r="BP32" s="21"/>
+      <c r="BQ32" s="21"/>
+      <c r="BR32" s="21"/>
+      <c r="BS32" s="21"/>
+      <c r="BT32" s="21"/>
+      <c r="BU32" s="21"/>
+      <c r="BV32" s="21"/>
+      <c r="BW32" s="21"/>
+      <c r="BX32" s="21"/>
+      <c r="BY32" s="21"/>
+      <c r="BZ32" s="21"/>
+      <c r="CA32" s="21"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
@@ -4250,27 +4253,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="26">
+      <c r="AP33" s="17">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="27" t="s">
+      <c r="AQ33" s="17"/>
+      <c r="AR33" s="17"/>
+      <c r="AS33" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="27"/>
-      <c r="AU33" s="27"/>
-      <c r="AV33" s="27"/>
-      <c r="AW33" s="27"/>
-      <c r="AX33" s="27"/>
-      <c r="AY33" s="27"/>
-      <c r="AZ33" s="27"/>
-      <c r="BA33" s="27"/>
-      <c r="BB33" s="27"/>
-      <c r="BC33" s="27"/>
-      <c r="BD33" s="27"/>
-      <c r="BE33" s="27"/>
-      <c r="BF33" s="27"/>
+      <c r="AT33" s="18"/>
+      <c r="AU33" s="18"/>
+      <c r="AV33" s="18"/>
+      <c r="AW33" s="18"/>
+      <c r="AX33" s="18"/>
+      <c r="AY33" s="18"/>
+      <c r="AZ33" s="18"/>
+      <c r="BA33" s="18"/>
+      <c r="BB33" s="18"/>
+      <c r="BC33" s="18"/>
+      <c r="BD33" s="18"/>
+      <c r="BE33" s="18"/>
+      <c r="BF33" s="18"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4294,10 +4297,10 @@
       <c r="CA33" s="12"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A34" s="18">
+      <c r="A34" s="13">
         <v>33</v>
       </c>
-      <c r="B34" s="18"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>50</v>
@@ -4578,36 +4581,36 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="29"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="30"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="15"/>
+      <c r="AD37" s="15"/>
+      <c r="AE37" s="16"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4666,41 +4669,41 @@
       <c r="CA37" s="12"/>
     </row>
     <row r="38" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A38" s="18">
+      <c r="A38" s="13">
         <v>37</v>
       </c>
-      <c r="B38" s="18"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="30"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
+      <c r="AC38" s="15"/>
+      <c r="AD38" s="15"/>
+      <c r="AE38" s="16"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4857,36 +4860,36 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="30"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="15"/>
+      <c r="AD40" s="15"/>
+      <c r="AE40" s="16"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -5038,41 +5041,41 @@
       <c r="CA41" s="12"/>
     </row>
     <row r="42" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A42" s="18">
+      <c r="A42" s="13">
         <v>41</v>
       </c>
-      <c r="B42" s="18"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="30"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
+      <c r="AD42" s="15"/>
+      <c r="AE42" s="16"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5136,36 +5139,36 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="30"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="15"/>
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="15"/>
+      <c r="AC43" s="15"/>
+      <c r="AD43" s="15"/>
+      <c r="AE43" s="16"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5229,36 +5232,36 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="30"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="15"/>
+      <c r="AA44" s="15"/>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="15"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="16"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -5410,10 +5413,10 @@
       <c r="CA45" s="12"/>
     </row>
     <row r="46" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A46" s="18">
+      <c r="A46" s="13">
         <v>45</v>
       </c>
-      <c r="B46" s="18"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="5"/>
       <c r="D46" s="9" t="s">
         <v>60</v>
@@ -5782,10 +5785,10 @@
       <c r="CA49" s="12"/>
     </row>
     <row r="50" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A50" s="18">
+      <c r="A50" s="13">
         <v>49</v>
       </c>
-      <c r="B50" s="18"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="5"/>
       <c r="D50" s="9" t="s">
         <v>65</v>
@@ -6154,10 +6157,10 @@
       <c r="CA53" s="12"/>
     </row>
     <row r="54" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A54" s="18">
+      <c r="A54" s="13">
         <v>53</v>
       </c>
-      <c r="B54" s="18"/>
+      <c r="B54" s="13"/>
       <c r="C54" s="5"/>
       <c r="D54" s="9" t="s">
         <v>69</v>
@@ -6526,10 +6529,10 @@
       <c r="CA57" s="12"/>
     </row>
     <row r="58" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A58" s="18">
+      <c r="A58" s="13">
         <v>57</v>
       </c>
-      <c r="B58" s="18"/>
+      <c r="B58" s="13"/>
       <c r="C58" s="5"/>
       <c r="D58" s="9" t="s">
         <v>75</v>
@@ -6898,10 +6901,10 @@
       <c r="CA61" s="12"/>
     </row>
     <row r="62" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A62" s="18">
+      <c r="A62" s="13">
         <v>61</v>
       </c>
-      <c r="B62" s="18"/>
+      <c r="B62" s="13"/>
       <c r="C62" s="5"/>
       <c r="D62" s="9" t="s">
         <v>78</v>
@@ -7268,10 +7271,10 @@
       <c r="CA65" s="12"/>
     </row>
     <row r="66" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A66" s="18">
+      <c r="A66" s="13">
         <v>65</v>
       </c>
-      <c r="B66" s="18"/>
+      <c r="B66" s="13"/>
       <c r="C66" s="5"/>
       <c r="D66" s="9" t="s">
         <v>85</v>
@@ -7640,10 +7643,10 @@
       <c r="CA69" s="12"/>
     </row>
     <row r="70" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A70" s="18">
+      <c r="A70" s="13">
         <v>69</v>
       </c>
-      <c r="B70" s="18"/>
+      <c r="B70" s="13"/>
       <c r="C70" s="5"/>
       <c r="D70" s="9" t="s">
         <v>90</v>
@@ -8012,10 +8015,10 @@
       <c r="CA73" s="12"/>
     </row>
     <row r="74" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A74" s="18">
+      <c r="A74" s="13">
         <v>73</v>
       </c>
-      <c r="B74" s="18"/>
+      <c r="B74" s="13"/>
       <c r="C74" s="5"/>
       <c r="D74" s="9" t="s">
         <v>93</v>
@@ -8384,10 +8387,10 @@
       <c r="CA77" s="12"/>
     </row>
     <row r="78" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A78" s="18">
+      <c r="A78" s="13">
         <v>77</v>
       </c>
-      <c r="B78" s="18"/>
+      <c r="B78" s="13"/>
       <c r="C78" s="5"/>
       <c r="D78" s="9" t="s">
         <v>97</v>
@@ -8756,10 +8759,10 @@
       <c r="CA81" s="12"/>
     </row>
     <row r="82" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A82" s="18">
+      <c r="A82" s="13">
         <v>81</v>
       </c>
-      <c r="B82" s="18"/>
+      <c r="B82" s="13"/>
       <c r="C82" s="5"/>
       <c r="D82" s="9" t="s">
         <v>99</v>
@@ -9128,10 +9131,10 @@
       <c r="CA85" s="12"/>
     </row>
     <row r="86" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A86" s="18">
+      <c r="A86" s="13">
         <v>85</v>
       </c>
-      <c r="B86" s="18"/>
+      <c r="B86" s="13"/>
       <c r="C86" s="5"/>
       <c r="D86" s="9" t="s">
         <v>99</v>
@@ -9496,10 +9499,10 @@
       <c r="CA89" s="12"/>
     </row>
     <row r="90" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A90" s="18">
+      <c r="A90" s="13">
         <v>89</v>
       </c>
-      <c r="B90" s="18"/>
+      <c r="B90" s="13"/>
       <c r="C90" s="5"/>
       <c r="D90" s="9" t="s">
         <v>105</v>
@@ -9864,10 +9867,10 @@
       <c r="CA93" s="12"/>
     </row>
     <row r="94" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A94" s="18">
+      <c r="A94" s="13">
         <v>93</v>
       </c>
-      <c r="B94" s="18"/>
+      <c r="B94" s="13"/>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
         <v>109</v>
@@ -10236,10 +10239,10 @@
       <c r="CA97" s="12"/>
     </row>
     <row r="98" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A98" s="18">
+      <c r="A98" s="13">
         <v>97</v>
       </c>
-      <c r="B98" s="18"/>
+      <c r="B98" s="13"/>
       <c r="C98" s="5"/>
       <c r="D98" s="9" t="s">
         <v>116</v>
@@ -10608,10 +10611,10 @@
       <c r="CA101" s="12"/>
     </row>
     <row r="102" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A102" s="18">
+      <c r="A102" s="13">
         <v>101</v>
       </c>
-      <c r="B102" s="18"/>
+      <c r="B102" s="13"/>
       <c r="C102" s="5"/>
       <c r="D102" s="9" t="s">
         <v>120</v>
@@ -10644,7 +10647,7 @@
       <c r="AD102" s="9"/>
       <c r="AE102" s="9"/>
       <c r="AF102" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AG102" s="10"/>
       <c r="AH102" s="10"/>
@@ -10658,7 +10661,7 @@
       <c r="AN102" s="9"/>
       <c r="AO102" s="9"/>
       <c r="AP102" s="11">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AQ102" s="11"/>
       <c r="AR102" s="11"/>
@@ -10707,7 +10710,7 @@
       <c r="B103" s="8"/>
       <c r="C103" s="5"/>
       <c r="D103" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E103" s="9"/>
       <c r="F103" s="9"/>
@@ -10751,7 +10754,7 @@
       <c r="AN103" s="9"/>
       <c r="AO103" s="9"/>
       <c r="AP103" s="11">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AQ103" s="11"/>
       <c r="AR103" s="11"/>
@@ -10799,7 +10802,9 @@
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="5"/>
-      <c r="D104" s="9"/>
+      <c r="D104" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
       <c r="G104" s="9"/>
@@ -10827,20 +10832,28 @@
       <c r="AC104" s="9"/>
       <c r="AD104" s="9"/>
       <c r="AE104" s="9"/>
-      <c r="AF104" s="10"/>
+      <c r="AF104" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="AG104" s="10"/>
       <c r="AH104" s="10"/>
       <c r="AI104" s="10"/>
       <c r="AJ104" s="10"/>
-      <c r="AK104" s="9"/>
+      <c r="AK104" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL104" s="9"/>
       <c r="AM104" s="9"/>
       <c r="AN104" s="9"/>
       <c r="AO104" s="9"/>
-      <c r="AP104" s="11"/>
+      <c r="AP104" s="11">
+        <v>0.4</v>
+      </c>
       <c r="AQ104" s="11"/>
       <c r="AR104" s="11"/>
-      <c r="AS104" s="9"/>
+      <c r="AS104" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT104" s="9"/>
       <c r="AU104" s="9"/>
       <c r="AV104" s="9"/>
@@ -10960,10 +10973,10 @@
       <c r="CA105" s="12"/>
     </row>
     <row r="106" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A106" s="18">
+      <c r="A106" s="13">
         <v>105</v>
       </c>
-      <c r="B106" s="18"/>
+      <c r="B106" s="13"/>
       <c r="C106" s="5"/>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
@@ -11292,10 +11305,10 @@
       <c r="CA109" s="12"/>
     </row>
     <row r="110" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A110" s="18">
+      <c r="A110" s="13">
         <v>109</v>
       </c>
-      <c r="B110" s="18"/>
+      <c r="B110" s="13"/>
       <c r="C110" s="5"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
@@ -11624,10 +11637,10 @@
       <c r="CA113" s="12"/>
     </row>
     <row r="114" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A114" s="18">
+      <c r="A114" s="13">
         <v>113</v>
       </c>
-      <c r="B114" s="18"/>
+      <c r="B114" s="13"/>
       <c r="C114" s="5"/>
       <c r="D114" s="9"/>
       <c r="E114" s="9"/>
@@ -11956,10 +11969,10 @@
       <c r="CA117" s="12"/>
     </row>
     <row r="118" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A118" s="18">
+      <c r="A118" s="13">
         <v>117</v>
       </c>
-      <c r="B118" s="18"/>
+      <c r="B118" s="13"/>
       <c r="C118" s="5"/>
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
@@ -12288,10 +12301,10 @@
       <c r="CA121" s="12"/>
     </row>
     <row r="122" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A122" s="18">
+      <c r="A122" s="13">
         <v>121</v>
       </c>
-      <c r="B122" s="18"/>
+      <c r="B122" s="13"/>
       <c r="C122" s="5"/>
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
@@ -12376,61 +12389,6 @@
       </c>
       <c r="B123" s="8"/>
       <c r="C123" s="5"/>
-      <c r="D123" s="9"/>
-      <c r="E123" s="9"/>
-      <c r="F123" s="9"/>
-      <c r="G123" s="9"/>
-      <c r="H123" s="9"/>
-      <c r="I123" s="9"/>
-      <c r="J123" s="9"/>
-      <c r="K123" s="9"/>
-      <c r="L123" s="9"/>
-      <c r="M123" s="9"/>
-      <c r="N123" s="9"/>
-      <c r="O123" s="9"/>
-      <c r="P123" s="9"/>
-      <c r="Q123" s="9"/>
-      <c r="R123" s="9"/>
-      <c r="S123" s="9"/>
-      <c r="T123" s="9"/>
-      <c r="U123" s="9"/>
-      <c r="V123" s="9"/>
-      <c r="W123" s="9"/>
-      <c r="X123" s="9"/>
-      <c r="Y123" s="9"/>
-      <c r="Z123" s="9"/>
-      <c r="AA123" s="9"/>
-      <c r="AB123" s="9"/>
-      <c r="AC123" s="9"/>
-      <c r="AD123" s="9"/>
-      <c r="AE123" s="9"/>
-      <c r="AF123" s="10"/>
-      <c r="AG123" s="10"/>
-      <c r="AH123" s="10"/>
-      <c r="AI123" s="10"/>
-      <c r="AJ123" s="10"/>
-      <c r="AK123" s="9"/>
-      <c r="AL123" s="9"/>
-      <c r="AM123" s="9"/>
-      <c r="AN123" s="9"/>
-      <c r="AO123" s="9"/>
-      <c r="AP123" s="11"/>
-      <c r="AQ123" s="11"/>
-      <c r="AR123" s="11"/>
-      <c r="AS123" s="9"/>
-      <c r="AT123" s="9"/>
-      <c r="AU123" s="9"/>
-      <c r="AV123" s="9"/>
-      <c r="AW123" s="9"/>
-      <c r="AX123" s="9"/>
-      <c r="AY123" s="9"/>
-      <c r="AZ123" s="9"/>
-      <c r="BA123" s="9"/>
-      <c r="BB123" s="9"/>
-      <c r="BC123" s="9"/>
-      <c r="BD123" s="9"/>
-      <c r="BE123" s="9"/>
-      <c r="BF123" s="9"/>
       <c r="BG123" s="12"/>
       <c r="BH123" s="12"/>
       <c r="BI123" s="12"/>
@@ -12454,494 +12412,352 @@
       <c r="CA123" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="861">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
+  <mergeCells count="856">
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12966,356 +12782,493 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">
@@ -13332,12 +13285,12 @@
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Info!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>AK3:AO123</xm:sqref>
+          <xm:sqref>AK2:AO122</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -13346,13 +13299,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>AS2:BF123</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Info!$A$1:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>AK2:AO2</xm:sqref>
+          <xm:sqref>AS2:BF122</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
báo cáo ngày 28/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="126">
   <si>
     <t>No.</t>
   </si>
@@ -392,6 +392,12 @@
   </si>
   <si>
     <t xml:space="preserve">Trang tạo mới  -Thực hiện đồng bộ </t>
+  </si>
+  <si>
+    <t>28/1/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Backup data</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1201,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP104" sqref="AP104:AR104"/>
+      <selection pane="bottomLeft" activeCell="D112" sqref="D112:AE112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10895,7 +10901,9 @@
       </c>
       <c r="B105" s="8"/>
       <c r="C105" s="5"/>
-      <c r="D105" s="9"/>
+      <c r="D105" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
       <c r="G105" s="9"/>
@@ -10923,20 +10931,28 @@
       <c r="AC105" s="9"/>
       <c r="AD105" s="9"/>
       <c r="AE105" s="9"/>
-      <c r="AF105" s="10"/>
+      <c r="AF105" s="10" t="s">
+        <v>124</v>
+      </c>
       <c r="AG105" s="10"/>
       <c r="AH105" s="10"/>
       <c r="AI105" s="10"/>
       <c r="AJ105" s="10"/>
-      <c r="AK105" s="9"/>
+      <c r="AK105" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL105" s="9"/>
       <c r="AM105" s="9"/>
       <c r="AN105" s="9"/>
       <c r="AO105" s="9"/>
-      <c r="AP105" s="11"/>
+      <c r="AP105" s="11">
+        <v>0.8</v>
+      </c>
       <c r="AQ105" s="11"/>
       <c r="AR105" s="11"/>
-      <c r="AS105" s="9"/>
+      <c r="AS105" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT105" s="9"/>
       <c r="AU105" s="9"/>
       <c r="AV105" s="9"/>
@@ -10978,7 +10994,9 @@
       </c>
       <c r="B106" s="13"/>
       <c r="C106" s="5"/>
-      <c r="D106" s="9"/>
+      <c r="D106" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
       <c r="G106" s="9"/>
@@ -11006,20 +11024,28 @@
       <c r="AC106" s="9"/>
       <c r="AD106" s="9"/>
       <c r="AE106" s="9"/>
-      <c r="AF106" s="10"/>
+      <c r="AF106" s="10" t="s">
+        <v>124</v>
+      </c>
       <c r="AG106" s="10"/>
       <c r="AH106" s="10"/>
       <c r="AI106" s="10"/>
       <c r="AJ106" s="10"/>
-      <c r="AK106" s="9"/>
+      <c r="AK106" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL106" s="9"/>
       <c r="AM106" s="9"/>
       <c r="AN106" s="9"/>
       <c r="AO106" s="9"/>
-      <c r="AP106" s="11"/>
+      <c r="AP106" s="11">
+        <v>0</v>
+      </c>
       <c r="AQ106" s="11"/>
       <c r="AR106" s="11"/>
-      <c r="AS106" s="9"/>
+      <c r="AS106" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT106" s="9"/>
       <c r="AU106" s="9"/>
       <c r="AV106" s="9"/>

</xml_diff>

<commit_message>
báo cáo ngày 29/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="127">
   <si>
     <t>No.</t>
   </si>
@@ -399,6 +399,9 @@
   <si>
     <t>Trang tạo mới  -Backup data</t>
   </si>
+  <si>
+    <t>29/1/2019</t>
+  </si>
 </sst>
 </file>
 
@@ -660,20 +663,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -693,6 +688,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,7 +801,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1189,7 +1192,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1201,7 +1204,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D112" sqref="D112:AE112"/>
+      <selection pane="bottomLeft" activeCell="AP108" sqref="AP108:AR108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,198 +1219,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="24" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="23" t="s">
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="25" t="s">
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="23" t="s">
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="23"/>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
-      <c r="BF1" s="23"/>
-      <c r="BG1" s="26" t="s">
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
+      <c r="AY1" s="15"/>
+      <c r="AZ1" s="15"/>
+      <c r="BA1" s="15"/>
+      <c r="BB1" s="15"/>
+      <c r="BC1" s="15"/>
+      <c r="BD1" s="15"/>
+      <c r="BE1" s="15"/>
+      <c r="BF1" s="15"/>
+      <c r="BG1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="26"/>
-      <c r="BI1" s="26"/>
-      <c r="BJ1" s="26"/>
-      <c r="BK1" s="26"/>
-      <c r="BL1" s="26"/>
-      <c r="BM1" s="26"/>
-      <c r="BN1" s="26"/>
-      <c r="BO1" s="26"/>
-      <c r="BP1" s="26"/>
-      <c r="BQ1" s="26"/>
-      <c r="BR1" s="26"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="26"/>
-      <c r="BU1" s="26"/>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="26"/>
-      <c r="BZ1" s="26"/>
-      <c r="CA1" s="26"/>
+      <c r="BH1" s="18"/>
+      <c r="BI1" s="18"/>
+      <c r="BJ1" s="18"/>
+      <c r="BK1" s="18"/>
+      <c r="BL1" s="18"/>
+      <c r="BM1" s="18"/>
+      <c r="BN1" s="18"/>
+      <c r="BO1" s="18"/>
+      <c r="BP1" s="18"/>
+      <c r="BQ1" s="18"/>
+      <c r="BR1" s="18"/>
+      <c r="BS1" s="18"/>
+      <c r="BT1" s="18"/>
+      <c r="BU1" s="18"/>
+      <c r="BV1" s="18"/>
+      <c r="BW1" s="18"/>
+      <c r="BX1" s="18"/>
+      <c r="BY1" s="18"/>
+      <c r="BZ1" s="18"/>
+      <c r="CA1" s="18"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="21">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="5"/>
       <c r="D3" s="9" t="s">
         <v>17</v>
@@ -1497,10 +1500,10 @@
       <c r="CA3" s="12"/>
     </row>
     <row r="4" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="5"/>
       <c r="D4" s="9" t="s">
         <v>18</v>
@@ -1590,10 +1593,10 @@
       <c r="CA4" s="12"/>
     </row>
     <row r="5" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="5"/>
       <c r="D5" s="9" t="s">
         <v>18</v>
@@ -1685,10 +1688,10 @@
       <c r="CA5" s="12"/>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -1778,10 +1781,10 @@
       <c r="CA6" s="12"/>
     </row>
     <row r="7" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
         <v>22</v>
@@ -1871,10 +1874,10 @@
       <c r="CA7" s="12"/>
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
         <v>24</v>
@@ -1964,10 +1967,10 @@
       <c r="CA8" s="12"/>
     </row>
     <row r="9" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
         <v>33</v>
@@ -2059,10 +2062,10 @@
       <c r="CA9" s="12"/>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
         <v>33</v>
@@ -2152,10 +2155,10 @@
       <c r="CA10" s="12"/>
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
         <v>33</v>
@@ -2245,10 +2248,10 @@
       <c r="CA11" s="12"/>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="9" t="s">
         <v>33</v>
@@ -2338,10 +2341,10 @@
       <c r="CA12" s="12"/>
     </row>
     <row r="13" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>33</v>
@@ -2433,10 +2436,10 @@
       <c r="CA13" s="12"/>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="13"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="5"/>
       <c r="D14" s="9" t="s">
         <v>33</v>
@@ -2528,10 +2531,10 @@
       <c r="CA14" s="12"/>
     </row>
     <row r="15" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
         <v>33</v>
@@ -2621,10 +2624,10 @@
       <c r="CA15" s="12"/>
     </row>
     <row r="16" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
         <v>36</v>
@@ -2714,10 +2717,10 @@
       <c r="CA16" s="12"/>
     </row>
     <row r="17" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
         <v>33</v>
@@ -2809,10 +2812,10 @@
       <c r="CA17" s="12"/>
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
         <v>38</v>
@@ -2902,10 +2905,10 @@
       <c r="CA18" s="12"/>
     </row>
     <row r="19" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
         <v>38</v>
@@ -2995,10 +2998,10 @@
       <c r="CA19" s="12"/>
     </row>
     <row r="20" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="13">
         <v>19</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="9" t="s">
         <v>38</v>
@@ -3088,10 +3091,10 @@
       <c r="CA20" s="12"/>
     </row>
     <row r="21" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="A21" s="13">
         <v>20</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="9" t="s">
         <v>38</v>
@@ -3181,10 +3184,10 @@
       <c r="CA21" s="12"/>
     </row>
     <row r="22" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="A22" s="8">
         <v>21</v>
       </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="5"/>
       <c r="D22" s="9" t="s">
         <v>44</v>
@@ -3276,10 +3279,10 @@
       <c r="CA22" s="12"/>
     </row>
     <row r="23" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="13">
         <v>22</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="9" t="s">
         <v>38</v>
@@ -3371,10 +3374,10 @@
       <c r="CA23" s="12"/>
     </row>
     <row r="24" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="13">
         <v>23</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="9" t="s">
         <v>33</v>
@@ -3464,10 +3467,10 @@
       <c r="CA24" s="12"/>
     </row>
     <row r="25" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8">
+      <c r="A25" s="13">
         <v>24</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="5"/>
       <c r="D25" s="9" t="s">
         <v>45</v>
@@ -3557,10 +3560,10 @@
       <c r="CA25" s="12"/>
     </row>
     <row r="26" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
+      <c r="A26" s="8">
         <v>25</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
         <v>38</v>
@@ -3650,10 +3653,10 @@
       <c r="CA26" s="12"/>
     </row>
     <row r="27" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="13">
         <v>26</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
         <v>33</v>
@@ -3743,10 +3746,10 @@
       <c r="CA27" s="12"/>
     </row>
     <row r="28" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="13">
         <v>27</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="9" t="s">
         <v>46</v>
@@ -3836,10 +3839,10 @@
       <c r="CA28" s="12"/>
     </row>
     <row r="29" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8">
+      <c r="A29" s="13">
         <v>28</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="9" t="s">
         <v>38</v>
@@ -3931,10 +3934,10 @@
       <c r="CA29" s="12"/>
     </row>
     <row r="30" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+      <c r="A30" s="8">
         <v>29</v>
       </c>
-      <c r="B30" s="13"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="5"/>
       <c r="D30" s="9" t="s">
         <v>48</v>
@@ -4024,10 +4027,10 @@
       <c r="CA30" s="12"/>
     </row>
     <row r="31" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="13">
         <v>30</v>
       </c>
-      <c r="B31" s="8"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="5"/>
       <c r="D31" s="9" t="s">
         <v>49</v>
@@ -4117,48 +4120,48 @@
       <c r="CA31" s="12"/>
     </row>
     <row r="32" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="13">
         <v>31</v>
       </c>
-      <c r="B32" s="8"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="19"/>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="19"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
-      <c r="AD32" s="19"/>
-      <c r="AE32" s="19"/>
-      <c r="AF32" s="20">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="24">
         <v>43293</v>
       </c>
-      <c r="AG32" s="20"/>
-      <c r="AH32" s="20"/>
-      <c r="AI32" s="20"/>
-      <c r="AJ32" s="20"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4187,33 +4190,33 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="21"/>
-      <c r="BH32" s="21"/>
-      <c r="BI32" s="21"/>
-      <c r="BJ32" s="21"/>
-      <c r="BK32" s="21"/>
-      <c r="BL32" s="21"/>
-      <c r="BM32" s="21"/>
-      <c r="BN32" s="21"/>
-      <c r="BO32" s="21"/>
-      <c r="BP32" s="21"/>
-      <c r="BQ32" s="21"/>
-      <c r="BR32" s="21"/>
-      <c r="BS32" s="21"/>
-      <c r="BT32" s="21"/>
-      <c r="BU32" s="21"/>
-      <c r="BV32" s="21"/>
-      <c r="BW32" s="21"/>
-      <c r="BX32" s="21"/>
-      <c r="BY32" s="21"/>
-      <c r="BZ32" s="21"/>
-      <c r="CA32" s="21"/>
+      <c r="BG32" s="25"/>
+      <c r="BH32" s="25"/>
+      <c r="BI32" s="25"/>
+      <c r="BJ32" s="25"/>
+      <c r="BK32" s="25"/>
+      <c r="BL32" s="25"/>
+      <c r="BM32" s="25"/>
+      <c r="BN32" s="25"/>
+      <c r="BO32" s="25"/>
+      <c r="BP32" s="25"/>
+      <c r="BQ32" s="25"/>
+      <c r="BR32" s="25"/>
+      <c r="BS32" s="25"/>
+      <c r="BT32" s="25"/>
+      <c r="BU32" s="25"/>
+      <c r="BV32" s="25"/>
+      <c r="BW32" s="25"/>
+      <c r="BX32" s="25"/>
+      <c r="BY32" s="25"/>
+      <c r="BZ32" s="25"/>
+      <c r="CA32" s="25"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
+      <c r="A33" s="13">
         <v>32</v>
       </c>
-      <c r="B33" s="8"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="7"/>
       <c r="D33" s="9" t="s">
         <v>50</v>
@@ -4259,27 +4262,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="17">
+      <c r="AP33" s="26">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="17"/>
-      <c r="AR33" s="17"/>
-      <c r="AS33" s="18" t="s">
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="18"/>
-      <c r="AU33" s="18"/>
-      <c r="AV33" s="18"/>
-      <c r="AW33" s="18"/>
-      <c r="AX33" s="18"/>
-      <c r="AY33" s="18"/>
-      <c r="AZ33" s="18"/>
-      <c r="BA33" s="18"/>
-      <c r="BB33" s="18"/>
-      <c r="BC33" s="18"/>
-      <c r="BD33" s="18"/>
-      <c r="BE33" s="18"/>
-      <c r="BF33" s="18"/>
+      <c r="AT33" s="27"/>
+      <c r="AU33" s="27"/>
+      <c r="AV33" s="27"/>
+      <c r="AW33" s="27"/>
+      <c r="AX33" s="27"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
+      <c r="BA33" s="27"/>
+      <c r="BB33" s="27"/>
+      <c r="BC33" s="27"/>
+      <c r="BD33" s="27"/>
+      <c r="BE33" s="27"/>
+      <c r="BF33" s="27"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4303,10 +4306,10 @@
       <c r="CA33" s="12"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
+      <c r="A34" s="8">
         <v>33</v>
       </c>
-      <c r="B34" s="13"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>50</v>
@@ -4396,10 +4399,10 @@
       <c r="CA34" s="12"/>
     </row>
     <row r="35" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="13">
         <v>34</v>
       </c>
-      <c r="B35" s="8"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
         <v>52</v>
@@ -4489,10 +4492,10 @@
       <c r="CA35" s="12"/>
     </row>
     <row r="36" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+      <c r="A36" s="13">
         <v>35</v>
       </c>
-      <c r="B36" s="8"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
         <v>52</v>
@@ -4582,41 +4585,41 @@
       <c r="CA36" s="12"/>
     </row>
     <row r="37" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8">
+      <c r="A37" s="13">
         <v>36</v>
       </c>
-      <c r="B37" s="8"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
-      <c r="V37" s="15"/>
-      <c r="W37" s="15"/>
-      <c r="X37" s="15"/>
-      <c r="Y37" s="15"/>
-      <c r="Z37" s="15"/>
-      <c r="AA37" s="15"/>
-      <c r="AB37" s="15"/>
-      <c r="AC37" s="15"/>
-      <c r="AD37" s="15"/>
-      <c r="AE37" s="16"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="30"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4675,41 +4678,41 @@
       <c r="CA37" s="12"/>
     </row>
     <row r="38" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
+      <c r="A38" s="8">
         <v>37</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="15"/>
-      <c r="Z38" s="15"/>
-      <c r="AA38" s="15"/>
-      <c r="AB38" s="15"/>
-      <c r="AC38" s="15"/>
-      <c r="AD38" s="15"/>
-      <c r="AE38" s="16"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="30"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4768,10 +4771,10 @@
       <c r="CA38" s="12"/>
     </row>
     <row r="39" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+      <c r="A39" s="13">
         <v>38</v>
       </c>
-      <c r="B39" s="8"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="5"/>
       <c r="D39" s="9" t="s">
         <v>53</v>
@@ -4861,41 +4864,41 @@
       <c r="CA39" s="12"/>
     </row>
     <row r="40" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+      <c r="A40" s="13">
         <v>39</v>
       </c>
-      <c r="B40" s="8"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
-      <c r="U40" s="15"/>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-      <c r="X40" s="15"/>
-      <c r="Y40" s="15"/>
-      <c r="Z40" s="15"/>
-      <c r="AA40" s="15"/>
-      <c r="AB40" s="15"/>
-      <c r="AC40" s="15"/>
-      <c r="AD40" s="15"/>
-      <c r="AE40" s="16"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="30"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4954,10 +4957,10 @@
       <c r="CA40" s="12"/>
     </row>
     <row r="41" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
+      <c r="A41" s="13">
         <v>40</v>
       </c>
-      <c r="B41" s="8"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="5"/>
       <c r="D41" s="9" t="s">
         <v>53</v>
@@ -5047,41 +5050,41 @@
       <c r="CA41" s="12"/>
     </row>
     <row r="42" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A42" s="13">
+      <c r="A42" s="8">
         <v>41</v>
       </c>
-      <c r="B42" s="13"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
-      <c r="U42" s="15"/>
-      <c r="V42" s="15"/>
-      <c r="W42" s="15"/>
-      <c r="X42" s="15"/>
-      <c r="Y42" s="15"/>
-      <c r="Z42" s="15"/>
-      <c r="AA42" s="15"/>
-      <c r="AB42" s="15"/>
-      <c r="AC42" s="15"/>
-      <c r="AD42" s="15"/>
-      <c r="AE42" s="16"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="30"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5140,41 +5143,41 @@
       <c r="CA42" s="12"/>
     </row>
     <row r="43" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
+      <c r="A43" s="13">
         <v>42</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="15"/>
-      <c r="AA43" s="15"/>
-      <c r="AB43" s="15"/>
-      <c r="AC43" s="15"/>
-      <c r="AD43" s="15"/>
-      <c r="AE43" s="16"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="30"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5233,41 +5236,41 @@
       <c r="CA43" s="12"/>
     </row>
     <row r="44" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
+      <c r="A44" s="13">
         <v>43</v>
       </c>
-      <c r="B44" s="8"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-      <c r="AA44" s="15"/>
-      <c r="AB44" s="15"/>
-      <c r="AC44" s="15"/>
-      <c r="AD44" s="15"/>
-      <c r="AE44" s="16"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="30"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -5326,10 +5329,10 @@
       <c r="CA44" s="12"/>
     </row>
     <row r="45" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8">
+      <c r="A45" s="13">
         <v>44</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="5"/>
       <c r="D45" s="9" t="s">
         <v>59</v>
@@ -5419,10 +5422,10 @@
       <c r="CA45" s="12"/>
     </row>
     <row r="46" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A46" s="13">
+      <c r="A46" s="8">
         <v>45</v>
       </c>
-      <c r="B46" s="13"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="9" t="s">
         <v>60</v>
@@ -5512,10 +5515,10 @@
       <c r="CA46" s="12"/>
     </row>
     <row r="47" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
+      <c r="A47" s="13">
         <v>46</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="5"/>
       <c r="D47" s="9" t="s">
         <v>62</v>
@@ -5605,10 +5608,10 @@
       <c r="CA47" s="12"/>
     </row>
     <row r="48" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
+      <c r="A48" s="13">
         <v>47</v>
       </c>
-      <c r="B48" s="8"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="5"/>
       <c r="D48" s="9" t="s">
         <v>62</v>
@@ -5698,10 +5701,10 @@
       <c r="CA48" s="12"/>
     </row>
     <row r="49" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="8">
+      <c r="A49" s="13">
         <v>48</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="5"/>
       <c r="D49" s="9" t="s">
         <v>64</v>
@@ -5791,10 +5794,10 @@
       <c r="CA49" s="12"/>
     </row>
     <row r="50" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A50" s="13">
+      <c r="A50" s="8">
         <v>49</v>
       </c>
-      <c r="B50" s="13"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="5"/>
       <c r="D50" s="9" t="s">
         <v>65</v>
@@ -5884,10 +5887,10 @@
       <c r="CA50" s="12"/>
     </row>
     <row r="51" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A51" s="8">
+      <c r="A51" s="13">
         <v>50</v>
       </c>
-      <c r="B51" s="8"/>
+      <c r="B51" s="13"/>
       <c r="C51" s="5"/>
       <c r="D51" s="9" t="s">
         <v>66</v>
@@ -5977,10 +5980,10 @@
       <c r="CA51" s="12"/>
     </row>
     <row r="52" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
+      <c r="A52" s="13">
         <v>51</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="13"/>
       <c r="C52" s="5"/>
       <c r="D52" s="9" t="s">
         <v>66</v>
@@ -6070,10 +6073,10 @@
       <c r="CA52" s="12"/>
     </row>
     <row r="53" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8">
+      <c r="A53" s="13">
         <v>52</v>
       </c>
-      <c r="B53" s="8"/>
+      <c r="B53" s="13"/>
       <c r="C53" s="5"/>
       <c r="D53" s="9" t="s">
         <v>68</v>
@@ -6163,10 +6166,10 @@
       <c r="CA53" s="12"/>
     </row>
     <row r="54" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A54" s="13">
+      <c r="A54" s="8">
         <v>53</v>
       </c>
-      <c r="B54" s="13"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="5"/>
       <c r="D54" s="9" t="s">
         <v>69</v>
@@ -6256,10 +6259,10 @@
       <c r="CA54" s="12"/>
     </row>
     <row r="55" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A55" s="8">
+      <c r="A55" s="13">
         <v>54</v>
       </c>
-      <c r="B55" s="8"/>
+      <c r="B55" s="13"/>
       <c r="C55" s="5"/>
       <c r="D55" s="9" t="s">
         <v>71</v>
@@ -6349,10 +6352,10 @@
       <c r="CA55" s="12"/>
     </row>
     <row r="56" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A56" s="8">
+      <c r="A56" s="13">
         <v>55</v>
       </c>
-      <c r="B56" s="8"/>
+      <c r="B56" s="13"/>
       <c r="C56" s="5"/>
       <c r="D56" s="9" t="s">
         <v>72</v>
@@ -6442,10 +6445,10 @@
       <c r="CA56" s="12"/>
     </row>
     <row r="57" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="8">
+      <c r="A57" s="13">
         <v>56</v>
       </c>
-      <c r="B57" s="8"/>
+      <c r="B57" s="13"/>
       <c r="C57" s="5"/>
       <c r="D57" s="9" t="s">
         <v>74</v>
@@ -6535,10 +6538,10 @@
       <c r="CA57" s="12"/>
     </row>
     <row r="58" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A58" s="13">
+      <c r="A58" s="8">
         <v>57</v>
       </c>
-      <c r="B58" s="13"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="5"/>
       <c r="D58" s="9" t="s">
         <v>75</v>
@@ -6628,10 +6631,10 @@
       <c r="CA58" s="12"/>
     </row>
     <row r="59" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A59" s="8">
+      <c r="A59" s="13">
         <v>58</v>
       </c>
-      <c r="B59" s="8"/>
+      <c r="B59" s="13"/>
       <c r="C59" s="5"/>
       <c r="D59" s="9" t="s">
         <v>77</v>
@@ -6721,10 +6724,10 @@
       <c r="CA59" s="12"/>
     </row>
     <row r="60" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A60" s="8">
+      <c r="A60" s="13">
         <v>59</v>
       </c>
-      <c r="B60" s="8"/>
+      <c r="B60" s="13"/>
       <c r="C60" s="5"/>
       <c r="D60" s="9" t="s">
         <v>75</v>
@@ -6814,10 +6817,10 @@
       <c r="CA60" s="12"/>
     </row>
     <row r="61" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="8">
+      <c r="A61" s="13">
         <v>60</v>
       </c>
-      <c r="B61" s="8"/>
+      <c r="B61" s="13"/>
       <c r="C61" s="5"/>
       <c r="D61" s="9" t="s">
         <v>80</v>
@@ -6907,10 +6910,10 @@
       <c r="CA61" s="12"/>
     </row>
     <row r="62" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A62" s="13">
+      <c r="A62" s="8">
         <v>61</v>
       </c>
-      <c r="B62" s="13"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="5"/>
       <c r="D62" s="9" t="s">
         <v>78</v>
@@ -7000,10 +7003,10 @@
       <c r="CA62" s="12"/>
     </row>
     <row r="63" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A63" s="8">
+      <c r="A63" s="13">
         <v>62</v>
       </c>
-      <c r="B63" s="8"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="5"/>
       <c r="D63" s="9" t="s">
         <v>84</v>
@@ -7093,10 +7096,10 @@
       <c r="CA63" s="12"/>
     </row>
     <row r="64" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A64" s="8">
+      <c r="A64" s="13">
         <v>63</v>
       </c>
-      <c r="B64" s="8"/>
+      <c r="B64" s="13"/>
       <c r="C64" s="5"/>
       <c r="D64" s="9" t="s">
         <v>84</v>
@@ -7186,10 +7189,10 @@
       <c r="CA64" s="12"/>
     </row>
     <row r="65" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="8">
+      <c r="A65" s="13">
         <v>64</v>
       </c>
-      <c r="B65" s="8"/>
+      <c r="B65" s="13"/>
       <c r="C65" s="5"/>
       <c r="D65" s="9" t="s">
         <v>83</v>
@@ -7277,10 +7280,10 @@
       <c r="CA65" s="12"/>
     </row>
     <row r="66" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A66" s="13">
+      <c r="A66" s="8">
         <v>65</v>
       </c>
-      <c r="B66" s="13"/>
+      <c r="B66" s="8"/>
       <c r="C66" s="5"/>
       <c r="D66" s="9" t="s">
         <v>85</v>
@@ -7370,10 +7373,10 @@
       <c r="CA66" s="12"/>
     </row>
     <row r="67" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A67" s="8">
+      <c r="A67" s="13">
         <v>66</v>
       </c>
-      <c r="B67" s="8"/>
+      <c r="B67" s="13"/>
       <c r="C67" s="5"/>
       <c r="D67" s="9" t="s">
         <v>87</v>
@@ -7463,10 +7466,10 @@
       <c r="CA67" s="12"/>
     </row>
     <row r="68" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A68" s="8">
+      <c r="A68" s="13">
         <v>67</v>
       </c>
-      <c r="B68" s="8"/>
+      <c r="B68" s="13"/>
       <c r="C68" s="5"/>
       <c r="D68" s="9" t="s">
         <v>87</v>
@@ -7556,10 +7559,10 @@
       <c r="CA68" s="12"/>
     </row>
     <row r="69" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="8">
+      <c r="A69" s="13">
         <v>68</v>
       </c>
-      <c r="B69" s="8"/>
+      <c r="B69" s="13"/>
       <c r="C69" s="5"/>
       <c r="D69" s="9" t="s">
         <v>88</v>
@@ -7649,10 +7652,10 @@
       <c r="CA69" s="12"/>
     </row>
     <row r="70" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A70" s="13">
+      <c r="A70" s="8">
         <v>69</v>
       </c>
-      <c r="B70" s="13"/>
+      <c r="B70" s="8"/>
       <c r="C70" s="5"/>
       <c r="D70" s="9" t="s">
         <v>90</v>
@@ -7742,10 +7745,10 @@
       <c r="CA70" s="12"/>
     </row>
     <row r="71" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
+      <c r="A71" s="13">
         <v>70</v>
       </c>
-      <c r="B71" s="8"/>
+      <c r="B71" s="13"/>
       <c r="C71" s="5"/>
       <c r="D71" s="9" t="s">
         <v>90</v>
@@ -7835,10 +7838,10 @@
       <c r="CA71" s="12"/>
     </row>
     <row r="72" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A72" s="8">
+      <c r="A72" s="13">
         <v>71</v>
       </c>
-      <c r="B72" s="8"/>
+      <c r="B72" s="13"/>
       <c r="C72" s="5"/>
       <c r="D72" s="9" t="s">
         <v>91</v>
@@ -7928,10 +7931,10 @@
       <c r="CA72" s="12"/>
     </row>
     <row r="73" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="8">
+      <c r="A73" s="13">
         <v>72</v>
       </c>
-      <c r="B73" s="8"/>
+      <c r="B73" s="13"/>
       <c r="C73" s="5"/>
       <c r="D73" s="9" t="s">
         <v>92</v>
@@ -8021,10 +8024,10 @@
       <c r="CA73" s="12"/>
     </row>
     <row r="74" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A74" s="13">
+      <c r="A74" s="8">
         <v>73</v>
       </c>
-      <c r="B74" s="13"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="5"/>
       <c r="D74" s="9" t="s">
         <v>93</v>
@@ -8114,10 +8117,10 @@
       <c r="CA74" s="12"/>
     </row>
     <row r="75" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A75" s="8">
+      <c r="A75" s="13">
         <v>74</v>
       </c>
-      <c r="B75" s="8"/>
+      <c r="B75" s="13"/>
       <c r="C75" s="5"/>
       <c r="D75" s="9" t="s">
         <v>94</v>
@@ -8207,10 +8210,10 @@
       <c r="CA75" s="12"/>
     </row>
     <row r="76" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
+      <c r="A76" s="13">
         <v>75</v>
       </c>
-      <c r="B76" s="8"/>
+      <c r="B76" s="13"/>
       <c r="C76" s="5"/>
       <c r="D76" s="9" t="s">
         <v>94</v>
@@ -8300,10 +8303,10 @@
       <c r="CA76" s="12"/>
     </row>
     <row r="77" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="8">
+      <c r="A77" s="13">
         <v>76</v>
       </c>
-      <c r="B77" s="8"/>
+      <c r="B77" s="13"/>
       <c r="C77" s="5"/>
       <c r="D77" s="9" t="s">
         <v>95</v>
@@ -8393,10 +8396,10 @@
       <c r="CA77" s="12"/>
     </row>
     <row r="78" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A78" s="13">
+      <c r="A78" s="8">
         <v>77</v>
       </c>
-      <c r="B78" s="13"/>
+      <c r="B78" s="8"/>
       <c r="C78" s="5"/>
       <c r="D78" s="9" t="s">
         <v>97</v>
@@ -8486,10 +8489,10 @@
       <c r="CA78" s="12"/>
     </row>
     <row r="79" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A79" s="8">
+      <c r="A79" s="13">
         <v>78</v>
       </c>
-      <c r="B79" s="8"/>
+      <c r="B79" s="13"/>
       <c r="C79" s="5"/>
       <c r="D79" s="9" t="s">
         <v>96</v>
@@ -8579,10 +8582,10 @@
       <c r="CA79" s="12"/>
     </row>
     <row r="80" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A80" s="8">
+      <c r="A80" s="13">
         <v>79</v>
       </c>
-      <c r="B80" s="8"/>
+      <c r="B80" s="13"/>
       <c r="C80" s="5"/>
       <c r="D80" s="9" t="s">
         <v>96</v>
@@ -8672,10 +8675,10 @@
       <c r="CA80" s="12"/>
     </row>
     <row r="81" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="8">
+      <c r="A81" s="13">
         <v>80</v>
       </c>
-      <c r="B81" s="8"/>
+      <c r="B81" s="13"/>
       <c r="C81" s="5"/>
       <c r="D81" s="9" t="s">
         <v>98</v>
@@ -8765,10 +8768,10 @@
       <c r="CA81" s="12"/>
     </row>
     <row r="82" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A82" s="13">
+      <c r="A82" s="8">
         <v>81</v>
       </c>
-      <c r="B82" s="13"/>
+      <c r="B82" s="8"/>
       <c r="C82" s="5"/>
       <c r="D82" s="9" t="s">
         <v>99</v>
@@ -8858,10 +8861,10 @@
       <c r="CA82" s="12"/>
     </row>
     <row r="83" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A83" s="8">
+      <c r="A83" s="13">
         <v>82</v>
       </c>
-      <c r="B83" s="8"/>
+      <c r="B83" s="13"/>
       <c r="C83" s="5"/>
       <c r="D83" s="9" t="s">
         <v>101</v>
@@ -8951,10 +8954,10 @@
       <c r="CA83" s="12"/>
     </row>
     <row r="84" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A84" s="8">
+      <c r="A84" s="13">
         <v>83</v>
       </c>
-      <c r="B84" s="8"/>
+      <c r="B84" s="13"/>
       <c r="C84" s="5"/>
       <c r="D84" s="9" t="s">
         <v>100</v>
@@ -9044,10 +9047,10 @@
       <c r="CA84" s="12"/>
     </row>
     <row r="85" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="8">
+      <c r="A85" s="13">
         <v>84</v>
       </c>
-      <c r="B85" s="8"/>
+      <c r="B85" s="13"/>
       <c r="C85" s="5"/>
       <c r="D85" s="9" t="s">
         <v>102</v>
@@ -9137,10 +9140,10 @@
       <c r="CA85" s="12"/>
     </row>
     <row r="86" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A86" s="13">
+      <c r="A86" s="8">
         <v>85</v>
       </c>
-      <c r="B86" s="13"/>
+      <c r="B86" s="8"/>
       <c r="C86" s="5"/>
       <c r="D86" s="9" t="s">
         <v>99</v>
@@ -9230,10 +9233,10 @@
       <c r="CA86" s="12"/>
     </row>
     <row r="87" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A87" s="8">
+      <c r="A87" s="13">
         <v>86</v>
       </c>
-      <c r="B87" s="8"/>
+      <c r="B87" s="13"/>
       <c r="C87" s="5"/>
       <c r="D87" s="9" t="s">
         <v>103</v>
@@ -9323,10 +9326,10 @@
       <c r="CA87" s="12"/>
     </row>
     <row r="88" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A88" s="8">
+      <c r="A88" s="13">
         <v>87</v>
       </c>
-      <c r="B88" s="8"/>
+      <c r="B88" s="13"/>
       <c r="C88" s="5"/>
       <c r="D88" s="9" t="s">
         <v>104</v>
@@ -9414,10 +9417,10 @@
       <c r="CA88" s="12"/>
     </row>
     <row r="89" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="8">
+      <c r="A89" s="13">
         <v>88</v>
       </c>
-      <c r="B89" s="8"/>
+      <c r="B89" s="13"/>
       <c r="C89" s="5"/>
       <c r="D89" s="9" t="s">
         <v>105</v>
@@ -9505,10 +9508,10 @@
       <c r="CA89" s="12"/>
     </row>
     <row r="90" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A90" s="13">
+      <c r="A90" s="8">
         <v>89</v>
       </c>
-      <c r="B90" s="13"/>
+      <c r="B90" s="8"/>
       <c r="C90" s="5"/>
       <c r="D90" s="9" t="s">
         <v>105</v>
@@ -9596,10 +9599,10 @@
       <c r="CA90" s="12"/>
     </row>
     <row r="91" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A91" s="8">
+      <c r="A91" s="13">
         <v>90</v>
       </c>
-      <c r="B91" s="8"/>
+      <c r="B91" s="13"/>
       <c r="C91" s="5"/>
       <c r="D91" s="9" t="s">
         <v>105</v>
@@ -9687,10 +9690,10 @@
       <c r="CA91" s="12"/>
     </row>
     <row r="92" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A92" s="8">
+      <c r="A92" s="13">
         <v>91</v>
       </c>
-      <c r="B92" s="8"/>
+      <c r="B92" s="13"/>
       <c r="C92" s="5"/>
       <c r="D92" s="9" t="s">
         <v>107</v>
@@ -9780,10 +9783,10 @@
       <c r="CA92" s="12"/>
     </row>
     <row r="93" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="8">
+      <c r="A93" s="13">
         <v>92</v>
       </c>
-      <c r="B93" s="8"/>
+      <c r="B93" s="13"/>
       <c r="C93" s="5"/>
       <c r="D93" s="9" t="s">
         <v>107</v>
@@ -9873,10 +9876,10 @@
       <c r="CA93" s="12"/>
     </row>
     <row r="94" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A94" s="13">
+      <c r="A94" s="8">
         <v>93</v>
       </c>
-      <c r="B94" s="13"/>
+      <c r="B94" s="8"/>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
         <v>109</v>
@@ -9966,10 +9969,10 @@
       <c r="CA94" s="12"/>
     </row>
     <row r="95" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A95" s="8">
+      <c r="A95" s="13">
         <v>94</v>
       </c>
-      <c r="B95" s="8"/>
+      <c r="B95" s="13"/>
       <c r="C95" s="5"/>
       <c r="D95" s="9" t="s">
         <v>111</v>
@@ -10059,10 +10062,10 @@
       <c r="CA95" s="12"/>
     </row>
     <row r="96" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A96" s="8">
+      <c r="A96" s="13">
         <v>95</v>
       </c>
-      <c r="B96" s="8"/>
+      <c r="B96" s="13"/>
       <c r="C96" s="5"/>
       <c r="D96" s="9" t="s">
         <v>114</v>
@@ -10152,10 +10155,10 @@
       <c r="CA96" s="12"/>
     </row>
     <row r="97" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="8">
+      <c r="A97" s="13">
         <v>96</v>
       </c>
-      <c r="B97" s="8"/>
+      <c r="B97" s="13"/>
       <c r="C97" s="5"/>
       <c r="D97" s="9" t="s">
         <v>115</v>
@@ -10245,10 +10248,10 @@
       <c r="CA97" s="12"/>
     </row>
     <row r="98" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A98" s="13">
+      <c r="A98" s="8">
         <v>97</v>
       </c>
-      <c r="B98" s="13"/>
+      <c r="B98" s="8"/>
       <c r="C98" s="5"/>
       <c r="D98" s="9" t="s">
         <v>116</v>
@@ -10338,10 +10341,10 @@
       <c r="CA98" s="12"/>
     </row>
     <row r="99" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A99" s="8">
+      <c r="A99" s="13">
         <v>98</v>
       </c>
-      <c r="B99" s="8"/>
+      <c r="B99" s="13"/>
       <c r="C99" s="5"/>
       <c r="D99" s="9" t="s">
         <v>117</v>
@@ -10431,10 +10434,10 @@
       <c r="CA99" s="12"/>
     </row>
     <row r="100" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A100" s="8">
+      <c r="A100" s="13">
         <v>99</v>
       </c>
-      <c r="B100" s="8"/>
+      <c r="B100" s="13"/>
       <c r="C100" s="5"/>
       <c r="D100" s="9" t="s">
         <v>117</v>
@@ -10524,10 +10527,10 @@
       <c r="CA100" s="12"/>
     </row>
     <row r="101" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="8">
+      <c r="A101" s="13">
         <v>100</v>
       </c>
-      <c r="B101" s="8"/>
+      <c r="B101" s="13"/>
       <c r="C101" s="5"/>
       <c r="D101" s="9" t="s">
         <v>119</v>
@@ -10617,10 +10620,10 @@
       <c r="CA101" s="12"/>
     </row>
     <row r="102" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A102" s="13">
+      <c r="A102" s="8">
         <v>101</v>
       </c>
-      <c r="B102" s="13"/>
+      <c r="B102" s="8"/>
       <c r="C102" s="5"/>
       <c r="D102" s="9" t="s">
         <v>120</v>
@@ -10710,10 +10713,10 @@
       <c r="CA102" s="12"/>
     </row>
     <row r="103" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A103" s="8">
+      <c r="A103" s="13">
         <v>102</v>
       </c>
-      <c r="B103" s="8"/>
+      <c r="B103" s="13"/>
       <c r="C103" s="5"/>
       <c r="D103" s="9" t="s">
         <v>120</v>
@@ -10803,10 +10806,10 @@
       <c r="CA103" s="12"/>
     </row>
     <row r="104" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A104" s="8">
+      <c r="A104" s="13">
         <v>103</v>
       </c>
-      <c r="B104" s="8"/>
+      <c r="B104" s="13"/>
       <c r="C104" s="5"/>
       <c r="D104" s="9" t="s">
         <v>123</v>
@@ -10896,10 +10899,10 @@
       <c r="CA104" s="12"/>
     </row>
     <row r="105" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="8">
+      <c r="A105" s="13">
         <v>104</v>
       </c>
-      <c r="B105" s="8"/>
+      <c r="B105" s="13"/>
       <c r="C105" s="5"/>
       <c r="D105" s="9" t="s">
         <v>123</v>
@@ -10989,10 +10992,10 @@
       <c r="CA105" s="12"/>
     </row>
     <row r="106" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A106" s="13">
+      <c r="A106" s="8">
         <v>105</v>
       </c>
-      <c r="B106" s="13"/>
+      <c r="B106" s="8"/>
       <c r="C106" s="5"/>
       <c r="D106" s="9" t="s">
         <v>125</v>
@@ -11082,12 +11085,14 @@
       <c r="CA106" s="12"/>
     </row>
     <row r="107" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A107" s="8">
+      <c r="A107" s="13">
         <v>106</v>
       </c>
-      <c r="B107" s="8"/>
+      <c r="B107" s="13"/>
       <c r="C107" s="5"/>
-      <c r="D107" s="9"/>
+      <c r="D107" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
       <c r="G107" s="9"/>
@@ -11115,20 +11120,28 @@
       <c r="AC107" s="9"/>
       <c r="AD107" s="9"/>
       <c r="AE107" s="9"/>
-      <c r="AF107" s="10"/>
+      <c r="AF107" s="10" t="s">
+        <v>126</v>
+      </c>
       <c r="AG107" s="10"/>
       <c r="AH107" s="10"/>
       <c r="AI107" s="10"/>
       <c r="AJ107" s="10"/>
-      <c r="AK107" s="9"/>
+      <c r="AK107" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL107" s="9"/>
       <c r="AM107" s="9"/>
       <c r="AN107" s="9"/>
       <c r="AO107" s="9"/>
-      <c r="AP107" s="11"/>
+      <c r="AP107" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ107" s="11"/>
       <c r="AR107" s="11"/>
-      <c r="AS107" s="9"/>
+      <c r="AS107" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT107" s="9"/>
       <c r="AU107" s="9"/>
       <c r="AV107" s="9"/>
@@ -11165,12 +11178,14 @@
       <c r="CA107" s="12"/>
     </row>
     <row r="108" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A108" s="8">
+      <c r="A108" s="13">
         <v>107</v>
       </c>
-      <c r="B108" s="8"/>
+      <c r="B108" s="13"/>
       <c r="C108" s="5"/>
-      <c r="D108" s="9"/>
+      <c r="D108" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="E108" s="9"/>
       <c r="F108" s="9"/>
       <c r="G108" s="9"/>
@@ -11198,20 +11213,28 @@
       <c r="AC108" s="9"/>
       <c r="AD108" s="9"/>
       <c r="AE108" s="9"/>
-      <c r="AF108" s="10"/>
+      <c r="AF108" s="10" t="s">
+        <v>126</v>
+      </c>
       <c r="AG108" s="10"/>
       <c r="AH108" s="10"/>
       <c r="AI108" s="10"/>
       <c r="AJ108" s="10"/>
-      <c r="AK108" s="9"/>
+      <c r="AK108" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL108" s="9"/>
       <c r="AM108" s="9"/>
       <c r="AN108" s="9"/>
       <c r="AO108" s="9"/>
-      <c r="AP108" s="11"/>
+      <c r="AP108" s="11">
+        <v>0.5</v>
+      </c>
       <c r="AQ108" s="11"/>
       <c r="AR108" s="11"/>
-      <c r="AS108" s="9"/>
+      <c r="AS108" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT108" s="9"/>
       <c r="AU108" s="9"/>
       <c r="AV108" s="9"/>
@@ -11248,10 +11271,10 @@
       <c r="CA108" s="12"/>
     </row>
     <row r="109" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="8">
+      <c r="A109" s="13">
         <v>108</v>
       </c>
-      <c r="B109" s="8"/>
+      <c r="B109" s="13"/>
       <c r="C109" s="5"/>
       <c r="D109" s="9"/>
       <c r="E109" s="9"/>
@@ -11331,10 +11354,10 @@
       <c r="CA109" s="12"/>
     </row>
     <row r="110" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A110" s="13">
+      <c r="A110" s="8">
         <v>109</v>
       </c>
-      <c r="B110" s="13"/>
+      <c r="B110" s="8"/>
       <c r="C110" s="5"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
@@ -11414,10 +11437,10 @@
       <c r="CA110" s="12"/>
     </row>
     <row r="111" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A111" s="8">
+      <c r="A111" s="13">
         <v>110</v>
       </c>
-      <c r="B111" s="8"/>
+      <c r="B111" s="13"/>
       <c r="C111" s="5"/>
       <c r="D111" s="9"/>
       <c r="E111" s="9"/>
@@ -11497,10 +11520,10 @@
       <c r="CA111" s="12"/>
     </row>
     <row r="112" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A112" s="8">
+      <c r="A112" s="13">
         <v>111</v>
       </c>
-      <c r="B112" s="8"/>
+      <c r="B112" s="13"/>
       <c r="C112" s="5"/>
       <c r="D112" s="9"/>
       <c r="E112" s="9"/>
@@ -11580,10 +11603,10 @@
       <c r="CA112" s="12"/>
     </row>
     <row r="113" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="8">
+      <c r="A113" s="13">
         <v>112</v>
       </c>
-      <c r="B113" s="8"/>
+      <c r="B113" s="13"/>
       <c r="C113" s="5"/>
       <c r="D113" s="9"/>
       <c r="E113" s="9"/>
@@ -11663,10 +11686,10 @@
       <c r="CA113" s="12"/>
     </row>
     <row r="114" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A114" s="13">
+      <c r="A114" s="8">
         <v>113</v>
       </c>
-      <c r="B114" s="13"/>
+      <c r="B114" s="8"/>
       <c r="C114" s="5"/>
       <c r="D114" s="9"/>
       <c r="E114" s="9"/>
@@ -11746,10 +11769,10 @@
       <c r="CA114" s="12"/>
     </row>
     <row r="115" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A115" s="8">
+      <c r="A115" s="13">
         <v>114</v>
       </c>
-      <c r="B115" s="8"/>
+      <c r="B115" s="13"/>
       <c r="C115" s="5"/>
       <c r="D115" s="9"/>
       <c r="E115" s="9"/>
@@ -11829,10 +11852,10 @@
       <c r="CA115" s="12"/>
     </row>
     <row r="116" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A116" s="8">
+      <c r="A116" s="13">
         <v>115</v>
       </c>
-      <c r="B116" s="8"/>
+      <c r="B116" s="13"/>
       <c r="C116" s="5"/>
       <c r="D116" s="9"/>
       <c r="E116" s="9"/>
@@ -11912,10 +11935,10 @@
       <c r="CA116" s="12"/>
     </row>
     <row r="117" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="8">
+      <c r="A117" s="13">
         <v>116</v>
       </c>
-      <c r="B117" s="8"/>
+      <c r="B117" s="13"/>
       <c r="C117" s="5"/>
       <c r="D117" s="9"/>
       <c r="E117" s="9"/>
@@ -11995,10 +12018,10 @@
       <c r="CA117" s="12"/>
     </row>
     <row r="118" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A118" s="13">
+      <c r="A118" s="8">
         <v>117</v>
       </c>
-      <c r="B118" s="13"/>
+      <c r="B118" s="8"/>
       <c r="C118" s="5"/>
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
@@ -12078,10 +12101,10 @@
       <c r="CA118" s="12"/>
     </row>
     <row r="119" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A119" s="8">
+      <c r="A119" s="13">
         <v>118</v>
       </c>
-      <c r="B119" s="8"/>
+      <c r="B119" s="13"/>
       <c r="C119" s="5"/>
       <c r="D119" s="9"/>
       <c r="E119" s="9"/>
@@ -12161,10 +12184,10 @@
       <c r="CA119" s="12"/>
     </row>
     <row r="120" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A120" s="8">
+      <c r="A120" s="13">
         <v>119</v>
       </c>
-      <c r="B120" s="8"/>
+      <c r="B120" s="13"/>
       <c r="C120" s="5"/>
       <c r="D120" s="9"/>
       <c r="E120" s="9"/>
@@ -12244,10 +12267,10 @@
       <c r="CA120" s="12"/>
     </row>
     <row r="121" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="8">
+      <c r="A121" s="13">
         <v>120</v>
       </c>
-      <c r="B121" s="8"/>
+      <c r="B121" s="13"/>
       <c r="C121" s="5"/>
       <c r="D121" s="9"/>
       <c r="E121" s="9"/>
@@ -12327,10 +12350,10 @@
       <c r="CA121" s="12"/>
     </row>
     <row r="122" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A122" s="13">
+      <c r="A122" s="8">
         <v>121</v>
       </c>
-      <c r="B122" s="13"/>
+      <c r="B122" s="8"/>
       <c r="C122" s="5"/>
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
@@ -12410,10 +12433,10 @@
       <c r="CA122" s="12"/>
     </row>
     <row r="123" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A123" s="8">
+      <c r="A123" s="13">
         <v>122</v>
       </c>
-      <c r="B123" s="8"/>
+      <c r="B123" s="13"/>
       <c r="C123" s="5"/>
       <c r="BG123" s="12"/>
       <c r="BH123" s="12"/>
@@ -12439,351 +12462,493 @@
     </row>
   </sheetData>
   <mergeCells count="856">
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12808,493 +12973,351 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
báo cáo ngày 31/1/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="130">
   <si>
     <t>No.</t>
   </si>
@@ -402,6 +402,15 @@
   <si>
     <t>29/1/2019</t>
   </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  import data</t>
+  </si>
+  <si>
+    <t>31/1/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data</t>
+  </si>
 </sst>
 </file>
 
@@ -663,12 +672,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -688,14 +705,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,7 +810,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1192,7 +1201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1204,7 +1213,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP108" sqref="AP108:AR108"/>
+      <selection pane="bottomLeft" activeCell="AK117" sqref="AK117:AO117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,198 +1228,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="16" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="15" t="s">
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="17" t="s">
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="17"/>
-      <c r="AR1" s="17"/>
-      <c r="AS1" s="15" t="s">
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="15"/>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
-      <c r="BG1" s="18" t="s">
+      <c r="AT1" s="23"/>
+      <c r="AU1" s="23"/>
+      <c r="AV1" s="23"/>
+      <c r="AW1" s="23"/>
+      <c r="AX1" s="23"/>
+      <c r="AY1" s="23"/>
+      <c r="AZ1" s="23"/>
+      <c r="BA1" s="23"/>
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23"/>
+      <c r="BG1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="18"/>
-      <c r="BI1" s="18"/>
-      <c r="BJ1" s="18"/>
-      <c r="BK1" s="18"/>
-      <c r="BL1" s="18"/>
-      <c r="BM1" s="18"/>
-      <c r="BN1" s="18"/>
-      <c r="BO1" s="18"/>
-      <c r="BP1" s="18"/>
-      <c r="BQ1" s="18"/>
-      <c r="BR1" s="18"/>
-      <c r="BS1" s="18"/>
-      <c r="BT1" s="18"/>
-      <c r="BU1" s="18"/>
-      <c r="BV1" s="18"/>
-      <c r="BW1" s="18"/>
-      <c r="BX1" s="18"/>
-      <c r="BY1" s="18"/>
-      <c r="BZ1" s="18"/>
-      <c r="CA1" s="18"/>
+      <c r="BH1" s="26"/>
+      <c r="BI1" s="26"/>
+      <c r="BJ1" s="26"/>
+      <c r="BK1" s="26"/>
+      <c r="BL1" s="26"/>
+      <c r="BM1" s="26"/>
+      <c r="BN1" s="26"/>
+      <c r="BO1" s="26"/>
+      <c r="BP1" s="26"/>
+      <c r="BQ1" s="26"/>
+      <c r="BR1" s="26"/>
+      <c r="BS1" s="26"/>
+      <c r="BT1" s="26"/>
+      <c r="BU1" s="26"/>
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26"/>
+      <c r="CA1" s="26"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="20" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="19" t="s">
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="21">
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="29">
         <v>1</v>
       </c>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="19" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
-      <c r="BN2" s="22"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2" s="22"/>
-      <c r="BQ2" s="22"/>
-      <c r="BR2" s="22"/>
-      <c r="BS2" s="22"/>
-      <c r="BT2" s="22"/>
-      <c r="BU2" s="22"/>
-      <c r="BV2" s="22"/>
-      <c r="BW2" s="22"/>
-      <c r="BX2" s="22"/>
-      <c r="BY2" s="22"/>
-      <c r="BZ2" s="22"/>
-      <c r="CA2" s="22"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="30"/>
+      <c r="BJ2" s="30"/>
+      <c r="BK2" s="30"/>
+      <c r="BL2" s="30"/>
+      <c r="BM2" s="30"/>
+      <c r="BN2" s="30"/>
+      <c r="BO2" s="30"/>
+      <c r="BP2" s="30"/>
+      <c r="BQ2" s="30"/>
+      <c r="BR2" s="30"/>
+      <c r="BS2" s="30"/>
+      <c r="BT2" s="30"/>
+      <c r="BU2" s="30"/>
+      <c r="BV2" s="30"/>
+      <c r="BW2" s="30"/>
+      <c r="BX2" s="30"/>
+      <c r="BY2" s="30"/>
+      <c r="BZ2" s="30"/>
+      <c r="CA2" s="30"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="5"/>
       <c r="D3" s="9" t="s">
         <v>17</v>
@@ -1500,10 +1509,10 @@
       <c r="CA3" s="12"/>
     </row>
     <row r="4" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="5"/>
       <c r="D4" s="9" t="s">
         <v>18</v>
@@ -1593,10 +1602,10 @@
       <c r="CA4" s="12"/>
     </row>
     <row r="5" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="5"/>
       <c r="D5" s="9" t="s">
         <v>18</v>
@@ -1688,10 +1697,10 @@
       <c r="CA5" s="12"/>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -1781,10 +1790,10 @@
       <c r="CA6" s="12"/>
     </row>
     <row r="7" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
         <v>22</v>
@@ -1874,10 +1883,10 @@
       <c r="CA7" s="12"/>
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
         <v>24</v>
@@ -1967,10 +1976,10 @@
       <c r="CA8" s="12"/>
     </row>
     <row r="9" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
         <v>33</v>
@@ -2062,10 +2071,10 @@
       <c r="CA9" s="12"/>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
         <v>33</v>
@@ -2155,10 +2164,10 @@
       <c r="CA10" s="12"/>
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
         <v>33</v>
@@ -2248,10 +2257,10 @@
       <c r="CA11" s="12"/>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="5"/>
       <c r="D12" s="9" t="s">
         <v>33</v>
@@ -2341,10 +2350,10 @@
       <c r="CA12" s="12"/>
     </row>
     <row r="13" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>33</v>
@@ -2436,10 +2445,10 @@
       <c r="CA13" s="12"/>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="9" t="s">
         <v>33</v>
@@ -2531,10 +2540,10 @@
       <c r="CA14" s="12"/>
     </row>
     <row r="15" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
         <v>33</v>
@@ -2624,10 +2633,10 @@
       <c r="CA15" s="12"/>
     </row>
     <row r="16" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="13"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
         <v>36</v>
@@ -2717,10 +2726,10 @@
       <c r="CA16" s="12"/>
     </row>
     <row r="17" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
         <v>33</v>
@@ -2812,10 +2821,10 @@
       <c r="CA17" s="12"/>
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
         <v>38</v>
@@ -2905,10 +2914,10 @@
       <c r="CA18" s="12"/>
     </row>
     <row r="19" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="13"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
         <v>38</v>
@@ -2998,10 +3007,10 @@
       <c r="CA19" s="12"/>
     </row>
     <row r="20" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="5"/>
       <c r="D20" s="9" t="s">
         <v>38</v>
@@ -3091,10 +3100,10 @@
       <c r="CA20" s="12"/>
     </row>
     <row r="21" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
+      <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="5"/>
       <c r="D21" s="9" t="s">
         <v>38</v>
@@ -3184,10 +3193,10 @@
       <c r="CA21" s="12"/>
     </row>
     <row r="22" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="13">
         <v>21</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="9" t="s">
         <v>44</v>
@@ -3279,10 +3288,10 @@
       <c r="CA22" s="12"/>
     </row>
     <row r="23" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+      <c r="A23" s="8">
         <v>22</v>
       </c>
-      <c r="B23" s="13"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="5"/>
       <c r="D23" s="9" t="s">
         <v>38</v>
@@ -3374,10 +3383,10 @@
       <c r="CA23" s="12"/>
     </row>
     <row r="24" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="A24" s="8">
         <v>23</v>
       </c>
-      <c r="B24" s="13"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="5"/>
       <c r="D24" s="9" t="s">
         <v>33</v>
@@ -3467,10 +3476,10 @@
       <c r="CA24" s="12"/>
     </row>
     <row r="25" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13">
+      <c r="A25" s="8">
         <v>24</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="5"/>
       <c r="D25" s="9" t="s">
         <v>45</v>
@@ -3560,10 +3569,10 @@
       <c r="CA25" s="12"/>
     </row>
     <row r="26" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="13">
         <v>25</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
         <v>38</v>
@@ -3653,10 +3662,10 @@
       <c r="CA26" s="12"/>
     </row>
     <row r="27" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+      <c r="A27" s="8">
         <v>26</v>
       </c>
-      <c r="B27" s="13"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
         <v>33</v>
@@ -3746,10 +3755,10 @@
       <c r="CA27" s="12"/>
     </row>
     <row r="28" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
+      <c r="A28" s="8">
         <v>27</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="5"/>
       <c r="D28" s="9" t="s">
         <v>46</v>
@@ -3839,10 +3848,10 @@
       <c r="CA28" s="12"/>
     </row>
     <row r="29" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="8">
         <v>28</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="5"/>
       <c r="D29" s="9" t="s">
         <v>38</v>
@@ -3934,10 +3943,10 @@
       <c r="CA29" s="12"/>
     </row>
     <row r="30" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="13">
         <v>29</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="5"/>
       <c r="D30" s="9" t="s">
         <v>48</v>
@@ -4027,10 +4036,10 @@
       <c r="CA30" s="12"/>
     </row>
     <row r="31" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
+      <c r="A31" s="8">
         <v>30</v>
       </c>
-      <c r="B31" s="13"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="5"/>
       <c r="D31" s="9" t="s">
         <v>49</v>
@@ -4120,48 +4129,48 @@
       <c r="CA31" s="12"/>
     </row>
     <row r="32" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
+      <c r="A32" s="8">
         <v>31</v>
       </c>
-      <c r="B32" s="13"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="23"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="23"/>
-      <c r="AD32" s="23"/>
-      <c r="AE32" s="23"/>
-      <c r="AF32" s="24">
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="19"/>
+      <c r="AC32" s="19"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="19"/>
+      <c r="AF32" s="20">
         <v>43293</v>
       </c>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="24"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="24"/>
+      <c r="AG32" s="20"/>
+      <c r="AH32" s="20"/>
+      <c r="AI32" s="20"/>
+      <c r="AJ32" s="20"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4190,33 +4199,33 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="25"/>
-      <c r="BH32" s="25"/>
-      <c r="BI32" s="25"/>
-      <c r="BJ32" s="25"/>
-      <c r="BK32" s="25"/>
-      <c r="BL32" s="25"/>
-      <c r="BM32" s="25"/>
-      <c r="BN32" s="25"/>
-      <c r="BO32" s="25"/>
-      <c r="BP32" s="25"/>
-      <c r="BQ32" s="25"/>
-      <c r="BR32" s="25"/>
-      <c r="BS32" s="25"/>
-      <c r="BT32" s="25"/>
-      <c r="BU32" s="25"/>
-      <c r="BV32" s="25"/>
-      <c r="BW32" s="25"/>
-      <c r="BX32" s="25"/>
-      <c r="BY32" s="25"/>
-      <c r="BZ32" s="25"/>
-      <c r="CA32" s="25"/>
+      <c r="BG32" s="21"/>
+      <c r="BH32" s="21"/>
+      <c r="BI32" s="21"/>
+      <c r="BJ32" s="21"/>
+      <c r="BK32" s="21"/>
+      <c r="BL32" s="21"/>
+      <c r="BM32" s="21"/>
+      <c r="BN32" s="21"/>
+      <c r="BO32" s="21"/>
+      <c r="BP32" s="21"/>
+      <c r="BQ32" s="21"/>
+      <c r="BR32" s="21"/>
+      <c r="BS32" s="21"/>
+      <c r="BT32" s="21"/>
+      <c r="BU32" s="21"/>
+      <c r="BV32" s="21"/>
+      <c r="BW32" s="21"/>
+      <c r="BX32" s="21"/>
+      <c r="BY32" s="21"/>
+      <c r="BZ32" s="21"/>
+      <c r="CA32" s="21"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13">
+      <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="13"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="7"/>
       <c r="D33" s="9" t="s">
         <v>50</v>
@@ -4262,27 +4271,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="26">
+      <c r="AP33" s="17">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="27" t="s">
+      <c r="AQ33" s="17"/>
+      <c r="AR33" s="17"/>
+      <c r="AS33" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="27"/>
-      <c r="AU33" s="27"/>
-      <c r="AV33" s="27"/>
-      <c r="AW33" s="27"/>
-      <c r="AX33" s="27"/>
-      <c r="AY33" s="27"/>
-      <c r="AZ33" s="27"/>
-      <c r="BA33" s="27"/>
-      <c r="BB33" s="27"/>
-      <c r="BC33" s="27"/>
-      <c r="BD33" s="27"/>
-      <c r="BE33" s="27"/>
-      <c r="BF33" s="27"/>
+      <c r="AT33" s="18"/>
+      <c r="AU33" s="18"/>
+      <c r="AV33" s="18"/>
+      <c r="AW33" s="18"/>
+      <c r="AX33" s="18"/>
+      <c r="AY33" s="18"/>
+      <c r="AZ33" s="18"/>
+      <c r="BA33" s="18"/>
+      <c r="BB33" s="18"/>
+      <c r="BC33" s="18"/>
+      <c r="BD33" s="18"/>
+      <c r="BE33" s="18"/>
+      <c r="BF33" s="18"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4306,10 +4315,10 @@
       <c r="CA33" s="12"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+      <c r="A34" s="13">
         <v>33</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>50</v>
@@ -4399,10 +4408,10 @@
       <c r="CA34" s="12"/>
     </row>
     <row r="35" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
+      <c r="A35" s="8">
         <v>34</v>
       </c>
-      <c r="B35" s="13"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
         <v>52</v>
@@ -4492,10 +4501,10 @@
       <c r="CA35" s="12"/>
     </row>
     <row r="36" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+      <c r="A36" s="8">
         <v>35</v>
       </c>
-      <c r="B36" s="13"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
         <v>52</v>
@@ -4585,41 +4594,41 @@
       <c r="CA36" s="12"/>
     </row>
     <row r="37" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13">
+      <c r="A37" s="8">
         <v>36</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="29"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="30"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="15"/>
+      <c r="AD37" s="15"/>
+      <c r="AE37" s="16"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4678,41 +4687,41 @@
       <c r="CA37" s="12"/>
     </row>
     <row r="38" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="A38" s="13">
         <v>37</v>
       </c>
-      <c r="B38" s="8"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="30"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
+      <c r="AC38" s="15"/>
+      <c r="AD38" s="15"/>
+      <c r="AE38" s="16"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4771,10 +4780,10 @@
       <c r="CA38" s="12"/>
     </row>
     <row r="39" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A39" s="13">
+      <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="13"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="5"/>
       <c r="D39" s="9" t="s">
         <v>53</v>
@@ -4864,41 +4873,41 @@
       <c r="CA39" s="12"/>
     </row>
     <row r="40" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+      <c r="A40" s="8">
         <v>39</v>
       </c>
-      <c r="B40" s="13"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="30"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="15"/>
+      <c r="AD40" s="15"/>
+      <c r="AE40" s="16"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4957,10 +4966,10 @@
       <c r="CA40" s="12"/>
     </row>
     <row r="41" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13">
+      <c r="A41" s="8">
         <v>40</v>
       </c>
-      <c r="B41" s="13"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="5"/>
       <c r="D41" s="9" t="s">
         <v>53</v>
@@ -5050,41 +5059,41 @@
       <c r="CA41" s="12"/>
     </row>
     <row r="42" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
+      <c r="A42" s="13">
         <v>41</v>
       </c>
-      <c r="B42" s="8"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="30"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
+      <c r="AD42" s="15"/>
+      <c r="AE42" s="16"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5143,41 +5152,41 @@
       <c r="CA42" s="12"/>
     </row>
     <row r="43" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A43" s="13">
+      <c r="A43" s="8">
         <v>42</v>
       </c>
-      <c r="B43" s="13"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="30"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="15"/>
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="15"/>
+      <c r="AC43" s="15"/>
+      <c r="AD43" s="15"/>
+      <c r="AE43" s="16"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5236,41 +5245,41 @@
       <c r="CA43" s="12"/>
     </row>
     <row r="44" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A44" s="13">
+      <c r="A44" s="8">
         <v>43</v>
       </c>
-      <c r="B44" s="13"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="30"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="15"/>
+      <c r="AA44" s="15"/>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="15"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="16"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -5329,10 +5338,10 @@
       <c r="CA44" s="12"/>
     </row>
     <row r="45" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13">
+      <c r="A45" s="8">
         <v>44</v>
       </c>
-      <c r="B45" s="13"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="5"/>
       <c r="D45" s="9" t="s">
         <v>59</v>
@@ -5422,10 +5431,10 @@
       <c r="CA45" s="12"/>
     </row>
     <row r="46" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
+      <c r="A46" s="13">
         <v>45</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="5"/>
       <c r="D46" s="9" t="s">
         <v>60</v>
@@ -5515,10 +5524,10 @@
       <c r="CA46" s="12"/>
     </row>
     <row r="47" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A47" s="13">
+      <c r="A47" s="8">
         <v>46</v>
       </c>
-      <c r="B47" s="13"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="5"/>
       <c r="D47" s="9" t="s">
         <v>62</v>
@@ -5608,10 +5617,10 @@
       <c r="CA47" s="12"/>
     </row>
     <row r="48" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A48" s="13">
+      <c r="A48" s="8">
         <v>47</v>
       </c>
-      <c r="B48" s="13"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="5"/>
       <c r="D48" s="9" t="s">
         <v>62</v>
@@ -5701,10 +5710,10 @@
       <c r="CA48" s="12"/>
     </row>
     <row r="49" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13">
+      <c r="A49" s="8">
         <v>48</v>
       </c>
-      <c r="B49" s="13"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="5"/>
       <c r="D49" s="9" t="s">
         <v>64</v>
@@ -5794,10 +5803,10 @@
       <c r="CA49" s="12"/>
     </row>
     <row r="50" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
+      <c r="A50" s="13">
         <v>49</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="5"/>
       <c r="D50" s="9" t="s">
         <v>65</v>
@@ -5887,10 +5896,10 @@
       <c r="CA50" s="12"/>
     </row>
     <row r="51" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A51" s="13">
+      <c r="A51" s="8">
         <v>50</v>
       </c>
-      <c r="B51" s="13"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="5"/>
       <c r="D51" s="9" t="s">
         <v>66</v>
@@ -5980,10 +5989,10 @@
       <c r="CA51" s="12"/>
     </row>
     <row r="52" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A52" s="13">
+      <c r="A52" s="8">
         <v>51</v>
       </c>
-      <c r="B52" s="13"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="5"/>
       <c r="D52" s="9" t="s">
         <v>66</v>
@@ -6073,10 +6082,10 @@
       <c r="CA52" s="12"/>
     </row>
     <row r="53" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13">
+      <c r="A53" s="8">
         <v>52</v>
       </c>
-      <c r="B53" s="13"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="5"/>
       <c r="D53" s="9" t="s">
         <v>68</v>
@@ -6166,10 +6175,10 @@
       <c r="CA53" s="12"/>
     </row>
     <row r="54" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
+      <c r="A54" s="13">
         <v>53</v>
       </c>
-      <c r="B54" s="8"/>
+      <c r="B54" s="13"/>
       <c r="C54" s="5"/>
       <c r="D54" s="9" t="s">
         <v>69</v>
@@ -6259,10 +6268,10 @@
       <c r="CA54" s="12"/>
     </row>
     <row r="55" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A55" s="13">
+      <c r="A55" s="8">
         <v>54</v>
       </c>
-      <c r="B55" s="13"/>
+      <c r="B55" s="8"/>
       <c r="C55" s="5"/>
       <c r="D55" s="9" t="s">
         <v>71</v>
@@ -6352,10 +6361,10 @@
       <c r="CA55" s="12"/>
     </row>
     <row r="56" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A56" s="13">
+      <c r="A56" s="8">
         <v>55</v>
       </c>
-      <c r="B56" s="13"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="5"/>
       <c r="D56" s="9" t="s">
         <v>72</v>
@@ -6445,10 +6454,10 @@
       <c r="CA56" s="12"/>
     </row>
     <row r="57" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13">
+      <c r="A57" s="8">
         <v>56</v>
       </c>
-      <c r="B57" s="13"/>
+      <c r="B57" s="8"/>
       <c r="C57" s="5"/>
       <c r="D57" s="9" t="s">
         <v>74</v>
@@ -6538,10 +6547,10 @@
       <c r="CA57" s="12"/>
     </row>
     <row r="58" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
+      <c r="A58" s="13">
         <v>57</v>
       </c>
-      <c r="B58" s="8"/>
+      <c r="B58" s="13"/>
       <c r="C58" s="5"/>
       <c r="D58" s="9" t="s">
         <v>75</v>
@@ -6631,10 +6640,10 @@
       <c r="CA58" s="12"/>
     </row>
     <row r="59" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A59" s="13">
+      <c r="A59" s="8">
         <v>58</v>
       </c>
-      <c r="B59" s="13"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="5"/>
       <c r="D59" s="9" t="s">
         <v>77</v>
@@ -6724,10 +6733,10 @@
       <c r="CA59" s="12"/>
     </row>
     <row r="60" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A60" s="13">
+      <c r="A60" s="8">
         <v>59</v>
       </c>
-      <c r="B60" s="13"/>
+      <c r="B60" s="8"/>
       <c r="C60" s="5"/>
       <c r="D60" s="9" t="s">
         <v>75</v>
@@ -6817,10 +6826,10 @@
       <c r="CA60" s="12"/>
     </row>
     <row r="61" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13">
+      <c r="A61" s="8">
         <v>60</v>
       </c>
-      <c r="B61" s="13"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="5"/>
       <c r="D61" s="9" t="s">
         <v>80</v>
@@ -6910,10 +6919,10 @@
       <c r="CA61" s="12"/>
     </row>
     <row r="62" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A62" s="8">
+      <c r="A62" s="13">
         <v>61</v>
       </c>
-      <c r="B62" s="8"/>
+      <c r="B62" s="13"/>
       <c r="C62" s="5"/>
       <c r="D62" s="9" t="s">
         <v>78</v>
@@ -7003,10 +7012,10 @@
       <c r="CA62" s="12"/>
     </row>
     <row r="63" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A63" s="13">
+      <c r="A63" s="8">
         <v>62</v>
       </c>
-      <c r="B63" s="13"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="5"/>
       <c r="D63" s="9" t="s">
         <v>84</v>
@@ -7096,10 +7105,10 @@
       <c r="CA63" s="12"/>
     </row>
     <row r="64" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A64" s="13">
+      <c r="A64" s="8">
         <v>63</v>
       </c>
-      <c r="B64" s="13"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="5"/>
       <c r="D64" s="9" t="s">
         <v>84</v>
@@ -7189,10 +7198,10 @@
       <c r="CA64" s="12"/>
     </row>
     <row r="65" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13">
+      <c r="A65" s="8">
         <v>64</v>
       </c>
-      <c r="B65" s="13"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="5"/>
       <c r="D65" s="9" t="s">
         <v>83</v>
@@ -7280,10 +7289,10 @@
       <c r="CA65" s="12"/>
     </row>
     <row r="66" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A66" s="8">
+      <c r="A66" s="13">
         <v>65</v>
       </c>
-      <c r="B66" s="8"/>
+      <c r="B66" s="13"/>
       <c r="C66" s="5"/>
       <c r="D66" s="9" t="s">
         <v>85</v>
@@ -7373,10 +7382,10 @@
       <c r="CA66" s="12"/>
     </row>
     <row r="67" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A67" s="13">
+      <c r="A67" s="8">
         <v>66</v>
       </c>
-      <c r="B67" s="13"/>
+      <c r="B67" s="8"/>
       <c r="C67" s="5"/>
       <c r="D67" s="9" t="s">
         <v>87</v>
@@ -7466,10 +7475,10 @@
       <c r="CA67" s="12"/>
     </row>
     <row r="68" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A68" s="13">
+      <c r="A68" s="8">
         <v>67</v>
       </c>
-      <c r="B68" s="13"/>
+      <c r="B68" s="8"/>
       <c r="C68" s="5"/>
       <c r="D68" s="9" t="s">
         <v>87</v>
@@ -7559,10 +7568,10 @@
       <c r="CA68" s="12"/>
     </row>
     <row r="69" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="13">
+      <c r="A69" s="8">
         <v>68</v>
       </c>
-      <c r="B69" s="13"/>
+      <c r="B69" s="8"/>
       <c r="C69" s="5"/>
       <c r="D69" s="9" t="s">
         <v>88</v>
@@ -7652,10 +7661,10 @@
       <c r="CA69" s="12"/>
     </row>
     <row r="70" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A70" s="8">
+      <c r="A70" s="13">
         <v>69</v>
       </c>
-      <c r="B70" s="8"/>
+      <c r="B70" s="13"/>
       <c r="C70" s="5"/>
       <c r="D70" s="9" t="s">
         <v>90</v>
@@ -7745,10 +7754,10 @@
       <c r="CA70" s="12"/>
     </row>
     <row r="71" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A71" s="13">
+      <c r="A71" s="8">
         <v>70</v>
       </c>
-      <c r="B71" s="13"/>
+      <c r="B71" s="8"/>
       <c r="C71" s="5"/>
       <c r="D71" s="9" t="s">
         <v>90</v>
@@ -7838,10 +7847,10 @@
       <c r="CA71" s="12"/>
     </row>
     <row r="72" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A72" s="13">
+      <c r="A72" s="8">
         <v>71</v>
       </c>
-      <c r="B72" s="13"/>
+      <c r="B72" s="8"/>
       <c r="C72" s="5"/>
       <c r="D72" s="9" t="s">
         <v>91</v>
@@ -7931,10 +7940,10 @@
       <c r="CA72" s="12"/>
     </row>
     <row r="73" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="13">
+      <c r="A73" s="8">
         <v>72</v>
       </c>
-      <c r="B73" s="13"/>
+      <c r="B73" s="8"/>
       <c r="C73" s="5"/>
       <c r="D73" s="9" t="s">
         <v>92</v>
@@ -8024,10 +8033,10 @@
       <c r="CA73" s="12"/>
     </row>
     <row r="74" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
+      <c r="A74" s="13">
         <v>73</v>
       </c>
-      <c r="B74" s="8"/>
+      <c r="B74" s="13"/>
       <c r="C74" s="5"/>
       <c r="D74" s="9" t="s">
         <v>93</v>
@@ -8117,10 +8126,10 @@
       <c r="CA74" s="12"/>
     </row>
     <row r="75" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A75" s="13">
+      <c r="A75" s="8">
         <v>74</v>
       </c>
-      <c r="B75" s="13"/>
+      <c r="B75" s="8"/>
       <c r="C75" s="5"/>
       <c r="D75" s="9" t="s">
         <v>94</v>
@@ -8210,10 +8219,10 @@
       <c r="CA75" s="12"/>
     </row>
     <row r="76" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A76" s="13">
+      <c r="A76" s="8">
         <v>75</v>
       </c>
-      <c r="B76" s="13"/>
+      <c r="B76" s="8"/>
       <c r="C76" s="5"/>
       <c r="D76" s="9" t="s">
         <v>94</v>
@@ -8303,10 +8312,10 @@
       <c r="CA76" s="12"/>
     </row>
     <row r="77" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="13">
+      <c r="A77" s="8">
         <v>76</v>
       </c>
-      <c r="B77" s="13"/>
+      <c r="B77" s="8"/>
       <c r="C77" s="5"/>
       <c r="D77" s="9" t="s">
         <v>95</v>
@@ -8396,10 +8405,10 @@
       <c r="CA77" s="12"/>
     </row>
     <row r="78" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
+      <c r="A78" s="13">
         <v>77</v>
       </c>
-      <c r="B78" s="8"/>
+      <c r="B78" s="13"/>
       <c r="C78" s="5"/>
       <c r="D78" s="9" t="s">
         <v>97</v>
@@ -8489,10 +8498,10 @@
       <c r="CA78" s="12"/>
     </row>
     <row r="79" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A79" s="13">
+      <c r="A79" s="8">
         <v>78</v>
       </c>
-      <c r="B79" s="13"/>
+      <c r="B79" s="8"/>
       <c r="C79" s="5"/>
       <c r="D79" s="9" t="s">
         <v>96</v>
@@ -8582,10 +8591,10 @@
       <c r="CA79" s="12"/>
     </row>
     <row r="80" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A80" s="13">
+      <c r="A80" s="8">
         <v>79</v>
       </c>
-      <c r="B80" s="13"/>
+      <c r="B80" s="8"/>
       <c r="C80" s="5"/>
       <c r="D80" s="9" t="s">
         <v>96</v>
@@ -8675,10 +8684,10 @@
       <c r="CA80" s="12"/>
     </row>
     <row r="81" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="13">
+      <c r="A81" s="8">
         <v>80</v>
       </c>
-      <c r="B81" s="13"/>
+      <c r="B81" s="8"/>
       <c r="C81" s="5"/>
       <c r="D81" s="9" t="s">
         <v>98</v>
@@ -8768,10 +8777,10 @@
       <c r="CA81" s="12"/>
     </row>
     <row r="82" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A82" s="8">
+      <c r="A82" s="13">
         <v>81</v>
       </c>
-      <c r="B82" s="8"/>
+      <c r="B82" s="13"/>
       <c r="C82" s="5"/>
       <c r="D82" s="9" t="s">
         <v>99</v>
@@ -8861,10 +8870,10 @@
       <c r="CA82" s="12"/>
     </row>
     <row r="83" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A83" s="13">
+      <c r="A83" s="8">
         <v>82</v>
       </c>
-      <c r="B83" s="13"/>
+      <c r="B83" s="8"/>
       <c r="C83" s="5"/>
       <c r="D83" s="9" t="s">
         <v>101</v>
@@ -8954,10 +8963,10 @@
       <c r="CA83" s="12"/>
     </row>
     <row r="84" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A84" s="13">
+      <c r="A84" s="8">
         <v>83</v>
       </c>
-      <c r="B84" s="13"/>
+      <c r="B84" s="8"/>
       <c r="C84" s="5"/>
       <c r="D84" s="9" t="s">
         <v>100</v>
@@ -9047,10 +9056,10 @@
       <c r="CA84" s="12"/>
     </row>
     <row r="85" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="13">
+      <c r="A85" s="8">
         <v>84</v>
       </c>
-      <c r="B85" s="13"/>
+      <c r="B85" s="8"/>
       <c r="C85" s="5"/>
       <c r="D85" s="9" t="s">
         <v>102</v>
@@ -9140,10 +9149,10 @@
       <c r="CA85" s="12"/>
     </row>
     <row r="86" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A86" s="8">
+      <c r="A86" s="13">
         <v>85</v>
       </c>
-      <c r="B86" s="8"/>
+      <c r="B86" s="13"/>
       <c r="C86" s="5"/>
       <c r="D86" s="9" t="s">
         <v>99</v>
@@ -9233,10 +9242,10 @@
       <c r="CA86" s="12"/>
     </row>
     <row r="87" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A87" s="13">
+      <c r="A87" s="8">
         <v>86</v>
       </c>
-      <c r="B87" s="13"/>
+      <c r="B87" s="8"/>
       <c r="C87" s="5"/>
       <c r="D87" s="9" t="s">
         <v>103</v>
@@ -9326,10 +9335,10 @@
       <c r="CA87" s="12"/>
     </row>
     <row r="88" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A88" s="13">
+      <c r="A88" s="8">
         <v>87</v>
       </c>
-      <c r="B88" s="13"/>
+      <c r="B88" s="8"/>
       <c r="C88" s="5"/>
       <c r="D88" s="9" t="s">
         <v>104</v>
@@ -9417,10 +9426,10 @@
       <c r="CA88" s="12"/>
     </row>
     <row r="89" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="13">
+      <c r="A89" s="8">
         <v>88</v>
       </c>
-      <c r="B89" s="13"/>
+      <c r="B89" s="8"/>
       <c r="C89" s="5"/>
       <c r="D89" s="9" t="s">
         <v>105</v>
@@ -9508,10 +9517,10 @@
       <c r="CA89" s="12"/>
     </row>
     <row r="90" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A90" s="8">
+      <c r="A90" s="13">
         <v>89</v>
       </c>
-      <c r="B90" s="8"/>
+      <c r="B90" s="13"/>
       <c r="C90" s="5"/>
       <c r="D90" s="9" t="s">
         <v>105</v>
@@ -9599,10 +9608,10 @@
       <c r="CA90" s="12"/>
     </row>
     <row r="91" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A91" s="13">
+      <c r="A91" s="8">
         <v>90</v>
       </c>
-      <c r="B91" s="13"/>
+      <c r="B91" s="8"/>
       <c r="C91" s="5"/>
       <c r="D91" s="9" t="s">
         <v>105</v>
@@ -9690,10 +9699,10 @@
       <c r="CA91" s="12"/>
     </row>
     <row r="92" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A92" s="13">
+      <c r="A92" s="8">
         <v>91</v>
       </c>
-      <c r="B92" s="13"/>
+      <c r="B92" s="8"/>
       <c r="C92" s="5"/>
       <c r="D92" s="9" t="s">
         <v>107</v>
@@ -9783,10 +9792,10 @@
       <c r="CA92" s="12"/>
     </row>
     <row r="93" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="13">
+      <c r="A93" s="8">
         <v>92</v>
       </c>
-      <c r="B93" s="13"/>
+      <c r="B93" s="8"/>
       <c r="C93" s="5"/>
       <c r="D93" s="9" t="s">
         <v>107</v>
@@ -9876,10 +9885,10 @@
       <c r="CA93" s="12"/>
     </row>
     <row r="94" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A94" s="8">
+      <c r="A94" s="13">
         <v>93</v>
       </c>
-      <c r="B94" s="8"/>
+      <c r="B94" s="13"/>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
         <v>109</v>
@@ -9969,10 +9978,10 @@
       <c r="CA94" s="12"/>
     </row>
     <row r="95" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A95" s="13">
+      <c r="A95" s="8">
         <v>94</v>
       </c>
-      <c r="B95" s="13"/>
+      <c r="B95" s="8"/>
       <c r="C95" s="5"/>
       <c r="D95" s="9" t="s">
         <v>111</v>
@@ -10062,10 +10071,10 @@
       <c r="CA95" s="12"/>
     </row>
     <row r="96" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A96" s="13">
+      <c r="A96" s="8">
         <v>95</v>
       </c>
-      <c r="B96" s="13"/>
+      <c r="B96" s="8"/>
       <c r="C96" s="5"/>
       <c r="D96" s="9" t="s">
         <v>114</v>
@@ -10155,10 +10164,10 @@
       <c r="CA96" s="12"/>
     </row>
     <row r="97" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="13">
+      <c r="A97" s="8">
         <v>96</v>
       </c>
-      <c r="B97" s="13"/>
+      <c r="B97" s="8"/>
       <c r="C97" s="5"/>
       <c r="D97" s="9" t="s">
         <v>115</v>
@@ -10248,10 +10257,10 @@
       <c r="CA97" s="12"/>
     </row>
     <row r="98" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A98" s="8">
+      <c r="A98" s="13">
         <v>97</v>
       </c>
-      <c r="B98" s="8"/>
+      <c r="B98" s="13"/>
       <c r="C98" s="5"/>
       <c r="D98" s="9" t="s">
         <v>116</v>
@@ -10341,10 +10350,10 @@
       <c r="CA98" s="12"/>
     </row>
     <row r="99" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A99" s="13">
+      <c r="A99" s="8">
         <v>98</v>
       </c>
-      <c r="B99" s="13"/>
+      <c r="B99" s="8"/>
       <c r="C99" s="5"/>
       <c r="D99" s="9" t="s">
         <v>117</v>
@@ -10434,10 +10443,10 @@
       <c r="CA99" s="12"/>
     </row>
     <row r="100" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A100" s="13">
+      <c r="A100" s="8">
         <v>99</v>
       </c>
-      <c r="B100" s="13"/>
+      <c r="B100" s="8"/>
       <c r="C100" s="5"/>
       <c r="D100" s="9" t="s">
         <v>117</v>
@@ -10527,10 +10536,10 @@
       <c r="CA100" s="12"/>
     </row>
     <row r="101" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="13">
+      <c r="A101" s="8">
         <v>100</v>
       </c>
-      <c r="B101" s="13"/>
+      <c r="B101" s="8"/>
       <c r="C101" s="5"/>
       <c r="D101" s="9" t="s">
         <v>119</v>
@@ -10620,10 +10629,10 @@
       <c r="CA101" s="12"/>
     </row>
     <row r="102" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A102" s="8">
+      <c r="A102" s="13">
         <v>101</v>
       </c>
-      <c r="B102" s="8"/>
+      <c r="B102" s="13"/>
       <c r="C102" s="5"/>
       <c r="D102" s="9" t="s">
         <v>120</v>
@@ -10713,10 +10722,10 @@
       <c r="CA102" s="12"/>
     </row>
     <row r="103" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A103" s="13">
+      <c r="A103" s="8">
         <v>102</v>
       </c>
-      <c r="B103" s="13"/>
+      <c r="B103" s="8"/>
       <c r="C103" s="5"/>
       <c r="D103" s="9" t="s">
         <v>120</v>
@@ -10806,10 +10815,10 @@
       <c r="CA103" s="12"/>
     </row>
     <row r="104" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A104" s="13">
+      <c r="A104" s="8">
         <v>103</v>
       </c>
-      <c r="B104" s="13"/>
+      <c r="B104" s="8"/>
       <c r="C104" s="5"/>
       <c r="D104" s="9" t="s">
         <v>123</v>
@@ -10899,10 +10908,10 @@
       <c r="CA104" s="12"/>
     </row>
     <row r="105" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="13">
+      <c r="A105" s="8">
         <v>104</v>
       </c>
-      <c r="B105" s="13"/>
+      <c r="B105" s="8"/>
       <c r="C105" s="5"/>
       <c r="D105" s="9" t="s">
         <v>123</v>
@@ -10992,10 +11001,10 @@
       <c r="CA105" s="12"/>
     </row>
     <row r="106" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A106" s="8">
+      <c r="A106" s="13">
         <v>105</v>
       </c>
-      <c r="B106" s="8"/>
+      <c r="B106" s="13"/>
       <c r="C106" s="5"/>
       <c r="D106" s="9" t="s">
         <v>125</v>
@@ -11085,10 +11094,10 @@
       <c r="CA106" s="12"/>
     </row>
     <row r="107" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A107" s="13">
+      <c r="A107" s="8">
         <v>106</v>
       </c>
-      <c r="B107" s="13"/>
+      <c r="B107" s="8"/>
       <c r="C107" s="5"/>
       <c r="D107" s="9" t="s">
         <v>123</v>
@@ -11178,10 +11187,10 @@
       <c r="CA107" s="12"/>
     </row>
     <row r="108" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A108" s="13">
+      <c r="A108" s="8">
         <v>107</v>
       </c>
-      <c r="B108" s="13"/>
+      <c r="B108" s="8"/>
       <c r="C108" s="5"/>
       <c r="D108" s="9" t="s">
         <v>125</v>
@@ -11271,12 +11280,14 @@
       <c r="CA108" s="12"/>
     </row>
     <row r="109" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="13">
+      <c r="A109" s="8">
         <v>108</v>
       </c>
-      <c r="B109" s="13"/>
+      <c r="B109" s="8"/>
       <c r="C109" s="5"/>
-      <c r="D109" s="9"/>
+      <c r="D109" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="E109" s="9"/>
       <c r="F109" s="9"/>
       <c r="G109" s="9"/>
@@ -11304,20 +11315,28 @@
       <c r="AC109" s="9"/>
       <c r="AD109" s="9"/>
       <c r="AE109" s="9"/>
-      <c r="AF109" s="10"/>
+      <c r="AF109" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="AG109" s="10"/>
       <c r="AH109" s="10"/>
       <c r="AI109" s="10"/>
       <c r="AJ109" s="10"/>
-      <c r="AK109" s="9"/>
+      <c r="AK109" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL109" s="9"/>
       <c r="AM109" s="9"/>
       <c r="AN109" s="9"/>
       <c r="AO109" s="9"/>
-      <c r="AP109" s="11"/>
+      <c r="AP109" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ109" s="11"/>
       <c r="AR109" s="11"/>
-      <c r="AS109" s="9"/>
+      <c r="AS109" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT109" s="9"/>
       <c r="AU109" s="9"/>
       <c r="AV109" s="9"/>
@@ -11354,12 +11373,14 @@
       <c r="CA109" s="12"/>
     </row>
     <row r="110" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A110" s="8">
+      <c r="A110" s="13">
         <v>109</v>
       </c>
-      <c r="B110" s="8"/>
+      <c r="B110" s="13"/>
       <c r="C110" s="5"/>
-      <c r="D110" s="9"/>
+      <c r="D110" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="E110" s="9"/>
       <c r="F110" s="9"/>
       <c r="G110" s="9"/>
@@ -11387,20 +11408,28 @@
       <c r="AC110" s="9"/>
       <c r="AD110" s="9"/>
       <c r="AE110" s="9"/>
-      <c r="AF110" s="10"/>
+      <c r="AF110" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="AG110" s="10"/>
       <c r="AH110" s="10"/>
       <c r="AI110" s="10"/>
       <c r="AJ110" s="10"/>
-      <c r="AK110" s="9"/>
+      <c r="AK110" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL110" s="9"/>
       <c r="AM110" s="9"/>
       <c r="AN110" s="9"/>
       <c r="AO110" s="9"/>
-      <c r="AP110" s="11"/>
+      <c r="AP110" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ110" s="11"/>
       <c r="AR110" s="11"/>
-      <c r="AS110" s="9"/>
+      <c r="AS110" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT110" s="9"/>
       <c r="AU110" s="9"/>
       <c r="AV110" s="9"/>
@@ -11437,12 +11466,14 @@
       <c r="CA110" s="12"/>
     </row>
     <row r="111" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A111" s="13">
+      <c r="A111" s="8">
         <v>110</v>
       </c>
-      <c r="B111" s="13"/>
+      <c r="B111" s="8"/>
       <c r="C111" s="5"/>
-      <c r="D111" s="9"/>
+      <c r="D111" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="E111" s="9"/>
       <c r="F111" s="9"/>
       <c r="G111" s="9"/>
@@ -11470,20 +11501,28 @@
       <c r="AC111" s="9"/>
       <c r="AD111" s="9"/>
       <c r="AE111" s="9"/>
-      <c r="AF111" s="10"/>
+      <c r="AF111" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="AG111" s="10"/>
       <c r="AH111" s="10"/>
       <c r="AI111" s="10"/>
       <c r="AJ111" s="10"/>
-      <c r="AK111" s="9"/>
+      <c r="AK111" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL111" s="9"/>
       <c r="AM111" s="9"/>
       <c r="AN111" s="9"/>
       <c r="AO111" s="9"/>
-      <c r="AP111" s="11"/>
+      <c r="AP111" s="11">
+        <v>0</v>
+      </c>
       <c r="AQ111" s="11"/>
       <c r="AR111" s="11"/>
-      <c r="AS111" s="9"/>
+      <c r="AS111" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT111" s="9"/>
       <c r="AU111" s="9"/>
       <c r="AV111" s="9"/>
@@ -11520,10 +11559,10 @@
       <c r="CA111" s="12"/>
     </row>
     <row r="112" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A112" s="13">
+      <c r="A112" s="8">
         <v>111</v>
       </c>
-      <c r="B112" s="13"/>
+      <c r="B112" s="8"/>
       <c r="C112" s="5"/>
       <c r="D112" s="9"/>
       <c r="E112" s="9"/>
@@ -11603,10 +11642,10 @@
       <c r="CA112" s="12"/>
     </row>
     <row r="113" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="13">
+      <c r="A113" s="8">
         <v>112</v>
       </c>
-      <c r="B113" s="13"/>
+      <c r="B113" s="8"/>
       <c r="C113" s="5"/>
       <c r="D113" s="9"/>
       <c r="E113" s="9"/>
@@ -11686,10 +11725,10 @@
       <c r="CA113" s="12"/>
     </row>
     <row r="114" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A114" s="8">
+      <c r="A114" s="13">
         <v>113</v>
       </c>
-      <c r="B114" s="8"/>
+      <c r="B114" s="13"/>
       <c r="C114" s="5"/>
       <c r="D114" s="9"/>
       <c r="E114" s="9"/>
@@ -11769,10 +11808,10 @@
       <c r="CA114" s="12"/>
     </row>
     <row r="115" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A115" s="13">
+      <c r="A115" s="8">
         <v>114</v>
       </c>
-      <c r="B115" s="13"/>
+      <c r="B115" s="8"/>
       <c r="C115" s="5"/>
       <c r="D115" s="9"/>
       <c r="E115" s="9"/>
@@ -11852,10 +11891,10 @@
       <c r="CA115" s="12"/>
     </row>
     <row r="116" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A116" s="13">
+      <c r="A116" s="8">
         <v>115</v>
       </c>
-      <c r="B116" s="13"/>
+      <c r="B116" s="8"/>
       <c r="C116" s="5"/>
       <c r="D116" s="9"/>
       <c r="E116" s="9"/>
@@ -11935,10 +11974,10 @@
       <c r="CA116" s="12"/>
     </row>
     <row r="117" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="13">
+      <c r="A117" s="8">
         <v>116</v>
       </c>
-      <c r="B117" s="13"/>
+      <c r="B117" s="8"/>
       <c r="C117" s="5"/>
       <c r="D117" s="9"/>
       <c r="E117" s="9"/>
@@ -12018,10 +12057,10 @@
       <c r="CA117" s="12"/>
     </row>
     <row r="118" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A118" s="8">
+      <c r="A118" s="13">
         <v>117</v>
       </c>
-      <c r="B118" s="8"/>
+      <c r="B118" s="13"/>
       <c r="C118" s="5"/>
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
@@ -12101,10 +12140,10 @@
       <c r="CA118" s="12"/>
     </row>
     <row r="119" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A119" s="13">
+      <c r="A119" s="8">
         <v>118</v>
       </c>
-      <c r="B119" s="13"/>
+      <c r="B119" s="8"/>
       <c r="C119" s="5"/>
       <c r="D119" s="9"/>
       <c r="E119" s="9"/>
@@ -12184,10 +12223,10 @@
       <c r="CA119" s="12"/>
     </row>
     <row r="120" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A120" s="13">
+      <c r="A120" s="8">
         <v>119</v>
       </c>
-      <c r="B120" s="13"/>
+      <c r="B120" s="8"/>
       <c r="C120" s="5"/>
       <c r="D120" s="9"/>
       <c r="E120" s="9"/>
@@ -12267,10 +12306,10 @@
       <c r="CA120" s="12"/>
     </row>
     <row r="121" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="13">
+      <c r="A121" s="8">
         <v>120</v>
       </c>
-      <c r="B121" s="13"/>
+      <c r="B121" s="8"/>
       <c r="C121" s="5"/>
       <c r="D121" s="9"/>
       <c r="E121" s="9"/>
@@ -12350,10 +12389,10 @@
       <c r="CA121" s="12"/>
     </row>
     <row r="122" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A122" s="8">
+      <c r="A122" s="13">
         <v>121</v>
       </c>
-      <c r="B122" s="8"/>
+      <c r="B122" s="13"/>
       <c r="C122" s="5"/>
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
@@ -12433,10 +12472,10 @@
       <c r="CA122" s="12"/>
     </row>
     <row r="123" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A123" s="13">
+      <c r="A123" s="8">
         <v>122</v>
       </c>
-      <c r="B123" s="13"/>
+      <c r="B123" s="8"/>
       <c r="C123" s="5"/>
       <c r="BG123" s="12"/>
       <c r="BH123" s="12"/>
@@ -12462,493 +12501,351 @@
     </row>
   </sheetData>
   <mergeCells count="856">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12973,351 +12870,493 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
báo cáo ngày 13/2/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="134">
   <si>
     <t>No.</t>
   </si>
@@ -411,6 +411,18 @@
   <si>
     <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data</t>
   </si>
+  <si>
+    <t>13/2/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data - Tạo câu lệnh sql để update bảng server đích</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data - Tạo file csv backup data bảng đích</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data - Lưu lịch sử chạy backup</t>
+  </si>
 </sst>
 </file>
 
@@ -672,20 +684,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -705,6 +709,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,7 +822,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1201,7 +1213,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1213,7 +1225,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK117" sqref="AK117:AO117"/>
+      <selection pane="bottomLeft" activeCell="AS115" sqref="AS115:BF115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,198 +1240,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="24" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="23" t="s">
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="25" t="s">
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="23" t="s">
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="23"/>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
-      <c r="BF1" s="23"/>
-      <c r="BG1" s="26" t="s">
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
+      <c r="AY1" s="15"/>
+      <c r="AZ1" s="15"/>
+      <c r="BA1" s="15"/>
+      <c r="BB1" s="15"/>
+      <c r="BC1" s="15"/>
+      <c r="BD1" s="15"/>
+      <c r="BE1" s="15"/>
+      <c r="BF1" s="15"/>
+      <c r="BG1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="26"/>
-      <c r="BI1" s="26"/>
-      <c r="BJ1" s="26"/>
-      <c r="BK1" s="26"/>
-      <c r="BL1" s="26"/>
-      <c r="BM1" s="26"/>
-      <c r="BN1" s="26"/>
-      <c r="BO1" s="26"/>
-      <c r="BP1" s="26"/>
-      <c r="BQ1" s="26"/>
-      <c r="BR1" s="26"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="26"/>
-      <c r="BU1" s="26"/>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="26"/>
-      <c r="BZ1" s="26"/>
-      <c r="CA1" s="26"/>
+      <c r="BH1" s="18"/>
+      <c r="BI1" s="18"/>
+      <c r="BJ1" s="18"/>
+      <c r="BK1" s="18"/>
+      <c r="BL1" s="18"/>
+      <c r="BM1" s="18"/>
+      <c r="BN1" s="18"/>
+      <c r="BO1" s="18"/>
+      <c r="BP1" s="18"/>
+      <c r="BQ1" s="18"/>
+      <c r="BR1" s="18"/>
+      <c r="BS1" s="18"/>
+      <c r="BT1" s="18"/>
+      <c r="BU1" s="18"/>
+      <c r="BV1" s="18"/>
+      <c r="BW1" s="18"/>
+      <c r="BX1" s="18"/>
+      <c r="BY1" s="18"/>
+      <c r="BZ1" s="18"/>
+      <c r="CA1" s="18"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="21">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="5"/>
       <c r="D3" s="9" t="s">
         <v>17</v>
@@ -1509,10 +1521,10 @@
       <c r="CA3" s="12"/>
     </row>
     <row r="4" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="5"/>
       <c r="D4" s="9" t="s">
         <v>18</v>
@@ -1602,10 +1614,10 @@
       <c r="CA4" s="12"/>
     </row>
     <row r="5" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="5"/>
       <c r="D5" s="9" t="s">
         <v>18</v>
@@ -1697,10 +1709,10 @@
       <c r="CA5" s="12"/>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -1790,10 +1802,10 @@
       <c r="CA6" s="12"/>
     </row>
     <row r="7" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
         <v>22</v>
@@ -1883,10 +1895,10 @@
       <c r="CA7" s="12"/>
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
         <v>24</v>
@@ -1976,10 +1988,10 @@
       <c r="CA8" s="12"/>
     </row>
     <row r="9" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
         <v>33</v>
@@ -2071,10 +2083,10 @@
       <c r="CA9" s="12"/>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
         <v>33</v>
@@ -2164,10 +2176,10 @@
       <c r="CA10" s="12"/>
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
         <v>33</v>
@@ -2257,10 +2269,10 @@
       <c r="CA11" s="12"/>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="9" t="s">
         <v>33</v>
@@ -2350,10 +2362,10 @@
       <c r="CA12" s="12"/>
     </row>
     <row r="13" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>33</v>
@@ -2445,10 +2457,10 @@
       <c r="CA13" s="12"/>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="13"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="5"/>
       <c r="D14" s="9" t="s">
         <v>33</v>
@@ -2540,10 +2552,10 @@
       <c r="CA14" s="12"/>
     </row>
     <row r="15" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
         <v>33</v>
@@ -2633,10 +2645,10 @@
       <c r="CA15" s="12"/>
     </row>
     <row r="16" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
         <v>36</v>
@@ -2726,10 +2738,10 @@
       <c r="CA16" s="12"/>
     </row>
     <row r="17" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
         <v>33</v>
@@ -2821,10 +2833,10 @@
       <c r="CA17" s="12"/>
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
         <v>38</v>
@@ -2914,10 +2926,10 @@
       <c r="CA18" s="12"/>
     </row>
     <row r="19" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
         <v>38</v>
@@ -3007,10 +3019,10 @@
       <c r="CA19" s="12"/>
     </row>
     <row r="20" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="13">
         <v>19</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="9" t="s">
         <v>38</v>
@@ -3100,10 +3112,10 @@
       <c r="CA20" s="12"/>
     </row>
     <row r="21" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="A21" s="13">
         <v>20</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="9" t="s">
         <v>38</v>
@@ -3193,10 +3205,10 @@
       <c r="CA21" s="12"/>
     </row>
     <row r="22" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="A22" s="8">
         <v>21</v>
       </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="5"/>
       <c r="D22" s="9" t="s">
         <v>44</v>
@@ -3288,10 +3300,10 @@
       <c r="CA22" s="12"/>
     </row>
     <row r="23" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="13">
         <v>22</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="9" t="s">
         <v>38</v>
@@ -3383,10 +3395,10 @@
       <c r="CA23" s="12"/>
     </row>
     <row r="24" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="13">
         <v>23</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="9" t="s">
         <v>33</v>
@@ -3476,10 +3488,10 @@
       <c r="CA24" s="12"/>
     </row>
     <row r="25" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8">
+      <c r="A25" s="13">
         <v>24</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="5"/>
       <c r="D25" s="9" t="s">
         <v>45</v>
@@ -3569,10 +3581,10 @@
       <c r="CA25" s="12"/>
     </row>
     <row r="26" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
+      <c r="A26" s="8">
         <v>25</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
         <v>38</v>
@@ -3662,10 +3674,10 @@
       <c r="CA26" s="12"/>
     </row>
     <row r="27" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="13">
         <v>26</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
         <v>33</v>
@@ -3755,10 +3767,10 @@
       <c r="CA27" s="12"/>
     </row>
     <row r="28" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="13">
         <v>27</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="9" t="s">
         <v>46</v>
@@ -3848,10 +3860,10 @@
       <c r="CA28" s="12"/>
     </row>
     <row r="29" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8">
+      <c r="A29" s="13">
         <v>28</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="9" t="s">
         <v>38</v>
@@ -3943,10 +3955,10 @@
       <c r="CA29" s="12"/>
     </row>
     <row r="30" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+      <c r="A30" s="8">
         <v>29</v>
       </c>
-      <c r="B30" s="13"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="5"/>
       <c r="D30" s="9" t="s">
         <v>48</v>
@@ -4036,10 +4048,10 @@
       <c r="CA30" s="12"/>
     </row>
     <row r="31" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="13">
         <v>30</v>
       </c>
-      <c r="B31" s="8"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="5"/>
       <c r="D31" s="9" t="s">
         <v>49</v>
@@ -4129,48 +4141,48 @@
       <c r="CA31" s="12"/>
     </row>
     <row r="32" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="13">
         <v>31</v>
       </c>
-      <c r="B32" s="8"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="19"/>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="19"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
-      <c r="AD32" s="19"/>
-      <c r="AE32" s="19"/>
-      <c r="AF32" s="20">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
+      <c r="AE32" s="23"/>
+      <c r="AF32" s="24">
         <v>43293</v>
       </c>
-      <c r="AG32" s="20"/>
-      <c r="AH32" s="20"/>
-      <c r="AI32" s="20"/>
-      <c r="AJ32" s="20"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4199,33 +4211,33 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="21"/>
-      <c r="BH32" s="21"/>
-      <c r="BI32" s="21"/>
-      <c r="BJ32" s="21"/>
-      <c r="BK32" s="21"/>
-      <c r="BL32" s="21"/>
-      <c r="BM32" s="21"/>
-      <c r="BN32" s="21"/>
-      <c r="BO32" s="21"/>
-      <c r="BP32" s="21"/>
-      <c r="BQ32" s="21"/>
-      <c r="BR32" s="21"/>
-      <c r="BS32" s="21"/>
-      <c r="BT32" s="21"/>
-      <c r="BU32" s="21"/>
-      <c r="BV32" s="21"/>
-      <c r="BW32" s="21"/>
-      <c r="BX32" s="21"/>
-      <c r="BY32" s="21"/>
-      <c r="BZ32" s="21"/>
-      <c r="CA32" s="21"/>
+      <c r="BG32" s="25"/>
+      <c r="BH32" s="25"/>
+      <c r="BI32" s="25"/>
+      <c r="BJ32" s="25"/>
+      <c r="BK32" s="25"/>
+      <c r="BL32" s="25"/>
+      <c r="BM32" s="25"/>
+      <c r="BN32" s="25"/>
+      <c r="BO32" s="25"/>
+      <c r="BP32" s="25"/>
+      <c r="BQ32" s="25"/>
+      <c r="BR32" s="25"/>
+      <c r="BS32" s="25"/>
+      <c r="BT32" s="25"/>
+      <c r="BU32" s="25"/>
+      <c r="BV32" s="25"/>
+      <c r="BW32" s="25"/>
+      <c r="BX32" s="25"/>
+      <c r="BY32" s="25"/>
+      <c r="BZ32" s="25"/>
+      <c r="CA32" s="25"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
+      <c r="A33" s="13">
         <v>32</v>
       </c>
-      <c r="B33" s="8"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="7"/>
       <c r="D33" s="9" t="s">
         <v>50</v>
@@ -4271,27 +4283,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="17">
+      <c r="AP33" s="26">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="17"/>
-      <c r="AR33" s="17"/>
-      <c r="AS33" s="18" t="s">
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="18"/>
-      <c r="AU33" s="18"/>
-      <c r="AV33" s="18"/>
-      <c r="AW33" s="18"/>
-      <c r="AX33" s="18"/>
-      <c r="AY33" s="18"/>
-      <c r="AZ33" s="18"/>
-      <c r="BA33" s="18"/>
-      <c r="BB33" s="18"/>
-      <c r="BC33" s="18"/>
-      <c r="BD33" s="18"/>
-      <c r="BE33" s="18"/>
-      <c r="BF33" s="18"/>
+      <c r="AT33" s="27"/>
+      <c r="AU33" s="27"/>
+      <c r="AV33" s="27"/>
+      <c r="AW33" s="27"/>
+      <c r="AX33" s="27"/>
+      <c r="AY33" s="27"/>
+      <c r="AZ33" s="27"/>
+      <c r="BA33" s="27"/>
+      <c r="BB33" s="27"/>
+      <c r="BC33" s="27"/>
+      <c r="BD33" s="27"/>
+      <c r="BE33" s="27"/>
+      <c r="BF33" s="27"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4315,10 +4327,10 @@
       <c r="CA33" s="12"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
+      <c r="A34" s="8">
         <v>33</v>
       </c>
-      <c r="B34" s="13"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>50</v>
@@ -4408,10 +4420,10 @@
       <c r="CA34" s="12"/>
     </row>
     <row r="35" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="13">
         <v>34</v>
       </c>
-      <c r="B35" s="8"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
         <v>52</v>
@@ -4501,10 +4513,10 @@
       <c r="CA35" s="12"/>
     </row>
     <row r="36" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+      <c r="A36" s="13">
         <v>35</v>
       </c>
-      <c r="B36" s="8"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
         <v>52</v>
@@ -4594,41 +4606,41 @@
       <c r="CA36" s="12"/>
     </row>
     <row r="37" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8">
+      <c r="A37" s="13">
         <v>36</v>
       </c>
-      <c r="B37" s="8"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
-      <c r="V37" s="15"/>
-      <c r="W37" s="15"/>
-      <c r="X37" s="15"/>
-      <c r="Y37" s="15"/>
-      <c r="Z37" s="15"/>
-      <c r="AA37" s="15"/>
-      <c r="AB37" s="15"/>
-      <c r="AC37" s="15"/>
-      <c r="AD37" s="15"/>
-      <c r="AE37" s="16"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="30"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4687,41 +4699,41 @@
       <c r="CA37" s="12"/>
     </row>
     <row r="38" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
+      <c r="A38" s="8">
         <v>37</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="15"/>
-      <c r="Z38" s="15"/>
-      <c r="AA38" s="15"/>
-      <c r="AB38" s="15"/>
-      <c r="AC38" s="15"/>
-      <c r="AD38" s="15"/>
-      <c r="AE38" s="16"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="30"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4780,10 +4792,10 @@
       <c r="CA38" s="12"/>
     </row>
     <row r="39" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+      <c r="A39" s="13">
         <v>38</v>
       </c>
-      <c r="B39" s="8"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="5"/>
       <c r="D39" s="9" t="s">
         <v>53</v>
@@ -4873,41 +4885,41 @@
       <c r="CA39" s="12"/>
     </row>
     <row r="40" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+      <c r="A40" s="13">
         <v>39</v>
       </c>
-      <c r="B40" s="8"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
-      <c r="U40" s="15"/>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-      <c r="X40" s="15"/>
-      <c r="Y40" s="15"/>
-      <c r="Z40" s="15"/>
-      <c r="AA40" s="15"/>
-      <c r="AB40" s="15"/>
-      <c r="AC40" s="15"/>
-      <c r="AD40" s="15"/>
-      <c r="AE40" s="16"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="30"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4966,10 +4978,10 @@
       <c r="CA40" s="12"/>
     </row>
     <row r="41" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
+      <c r="A41" s="13">
         <v>40</v>
       </c>
-      <c r="B41" s="8"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="5"/>
       <c r="D41" s="9" t="s">
         <v>53</v>
@@ -5059,41 +5071,41 @@
       <c r="CA41" s="12"/>
     </row>
     <row r="42" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A42" s="13">
+      <c r="A42" s="8">
         <v>41</v>
       </c>
-      <c r="B42" s="13"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
-      <c r="U42" s="15"/>
-      <c r="V42" s="15"/>
-      <c r="W42" s="15"/>
-      <c r="X42" s="15"/>
-      <c r="Y42" s="15"/>
-      <c r="Z42" s="15"/>
-      <c r="AA42" s="15"/>
-      <c r="AB42" s="15"/>
-      <c r="AC42" s="15"/>
-      <c r="AD42" s="15"/>
-      <c r="AE42" s="16"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="30"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5152,41 +5164,41 @@
       <c r="CA42" s="12"/>
     </row>
     <row r="43" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
+      <c r="A43" s="13">
         <v>42</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="15"/>
-      <c r="AA43" s="15"/>
-      <c r="AB43" s="15"/>
-      <c r="AC43" s="15"/>
-      <c r="AD43" s="15"/>
-      <c r="AE43" s="16"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="30"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5245,41 +5257,41 @@
       <c r="CA43" s="12"/>
     </row>
     <row r="44" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
+      <c r="A44" s="13">
         <v>43</v>
       </c>
-      <c r="B44" s="8"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-      <c r="AA44" s="15"/>
-      <c r="AB44" s="15"/>
-      <c r="AC44" s="15"/>
-      <c r="AD44" s="15"/>
-      <c r="AE44" s="16"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="30"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -5338,10 +5350,10 @@
       <c r="CA44" s="12"/>
     </row>
     <row r="45" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8">
+      <c r="A45" s="13">
         <v>44</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="5"/>
       <c r="D45" s="9" t="s">
         <v>59</v>
@@ -5431,10 +5443,10 @@
       <c r="CA45" s="12"/>
     </row>
     <row r="46" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A46" s="13">
+      <c r="A46" s="8">
         <v>45</v>
       </c>
-      <c r="B46" s="13"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="9" t="s">
         <v>60</v>
@@ -5524,10 +5536,10 @@
       <c r="CA46" s="12"/>
     </row>
     <row r="47" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
+      <c r="A47" s="13">
         <v>46</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="5"/>
       <c r="D47" s="9" t="s">
         <v>62</v>
@@ -5617,10 +5629,10 @@
       <c r="CA47" s="12"/>
     </row>
     <row r="48" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
+      <c r="A48" s="13">
         <v>47</v>
       </c>
-      <c r="B48" s="8"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="5"/>
       <c r="D48" s="9" t="s">
         <v>62</v>
@@ -5710,10 +5722,10 @@
       <c r="CA48" s="12"/>
     </row>
     <row r="49" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="8">
+      <c r="A49" s="13">
         <v>48</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="5"/>
       <c r="D49" s="9" t="s">
         <v>64</v>
@@ -5803,10 +5815,10 @@
       <c r="CA49" s="12"/>
     </row>
     <row r="50" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A50" s="13">
+      <c r="A50" s="8">
         <v>49</v>
       </c>
-      <c r="B50" s="13"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="5"/>
       <c r="D50" s="9" t="s">
         <v>65</v>
@@ -5896,10 +5908,10 @@
       <c r="CA50" s="12"/>
     </row>
     <row r="51" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A51" s="8">
+      <c r="A51" s="13">
         <v>50</v>
       </c>
-      <c r="B51" s="8"/>
+      <c r="B51" s="13"/>
       <c r="C51" s="5"/>
       <c r="D51" s="9" t="s">
         <v>66</v>
@@ -5989,10 +6001,10 @@
       <c r="CA51" s="12"/>
     </row>
     <row r="52" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
+      <c r="A52" s="13">
         <v>51</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="13"/>
       <c r="C52" s="5"/>
       <c r="D52" s="9" t="s">
         <v>66</v>
@@ -6082,10 +6094,10 @@
       <c r="CA52" s="12"/>
     </row>
     <row r="53" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8">
+      <c r="A53" s="13">
         <v>52</v>
       </c>
-      <c r="B53" s="8"/>
+      <c r="B53" s="13"/>
       <c r="C53" s="5"/>
       <c r="D53" s="9" t="s">
         <v>68</v>
@@ -6175,10 +6187,10 @@
       <c r="CA53" s="12"/>
     </row>
     <row r="54" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A54" s="13">
+      <c r="A54" s="8">
         <v>53</v>
       </c>
-      <c r="B54" s="13"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="5"/>
       <c r="D54" s="9" t="s">
         <v>69</v>
@@ -6268,10 +6280,10 @@
       <c r="CA54" s="12"/>
     </row>
     <row r="55" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A55" s="8">
+      <c r="A55" s="13">
         <v>54</v>
       </c>
-      <c r="B55" s="8"/>
+      <c r="B55" s="13"/>
       <c r="C55" s="5"/>
       <c r="D55" s="9" t="s">
         <v>71</v>
@@ -6361,10 +6373,10 @@
       <c r="CA55" s="12"/>
     </row>
     <row r="56" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A56" s="8">
+      <c r="A56" s="13">
         <v>55</v>
       </c>
-      <c r="B56" s="8"/>
+      <c r="B56" s="13"/>
       <c r="C56" s="5"/>
       <c r="D56" s="9" t="s">
         <v>72</v>
@@ -6454,10 +6466,10 @@
       <c r="CA56" s="12"/>
     </row>
     <row r="57" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="8">
+      <c r="A57" s="13">
         <v>56</v>
       </c>
-      <c r="B57" s="8"/>
+      <c r="B57" s="13"/>
       <c r="C57" s="5"/>
       <c r="D57" s="9" t="s">
         <v>74</v>
@@ -6547,10 +6559,10 @@
       <c r="CA57" s="12"/>
     </row>
     <row r="58" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A58" s="13">
+      <c r="A58" s="8">
         <v>57</v>
       </c>
-      <c r="B58" s="13"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="5"/>
       <c r="D58" s="9" t="s">
         <v>75</v>
@@ -6640,10 +6652,10 @@
       <c r="CA58" s="12"/>
     </row>
     <row r="59" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A59" s="8">
+      <c r="A59" s="13">
         <v>58</v>
       </c>
-      <c r="B59" s="8"/>
+      <c r="B59" s="13"/>
       <c r="C59" s="5"/>
       <c r="D59" s="9" t="s">
         <v>77</v>
@@ -6733,10 +6745,10 @@
       <c r="CA59" s="12"/>
     </row>
     <row r="60" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A60" s="8">
+      <c r="A60" s="13">
         <v>59</v>
       </c>
-      <c r="B60" s="8"/>
+      <c r="B60" s="13"/>
       <c r="C60" s="5"/>
       <c r="D60" s="9" t="s">
         <v>75</v>
@@ -6826,10 +6838,10 @@
       <c r="CA60" s="12"/>
     </row>
     <row r="61" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="8">
+      <c r="A61" s="13">
         <v>60</v>
       </c>
-      <c r="B61" s="8"/>
+      <c r="B61" s="13"/>
       <c r="C61" s="5"/>
       <c r="D61" s="9" t="s">
         <v>80</v>
@@ -6919,10 +6931,10 @@
       <c r="CA61" s="12"/>
     </row>
     <row r="62" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A62" s="13">
+      <c r="A62" s="8">
         <v>61</v>
       </c>
-      <c r="B62" s="13"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="5"/>
       <c r="D62" s="9" t="s">
         <v>78</v>
@@ -7012,10 +7024,10 @@
       <c r="CA62" s="12"/>
     </row>
     <row r="63" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A63" s="8">
+      <c r="A63" s="13">
         <v>62</v>
       </c>
-      <c r="B63" s="8"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="5"/>
       <c r="D63" s="9" t="s">
         <v>84</v>
@@ -7105,10 +7117,10 @@
       <c r="CA63" s="12"/>
     </row>
     <row r="64" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A64" s="8">
+      <c r="A64" s="13">
         <v>63</v>
       </c>
-      <c r="B64" s="8"/>
+      <c r="B64" s="13"/>
       <c r="C64" s="5"/>
       <c r="D64" s="9" t="s">
         <v>84</v>
@@ -7198,10 +7210,10 @@
       <c r="CA64" s="12"/>
     </row>
     <row r="65" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="8">
+      <c r="A65" s="13">
         <v>64</v>
       </c>
-      <c r="B65" s="8"/>
+      <c r="B65" s="13"/>
       <c r="C65" s="5"/>
       <c r="D65" s="9" t="s">
         <v>83</v>
@@ -7289,10 +7301,10 @@
       <c r="CA65" s="12"/>
     </row>
     <row r="66" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A66" s="13">
+      <c r="A66" s="8">
         <v>65</v>
       </c>
-      <c r="B66" s="13"/>
+      <c r="B66" s="8"/>
       <c r="C66" s="5"/>
       <c r="D66" s="9" t="s">
         <v>85</v>
@@ -7382,10 +7394,10 @@
       <c r="CA66" s="12"/>
     </row>
     <row r="67" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A67" s="8">
+      <c r="A67" s="13">
         <v>66</v>
       </c>
-      <c r="B67" s="8"/>
+      <c r="B67" s="13"/>
       <c r="C67" s="5"/>
       <c r="D67" s="9" t="s">
         <v>87</v>
@@ -7475,10 +7487,10 @@
       <c r="CA67" s="12"/>
     </row>
     <row r="68" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A68" s="8">
+      <c r="A68" s="13">
         <v>67</v>
       </c>
-      <c r="B68" s="8"/>
+      <c r="B68" s="13"/>
       <c r="C68" s="5"/>
       <c r="D68" s="9" t="s">
         <v>87</v>
@@ -7568,10 +7580,10 @@
       <c r="CA68" s="12"/>
     </row>
     <row r="69" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="8">
+      <c r="A69" s="13">
         <v>68</v>
       </c>
-      <c r="B69" s="8"/>
+      <c r="B69" s="13"/>
       <c r="C69" s="5"/>
       <c r="D69" s="9" t="s">
         <v>88</v>
@@ -7661,10 +7673,10 @@
       <c r="CA69" s="12"/>
     </row>
     <row r="70" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A70" s="13">
+      <c r="A70" s="8">
         <v>69</v>
       </c>
-      <c r="B70" s="13"/>
+      <c r="B70" s="8"/>
       <c r="C70" s="5"/>
       <c r="D70" s="9" t="s">
         <v>90</v>
@@ -7754,10 +7766,10 @@
       <c r="CA70" s="12"/>
     </row>
     <row r="71" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
+      <c r="A71" s="13">
         <v>70</v>
       </c>
-      <c r="B71" s="8"/>
+      <c r="B71" s="13"/>
       <c r="C71" s="5"/>
       <c r="D71" s="9" t="s">
         <v>90</v>
@@ -7847,10 +7859,10 @@
       <c r="CA71" s="12"/>
     </row>
     <row r="72" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A72" s="8">
+      <c r="A72" s="13">
         <v>71</v>
       </c>
-      <c r="B72" s="8"/>
+      <c r="B72" s="13"/>
       <c r="C72" s="5"/>
       <c r="D72" s="9" t="s">
         <v>91</v>
@@ -7940,10 +7952,10 @@
       <c r="CA72" s="12"/>
     </row>
     <row r="73" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="8">
+      <c r="A73" s="13">
         <v>72</v>
       </c>
-      <c r="B73" s="8"/>
+      <c r="B73" s="13"/>
       <c r="C73" s="5"/>
       <c r="D73" s="9" t="s">
         <v>92</v>
@@ -8033,10 +8045,10 @@
       <c r="CA73" s="12"/>
     </row>
     <row r="74" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A74" s="13">
+      <c r="A74" s="8">
         <v>73</v>
       </c>
-      <c r="B74" s="13"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="5"/>
       <c r="D74" s="9" t="s">
         <v>93</v>
@@ -8126,10 +8138,10 @@
       <c r="CA74" s="12"/>
     </row>
     <row r="75" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A75" s="8">
+      <c r="A75" s="13">
         <v>74</v>
       </c>
-      <c r="B75" s="8"/>
+      <c r="B75" s="13"/>
       <c r="C75" s="5"/>
       <c r="D75" s="9" t="s">
         <v>94</v>
@@ -8219,10 +8231,10 @@
       <c r="CA75" s="12"/>
     </row>
     <row r="76" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
+      <c r="A76" s="13">
         <v>75</v>
       </c>
-      <c r="B76" s="8"/>
+      <c r="B76" s="13"/>
       <c r="C76" s="5"/>
       <c r="D76" s="9" t="s">
         <v>94</v>
@@ -8312,10 +8324,10 @@
       <c r="CA76" s="12"/>
     </row>
     <row r="77" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="8">
+      <c r="A77" s="13">
         <v>76</v>
       </c>
-      <c r="B77" s="8"/>
+      <c r="B77" s="13"/>
       <c r="C77" s="5"/>
       <c r="D77" s="9" t="s">
         <v>95</v>
@@ -8405,10 +8417,10 @@
       <c r="CA77" s="12"/>
     </row>
     <row r="78" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A78" s="13">
+      <c r="A78" s="8">
         <v>77</v>
       </c>
-      <c r="B78" s="13"/>
+      <c r="B78" s="8"/>
       <c r="C78" s="5"/>
       <c r="D78" s="9" t="s">
         <v>97</v>
@@ -8498,10 +8510,10 @@
       <c r="CA78" s="12"/>
     </row>
     <row r="79" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A79" s="8">
+      <c r="A79" s="13">
         <v>78</v>
       </c>
-      <c r="B79" s="8"/>
+      <c r="B79" s="13"/>
       <c r="C79" s="5"/>
       <c r="D79" s="9" t="s">
         <v>96</v>
@@ -8591,10 +8603,10 @@
       <c r="CA79" s="12"/>
     </row>
     <row r="80" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A80" s="8">
+      <c r="A80" s="13">
         <v>79</v>
       </c>
-      <c r="B80" s="8"/>
+      <c r="B80" s="13"/>
       <c r="C80" s="5"/>
       <c r="D80" s="9" t="s">
         <v>96</v>
@@ -8684,10 +8696,10 @@
       <c r="CA80" s="12"/>
     </row>
     <row r="81" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="8">
+      <c r="A81" s="13">
         <v>80</v>
       </c>
-      <c r="B81" s="8"/>
+      <c r="B81" s="13"/>
       <c r="C81" s="5"/>
       <c r="D81" s="9" t="s">
         <v>98</v>
@@ -8777,10 +8789,10 @@
       <c r="CA81" s="12"/>
     </row>
     <row r="82" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A82" s="13">
+      <c r="A82" s="8">
         <v>81</v>
       </c>
-      <c r="B82" s="13"/>
+      <c r="B82" s="8"/>
       <c r="C82" s="5"/>
       <c r="D82" s="9" t="s">
         <v>99</v>
@@ -8870,10 +8882,10 @@
       <c r="CA82" s="12"/>
     </row>
     <row r="83" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A83" s="8">
+      <c r="A83" s="13">
         <v>82</v>
       </c>
-      <c r="B83" s="8"/>
+      <c r="B83" s="13"/>
       <c r="C83" s="5"/>
       <c r="D83" s="9" t="s">
         <v>101</v>
@@ -8963,10 +8975,10 @@
       <c r="CA83" s="12"/>
     </row>
     <row r="84" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A84" s="8">
+      <c r="A84" s="13">
         <v>83</v>
       </c>
-      <c r="B84" s="8"/>
+      <c r="B84" s="13"/>
       <c r="C84" s="5"/>
       <c r="D84" s="9" t="s">
         <v>100</v>
@@ -9056,10 +9068,10 @@
       <c r="CA84" s="12"/>
     </row>
     <row r="85" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="8">
+      <c r="A85" s="13">
         <v>84</v>
       </c>
-      <c r="B85" s="8"/>
+      <c r="B85" s="13"/>
       <c r="C85" s="5"/>
       <c r="D85" s="9" t="s">
         <v>102</v>
@@ -9149,10 +9161,10 @@
       <c r="CA85" s="12"/>
     </row>
     <row r="86" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A86" s="13">
+      <c r="A86" s="8">
         <v>85</v>
       </c>
-      <c r="B86" s="13"/>
+      <c r="B86" s="8"/>
       <c r="C86" s="5"/>
       <c r="D86" s="9" t="s">
         <v>99</v>
@@ -9242,10 +9254,10 @@
       <c r="CA86" s="12"/>
     </row>
     <row r="87" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A87" s="8">
+      <c r="A87" s="13">
         <v>86</v>
       </c>
-      <c r="B87" s="8"/>
+      <c r="B87" s="13"/>
       <c r="C87" s="5"/>
       <c r="D87" s="9" t="s">
         <v>103</v>
@@ -9335,10 +9347,10 @@
       <c r="CA87" s="12"/>
     </row>
     <row r="88" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A88" s="8">
+      <c r="A88" s="13">
         <v>87</v>
       </c>
-      <c r="B88" s="8"/>
+      <c r="B88" s="13"/>
       <c r="C88" s="5"/>
       <c r="D88" s="9" t="s">
         <v>104</v>
@@ -9426,10 +9438,10 @@
       <c r="CA88" s="12"/>
     </row>
     <row r="89" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="8">
+      <c r="A89" s="13">
         <v>88</v>
       </c>
-      <c r="B89" s="8"/>
+      <c r="B89" s="13"/>
       <c r="C89" s="5"/>
       <c r="D89" s="9" t="s">
         <v>105</v>
@@ -9517,10 +9529,10 @@
       <c r="CA89" s="12"/>
     </row>
     <row r="90" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A90" s="13">
+      <c r="A90" s="8">
         <v>89</v>
       </c>
-      <c r="B90" s="13"/>
+      <c r="B90" s="8"/>
       <c r="C90" s="5"/>
       <c r="D90" s="9" t="s">
         <v>105</v>
@@ -9608,10 +9620,10 @@
       <c r="CA90" s="12"/>
     </row>
     <row r="91" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A91" s="8">
+      <c r="A91" s="13">
         <v>90</v>
       </c>
-      <c r="B91" s="8"/>
+      <c r="B91" s="13"/>
       <c r="C91" s="5"/>
       <c r="D91" s="9" t="s">
         <v>105</v>
@@ -9699,10 +9711,10 @@
       <c r="CA91" s="12"/>
     </row>
     <row r="92" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A92" s="8">
+      <c r="A92" s="13">
         <v>91</v>
       </c>
-      <c r="B92" s="8"/>
+      <c r="B92" s="13"/>
       <c r="C92" s="5"/>
       <c r="D92" s="9" t="s">
         <v>107</v>
@@ -9792,10 +9804,10 @@
       <c r="CA92" s="12"/>
     </row>
     <row r="93" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="8">
+      <c r="A93" s="13">
         <v>92</v>
       </c>
-      <c r="B93" s="8"/>
+      <c r="B93" s="13"/>
       <c r="C93" s="5"/>
       <c r="D93" s="9" t="s">
         <v>107</v>
@@ -9885,10 +9897,10 @@
       <c r="CA93" s="12"/>
     </row>
     <row r="94" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A94" s="13">
+      <c r="A94" s="8">
         <v>93</v>
       </c>
-      <c r="B94" s="13"/>
+      <c r="B94" s="8"/>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
         <v>109</v>
@@ -9978,10 +9990,10 @@
       <c r="CA94" s="12"/>
     </row>
     <row r="95" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A95" s="8">
+      <c r="A95" s="13">
         <v>94</v>
       </c>
-      <c r="B95" s="8"/>
+      <c r="B95" s="13"/>
       <c r="C95" s="5"/>
       <c r="D95" s="9" t="s">
         <v>111</v>
@@ -10071,10 +10083,10 @@
       <c r="CA95" s="12"/>
     </row>
     <row r="96" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A96" s="8">
+      <c r="A96" s="13">
         <v>95</v>
       </c>
-      <c r="B96" s="8"/>
+      <c r="B96" s="13"/>
       <c r="C96" s="5"/>
       <c r="D96" s="9" t="s">
         <v>114</v>
@@ -10164,10 +10176,10 @@
       <c r="CA96" s="12"/>
     </row>
     <row r="97" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="8">
+      <c r="A97" s="13">
         <v>96</v>
       </c>
-      <c r="B97" s="8"/>
+      <c r="B97" s="13"/>
       <c r="C97" s="5"/>
       <c r="D97" s="9" t="s">
         <v>115</v>
@@ -10257,10 +10269,10 @@
       <c r="CA97" s="12"/>
     </row>
     <row r="98" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A98" s="13">
+      <c r="A98" s="8">
         <v>97</v>
       </c>
-      <c r="B98" s="13"/>
+      <c r="B98" s="8"/>
       <c r="C98" s="5"/>
       <c r="D98" s="9" t="s">
         <v>116</v>
@@ -10350,10 +10362,10 @@
       <c r="CA98" s="12"/>
     </row>
     <row r="99" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A99" s="8">
+      <c r="A99" s="13">
         <v>98</v>
       </c>
-      <c r="B99" s="8"/>
+      <c r="B99" s="13"/>
       <c r="C99" s="5"/>
       <c r="D99" s="9" t="s">
         <v>117</v>
@@ -10443,10 +10455,10 @@
       <c r="CA99" s="12"/>
     </row>
     <row r="100" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A100" s="8">
+      <c r="A100" s="13">
         <v>99</v>
       </c>
-      <c r="B100" s="8"/>
+      <c r="B100" s="13"/>
       <c r="C100" s="5"/>
       <c r="D100" s="9" t="s">
         <v>117</v>
@@ -10536,10 +10548,10 @@
       <c r="CA100" s="12"/>
     </row>
     <row r="101" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="8">
+      <c r="A101" s="13">
         <v>100</v>
       </c>
-      <c r="B101" s="8"/>
+      <c r="B101" s="13"/>
       <c r="C101" s="5"/>
       <c r="D101" s="9" t="s">
         <v>119</v>
@@ -10629,10 +10641,10 @@
       <c r="CA101" s="12"/>
     </row>
     <row r="102" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A102" s="13">
+      <c r="A102" s="8">
         <v>101</v>
       </c>
-      <c r="B102" s="13"/>
+      <c r="B102" s="8"/>
       <c r="C102" s="5"/>
       <c r="D102" s="9" t="s">
         <v>120</v>
@@ -10722,10 +10734,10 @@
       <c r="CA102" s="12"/>
     </row>
     <row r="103" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A103" s="8">
+      <c r="A103" s="13">
         <v>102</v>
       </c>
-      <c r="B103" s="8"/>
+      <c r="B103" s="13"/>
       <c r="C103" s="5"/>
       <c r="D103" s="9" t="s">
         <v>120</v>
@@ -10815,10 +10827,10 @@
       <c r="CA103" s="12"/>
     </row>
     <row r="104" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A104" s="8">
+      <c r="A104" s="13">
         <v>103</v>
       </c>
-      <c r="B104" s="8"/>
+      <c r="B104" s="13"/>
       <c r="C104" s="5"/>
       <c r="D104" s="9" t="s">
         <v>123</v>
@@ -10908,10 +10920,10 @@
       <c r="CA104" s="12"/>
     </row>
     <row r="105" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="8">
+      <c r="A105" s="13">
         <v>104</v>
       </c>
-      <c r="B105" s="8"/>
+      <c r="B105" s="13"/>
       <c r="C105" s="5"/>
       <c r="D105" s="9" t="s">
         <v>123</v>
@@ -11001,10 +11013,10 @@
       <c r="CA105" s="12"/>
     </row>
     <row r="106" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A106" s="13">
+      <c r="A106" s="8">
         <v>105</v>
       </c>
-      <c r="B106" s="13"/>
+      <c r="B106" s="8"/>
       <c r="C106" s="5"/>
       <c r="D106" s="9" t="s">
         <v>125</v>
@@ -11094,10 +11106,10 @@
       <c r="CA106" s="12"/>
     </row>
     <row r="107" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A107" s="8">
+      <c r="A107" s="13">
         <v>106</v>
       </c>
-      <c r="B107" s="8"/>
+      <c r="B107" s="13"/>
       <c r="C107" s="5"/>
       <c r="D107" s="9" t="s">
         <v>123</v>
@@ -11187,10 +11199,10 @@
       <c r="CA107" s="12"/>
     </row>
     <row r="108" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A108" s="8">
+      <c r="A108" s="13">
         <v>107</v>
       </c>
-      <c r="B108" s="8"/>
+      <c r="B108" s="13"/>
       <c r="C108" s="5"/>
       <c r="D108" s="9" t="s">
         <v>125</v>
@@ -11280,10 +11292,10 @@
       <c r="CA108" s="12"/>
     </row>
     <row r="109" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="8">
+      <c r="A109" s="13">
         <v>108</v>
       </c>
-      <c r="B109" s="8"/>
+      <c r="B109" s="13"/>
       <c r="C109" s="5"/>
       <c r="D109" s="9" t="s">
         <v>125</v>
@@ -11373,10 +11385,10 @@
       <c r="CA109" s="12"/>
     </row>
     <row r="110" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A110" s="13">
+      <c r="A110" s="8">
         <v>109</v>
       </c>
-      <c r="B110" s="13"/>
+      <c r="B110" s="8"/>
       <c r="C110" s="5"/>
       <c r="D110" s="9" t="s">
         <v>127</v>
@@ -11466,10 +11478,10 @@
       <c r="CA110" s="12"/>
     </row>
     <row r="111" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A111" s="8">
+      <c r="A111" s="13">
         <v>110</v>
       </c>
-      <c r="B111" s="8"/>
+      <c r="B111" s="13"/>
       <c r="C111" s="5"/>
       <c r="D111" s="9" t="s">
         <v>129</v>
@@ -11559,12 +11571,14 @@
       <c r="CA111" s="12"/>
     </row>
     <row r="112" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A112" s="8">
+      <c r="A112" s="13">
         <v>111</v>
       </c>
-      <c r="B112" s="8"/>
+      <c r="B112" s="13"/>
       <c r="C112" s="5"/>
-      <c r="D112" s="9"/>
+      <c r="D112" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="E112" s="9"/>
       <c r="F112" s="9"/>
       <c r="G112" s="9"/>
@@ -11592,20 +11606,28 @@
       <c r="AC112" s="9"/>
       <c r="AD112" s="9"/>
       <c r="AE112" s="9"/>
-      <c r="AF112" s="10"/>
+      <c r="AF112" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="AG112" s="10"/>
       <c r="AH112" s="10"/>
       <c r="AI112" s="10"/>
       <c r="AJ112" s="10"/>
-      <c r="AK112" s="9"/>
+      <c r="AK112" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL112" s="9"/>
       <c r="AM112" s="9"/>
       <c r="AN112" s="9"/>
       <c r="AO112" s="9"/>
-      <c r="AP112" s="11"/>
+      <c r="AP112" s="11">
+        <v>0.8</v>
+      </c>
       <c r="AQ112" s="11"/>
       <c r="AR112" s="11"/>
-      <c r="AS112" s="9"/>
+      <c r="AS112" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT112" s="9"/>
       <c r="AU112" s="9"/>
       <c r="AV112" s="9"/>
@@ -11642,12 +11664,14 @@
       <c r="CA112" s="12"/>
     </row>
     <row r="113" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="8">
+      <c r="A113" s="13">
         <v>112</v>
       </c>
-      <c r="B113" s="8"/>
+      <c r="B113" s="13"/>
       <c r="C113" s="5"/>
-      <c r="D113" s="9"/>
+      <c r="D113" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="E113" s="9"/>
       <c r="F113" s="9"/>
       <c r="G113" s="9"/>
@@ -11675,20 +11699,28 @@
       <c r="AC113" s="9"/>
       <c r="AD113" s="9"/>
       <c r="AE113" s="9"/>
-      <c r="AF113" s="10"/>
+      <c r="AF113" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="AG113" s="10"/>
       <c r="AH113" s="10"/>
       <c r="AI113" s="10"/>
       <c r="AJ113" s="10"/>
-      <c r="AK113" s="9"/>
+      <c r="AK113" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL113" s="9"/>
       <c r="AM113" s="9"/>
       <c r="AN113" s="9"/>
       <c r="AO113" s="9"/>
-      <c r="AP113" s="11"/>
+      <c r="AP113" s="11">
+        <v>0.5</v>
+      </c>
       <c r="AQ113" s="11"/>
       <c r="AR113" s="11"/>
-      <c r="AS113" s="9"/>
+      <c r="AS113" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT113" s="9"/>
       <c r="AU113" s="9"/>
       <c r="AV113" s="9"/>
@@ -11725,12 +11757,14 @@
       <c r="CA113" s="12"/>
     </row>
     <row r="114" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A114" s="13">
+      <c r="A114" s="8">
         <v>113</v>
       </c>
-      <c r="B114" s="13"/>
+      <c r="B114" s="8"/>
       <c r="C114" s="5"/>
-      <c r="D114" s="9"/>
+      <c r="D114" s="9" t="s">
+        <v>133</v>
+      </c>
       <c r="E114" s="9"/>
       <c r="F114" s="9"/>
       <c r="G114" s="9"/>
@@ -11758,20 +11792,28 @@
       <c r="AC114" s="9"/>
       <c r="AD114" s="9"/>
       <c r="AE114" s="9"/>
-      <c r="AF114" s="10"/>
+      <c r="AF114" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="AG114" s="10"/>
       <c r="AH114" s="10"/>
       <c r="AI114" s="10"/>
       <c r="AJ114" s="10"/>
-      <c r="AK114" s="9"/>
+      <c r="AK114" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL114" s="9"/>
       <c r="AM114" s="9"/>
       <c r="AN114" s="9"/>
       <c r="AO114" s="9"/>
-      <c r="AP114" s="11"/>
+      <c r="AP114" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ114" s="11"/>
       <c r="AR114" s="11"/>
-      <c r="AS114" s="9"/>
+      <c r="AS114" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT114" s="9"/>
       <c r="AU114" s="9"/>
       <c r="AV114" s="9"/>
@@ -11808,10 +11850,10 @@
       <c r="CA114" s="12"/>
     </row>
     <row r="115" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A115" s="8">
+      <c r="A115" s="13">
         <v>114</v>
       </c>
-      <c r="B115" s="8"/>
+      <c r="B115" s="13"/>
       <c r="C115" s="5"/>
       <c r="D115" s="9"/>
       <c r="E115" s="9"/>
@@ -11891,10 +11933,10 @@
       <c r="CA115" s="12"/>
     </row>
     <row r="116" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A116" s="8">
+      <c r="A116" s="13">
         <v>115</v>
       </c>
-      <c r="B116" s="8"/>
+      <c r="B116" s="13"/>
       <c r="C116" s="5"/>
       <c r="D116" s="9"/>
       <c r="E116" s="9"/>
@@ -11974,10 +12016,10 @@
       <c r="CA116" s="12"/>
     </row>
     <row r="117" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="8">
+      <c r="A117" s="13">
         <v>116</v>
       </c>
-      <c r="B117" s="8"/>
+      <c r="B117" s="13"/>
       <c r="C117" s="5"/>
       <c r="D117" s="9"/>
       <c r="E117" s="9"/>
@@ -12057,10 +12099,10 @@
       <c r="CA117" s="12"/>
     </row>
     <row r="118" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A118" s="13">
+      <c r="A118" s="8">
         <v>117</v>
       </c>
-      <c r="B118" s="13"/>
+      <c r="B118" s="8"/>
       <c r="C118" s="5"/>
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
@@ -12140,10 +12182,10 @@
       <c r="CA118" s="12"/>
     </row>
     <row r="119" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A119" s="8">
+      <c r="A119" s="13">
         <v>118</v>
       </c>
-      <c r="B119" s="8"/>
+      <c r="B119" s="13"/>
       <c r="C119" s="5"/>
       <c r="D119" s="9"/>
       <c r="E119" s="9"/>
@@ -12223,10 +12265,10 @@
       <c r="CA119" s="12"/>
     </row>
     <row r="120" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A120" s="8">
+      <c r="A120" s="13">
         <v>119</v>
       </c>
-      <c r="B120" s="8"/>
+      <c r="B120" s="13"/>
       <c r="C120" s="5"/>
       <c r="D120" s="9"/>
       <c r="E120" s="9"/>
@@ -12306,10 +12348,10 @@
       <c r="CA120" s="12"/>
     </row>
     <row r="121" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="8">
+      <c r="A121" s="13">
         <v>120</v>
       </c>
-      <c r="B121" s="8"/>
+      <c r="B121" s="13"/>
       <c r="C121" s="5"/>
       <c r="D121" s="9"/>
       <c r="E121" s="9"/>
@@ -12389,10 +12431,10 @@
       <c r="CA121" s="12"/>
     </row>
     <row r="122" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A122" s="13">
+      <c r="A122" s="8">
         <v>121</v>
       </c>
-      <c r="B122" s="13"/>
+      <c r="B122" s="8"/>
       <c r="C122" s="5"/>
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
@@ -12472,10 +12514,10 @@
       <c r="CA122" s="12"/>
     </row>
     <row r="123" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A123" s="8">
+      <c r="A123" s="13">
         <v>122</v>
       </c>
-      <c r="B123" s="8"/>
+      <c r="B123" s="13"/>
       <c r="C123" s="5"/>
       <c r="BG123" s="12"/>
       <c r="BH123" s="12"/>
@@ -12501,351 +12543,493 @@
     </row>
   </sheetData>
   <mergeCells count="856">
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -12870,493 +13054,351 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
Báo cáo ngày 16/2/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="136">
   <si>
     <t>No.</t>
   </si>
@@ -423,6 +423,12 @@
   <si>
     <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data - Lưu lịch sử chạy backup</t>
   </si>
+  <si>
+    <t>16/2/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data - Hoàn thành việc update dữ liệu</t>
+  </si>
 </sst>
 </file>
 
@@ -684,12 +690,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -709,14 +723,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,7 +828,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1213,7 +1219,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1225,7 +1231,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS115" sqref="AS115:BF115"/>
+      <selection pane="bottomLeft" activeCell="AP118" sqref="AP118:AR118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,198 +1246,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="16" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="15" t="s">
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="17" t="s">
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="17"/>
-      <c r="AR1" s="17"/>
-      <c r="AS1" s="15" t="s">
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="15"/>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
-      <c r="BG1" s="18" t="s">
+      <c r="AT1" s="23"/>
+      <c r="AU1" s="23"/>
+      <c r="AV1" s="23"/>
+      <c r="AW1" s="23"/>
+      <c r="AX1" s="23"/>
+      <c r="AY1" s="23"/>
+      <c r="AZ1" s="23"/>
+      <c r="BA1" s="23"/>
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23"/>
+      <c r="BG1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="18"/>
-      <c r="BI1" s="18"/>
-      <c r="BJ1" s="18"/>
-      <c r="BK1" s="18"/>
-      <c r="BL1" s="18"/>
-      <c r="BM1" s="18"/>
-      <c r="BN1" s="18"/>
-      <c r="BO1" s="18"/>
-      <c r="BP1" s="18"/>
-      <c r="BQ1" s="18"/>
-      <c r="BR1" s="18"/>
-      <c r="BS1" s="18"/>
-      <c r="BT1" s="18"/>
-      <c r="BU1" s="18"/>
-      <c r="BV1" s="18"/>
-      <c r="BW1" s="18"/>
-      <c r="BX1" s="18"/>
-      <c r="BY1" s="18"/>
-      <c r="BZ1" s="18"/>
-      <c r="CA1" s="18"/>
+      <c r="BH1" s="26"/>
+      <c r="BI1" s="26"/>
+      <c r="BJ1" s="26"/>
+      <c r="BK1" s="26"/>
+      <c r="BL1" s="26"/>
+      <c r="BM1" s="26"/>
+      <c r="BN1" s="26"/>
+      <c r="BO1" s="26"/>
+      <c r="BP1" s="26"/>
+      <c r="BQ1" s="26"/>
+      <c r="BR1" s="26"/>
+      <c r="BS1" s="26"/>
+      <c r="BT1" s="26"/>
+      <c r="BU1" s="26"/>
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26"/>
+      <c r="CA1" s="26"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="20" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="19" t="s">
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="21">
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="29">
         <v>1</v>
       </c>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="19" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
-      <c r="BN2" s="22"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2" s="22"/>
-      <c r="BQ2" s="22"/>
-      <c r="BR2" s="22"/>
-      <c r="BS2" s="22"/>
-      <c r="BT2" s="22"/>
-      <c r="BU2" s="22"/>
-      <c r="BV2" s="22"/>
-      <c r="BW2" s="22"/>
-      <c r="BX2" s="22"/>
-      <c r="BY2" s="22"/>
-      <c r="BZ2" s="22"/>
-      <c r="CA2" s="22"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="30"/>
+      <c r="BJ2" s="30"/>
+      <c r="BK2" s="30"/>
+      <c r="BL2" s="30"/>
+      <c r="BM2" s="30"/>
+      <c r="BN2" s="30"/>
+      <c r="BO2" s="30"/>
+      <c r="BP2" s="30"/>
+      <c r="BQ2" s="30"/>
+      <c r="BR2" s="30"/>
+      <c r="BS2" s="30"/>
+      <c r="BT2" s="30"/>
+      <c r="BU2" s="30"/>
+      <c r="BV2" s="30"/>
+      <c r="BW2" s="30"/>
+      <c r="BX2" s="30"/>
+      <c r="BY2" s="30"/>
+      <c r="BZ2" s="30"/>
+      <c r="CA2" s="30"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="5"/>
       <c r="D3" s="9" t="s">
         <v>17</v>
@@ -1521,10 +1527,10 @@
       <c r="CA3" s="12"/>
     </row>
     <row r="4" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="5"/>
       <c r="D4" s="9" t="s">
         <v>18</v>
@@ -1614,10 +1620,10 @@
       <c r="CA4" s="12"/>
     </row>
     <row r="5" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="5"/>
       <c r="D5" s="9" t="s">
         <v>18</v>
@@ -1709,10 +1715,10 @@
       <c r="CA5" s="12"/>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -1802,10 +1808,10 @@
       <c r="CA6" s="12"/>
     </row>
     <row r="7" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
         <v>22</v>
@@ -1895,10 +1901,10 @@
       <c r="CA7" s="12"/>
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
         <v>24</v>
@@ -1988,10 +1994,10 @@
       <c r="CA8" s="12"/>
     </row>
     <row r="9" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
         <v>33</v>
@@ -2083,10 +2089,10 @@
       <c r="CA9" s="12"/>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
         <v>33</v>
@@ -2176,10 +2182,10 @@
       <c r="CA10" s="12"/>
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
         <v>33</v>
@@ -2269,10 +2275,10 @@
       <c r="CA11" s="12"/>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="5"/>
       <c r="D12" s="9" t="s">
         <v>33</v>
@@ -2362,10 +2368,10 @@
       <c r="CA12" s="12"/>
     </row>
     <row r="13" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>33</v>
@@ -2457,10 +2463,10 @@
       <c r="CA13" s="12"/>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="9" t="s">
         <v>33</v>
@@ -2552,10 +2558,10 @@
       <c r="CA14" s="12"/>
     </row>
     <row r="15" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
         <v>33</v>
@@ -2645,10 +2651,10 @@
       <c r="CA15" s="12"/>
     </row>
     <row r="16" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="13"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
         <v>36</v>
@@ -2738,10 +2744,10 @@
       <c r="CA16" s="12"/>
     </row>
     <row r="17" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
         <v>33</v>
@@ -2833,10 +2839,10 @@
       <c r="CA17" s="12"/>
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="5"/>
       <c r="D18" s="9" t="s">
         <v>38</v>
@@ -2926,10 +2932,10 @@
       <c r="CA18" s="12"/>
     </row>
     <row r="19" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="13"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
         <v>38</v>
@@ -3019,10 +3025,10 @@
       <c r="CA19" s="12"/>
     </row>
     <row r="20" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="5"/>
       <c r="D20" s="9" t="s">
         <v>38</v>
@@ -3112,10 +3118,10 @@
       <c r="CA20" s="12"/>
     </row>
     <row r="21" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
+      <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="5"/>
       <c r="D21" s="9" t="s">
         <v>38</v>
@@ -3205,10 +3211,10 @@
       <c r="CA21" s="12"/>
     </row>
     <row r="22" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="13">
         <v>21</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="9" t="s">
         <v>44</v>
@@ -3300,10 +3306,10 @@
       <c r="CA22" s="12"/>
     </row>
     <row r="23" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+      <c r="A23" s="8">
         <v>22</v>
       </c>
-      <c r="B23" s="13"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="5"/>
       <c r="D23" s="9" t="s">
         <v>38</v>
@@ -3395,10 +3401,10 @@
       <c r="CA23" s="12"/>
     </row>
     <row r="24" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="A24" s="8">
         <v>23</v>
       </c>
-      <c r="B24" s="13"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="5"/>
       <c r="D24" s="9" t="s">
         <v>33</v>
@@ -3488,10 +3494,10 @@
       <c r="CA24" s="12"/>
     </row>
     <row r="25" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13">
+      <c r="A25" s="8">
         <v>24</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="5"/>
       <c r="D25" s="9" t="s">
         <v>45</v>
@@ -3581,10 +3587,10 @@
       <c r="CA25" s="12"/>
     </row>
     <row r="26" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="13">
         <v>25</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="9" t="s">
         <v>38</v>
@@ -3674,10 +3680,10 @@
       <c r="CA26" s="12"/>
     </row>
     <row r="27" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+      <c r="A27" s="8">
         <v>26</v>
       </c>
-      <c r="B27" s="13"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="D27" s="9" t="s">
         <v>33</v>
@@ -3767,10 +3773,10 @@
       <c r="CA27" s="12"/>
     </row>
     <row r="28" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
+      <c r="A28" s="8">
         <v>27</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="5"/>
       <c r="D28" s="9" t="s">
         <v>46</v>
@@ -3860,10 +3866,10 @@
       <c r="CA28" s="12"/>
     </row>
     <row r="29" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="8">
         <v>28</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="5"/>
       <c r="D29" s="9" t="s">
         <v>38</v>
@@ -3955,10 +3961,10 @@
       <c r="CA29" s="12"/>
     </row>
     <row r="30" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="13">
         <v>29</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="5"/>
       <c r="D30" s="9" t="s">
         <v>48</v>
@@ -4048,10 +4054,10 @@
       <c r="CA30" s="12"/>
     </row>
     <row r="31" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
+      <c r="A31" s="8">
         <v>30</v>
       </c>
-      <c r="B31" s="13"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="5"/>
       <c r="D31" s="9" t="s">
         <v>49</v>
@@ -4141,48 +4147,48 @@
       <c r="CA31" s="12"/>
     </row>
     <row r="32" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
+      <c r="A32" s="8">
         <v>31</v>
       </c>
-      <c r="B32" s="13"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="23"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="23"/>
-      <c r="AD32" s="23"/>
-      <c r="AE32" s="23"/>
-      <c r="AF32" s="24">
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="19"/>
+      <c r="AC32" s="19"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="19"/>
+      <c r="AF32" s="20">
         <v>43293</v>
       </c>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="24"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="24"/>
+      <c r="AG32" s="20"/>
+      <c r="AH32" s="20"/>
+      <c r="AI32" s="20"/>
+      <c r="AJ32" s="20"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4211,33 +4217,33 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="25"/>
-      <c r="BH32" s="25"/>
-      <c r="BI32" s="25"/>
-      <c r="BJ32" s="25"/>
-      <c r="BK32" s="25"/>
-      <c r="BL32" s="25"/>
-      <c r="BM32" s="25"/>
-      <c r="BN32" s="25"/>
-      <c r="BO32" s="25"/>
-      <c r="BP32" s="25"/>
-      <c r="BQ32" s="25"/>
-      <c r="BR32" s="25"/>
-      <c r="BS32" s="25"/>
-      <c r="BT32" s="25"/>
-      <c r="BU32" s="25"/>
-      <c r="BV32" s="25"/>
-      <c r="BW32" s="25"/>
-      <c r="BX32" s="25"/>
-      <c r="BY32" s="25"/>
-      <c r="BZ32" s="25"/>
-      <c r="CA32" s="25"/>
+      <c r="BG32" s="21"/>
+      <c r="BH32" s="21"/>
+      <c r="BI32" s="21"/>
+      <c r="BJ32" s="21"/>
+      <c r="BK32" s="21"/>
+      <c r="BL32" s="21"/>
+      <c r="BM32" s="21"/>
+      <c r="BN32" s="21"/>
+      <c r="BO32" s="21"/>
+      <c r="BP32" s="21"/>
+      <c r="BQ32" s="21"/>
+      <c r="BR32" s="21"/>
+      <c r="BS32" s="21"/>
+      <c r="BT32" s="21"/>
+      <c r="BU32" s="21"/>
+      <c r="BV32" s="21"/>
+      <c r="BW32" s="21"/>
+      <c r="BX32" s="21"/>
+      <c r="BY32" s="21"/>
+      <c r="BZ32" s="21"/>
+      <c r="CA32" s="21"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13">
+      <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="13"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="7"/>
       <c r="D33" s="9" t="s">
         <v>50</v>
@@ -4283,27 +4289,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="26">
+      <c r="AP33" s="17">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="27" t="s">
+      <c r="AQ33" s="17"/>
+      <c r="AR33" s="17"/>
+      <c r="AS33" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="27"/>
-      <c r="AU33" s="27"/>
-      <c r="AV33" s="27"/>
-      <c r="AW33" s="27"/>
-      <c r="AX33" s="27"/>
-      <c r="AY33" s="27"/>
-      <c r="AZ33" s="27"/>
-      <c r="BA33" s="27"/>
-      <c r="BB33" s="27"/>
-      <c r="BC33" s="27"/>
-      <c r="BD33" s="27"/>
-      <c r="BE33" s="27"/>
-      <c r="BF33" s="27"/>
+      <c r="AT33" s="18"/>
+      <c r="AU33" s="18"/>
+      <c r="AV33" s="18"/>
+      <c r="AW33" s="18"/>
+      <c r="AX33" s="18"/>
+      <c r="AY33" s="18"/>
+      <c r="AZ33" s="18"/>
+      <c r="BA33" s="18"/>
+      <c r="BB33" s="18"/>
+      <c r="BC33" s="18"/>
+      <c r="BD33" s="18"/>
+      <c r="BE33" s="18"/>
+      <c r="BF33" s="18"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -4327,10 +4333,10 @@
       <c r="CA33" s="12"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+      <c r="A34" s="13">
         <v>33</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="5"/>
       <c r="D34" s="9" t="s">
         <v>50</v>
@@ -4420,10 +4426,10 @@
       <c r="CA34" s="12"/>
     </row>
     <row r="35" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
+      <c r="A35" s="8">
         <v>34</v>
       </c>
-      <c r="B35" s="13"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="5"/>
       <c r="D35" s="9" t="s">
         <v>52</v>
@@ -4513,10 +4519,10 @@
       <c r="CA35" s="12"/>
     </row>
     <row r="36" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+      <c r="A36" s="8">
         <v>35</v>
       </c>
-      <c r="B36" s="13"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="5"/>
       <c r="D36" s="9" t="s">
         <v>52</v>
@@ -4606,41 +4612,41 @@
       <c r="CA36" s="12"/>
     </row>
     <row r="37" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13">
+      <c r="A37" s="8">
         <v>36</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="29"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="30"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="15"/>
+      <c r="AD37" s="15"/>
+      <c r="AE37" s="16"/>
       <c r="AF37" s="10">
         <v>43416</v>
       </c>
@@ -4699,41 +4705,41 @@
       <c r="CA37" s="12"/>
     </row>
     <row r="38" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="A38" s="13">
         <v>37</v>
       </c>
-      <c r="B38" s="8"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="30"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
+      <c r="AC38" s="15"/>
+      <c r="AD38" s="15"/>
+      <c r="AE38" s="16"/>
       <c r="AF38" s="10">
         <v>43446</v>
       </c>
@@ -4792,10 +4798,10 @@
       <c r="CA38" s="12"/>
     </row>
     <row r="39" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A39" s="13">
+      <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="13"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="5"/>
       <c r="D39" s="9" t="s">
         <v>53</v>
@@ -4885,41 +4891,41 @@
       <c r="CA39" s="12"/>
     </row>
     <row r="40" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+      <c r="A40" s="8">
         <v>39</v>
       </c>
-      <c r="B40" s="13"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="30"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="15"/>
+      <c r="AD40" s="15"/>
+      <c r="AE40" s="16"/>
       <c r="AF40" s="10">
         <v>43447</v>
       </c>
@@ -4978,10 +4984,10 @@
       <c r="CA40" s="12"/>
     </row>
     <row r="41" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13">
+      <c r="A41" s="8">
         <v>40</v>
       </c>
-      <c r="B41" s="13"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="5"/>
       <c r="D41" s="9" t="s">
         <v>53</v>
@@ -5071,41 +5077,41 @@
       <c r="CA41" s="12"/>
     </row>
     <row r="42" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
+      <c r="A42" s="13">
         <v>41</v>
       </c>
-      <c r="B42" s="8"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="30"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
+      <c r="AD42" s="15"/>
+      <c r="AE42" s="16"/>
       <c r="AF42" s="10" t="s">
         <v>55</v>
       </c>
@@ -5164,41 +5170,41 @@
       <c r="CA42" s="12"/>
     </row>
     <row r="43" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A43" s="13">
+      <c r="A43" s="8">
         <v>42</v>
       </c>
-      <c r="B43" s="13"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="30"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="15"/>
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="15"/>
+      <c r="AC43" s="15"/>
+      <c r="AD43" s="15"/>
+      <c r="AE43" s="16"/>
       <c r="AF43" s="10" t="s">
         <v>55</v>
       </c>
@@ -5257,41 +5263,41 @@
       <c r="CA43" s="12"/>
     </row>
     <row r="44" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A44" s="13">
+      <c r="A44" s="8">
         <v>43</v>
       </c>
-      <c r="B44" s="13"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="30"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="15"/>
+      <c r="AA44" s="15"/>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="15"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="16"/>
       <c r="AF44" s="10" t="s">
         <v>58</v>
       </c>
@@ -5350,10 +5356,10 @@
       <c r="CA44" s="12"/>
     </row>
     <row r="45" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13">
+      <c r="A45" s="8">
         <v>44</v>
       </c>
-      <c r="B45" s="13"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="5"/>
       <c r="D45" s="9" t="s">
         <v>59</v>
@@ -5443,10 +5449,10 @@
       <c r="CA45" s="12"/>
     </row>
     <row r="46" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
+      <c r="A46" s="13">
         <v>45</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="5"/>
       <c r="D46" s="9" t="s">
         <v>60</v>
@@ -5536,10 +5542,10 @@
       <c r="CA46" s="12"/>
     </row>
     <row r="47" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A47" s="13">
+      <c r="A47" s="8">
         <v>46</v>
       </c>
-      <c r="B47" s="13"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="5"/>
       <c r="D47" s="9" t="s">
         <v>62</v>
@@ -5629,10 +5635,10 @@
       <c r="CA47" s="12"/>
     </row>
     <row r="48" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A48" s="13">
+      <c r="A48" s="8">
         <v>47</v>
       </c>
-      <c r="B48" s="13"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="5"/>
       <c r="D48" s="9" t="s">
         <v>62</v>
@@ -5722,10 +5728,10 @@
       <c r="CA48" s="12"/>
     </row>
     <row r="49" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13">
+      <c r="A49" s="8">
         <v>48</v>
       </c>
-      <c r="B49" s="13"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="5"/>
       <c r="D49" s="9" t="s">
         <v>64</v>
@@ -5815,10 +5821,10 @@
       <c r="CA49" s="12"/>
     </row>
     <row r="50" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
+      <c r="A50" s="13">
         <v>49</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="5"/>
       <c r="D50" s="9" t="s">
         <v>65</v>
@@ -5908,10 +5914,10 @@
       <c r="CA50" s="12"/>
     </row>
     <row r="51" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A51" s="13">
+      <c r="A51" s="8">
         <v>50</v>
       </c>
-      <c r="B51" s="13"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="5"/>
       <c r="D51" s="9" t="s">
         <v>66</v>
@@ -6001,10 +6007,10 @@
       <c r="CA51" s="12"/>
     </row>
     <row r="52" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A52" s="13">
+      <c r="A52" s="8">
         <v>51</v>
       </c>
-      <c r="B52" s="13"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="5"/>
       <c r="D52" s="9" t="s">
         <v>66</v>
@@ -6094,10 +6100,10 @@
       <c r="CA52" s="12"/>
     </row>
     <row r="53" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13">
+      <c r="A53" s="8">
         <v>52</v>
       </c>
-      <c r="B53" s="13"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="5"/>
       <c r="D53" s="9" t="s">
         <v>68</v>
@@ -6187,10 +6193,10 @@
       <c r="CA53" s="12"/>
     </row>
     <row r="54" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
+      <c r="A54" s="13">
         <v>53</v>
       </c>
-      <c r="B54" s="8"/>
+      <c r="B54" s="13"/>
       <c r="C54" s="5"/>
       <c r="D54" s="9" t="s">
         <v>69</v>
@@ -6280,10 +6286,10 @@
       <c r="CA54" s="12"/>
     </row>
     <row r="55" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A55" s="13">
+      <c r="A55" s="8">
         <v>54</v>
       </c>
-      <c r="B55" s="13"/>
+      <c r="B55" s="8"/>
       <c r="C55" s="5"/>
       <c r="D55" s="9" t="s">
         <v>71</v>
@@ -6373,10 +6379,10 @@
       <c r="CA55" s="12"/>
     </row>
     <row r="56" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A56" s="13">
+      <c r="A56" s="8">
         <v>55</v>
       </c>
-      <c r="B56" s="13"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="5"/>
       <c r="D56" s="9" t="s">
         <v>72</v>
@@ -6466,10 +6472,10 @@
       <c r="CA56" s="12"/>
     </row>
     <row r="57" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13">
+      <c r="A57" s="8">
         <v>56</v>
       </c>
-      <c r="B57" s="13"/>
+      <c r="B57" s="8"/>
       <c r="C57" s="5"/>
       <c r="D57" s="9" t="s">
         <v>74</v>
@@ -6559,10 +6565,10 @@
       <c r="CA57" s="12"/>
     </row>
     <row r="58" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
+      <c r="A58" s="13">
         <v>57</v>
       </c>
-      <c r="B58" s="8"/>
+      <c r="B58" s="13"/>
       <c r="C58" s="5"/>
       <c r="D58" s="9" t="s">
         <v>75</v>
@@ -6652,10 +6658,10 @@
       <c r="CA58" s="12"/>
     </row>
     <row r="59" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A59" s="13">
+      <c r="A59" s="8">
         <v>58</v>
       </c>
-      <c r="B59" s="13"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="5"/>
       <c r="D59" s="9" t="s">
         <v>77</v>
@@ -6745,10 +6751,10 @@
       <c r="CA59" s="12"/>
     </row>
     <row r="60" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A60" s="13">
+      <c r="A60" s="8">
         <v>59</v>
       </c>
-      <c r="B60" s="13"/>
+      <c r="B60" s="8"/>
       <c r="C60" s="5"/>
       <c r="D60" s="9" t="s">
         <v>75</v>
@@ -6838,10 +6844,10 @@
       <c r="CA60" s="12"/>
     </row>
     <row r="61" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13">
+      <c r="A61" s="8">
         <v>60</v>
       </c>
-      <c r="B61" s="13"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="5"/>
       <c r="D61" s="9" t="s">
         <v>80</v>
@@ -6931,10 +6937,10 @@
       <c r="CA61" s="12"/>
     </row>
     <row r="62" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A62" s="8">
+      <c r="A62" s="13">
         <v>61</v>
       </c>
-      <c r="B62" s="8"/>
+      <c r="B62" s="13"/>
       <c r="C62" s="5"/>
       <c r="D62" s="9" t="s">
         <v>78</v>
@@ -7024,10 +7030,10 @@
       <c r="CA62" s="12"/>
     </row>
     <row r="63" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A63" s="13">
+      <c r="A63" s="8">
         <v>62</v>
       </c>
-      <c r="B63" s="13"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="5"/>
       <c r="D63" s="9" t="s">
         <v>84</v>
@@ -7117,10 +7123,10 @@
       <c r="CA63" s="12"/>
     </row>
     <row r="64" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A64" s="13">
+      <c r="A64" s="8">
         <v>63</v>
       </c>
-      <c r="B64" s="13"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="5"/>
       <c r="D64" s="9" t="s">
         <v>84</v>
@@ -7210,10 +7216,10 @@
       <c r="CA64" s="12"/>
     </row>
     <row r="65" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13">
+      <c r="A65" s="8">
         <v>64</v>
       </c>
-      <c r="B65" s="13"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="5"/>
       <c r="D65" s="9" t="s">
         <v>83</v>
@@ -7301,10 +7307,10 @@
       <c r="CA65" s="12"/>
     </row>
     <row r="66" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A66" s="8">
+      <c r="A66" s="13">
         <v>65</v>
       </c>
-      <c r="B66" s="8"/>
+      <c r="B66" s="13"/>
       <c r="C66" s="5"/>
       <c r="D66" s="9" t="s">
         <v>85</v>
@@ -7394,10 +7400,10 @@
       <c r="CA66" s="12"/>
     </row>
     <row r="67" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A67" s="13">
+      <c r="A67" s="8">
         <v>66</v>
       </c>
-      <c r="B67" s="13"/>
+      <c r="B67" s="8"/>
       <c r="C67" s="5"/>
       <c r="D67" s="9" t="s">
         <v>87</v>
@@ -7487,10 +7493,10 @@
       <c r="CA67" s="12"/>
     </row>
     <row r="68" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A68" s="13">
+      <c r="A68" s="8">
         <v>67</v>
       </c>
-      <c r="B68" s="13"/>
+      <c r="B68" s="8"/>
       <c r="C68" s="5"/>
       <c r="D68" s="9" t="s">
         <v>87</v>
@@ -7580,10 +7586,10 @@
       <c r="CA68" s="12"/>
     </row>
     <row r="69" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="13">
+      <c r="A69" s="8">
         <v>68</v>
       </c>
-      <c r="B69" s="13"/>
+      <c r="B69" s="8"/>
       <c r="C69" s="5"/>
       <c r="D69" s="9" t="s">
         <v>88</v>
@@ -7673,10 +7679,10 @@
       <c r="CA69" s="12"/>
     </row>
     <row r="70" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A70" s="8">
+      <c r="A70" s="13">
         <v>69</v>
       </c>
-      <c r="B70" s="8"/>
+      <c r="B70" s="13"/>
       <c r="C70" s="5"/>
       <c r="D70" s="9" t="s">
         <v>90</v>
@@ -7766,10 +7772,10 @@
       <c r="CA70" s="12"/>
     </row>
     <row r="71" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A71" s="13">
+      <c r="A71" s="8">
         <v>70</v>
       </c>
-      <c r="B71" s="13"/>
+      <c r="B71" s="8"/>
       <c r="C71" s="5"/>
       <c r="D71" s="9" t="s">
         <v>90</v>
@@ -7859,10 +7865,10 @@
       <c r="CA71" s="12"/>
     </row>
     <row r="72" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A72" s="13">
+      <c r="A72" s="8">
         <v>71</v>
       </c>
-      <c r="B72" s="13"/>
+      <c r="B72" s="8"/>
       <c r="C72" s="5"/>
       <c r="D72" s="9" t="s">
         <v>91</v>
@@ -7952,10 +7958,10 @@
       <c r="CA72" s="12"/>
     </row>
     <row r="73" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="13">
+      <c r="A73" s="8">
         <v>72</v>
       </c>
-      <c r="B73" s="13"/>
+      <c r="B73" s="8"/>
       <c r="C73" s="5"/>
       <c r="D73" s="9" t="s">
         <v>92</v>
@@ -8045,10 +8051,10 @@
       <c r="CA73" s="12"/>
     </row>
     <row r="74" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
+      <c r="A74" s="13">
         <v>73</v>
       </c>
-      <c r="B74" s="8"/>
+      <c r="B74" s="13"/>
       <c r="C74" s="5"/>
       <c r="D74" s="9" t="s">
         <v>93</v>
@@ -8138,10 +8144,10 @@
       <c r="CA74" s="12"/>
     </row>
     <row r="75" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A75" s="13">
+      <c r="A75" s="8">
         <v>74</v>
       </c>
-      <c r="B75" s="13"/>
+      <c r="B75" s="8"/>
       <c r="C75" s="5"/>
       <c r="D75" s="9" t="s">
         <v>94</v>
@@ -8231,10 +8237,10 @@
       <c r="CA75" s="12"/>
     </row>
     <row r="76" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A76" s="13">
+      <c r="A76" s="8">
         <v>75</v>
       </c>
-      <c r="B76" s="13"/>
+      <c r="B76" s="8"/>
       <c r="C76" s="5"/>
       <c r="D76" s="9" t="s">
         <v>94</v>
@@ -8324,10 +8330,10 @@
       <c r="CA76" s="12"/>
     </row>
     <row r="77" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="13">
+      <c r="A77" s="8">
         <v>76</v>
       </c>
-      <c r="B77" s="13"/>
+      <c r="B77" s="8"/>
       <c r="C77" s="5"/>
       <c r="D77" s="9" t="s">
         <v>95</v>
@@ -8417,10 +8423,10 @@
       <c r="CA77" s="12"/>
     </row>
     <row r="78" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
+      <c r="A78" s="13">
         <v>77</v>
       </c>
-      <c r="B78" s="8"/>
+      <c r="B78" s="13"/>
       <c r="C78" s="5"/>
       <c r="D78" s="9" t="s">
         <v>97</v>
@@ -8510,10 +8516,10 @@
       <c r="CA78" s="12"/>
     </row>
     <row r="79" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A79" s="13">
+      <c r="A79" s="8">
         <v>78</v>
       </c>
-      <c r="B79" s="13"/>
+      <c r="B79" s="8"/>
       <c r="C79" s="5"/>
       <c r="D79" s="9" t="s">
         <v>96</v>
@@ -8603,10 +8609,10 @@
       <c r="CA79" s="12"/>
     </row>
     <row r="80" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A80" s="13">
+      <c r="A80" s="8">
         <v>79</v>
       </c>
-      <c r="B80" s="13"/>
+      <c r="B80" s="8"/>
       <c r="C80" s="5"/>
       <c r="D80" s="9" t="s">
         <v>96</v>
@@ -8696,10 +8702,10 @@
       <c r="CA80" s="12"/>
     </row>
     <row r="81" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="13">
+      <c r="A81" s="8">
         <v>80</v>
       </c>
-      <c r="B81" s="13"/>
+      <c r="B81" s="8"/>
       <c r="C81" s="5"/>
       <c r="D81" s="9" t="s">
         <v>98</v>
@@ -8789,10 +8795,10 @@
       <c r="CA81" s="12"/>
     </row>
     <row r="82" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A82" s="8">
+      <c r="A82" s="13">
         <v>81</v>
       </c>
-      <c r="B82" s="8"/>
+      <c r="B82" s="13"/>
       <c r="C82" s="5"/>
       <c r="D82" s="9" t="s">
         <v>99</v>
@@ -8882,10 +8888,10 @@
       <c r="CA82" s="12"/>
     </row>
     <row r="83" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A83" s="13">
+      <c r="A83" s="8">
         <v>82</v>
       </c>
-      <c r="B83" s="13"/>
+      <c r="B83" s="8"/>
       <c r="C83" s="5"/>
       <c r="D83" s="9" t="s">
         <v>101</v>
@@ -8975,10 +8981,10 @@
       <c r="CA83" s="12"/>
     </row>
     <row r="84" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A84" s="13">
+      <c r="A84" s="8">
         <v>83</v>
       </c>
-      <c r="B84" s="13"/>
+      <c r="B84" s="8"/>
       <c r="C84" s="5"/>
       <c r="D84" s="9" t="s">
         <v>100</v>
@@ -9068,10 +9074,10 @@
       <c r="CA84" s="12"/>
     </row>
     <row r="85" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="13">
+      <c r="A85" s="8">
         <v>84</v>
       </c>
-      <c r="B85" s="13"/>
+      <c r="B85" s="8"/>
       <c r="C85" s="5"/>
       <c r="D85" s="9" t="s">
         <v>102</v>
@@ -9161,10 +9167,10 @@
       <c r="CA85" s="12"/>
     </row>
     <row r="86" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A86" s="8">
+      <c r="A86" s="13">
         <v>85</v>
       </c>
-      <c r="B86" s="8"/>
+      <c r="B86" s="13"/>
       <c r="C86" s="5"/>
       <c r="D86" s="9" t="s">
         <v>99</v>
@@ -9254,10 +9260,10 @@
       <c r="CA86" s="12"/>
     </row>
     <row r="87" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A87" s="13">
+      <c r="A87" s="8">
         <v>86</v>
       </c>
-      <c r="B87" s="13"/>
+      <c r="B87" s="8"/>
       <c r="C87" s="5"/>
       <c r="D87" s="9" t="s">
         <v>103</v>
@@ -9347,10 +9353,10 @@
       <c r="CA87" s="12"/>
     </row>
     <row r="88" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A88" s="13">
+      <c r="A88" s="8">
         <v>87</v>
       </c>
-      <c r="B88" s="13"/>
+      <c r="B88" s="8"/>
       <c r="C88" s="5"/>
       <c r="D88" s="9" t="s">
         <v>104</v>
@@ -9438,10 +9444,10 @@
       <c r="CA88" s="12"/>
     </row>
     <row r="89" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="13">
+      <c r="A89" s="8">
         <v>88</v>
       </c>
-      <c r="B89" s="13"/>
+      <c r="B89" s="8"/>
       <c r="C89" s="5"/>
       <c r="D89" s="9" t="s">
         <v>105</v>
@@ -9529,10 +9535,10 @@
       <c r="CA89" s="12"/>
     </row>
     <row r="90" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A90" s="8">
+      <c r="A90" s="13">
         <v>89</v>
       </c>
-      <c r="B90" s="8"/>
+      <c r="B90" s="13"/>
       <c r="C90" s="5"/>
       <c r="D90" s="9" t="s">
         <v>105</v>
@@ -9620,10 +9626,10 @@
       <c r="CA90" s="12"/>
     </row>
     <row r="91" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A91" s="13">
+      <c r="A91" s="8">
         <v>90</v>
       </c>
-      <c r="B91" s="13"/>
+      <c r="B91" s="8"/>
       <c r="C91" s="5"/>
       <c r="D91" s="9" t="s">
         <v>105</v>
@@ -9711,10 +9717,10 @@
       <c r="CA91" s="12"/>
     </row>
     <row r="92" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A92" s="13">
+      <c r="A92" s="8">
         <v>91</v>
       </c>
-      <c r="B92" s="13"/>
+      <c r="B92" s="8"/>
       <c r="C92" s="5"/>
       <c r="D92" s="9" t="s">
         <v>107</v>
@@ -9804,10 +9810,10 @@
       <c r="CA92" s="12"/>
     </row>
     <row r="93" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="13">
+      <c r="A93" s="8">
         <v>92</v>
       </c>
-      <c r="B93" s="13"/>
+      <c r="B93" s="8"/>
       <c r="C93" s="5"/>
       <c r="D93" s="9" t="s">
         <v>107</v>
@@ -9897,10 +9903,10 @@
       <c r="CA93" s="12"/>
     </row>
     <row r="94" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A94" s="8">
+      <c r="A94" s="13">
         <v>93</v>
       </c>
-      <c r="B94" s="8"/>
+      <c r="B94" s="13"/>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
         <v>109</v>
@@ -9990,10 +9996,10 @@
       <c r="CA94" s="12"/>
     </row>
     <row r="95" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A95" s="13">
+      <c r="A95" s="8">
         <v>94</v>
       </c>
-      <c r="B95" s="13"/>
+      <c r="B95" s="8"/>
       <c r="C95" s="5"/>
       <c r="D95" s="9" t="s">
         <v>111</v>
@@ -10083,10 +10089,10 @@
       <c r="CA95" s="12"/>
     </row>
     <row r="96" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A96" s="13">
+      <c r="A96" s="8">
         <v>95</v>
       </c>
-      <c r="B96" s="13"/>
+      <c r="B96" s="8"/>
       <c r="C96" s="5"/>
       <c r="D96" s="9" t="s">
         <v>114</v>
@@ -10176,10 +10182,10 @@
       <c r="CA96" s="12"/>
     </row>
     <row r="97" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="13">
+      <c r="A97" s="8">
         <v>96</v>
       </c>
-      <c r="B97" s="13"/>
+      <c r="B97" s="8"/>
       <c r="C97" s="5"/>
       <c r="D97" s="9" t="s">
         <v>115</v>
@@ -10269,10 +10275,10 @@
       <c r="CA97" s="12"/>
     </row>
     <row r="98" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A98" s="8">
+      <c r="A98" s="13">
         <v>97</v>
       </c>
-      <c r="B98" s="8"/>
+      <c r="B98" s="13"/>
       <c r="C98" s="5"/>
       <c r="D98" s="9" t="s">
         <v>116</v>
@@ -10362,10 +10368,10 @@
       <c r="CA98" s="12"/>
     </row>
     <row r="99" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A99" s="13">
+      <c r="A99" s="8">
         <v>98</v>
       </c>
-      <c r="B99" s="13"/>
+      <c r="B99" s="8"/>
       <c r="C99" s="5"/>
       <c r="D99" s="9" t="s">
         <v>117</v>
@@ -10455,10 +10461,10 @@
       <c r="CA99" s="12"/>
     </row>
     <row r="100" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A100" s="13">
+      <c r="A100" s="8">
         <v>99</v>
       </c>
-      <c r="B100" s="13"/>
+      <c r="B100" s="8"/>
       <c r="C100" s="5"/>
       <c r="D100" s="9" t="s">
         <v>117</v>
@@ -10548,10 +10554,10 @@
       <c r="CA100" s="12"/>
     </row>
     <row r="101" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="13">
+      <c r="A101" s="8">
         <v>100</v>
       </c>
-      <c r="B101" s="13"/>
+      <c r="B101" s="8"/>
       <c r="C101" s="5"/>
       <c r="D101" s="9" t="s">
         <v>119</v>
@@ -10641,10 +10647,10 @@
       <c r="CA101" s="12"/>
     </row>
     <row r="102" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A102" s="8">
+      <c r="A102" s="13">
         <v>101</v>
       </c>
-      <c r="B102" s="8"/>
+      <c r="B102" s="13"/>
       <c r="C102" s="5"/>
       <c r="D102" s="9" t="s">
         <v>120</v>
@@ -10734,10 +10740,10 @@
       <c r="CA102" s="12"/>
     </row>
     <row r="103" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A103" s="13">
+      <c r="A103" s="8">
         <v>102</v>
       </c>
-      <c r="B103" s="13"/>
+      <c r="B103" s="8"/>
       <c r="C103" s="5"/>
       <c r="D103" s="9" t="s">
         <v>120</v>
@@ -10827,10 +10833,10 @@
       <c r="CA103" s="12"/>
     </row>
     <row r="104" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A104" s="13">
+      <c r="A104" s="8">
         <v>103</v>
       </c>
-      <c r="B104" s="13"/>
+      <c r="B104" s="8"/>
       <c r="C104" s="5"/>
       <c r="D104" s="9" t="s">
         <v>123</v>
@@ -10920,10 +10926,10 @@
       <c r="CA104" s="12"/>
     </row>
     <row r="105" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="13">
+      <c r="A105" s="8">
         <v>104</v>
       </c>
-      <c r="B105" s="13"/>
+      <c r="B105" s="8"/>
       <c r="C105" s="5"/>
       <c r="D105" s="9" t="s">
         <v>123</v>
@@ -11013,10 +11019,10 @@
       <c r="CA105" s="12"/>
     </row>
     <row r="106" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A106" s="8">
+      <c r="A106" s="13">
         <v>105</v>
       </c>
-      <c r="B106" s="8"/>
+      <c r="B106" s="13"/>
       <c r="C106" s="5"/>
       <c r="D106" s="9" t="s">
         <v>125</v>
@@ -11106,10 +11112,10 @@
       <c r="CA106" s="12"/>
     </row>
     <row r="107" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A107" s="13">
+      <c r="A107" s="8">
         <v>106</v>
       </c>
-      <c r="B107" s="13"/>
+      <c r="B107" s="8"/>
       <c r="C107" s="5"/>
       <c r="D107" s="9" t="s">
         <v>123</v>
@@ -11199,10 +11205,10 @@
       <c r="CA107" s="12"/>
     </row>
     <row r="108" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A108" s="13">
+      <c r="A108" s="8">
         <v>107</v>
       </c>
-      <c r="B108" s="13"/>
+      <c r="B108" s="8"/>
       <c r="C108" s="5"/>
       <c r="D108" s="9" t="s">
         <v>125</v>
@@ -11292,10 +11298,10 @@
       <c r="CA108" s="12"/>
     </row>
     <row r="109" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="13">
+      <c r="A109" s="8">
         <v>108</v>
       </c>
-      <c r="B109" s="13"/>
+      <c r="B109" s="8"/>
       <c r="C109" s="5"/>
       <c r="D109" s="9" t="s">
         <v>125</v>
@@ -11385,10 +11391,10 @@
       <c r="CA109" s="12"/>
     </row>
     <row r="110" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A110" s="8">
+      <c r="A110" s="13">
         <v>109</v>
       </c>
-      <c r="B110" s="8"/>
+      <c r="B110" s="13"/>
       <c r="C110" s="5"/>
       <c r="D110" s="9" t="s">
         <v>127</v>
@@ -11478,10 +11484,10 @@
       <c r="CA110" s="12"/>
     </row>
     <row r="111" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A111" s="13">
+      <c r="A111" s="8">
         <v>110</v>
       </c>
-      <c r="B111" s="13"/>
+      <c r="B111" s="8"/>
       <c r="C111" s="5"/>
       <c r="D111" s="9" t="s">
         <v>129</v>
@@ -11571,10 +11577,10 @@
       <c r="CA111" s="12"/>
     </row>
     <row r="112" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A112" s="13">
+      <c r="A112" s="8">
         <v>111</v>
       </c>
-      <c r="B112" s="13"/>
+      <c r="B112" s="8"/>
       <c r="C112" s="5"/>
       <c r="D112" s="9" t="s">
         <v>131</v>
@@ -11664,10 +11670,10 @@
       <c r="CA112" s="12"/>
     </row>
     <row r="113" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="13">
+      <c r="A113" s="8">
         <v>112</v>
       </c>
-      <c r="B113" s="13"/>
+      <c r="B113" s="8"/>
       <c r="C113" s="5"/>
       <c r="D113" s="9" t="s">
         <v>132</v>
@@ -11757,10 +11763,10 @@
       <c r="CA113" s="12"/>
     </row>
     <row r="114" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A114" s="8">
+      <c r="A114" s="13">
         <v>113</v>
       </c>
-      <c r="B114" s="8"/>
+      <c r="B114" s="13"/>
       <c r="C114" s="5"/>
       <c r="D114" s="9" t="s">
         <v>133</v>
@@ -11850,12 +11856,14 @@
       <c r="CA114" s="12"/>
     </row>
     <row r="115" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A115" s="13">
+      <c r="A115" s="8">
         <v>114</v>
       </c>
-      <c r="B115" s="13"/>
+      <c r="B115" s="8"/>
       <c r="C115" s="5"/>
-      <c r="D115" s="9"/>
+      <c r="D115" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="E115" s="9"/>
       <c r="F115" s="9"/>
       <c r="G115" s="9"/>
@@ -11883,20 +11891,28 @@
       <c r="AC115" s="9"/>
       <c r="AD115" s="9"/>
       <c r="AE115" s="9"/>
-      <c r="AF115" s="10"/>
+      <c r="AF115" s="10" t="s">
+        <v>134</v>
+      </c>
       <c r="AG115" s="10"/>
       <c r="AH115" s="10"/>
       <c r="AI115" s="10"/>
       <c r="AJ115" s="10"/>
-      <c r="AK115" s="9"/>
+      <c r="AK115" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL115" s="9"/>
       <c r="AM115" s="9"/>
       <c r="AN115" s="9"/>
       <c r="AO115" s="9"/>
-      <c r="AP115" s="11"/>
+      <c r="AP115" s="11">
+        <v>0.8</v>
+      </c>
       <c r="AQ115" s="11"/>
       <c r="AR115" s="11"/>
-      <c r="AS115" s="9"/>
+      <c r="AS115" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT115" s="9"/>
       <c r="AU115" s="9"/>
       <c r="AV115" s="9"/>
@@ -11933,12 +11949,14 @@
       <c r="CA115" s="12"/>
     </row>
     <row r="116" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A116" s="13">
+      <c r="A116" s="8">
         <v>115</v>
       </c>
-      <c r="B116" s="13"/>
+      <c r="B116" s="8"/>
       <c r="C116" s="5"/>
-      <c r="D116" s="9"/>
+      <c r="D116" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="E116" s="9"/>
       <c r="F116" s="9"/>
       <c r="G116" s="9"/>
@@ -11966,20 +11984,28 @@
       <c r="AC116" s="9"/>
       <c r="AD116" s="9"/>
       <c r="AE116" s="9"/>
-      <c r="AF116" s="10"/>
+      <c r="AF116" s="10" t="s">
+        <v>134</v>
+      </c>
       <c r="AG116" s="10"/>
       <c r="AH116" s="10"/>
       <c r="AI116" s="10"/>
       <c r="AJ116" s="10"/>
-      <c r="AK116" s="9"/>
+      <c r="AK116" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL116" s="9"/>
       <c r="AM116" s="9"/>
       <c r="AN116" s="9"/>
       <c r="AO116" s="9"/>
-      <c r="AP116" s="11"/>
+      <c r="AP116" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ116" s="11"/>
       <c r="AR116" s="11"/>
-      <c r="AS116" s="9"/>
+      <c r="AS116" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT116" s="9"/>
       <c r="AU116" s="9"/>
       <c r="AV116" s="9"/>
@@ -12016,12 +12042,14 @@
       <c r="CA116" s="12"/>
     </row>
     <row r="117" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="13">
+      <c r="A117" s="8">
         <v>116</v>
       </c>
-      <c r="B117" s="13"/>
+      <c r="B117" s="8"/>
       <c r="C117" s="5"/>
-      <c r="D117" s="9"/>
+      <c r="D117" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="E117" s="9"/>
       <c r="F117" s="9"/>
       <c r="G117" s="9"/>
@@ -12049,20 +12077,28 @@
       <c r="AC117" s="9"/>
       <c r="AD117" s="9"/>
       <c r="AE117" s="9"/>
-      <c r="AF117" s="10"/>
+      <c r="AF117" s="10" t="s">
+        <v>134</v>
+      </c>
       <c r="AG117" s="10"/>
       <c r="AH117" s="10"/>
       <c r="AI117" s="10"/>
       <c r="AJ117" s="10"/>
-      <c r="AK117" s="9"/>
+      <c r="AK117" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL117" s="9"/>
       <c r="AM117" s="9"/>
       <c r="AN117" s="9"/>
       <c r="AO117" s="9"/>
-      <c r="AP117" s="11"/>
+      <c r="AP117" s="11">
+        <v>0.5</v>
+      </c>
       <c r="AQ117" s="11"/>
       <c r="AR117" s="11"/>
-      <c r="AS117" s="9"/>
+      <c r="AS117" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT117" s="9"/>
       <c r="AU117" s="9"/>
       <c r="AV117" s="9"/>
@@ -12099,10 +12135,10 @@
       <c r="CA117" s="12"/>
     </row>
     <row r="118" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A118" s="8">
+      <c r="A118" s="13">
         <v>117</v>
       </c>
-      <c r="B118" s="8"/>
+      <c r="B118" s="13"/>
       <c r="C118" s="5"/>
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
@@ -12182,10 +12218,10 @@
       <c r="CA118" s="12"/>
     </row>
     <row r="119" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A119" s="13">
+      <c r="A119" s="8">
         <v>118</v>
       </c>
-      <c r="B119" s="13"/>
+      <c r="B119" s="8"/>
       <c r="C119" s="5"/>
       <c r="D119" s="9"/>
       <c r="E119" s="9"/>
@@ -12265,10 +12301,10 @@
       <c r="CA119" s="12"/>
     </row>
     <row r="120" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A120" s="13">
+      <c r="A120" s="8">
         <v>119</v>
       </c>
-      <c r="B120" s="13"/>
+      <c r="B120" s="8"/>
       <c r="C120" s="5"/>
       <c r="D120" s="9"/>
       <c r="E120" s="9"/>
@@ -12348,10 +12384,10 @@
       <c r="CA120" s="12"/>
     </row>
     <row r="121" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="13">
+      <c r="A121" s="8">
         <v>120</v>
       </c>
-      <c r="B121" s="13"/>
+      <c r="B121" s="8"/>
       <c r="C121" s="5"/>
       <c r="D121" s="9"/>
       <c r="E121" s="9"/>
@@ -12431,10 +12467,10 @@
       <c r="CA121" s="12"/>
     </row>
     <row r="122" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A122" s="8">
+      <c r="A122" s="13">
         <v>121</v>
       </c>
-      <c r="B122" s="8"/>
+      <c r="B122" s="13"/>
       <c r="C122" s="5"/>
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
@@ -12514,10 +12550,10 @@
       <c r="CA122" s="12"/>
     </row>
     <row r="123" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A123" s="13">
+      <c r="A123" s="8">
         <v>122</v>
       </c>
-      <c r="B123" s="13"/>
+      <c r="B123" s="8"/>
       <c r="C123" s="5"/>
       <c r="BG123" s="12"/>
       <c r="BH123" s="12"/>
@@ -12543,493 +12579,351 @@
     </row>
   </sheetData>
   <mergeCells count="856">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="D70:AE70"/>
     <mergeCell ref="AF70:AJ70"/>
@@ -13054,351 +12948,493 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:AE3"/>
     <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">

</xml_diff>

<commit_message>
báo cáo ngày 19/2/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="140">
   <si>
     <t>No.</t>
   </si>
@@ -429,6 +429,18 @@
   <si>
     <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data - Hoàn thành việc update dữ liệu</t>
   </si>
+  <si>
+    <t>19/2/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  delete data - Tạo câu lệnh sql để delete bảng server đích</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  delete data - Sửa lỗi chính tả khi thêm vào db đích</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  delete data - Sửa lỗi back up dữ liệu khi sửa dữ liệu</t>
+  </si>
 </sst>
 </file>
 
@@ -679,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -723,6 +735,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1227,11 +1245,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA123"/>
+  <dimension ref="A1:CA142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP118" sqref="AP118:AR118"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D127" sqref="D127:AE127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12223,61 +12241,71 @@
       </c>
       <c r="B119" s="8"/>
       <c r="C119" s="5"/>
-      <c r="D119" s="9"/>
-      <c r="E119" s="9"/>
-      <c r="F119" s="9"/>
-      <c r="G119" s="9"/>
-      <c r="H119" s="9"/>
-      <c r="I119" s="9"/>
-      <c r="J119" s="9"/>
-      <c r="K119" s="9"/>
-      <c r="L119" s="9"/>
-      <c r="M119" s="9"/>
-      <c r="N119" s="9"/>
-      <c r="O119" s="9"/>
-      <c r="P119" s="9"/>
-      <c r="Q119" s="9"/>
-      <c r="R119" s="9"/>
-      <c r="S119" s="9"/>
-      <c r="T119" s="9"/>
-      <c r="U119" s="9"/>
-      <c r="V119" s="9"/>
-      <c r="W119" s="9"/>
-      <c r="X119" s="9"/>
-      <c r="Y119" s="9"/>
-      <c r="Z119" s="9"/>
-      <c r="AA119" s="9"/>
-      <c r="AB119" s="9"/>
-      <c r="AC119" s="9"/>
-      <c r="AD119" s="9"/>
-      <c r="AE119" s="9"/>
-      <c r="AF119" s="10"/>
-      <c r="AG119" s="10"/>
-      <c r="AH119" s="10"/>
-      <c r="AI119" s="10"/>
-      <c r="AJ119" s="10"/>
-      <c r="AK119" s="9"/>
-      <c r="AL119" s="9"/>
-      <c r="AM119" s="9"/>
-      <c r="AN119" s="9"/>
-      <c r="AO119" s="9"/>
-      <c r="AP119" s="11"/>
-      <c r="AQ119" s="11"/>
-      <c r="AR119" s="11"/>
-      <c r="AS119" s="9"/>
-      <c r="AT119" s="9"/>
-      <c r="AU119" s="9"/>
-      <c r="AV119" s="9"/>
-      <c r="AW119" s="9"/>
-      <c r="AX119" s="9"/>
-      <c r="AY119" s="9"/>
-      <c r="AZ119" s="9"/>
-      <c r="BA119" s="9"/>
-      <c r="BB119" s="9"/>
-      <c r="BC119" s="9"/>
-      <c r="BD119" s="9"/>
-      <c r="BE119" s="9"/>
-      <c r="BF119" s="9"/>
+      <c r="D119" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E119" s="15"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+      <c r="I119" s="15"/>
+      <c r="J119" s="15"/>
+      <c r="K119" s="15"/>
+      <c r="L119" s="15"/>
+      <c r="M119" s="15"/>
+      <c r="N119" s="15"/>
+      <c r="O119" s="15"/>
+      <c r="P119" s="15"/>
+      <c r="Q119" s="15"/>
+      <c r="R119" s="15"/>
+      <c r="S119" s="15"/>
+      <c r="T119" s="15"/>
+      <c r="U119" s="15"/>
+      <c r="V119" s="15"/>
+      <c r="W119" s="15"/>
+      <c r="X119" s="15"/>
+      <c r="Y119" s="15"/>
+      <c r="Z119" s="15"/>
+      <c r="AA119" s="15"/>
+      <c r="AB119" s="15"/>
+      <c r="AC119" s="15"/>
+      <c r="AD119" s="15"/>
+      <c r="AE119" s="16"/>
+      <c r="AF119" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG119" s="35"/>
+      <c r="AH119" s="35"/>
+      <c r="AI119" s="35"/>
+      <c r="AJ119" s="36"/>
+      <c r="AK119" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL119" s="15"/>
+      <c r="AM119" s="15"/>
+      <c r="AN119" s="15"/>
+      <c r="AO119" s="16"/>
+      <c r="AP119" s="31">
+        <v>1</v>
+      </c>
+      <c r="AQ119" s="32"/>
+      <c r="AR119" s="33"/>
+      <c r="AS119" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT119" s="15"/>
+      <c r="AU119" s="15"/>
+      <c r="AV119" s="15"/>
+      <c r="AW119" s="15"/>
+      <c r="AX119" s="15"/>
+      <c r="AY119" s="15"/>
+      <c r="AZ119" s="15"/>
+      <c r="BA119" s="15"/>
+      <c r="BB119" s="15"/>
+      <c r="BC119" s="15"/>
+      <c r="BD119" s="15"/>
+      <c r="BE119" s="15"/>
+      <c r="BF119" s="16"/>
       <c r="BG119" s="12"/>
       <c r="BH119" s="12"/>
       <c r="BI119" s="12"/>
@@ -12306,7 +12334,9 @@
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="5"/>
-      <c r="D120" s="9"/>
+      <c r="D120" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="E120" s="9"/>
       <c r="F120" s="9"/>
       <c r="G120" s="9"/>
@@ -12334,20 +12364,28 @@
       <c r="AC120" s="9"/>
       <c r="AD120" s="9"/>
       <c r="AE120" s="9"/>
-      <c r="AF120" s="10"/>
+      <c r="AF120" s="10" t="s">
+        <v>136</v>
+      </c>
       <c r="AG120" s="10"/>
       <c r="AH120" s="10"/>
       <c r="AI120" s="10"/>
       <c r="AJ120" s="10"/>
-      <c r="AK120" s="9"/>
+      <c r="AK120" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL120" s="9"/>
       <c r="AM120" s="9"/>
       <c r="AN120" s="9"/>
       <c r="AO120" s="9"/>
-      <c r="AP120" s="11"/>
+      <c r="AP120" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ120" s="11"/>
       <c r="AR120" s="11"/>
-      <c r="AS120" s="9"/>
+      <c r="AS120" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT120" s="9"/>
       <c r="AU120" s="9"/>
       <c r="AV120" s="9"/>
@@ -12389,7 +12427,9 @@
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="5"/>
-      <c r="D121" s="9"/>
+      <c r="D121" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="E121" s="9"/>
       <c r="F121" s="9"/>
       <c r="G121" s="9"/>
@@ -12417,20 +12457,28 @@
       <c r="AC121" s="9"/>
       <c r="AD121" s="9"/>
       <c r="AE121" s="9"/>
-      <c r="AF121" s="10"/>
+      <c r="AF121" s="10" t="s">
+        <v>136</v>
+      </c>
       <c r="AG121" s="10"/>
       <c r="AH121" s="10"/>
       <c r="AI121" s="10"/>
       <c r="AJ121" s="10"/>
-      <c r="AK121" s="9"/>
+      <c r="AK121" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL121" s="9"/>
       <c r="AM121" s="9"/>
       <c r="AN121" s="9"/>
       <c r="AO121" s="9"/>
-      <c r="AP121" s="11"/>
+      <c r="AP121" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ121" s="11"/>
       <c r="AR121" s="11"/>
-      <c r="AS121" s="9"/>
+      <c r="AS121" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT121" s="9"/>
       <c r="AU121" s="9"/>
       <c r="AV121" s="9"/>
@@ -12472,7 +12520,9 @@
       </c>
       <c r="B122" s="13"/>
       <c r="C122" s="5"/>
-      <c r="D122" s="9"/>
+      <c r="D122" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="E122" s="9"/>
       <c r="F122" s="9"/>
       <c r="G122" s="9"/>
@@ -12500,20 +12550,28 @@
       <c r="AC122" s="9"/>
       <c r="AD122" s="9"/>
       <c r="AE122" s="9"/>
-      <c r="AF122" s="10"/>
+      <c r="AF122" s="10" t="s">
+        <v>136</v>
+      </c>
       <c r="AG122" s="10"/>
       <c r="AH122" s="10"/>
       <c r="AI122" s="10"/>
       <c r="AJ122" s="10"/>
-      <c r="AK122" s="9"/>
+      <c r="AK122" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL122" s="9"/>
       <c r="AM122" s="9"/>
       <c r="AN122" s="9"/>
       <c r="AO122" s="9"/>
-      <c r="AP122" s="11"/>
+      <c r="AP122" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ122" s="11"/>
       <c r="AR122" s="11"/>
-      <c r="AS122" s="9"/>
+      <c r="AS122" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT122" s="9"/>
       <c r="AU122" s="9"/>
       <c r="AV122" s="9"/>
@@ -12555,6 +12613,71 @@
       </c>
       <c r="B123" s="8"/>
       <c r="C123" s="5"/>
+      <c r="D123" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="9"/>
+      <c r="J123" s="9"/>
+      <c r="K123" s="9"/>
+      <c r="L123" s="9"/>
+      <c r="M123" s="9"/>
+      <c r="N123" s="9"/>
+      <c r="O123" s="9"/>
+      <c r="P123" s="9"/>
+      <c r="Q123" s="9"/>
+      <c r="R123" s="9"/>
+      <c r="S123" s="9"/>
+      <c r="T123" s="9"/>
+      <c r="U123" s="9"/>
+      <c r="V123" s="9"/>
+      <c r="W123" s="9"/>
+      <c r="X123" s="9"/>
+      <c r="Y123" s="9"/>
+      <c r="Z123" s="9"/>
+      <c r="AA123" s="9"/>
+      <c r="AB123" s="9"/>
+      <c r="AC123" s="9"/>
+      <c r="AD123" s="9"/>
+      <c r="AE123" s="9"/>
+      <c r="AF123" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG123" s="10"/>
+      <c r="AH123" s="10"/>
+      <c r="AI123" s="10"/>
+      <c r="AJ123" s="10"/>
+      <c r="AK123" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL123" s="9"/>
+      <c r="AM123" s="9"/>
+      <c r="AN123" s="9"/>
+      <c r="AO123" s="9"/>
+      <c r="AP123" s="11">
+        <v>1</v>
+      </c>
+      <c r="AQ123" s="11"/>
+      <c r="AR123" s="11"/>
+      <c r="AS123" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT123" s="9"/>
+      <c r="AU123" s="9"/>
+      <c r="AV123" s="9"/>
+      <c r="AW123" s="9"/>
+      <c r="AX123" s="9"/>
+      <c r="AY123" s="9"/>
+      <c r="AZ123" s="9"/>
+      <c r="BA123" s="9"/>
+      <c r="BB123" s="9"/>
+      <c r="BC123" s="9"/>
+      <c r="BD123" s="9"/>
+      <c r="BE123" s="9"/>
+      <c r="BF123" s="9"/>
       <c r="BG123" s="12"/>
       <c r="BH123" s="12"/>
       <c r="BI123" s="12"/>
@@ -12577,8 +12700,1744 @@
       <c r="BZ123" s="12"/>
       <c r="CA123" s="12"/>
     </row>
+    <row r="124" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A124" s="8">
+        <v>123</v>
+      </c>
+      <c r="B124" s="8"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
+      <c r="H124" s="9"/>
+      <c r="I124" s="9"/>
+      <c r="J124" s="9"/>
+      <c r="K124" s="9"/>
+      <c r="L124" s="9"/>
+      <c r="M124" s="9"/>
+      <c r="N124" s="9"/>
+      <c r="O124" s="9"/>
+      <c r="P124" s="9"/>
+      <c r="Q124" s="9"/>
+      <c r="R124" s="9"/>
+      <c r="S124" s="9"/>
+      <c r="T124" s="9"/>
+      <c r="U124" s="9"/>
+      <c r="V124" s="9"/>
+      <c r="W124" s="9"/>
+      <c r="X124" s="9"/>
+      <c r="Y124" s="9"/>
+      <c r="Z124" s="9"/>
+      <c r="AA124" s="9"/>
+      <c r="AB124" s="9"/>
+      <c r="AC124" s="9"/>
+      <c r="AD124" s="9"/>
+      <c r="AE124" s="9"/>
+      <c r="AF124" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG124" s="10"/>
+      <c r="AH124" s="10"/>
+      <c r="AI124" s="10"/>
+      <c r="AJ124" s="10"/>
+      <c r="AK124" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL124" s="9"/>
+      <c r="AM124" s="9"/>
+      <c r="AN124" s="9"/>
+      <c r="AO124" s="9"/>
+      <c r="AP124" s="11">
+        <v>1</v>
+      </c>
+      <c r="AQ124" s="11"/>
+      <c r="AR124" s="11"/>
+      <c r="AS124" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT124" s="9"/>
+      <c r="AU124" s="9"/>
+      <c r="AV124" s="9"/>
+      <c r="AW124" s="9"/>
+      <c r="AX124" s="9"/>
+      <c r="AY124" s="9"/>
+      <c r="AZ124" s="9"/>
+      <c r="BA124" s="9"/>
+      <c r="BB124" s="9"/>
+      <c r="BC124" s="9"/>
+      <c r="BD124" s="9"/>
+      <c r="BE124" s="9"/>
+      <c r="BF124" s="9"/>
+      <c r="BG124" s="12"/>
+      <c r="BH124" s="12"/>
+      <c r="BI124" s="12"/>
+      <c r="BJ124" s="12"/>
+      <c r="BK124" s="12"/>
+      <c r="BL124" s="12"/>
+      <c r="BM124" s="12"/>
+      <c r="BN124" s="12"/>
+      <c r="BO124" s="12"/>
+      <c r="BP124" s="12"/>
+      <c r="BQ124" s="12"/>
+      <c r="BR124" s="12"/>
+      <c r="BS124" s="12"/>
+      <c r="BT124" s="12"/>
+      <c r="BU124" s="12"/>
+      <c r="BV124" s="12"/>
+      <c r="BW124" s="12"/>
+      <c r="BX124" s="12"/>
+      <c r="BY124" s="12"/>
+      <c r="BZ124" s="12"/>
+      <c r="CA124" s="12"/>
+    </row>
+    <row r="125" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A125" s="8">
+        <v>124</v>
+      </c>
+      <c r="B125" s="8"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9"/>
+      <c r="F125" s="9"/>
+      <c r="G125" s="9"/>
+      <c r="H125" s="9"/>
+      <c r="I125" s="9"/>
+      <c r="J125" s="9"/>
+      <c r="K125" s="9"/>
+      <c r="L125" s="9"/>
+      <c r="M125" s="9"/>
+      <c r="N125" s="9"/>
+      <c r="O125" s="9"/>
+      <c r="P125" s="9"/>
+      <c r="Q125" s="9"/>
+      <c r="R125" s="9"/>
+      <c r="S125" s="9"/>
+      <c r="T125" s="9"/>
+      <c r="U125" s="9"/>
+      <c r="V125" s="9"/>
+      <c r="W125" s="9"/>
+      <c r="X125" s="9"/>
+      <c r="Y125" s="9"/>
+      <c r="Z125" s="9"/>
+      <c r="AA125" s="9"/>
+      <c r="AB125" s="9"/>
+      <c r="AC125" s="9"/>
+      <c r="AD125" s="9"/>
+      <c r="AE125" s="9"/>
+      <c r="AF125" s="10"/>
+      <c r="AG125" s="10"/>
+      <c r="AH125" s="10"/>
+      <c r="AI125" s="10"/>
+      <c r="AJ125" s="10"/>
+      <c r="AK125" s="9"/>
+      <c r="AL125" s="9"/>
+      <c r="AM125" s="9"/>
+      <c r="AN125" s="9"/>
+      <c r="AO125" s="9"/>
+      <c r="AP125" s="11"/>
+      <c r="AQ125" s="11"/>
+      <c r="AR125" s="11"/>
+      <c r="AS125" s="9"/>
+      <c r="AT125" s="9"/>
+      <c r="AU125" s="9"/>
+      <c r="AV125" s="9"/>
+      <c r="AW125" s="9"/>
+      <c r="AX125" s="9"/>
+      <c r="AY125" s="9"/>
+      <c r="AZ125" s="9"/>
+      <c r="BA125" s="9"/>
+      <c r="BB125" s="9"/>
+      <c r="BC125" s="9"/>
+      <c r="BD125" s="9"/>
+      <c r="BE125" s="9"/>
+      <c r="BF125" s="9"/>
+      <c r="BG125" s="12"/>
+      <c r="BH125" s="12"/>
+      <c r="BI125" s="12"/>
+      <c r="BJ125" s="12"/>
+      <c r="BK125" s="12"/>
+      <c r="BL125" s="12"/>
+      <c r="BM125" s="12"/>
+      <c r="BN125" s="12"/>
+      <c r="BO125" s="12"/>
+      <c r="BP125" s="12"/>
+      <c r="BQ125" s="12"/>
+      <c r="BR125" s="12"/>
+      <c r="BS125" s="12"/>
+      <c r="BT125" s="12"/>
+      <c r="BU125" s="12"/>
+      <c r="BV125" s="12"/>
+      <c r="BW125" s="12"/>
+      <c r="BX125" s="12"/>
+      <c r="BY125" s="12"/>
+      <c r="BZ125" s="12"/>
+      <c r="CA125" s="12"/>
+    </row>
+    <row r="126" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A126" s="8">
+        <v>124</v>
+      </c>
+      <c r="B126" s="8"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
+      <c r="G126" s="9"/>
+      <c r="H126" s="9"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="9"/>
+      <c r="K126" s="9"/>
+      <c r="L126" s="9"/>
+      <c r="M126" s="9"/>
+      <c r="N126" s="9"/>
+      <c r="O126" s="9"/>
+      <c r="P126" s="9"/>
+      <c r="Q126" s="9"/>
+      <c r="R126" s="9"/>
+      <c r="S126" s="9"/>
+      <c r="T126" s="9"/>
+      <c r="U126" s="9"/>
+      <c r="V126" s="9"/>
+      <c r="W126" s="9"/>
+      <c r="X126" s="9"/>
+      <c r="Y126" s="9"/>
+      <c r="Z126" s="9"/>
+      <c r="AA126" s="9"/>
+      <c r="AB126" s="9"/>
+      <c r="AC126" s="9"/>
+      <c r="AD126" s="9"/>
+      <c r="AE126" s="9"/>
+      <c r="AF126" s="10"/>
+      <c r="AG126" s="10"/>
+      <c r="AH126" s="10"/>
+      <c r="AI126" s="10"/>
+      <c r="AJ126" s="10"/>
+      <c r="AK126" s="9"/>
+      <c r="AL126" s="9"/>
+      <c r="AM126" s="9"/>
+      <c r="AN126" s="9"/>
+      <c r="AO126" s="9"/>
+      <c r="AP126" s="11"/>
+      <c r="AQ126" s="11"/>
+      <c r="AR126" s="11"/>
+      <c r="AS126" s="9"/>
+      <c r="AT126" s="9"/>
+      <c r="AU126" s="9"/>
+      <c r="AV126" s="9"/>
+      <c r="AW126" s="9"/>
+      <c r="AX126" s="9"/>
+      <c r="AY126" s="9"/>
+      <c r="AZ126" s="9"/>
+      <c r="BA126" s="9"/>
+      <c r="BB126" s="9"/>
+      <c r="BC126" s="9"/>
+      <c r="BD126" s="9"/>
+      <c r="BE126" s="9"/>
+      <c r="BF126" s="9"/>
+      <c r="BG126" s="12"/>
+      <c r="BH126" s="12"/>
+      <c r="BI126" s="12"/>
+      <c r="BJ126" s="12"/>
+      <c r="BK126" s="12"/>
+      <c r="BL126" s="12"/>
+      <c r="BM126" s="12"/>
+      <c r="BN126" s="12"/>
+      <c r="BO126" s="12"/>
+      <c r="BP126" s="12"/>
+      <c r="BQ126" s="12"/>
+      <c r="BR126" s="12"/>
+      <c r="BS126" s="12"/>
+      <c r="BT126" s="12"/>
+      <c r="BU126" s="12"/>
+      <c r="BV126" s="12"/>
+      <c r="BW126" s="12"/>
+      <c r="BX126" s="12"/>
+      <c r="BY126" s="12"/>
+      <c r="BZ126" s="12"/>
+      <c r="CA126" s="12"/>
+    </row>
+    <row r="127" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A127" s="8">
+        <v>124</v>
+      </c>
+      <c r="B127" s="8"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="9"/>
+      <c r="H127" s="9"/>
+      <c r="I127" s="9"/>
+      <c r="J127" s="9"/>
+      <c r="K127" s="9"/>
+      <c r="L127" s="9"/>
+      <c r="M127" s="9"/>
+      <c r="N127" s="9"/>
+      <c r="O127" s="9"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="9"/>
+      <c r="R127" s="9"/>
+      <c r="S127" s="9"/>
+      <c r="T127" s="9"/>
+      <c r="U127" s="9"/>
+      <c r="V127" s="9"/>
+      <c r="W127" s="9"/>
+      <c r="X127" s="9"/>
+      <c r="Y127" s="9"/>
+      <c r="Z127" s="9"/>
+      <c r="AA127" s="9"/>
+      <c r="AB127" s="9"/>
+      <c r="AC127" s="9"/>
+      <c r="AD127" s="9"/>
+      <c r="AE127" s="9"/>
+      <c r="AF127" s="10"/>
+      <c r="AG127" s="10"/>
+      <c r="AH127" s="10"/>
+      <c r="AI127" s="10"/>
+      <c r="AJ127" s="10"/>
+      <c r="AK127" s="9"/>
+      <c r="AL127" s="9"/>
+      <c r="AM127" s="9"/>
+      <c r="AN127" s="9"/>
+      <c r="AO127" s="9"/>
+      <c r="AP127" s="11"/>
+      <c r="AQ127" s="11"/>
+      <c r="AR127" s="11"/>
+      <c r="AS127" s="9"/>
+      <c r="AT127" s="9"/>
+      <c r="AU127" s="9"/>
+      <c r="AV127" s="9"/>
+      <c r="AW127" s="9"/>
+      <c r="AX127" s="9"/>
+      <c r="AY127" s="9"/>
+      <c r="AZ127" s="9"/>
+      <c r="BA127" s="9"/>
+      <c r="BB127" s="9"/>
+      <c r="BC127" s="9"/>
+      <c r="BD127" s="9"/>
+      <c r="BE127" s="9"/>
+      <c r="BF127" s="9"/>
+      <c r="BG127" s="12"/>
+      <c r="BH127" s="12"/>
+      <c r="BI127" s="12"/>
+      <c r="BJ127" s="12"/>
+      <c r="BK127" s="12"/>
+      <c r="BL127" s="12"/>
+      <c r="BM127" s="12"/>
+      <c r="BN127" s="12"/>
+      <c r="BO127" s="12"/>
+      <c r="BP127" s="12"/>
+      <c r="BQ127" s="12"/>
+      <c r="BR127" s="12"/>
+      <c r="BS127" s="12"/>
+      <c r="BT127" s="12"/>
+      <c r="BU127" s="12"/>
+      <c r="BV127" s="12"/>
+      <c r="BW127" s="12"/>
+      <c r="BX127" s="12"/>
+      <c r="BY127" s="12"/>
+      <c r="BZ127" s="12"/>
+      <c r="CA127" s="12"/>
+    </row>
+    <row r="128" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A128" s="8">
+        <v>124</v>
+      </c>
+      <c r="B128" s="8"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+      <c r="H128" s="9"/>
+      <c r="I128" s="9"/>
+      <c r="J128" s="9"/>
+      <c r="K128" s="9"/>
+      <c r="L128" s="9"/>
+      <c r="M128" s="9"/>
+      <c r="N128" s="9"/>
+      <c r="O128" s="9"/>
+      <c r="P128" s="9"/>
+      <c r="Q128" s="9"/>
+      <c r="R128" s="9"/>
+      <c r="S128" s="9"/>
+      <c r="T128" s="9"/>
+      <c r="U128" s="9"/>
+      <c r="V128" s="9"/>
+      <c r="W128" s="9"/>
+      <c r="X128" s="9"/>
+      <c r="Y128" s="9"/>
+      <c r="Z128" s="9"/>
+      <c r="AA128" s="9"/>
+      <c r="AB128" s="9"/>
+      <c r="AC128" s="9"/>
+      <c r="AD128" s="9"/>
+      <c r="AE128" s="9"/>
+      <c r="AF128" s="10"/>
+      <c r="AG128" s="10"/>
+      <c r="AH128" s="10"/>
+      <c r="AI128" s="10"/>
+      <c r="AJ128" s="10"/>
+      <c r="AK128" s="9"/>
+      <c r="AL128" s="9"/>
+      <c r="AM128" s="9"/>
+      <c r="AN128" s="9"/>
+      <c r="AO128" s="9"/>
+      <c r="AP128" s="11"/>
+      <c r="AQ128" s="11"/>
+      <c r="AR128" s="11"/>
+      <c r="AS128" s="9"/>
+      <c r="AT128" s="9"/>
+      <c r="AU128" s="9"/>
+      <c r="AV128" s="9"/>
+      <c r="AW128" s="9"/>
+      <c r="AX128" s="9"/>
+      <c r="AY128" s="9"/>
+      <c r="AZ128" s="9"/>
+      <c r="BA128" s="9"/>
+      <c r="BB128" s="9"/>
+      <c r="BC128" s="9"/>
+      <c r="BD128" s="9"/>
+      <c r="BE128" s="9"/>
+      <c r="BF128" s="9"/>
+      <c r="BG128" s="12"/>
+      <c r="BH128" s="12"/>
+      <c r="BI128" s="12"/>
+      <c r="BJ128" s="12"/>
+      <c r="BK128" s="12"/>
+      <c r="BL128" s="12"/>
+      <c r="BM128" s="12"/>
+      <c r="BN128" s="12"/>
+      <c r="BO128" s="12"/>
+      <c r="BP128" s="12"/>
+      <c r="BQ128" s="12"/>
+      <c r="BR128" s="12"/>
+      <c r="BS128" s="12"/>
+      <c r="BT128" s="12"/>
+      <c r="BU128" s="12"/>
+      <c r="BV128" s="12"/>
+      <c r="BW128" s="12"/>
+      <c r="BX128" s="12"/>
+      <c r="BY128" s="12"/>
+      <c r="BZ128" s="12"/>
+      <c r="CA128" s="12"/>
+    </row>
+    <row r="129" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A129" s="8">
+        <v>124</v>
+      </c>
+      <c r="B129" s="8"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9"/>
+      <c r="H129" s="9"/>
+      <c r="I129" s="9"/>
+      <c r="J129" s="9"/>
+      <c r="K129" s="9"/>
+      <c r="L129" s="9"/>
+      <c r="M129" s="9"/>
+      <c r="N129" s="9"/>
+      <c r="O129" s="9"/>
+      <c r="P129" s="9"/>
+      <c r="Q129" s="9"/>
+      <c r="R129" s="9"/>
+      <c r="S129" s="9"/>
+      <c r="T129" s="9"/>
+      <c r="U129" s="9"/>
+      <c r="V129" s="9"/>
+      <c r="W129" s="9"/>
+      <c r="X129" s="9"/>
+      <c r="Y129" s="9"/>
+      <c r="Z129" s="9"/>
+      <c r="AA129" s="9"/>
+      <c r="AB129" s="9"/>
+      <c r="AC129" s="9"/>
+      <c r="AD129" s="9"/>
+      <c r="AE129" s="9"/>
+      <c r="AF129" s="10"/>
+      <c r="AG129" s="10"/>
+      <c r="AH129" s="10"/>
+      <c r="AI129" s="10"/>
+      <c r="AJ129" s="10"/>
+      <c r="AK129" s="9"/>
+      <c r="AL129" s="9"/>
+      <c r="AM129" s="9"/>
+      <c r="AN129" s="9"/>
+      <c r="AO129" s="9"/>
+      <c r="AP129" s="11"/>
+      <c r="AQ129" s="11"/>
+      <c r="AR129" s="11"/>
+      <c r="AS129" s="9"/>
+      <c r="AT129" s="9"/>
+      <c r="AU129" s="9"/>
+      <c r="AV129" s="9"/>
+      <c r="AW129" s="9"/>
+      <c r="AX129" s="9"/>
+      <c r="AY129" s="9"/>
+      <c r="AZ129" s="9"/>
+      <c r="BA129" s="9"/>
+      <c r="BB129" s="9"/>
+      <c r="BC129" s="9"/>
+      <c r="BD129" s="9"/>
+      <c r="BE129" s="9"/>
+      <c r="BF129" s="9"/>
+      <c r="BG129" s="12"/>
+      <c r="BH129" s="12"/>
+      <c r="BI129" s="12"/>
+      <c r="BJ129" s="12"/>
+      <c r="BK129" s="12"/>
+      <c r="BL129" s="12"/>
+      <c r="BM129" s="12"/>
+      <c r="BN129" s="12"/>
+      <c r="BO129" s="12"/>
+      <c r="BP129" s="12"/>
+      <c r="BQ129" s="12"/>
+      <c r="BR129" s="12"/>
+      <c r="BS129" s="12"/>
+      <c r="BT129" s="12"/>
+      <c r="BU129" s="12"/>
+      <c r="BV129" s="12"/>
+      <c r="BW129" s="12"/>
+      <c r="BX129" s="12"/>
+      <c r="BY129" s="12"/>
+      <c r="BZ129" s="12"/>
+      <c r="CA129" s="12"/>
+    </row>
+    <row r="130" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A130" s="8">
+        <v>124</v>
+      </c>
+      <c r="B130" s="8"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="9"/>
+      <c r="H130" s="9"/>
+      <c r="I130" s="9"/>
+      <c r="J130" s="9"/>
+      <c r="K130" s="9"/>
+      <c r="L130" s="9"/>
+      <c r="M130" s="9"/>
+      <c r="N130" s="9"/>
+      <c r="O130" s="9"/>
+      <c r="P130" s="9"/>
+      <c r="Q130" s="9"/>
+      <c r="R130" s="9"/>
+      <c r="S130" s="9"/>
+      <c r="T130" s="9"/>
+      <c r="U130" s="9"/>
+      <c r="V130" s="9"/>
+      <c r="W130" s="9"/>
+      <c r="X130" s="9"/>
+      <c r="Y130" s="9"/>
+      <c r="Z130" s="9"/>
+      <c r="AA130" s="9"/>
+      <c r="AB130" s="9"/>
+      <c r="AC130" s="9"/>
+      <c r="AD130" s="9"/>
+      <c r="AE130" s="9"/>
+      <c r="AF130" s="10"/>
+      <c r="AG130" s="10"/>
+      <c r="AH130" s="10"/>
+      <c r="AI130" s="10"/>
+      <c r="AJ130" s="10"/>
+      <c r="AK130" s="9"/>
+      <c r="AL130" s="9"/>
+      <c r="AM130" s="9"/>
+      <c r="AN130" s="9"/>
+      <c r="AO130" s="9"/>
+      <c r="AP130" s="11"/>
+      <c r="AQ130" s="11"/>
+      <c r="AR130" s="11"/>
+      <c r="AS130" s="9"/>
+      <c r="AT130" s="9"/>
+      <c r="AU130" s="9"/>
+      <c r="AV130" s="9"/>
+      <c r="AW130" s="9"/>
+      <c r="AX130" s="9"/>
+      <c r="AY130" s="9"/>
+      <c r="AZ130" s="9"/>
+      <c r="BA130" s="9"/>
+      <c r="BB130" s="9"/>
+      <c r="BC130" s="9"/>
+      <c r="BD130" s="9"/>
+      <c r="BE130" s="9"/>
+      <c r="BF130" s="9"/>
+      <c r="BG130" s="12"/>
+      <c r="BH130" s="12"/>
+      <c r="BI130" s="12"/>
+      <c r="BJ130" s="12"/>
+      <c r="BK130" s="12"/>
+      <c r="BL130" s="12"/>
+      <c r="BM130" s="12"/>
+      <c r="BN130" s="12"/>
+      <c r="BO130" s="12"/>
+      <c r="BP130" s="12"/>
+      <c r="BQ130" s="12"/>
+      <c r="BR130" s="12"/>
+      <c r="BS130" s="12"/>
+      <c r="BT130" s="12"/>
+      <c r="BU130" s="12"/>
+      <c r="BV130" s="12"/>
+      <c r="BW130" s="12"/>
+      <c r="BX130" s="12"/>
+      <c r="BY130" s="12"/>
+      <c r="BZ130" s="12"/>
+      <c r="CA130" s="12"/>
+    </row>
+    <row r="131" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A131" s="8">
+        <v>124</v>
+      </c>
+      <c r="B131" s="8"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="9"/>
+      <c r="K131" s="9"/>
+      <c r="L131" s="9"/>
+      <c r="M131" s="9"/>
+      <c r="N131" s="9"/>
+      <c r="O131" s="9"/>
+      <c r="P131" s="9"/>
+      <c r="Q131" s="9"/>
+      <c r="R131" s="9"/>
+      <c r="S131" s="9"/>
+      <c r="T131" s="9"/>
+      <c r="U131" s="9"/>
+      <c r="V131" s="9"/>
+      <c r="W131" s="9"/>
+      <c r="X131" s="9"/>
+      <c r="Y131" s="9"/>
+      <c r="Z131" s="9"/>
+      <c r="AA131" s="9"/>
+      <c r="AB131" s="9"/>
+      <c r="AC131" s="9"/>
+      <c r="AD131" s="9"/>
+      <c r="AE131" s="9"/>
+      <c r="AF131" s="10"/>
+      <c r="AG131" s="10"/>
+      <c r="AH131" s="10"/>
+      <c r="AI131" s="10"/>
+      <c r="AJ131" s="10"/>
+      <c r="AK131" s="9"/>
+      <c r="AL131" s="9"/>
+      <c r="AM131" s="9"/>
+      <c r="AN131" s="9"/>
+      <c r="AO131" s="9"/>
+      <c r="AP131" s="11"/>
+      <c r="AQ131" s="11"/>
+      <c r="AR131" s="11"/>
+      <c r="AS131" s="9"/>
+      <c r="AT131" s="9"/>
+      <c r="AU131" s="9"/>
+      <c r="AV131" s="9"/>
+      <c r="AW131" s="9"/>
+      <c r="AX131" s="9"/>
+      <c r="AY131" s="9"/>
+      <c r="AZ131" s="9"/>
+      <c r="BA131" s="9"/>
+      <c r="BB131" s="9"/>
+      <c r="BC131" s="9"/>
+      <c r="BD131" s="9"/>
+      <c r="BE131" s="9"/>
+      <c r="BF131" s="9"/>
+      <c r="BG131" s="12"/>
+      <c r="BH131" s="12"/>
+      <c r="BI131" s="12"/>
+      <c r="BJ131" s="12"/>
+      <c r="BK131" s="12"/>
+      <c r="BL131" s="12"/>
+      <c r="BM131" s="12"/>
+      <c r="BN131" s="12"/>
+      <c r="BO131" s="12"/>
+      <c r="BP131" s="12"/>
+      <c r="BQ131" s="12"/>
+      <c r="BR131" s="12"/>
+      <c r="BS131" s="12"/>
+      <c r="BT131" s="12"/>
+      <c r="BU131" s="12"/>
+      <c r="BV131" s="12"/>
+      <c r="BW131" s="12"/>
+      <c r="BX131" s="12"/>
+      <c r="BY131" s="12"/>
+      <c r="BZ131" s="12"/>
+      <c r="CA131" s="12"/>
+    </row>
+    <row r="132" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A132" s="8">
+        <v>124</v>
+      </c>
+      <c r="B132" s="8"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="9"/>
+      <c r="J132" s="9"/>
+      <c r="K132" s="9"/>
+      <c r="L132" s="9"/>
+      <c r="M132" s="9"/>
+      <c r="N132" s="9"/>
+      <c r="O132" s="9"/>
+      <c r="P132" s="9"/>
+      <c r="Q132" s="9"/>
+      <c r="R132" s="9"/>
+      <c r="S132" s="9"/>
+      <c r="T132" s="9"/>
+      <c r="U132" s="9"/>
+      <c r="V132" s="9"/>
+      <c r="W132" s="9"/>
+      <c r="X132" s="9"/>
+      <c r="Y132" s="9"/>
+      <c r="Z132" s="9"/>
+      <c r="AA132" s="9"/>
+      <c r="AB132" s="9"/>
+      <c r="AC132" s="9"/>
+      <c r="AD132" s="9"/>
+      <c r="AE132" s="9"/>
+      <c r="AF132" s="10"/>
+      <c r="AG132" s="10"/>
+      <c r="AH132" s="10"/>
+      <c r="AI132" s="10"/>
+      <c r="AJ132" s="10"/>
+      <c r="AK132" s="9"/>
+      <c r="AL132" s="9"/>
+      <c r="AM132" s="9"/>
+      <c r="AN132" s="9"/>
+      <c r="AO132" s="9"/>
+      <c r="AP132" s="11"/>
+      <c r="AQ132" s="11"/>
+      <c r="AR132" s="11"/>
+      <c r="AS132" s="9"/>
+      <c r="AT132" s="9"/>
+      <c r="AU132" s="9"/>
+      <c r="AV132" s="9"/>
+      <c r="AW132" s="9"/>
+      <c r="AX132" s="9"/>
+      <c r="AY132" s="9"/>
+      <c r="AZ132" s="9"/>
+      <c r="BA132" s="9"/>
+      <c r="BB132" s="9"/>
+      <c r="BC132" s="9"/>
+      <c r="BD132" s="9"/>
+      <c r="BE132" s="9"/>
+      <c r="BF132" s="9"/>
+      <c r="BG132" s="12"/>
+      <c r="BH132" s="12"/>
+      <c r="BI132" s="12"/>
+      <c r="BJ132" s="12"/>
+      <c r="BK132" s="12"/>
+      <c r="BL132" s="12"/>
+      <c r="BM132" s="12"/>
+      <c r="BN132" s="12"/>
+      <c r="BO132" s="12"/>
+      <c r="BP132" s="12"/>
+      <c r="BQ132" s="12"/>
+      <c r="BR132" s="12"/>
+      <c r="BS132" s="12"/>
+      <c r="BT132" s="12"/>
+      <c r="BU132" s="12"/>
+      <c r="BV132" s="12"/>
+      <c r="BW132" s="12"/>
+      <c r="BX132" s="12"/>
+      <c r="BY132" s="12"/>
+      <c r="BZ132" s="12"/>
+      <c r="CA132" s="12"/>
+    </row>
+    <row r="133" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A133" s="8">
+        <v>124</v>
+      </c>
+      <c r="B133" s="8"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="9"/>
+      <c r="K133" s="9"/>
+      <c r="L133" s="9"/>
+      <c r="M133" s="9"/>
+      <c r="N133" s="9"/>
+      <c r="O133" s="9"/>
+      <c r="P133" s="9"/>
+      <c r="Q133" s="9"/>
+      <c r="R133" s="9"/>
+      <c r="S133" s="9"/>
+      <c r="T133" s="9"/>
+      <c r="U133" s="9"/>
+      <c r="V133" s="9"/>
+      <c r="W133" s="9"/>
+      <c r="X133" s="9"/>
+      <c r="Y133" s="9"/>
+      <c r="Z133" s="9"/>
+      <c r="AA133" s="9"/>
+      <c r="AB133" s="9"/>
+      <c r="AC133" s="9"/>
+      <c r="AD133" s="9"/>
+      <c r="AE133" s="9"/>
+      <c r="AF133" s="10"/>
+      <c r="AG133" s="10"/>
+      <c r="AH133" s="10"/>
+      <c r="AI133" s="10"/>
+      <c r="AJ133" s="10"/>
+      <c r="AK133" s="9"/>
+      <c r="AL133" s="9"/>
+      <c r="AM133" s="9"/>
+      <c r="AN133" s="9"/>
+      <c r="AO133" s="9"/>
+      <c r="AP133" s="11"/>
+      <c r="AQ133" s="11"/>
+      <c r="AR133" s="11"/>
+      <c r="AS133" s="9"/>
+      <c r="AT133" s="9"/>
+      <c r="AU133" s="9"/>
+      <c r="AV133" s="9"/>
+      <c r="AW133" s="9"/>
+      <c r="AX133" s="9"/>
+      <c r="AY133" s="9"/>
+      <c r="AZ133" s="9"/>
+      <c r="BA133" s="9"/>
+      <c r="BB133" s="9"/>
+      <c r="BC133" s="9"/>
+      <c r="BD133" s="9"/>
+      <c r="BE133" s="9"/>
+      <c r="BF133" s="9"/>
+      <c r="BG133" s="12"/>
+      <c r="BH133" s="12"/>
+      <c r="BI133" s="12"/>
+      <c r="BJ133" s="12"/>
+      <c r="BK133" s="12"/>
+      <c r="BL133" s="12"/>
+      <c r="BM133" s="12"/>
+      <c r="BN133" s="12"/>
+      <c r="BO133" s="12"/>
+      <c r="BP133" s="12"/>
+      <c r="BQ133" s="12"/>
+      <c r="BR133" s="12"/>
+      <c r="BS133" s="12"/>
+      <c r="BT133" s="12"/>
+      <c r="BU133" s="12"/>
+      <c r="BV133" s="12"/>
+      <c r="BW133" s="12"/>
+      <c r="BX133" s="12"/>
+      <c r="BY133" s="12"/>
+      <c r="BZ133" s="12"/>
+      <c r="CA133" s="12"/>
+    </row>
+    <row r="134" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A134" s="8">
+        <v>124</v>
+      </c>
+      <c r="B134" s="8"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="9"/>
+      <c r="K134" s="9"/>
+      <c r="L134" s="9"/>
+      <c r="M134" s="9"/>
+      <c r="N134" s="9"/>
+      <c r="O134" s="9"/>
+      <c r="P134" s="9"/>
+      <c r="Q134" s="9"/>
+      <c r="R134" s="9"/>
+      <c r="S134" s="9"/>
+      <c r="T134" s="9"/>
+      <c r="U134" s="9"/>
+      <c r="V134" s="9"/>
+      <c r="W134" s="9"/>
+      <c r="X134" s="9"/>
+      <c r="Y134" s="9"/>
+      <c r="Z134" s="9"/>
+      <c r="AA134" s="9"/>
+      <c r="AB134" s="9"/>
+      <c r="AC134" s="9"/>
+      <c r="AD134" s="9"/>
+      <c r="AE134" s="9"/>
+      <c r="AF134" s="10"/>
+      <c r="AG134" s="10"/>
+      <c r="AH134" s="10"/>
+      <c r="AI134" s="10"/>
+      <c r="AJ134" s="10"/>
+      <c r="AK134" s="9"/>
+      <c r="AL134" s="9"/>
+      <c r="AM134" s="9"/>
+      <c r="AN134" s="9"/>
+      <c r="AO134" s="9"/>
+      <c r="AP134" s="11"/>
+      <c r="AQ134" s="11"/>
+      <c r="AR134" s="11"/>
+      <c r="AS134" s="9"/>
+      <c r="AT134" s="9"/>
+      <c r="AU134" s="9"/>
+      <c r="AV134" s="9"/>
+      <c r="AW134" s="9"/>
+      <c r="AX134" s="9"/>
+      <c r="AY134" s="9"/>
+      <c r="AZ134" s="9"/>
+      <c r="BA134" s="9"/>
+      <c r="BB134" s="9"/>
+      <c r="BC134" s="9"/>
+      <c r="BD134" s="9"/>
+      <c r="BE134" s="9"/>
+      <c r="BF134" s="9"/>
+      <c r="BG134" s="12"/>
+      <c r="BH134" s="12"/>
+      <c r="BI134" s="12"/>
+      <c r="BJ134" s="12"/>
+      <c r="BK134" s="12"/>
+      <c r="BL134" s="12"/>
+      <c r="BM134" s="12"/>
+      <c r="BN134" s="12"/>
+      <c r="BO134" s="12"/>
+      <c r="BP134" s="12"/>
+      <c r="BQ134" s="12"/>
+      <c r="BR134" s="12"/>
+      <c r="BS134" s="12"/>
+      <c r="BT134" s="12"/>
+      <c r="BU134" s="12"/>
+      <c r="BV134" s="12"/>
+      <c r="BW134" s="12"/>
+      <c r="BX134" s="12"/>
+      <c r="BY134" s="12"/>
+      <c r="BZ134" s="12"/>
+      <c r="CA134" s="12"/>
+    </row>
+    <row r="135" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A135" s="8">
+        <v>124</v>
+      </c>
+      <c r="B135" s="8"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="9"/>
+      <c r="K135" s="9"/>
+      <c r="L135" s="9"/>
+      <c r="M135" s="9"/>
+      <c r="N135" s="9"/>
+      <c r="O135" s="9"/>
+      <c r="P135" s="9"/>
+      <c r="Q135" s="9"/>
+      <c r="R135" s="9"/>
+      <c r="S135" s="9"/>
+      <c r="T135" s="9"/>
+      <c r="U135" s="9"/>
+      <c r="V135" s="9"/>
+      <c r="W135" s="9"/>
+      <c r="X135" s="9"/>
+      <c r="Y135" s="9"/>
+      <c r="Z135" s="9"/>
+      <c r="AA135" s="9"/>
+      <c r="AB135" s="9"/>
+      <c r="AC135" s="9"/>
+      <c r="AD135" s="9"/>
+      <c r="AE135" s="9"/>
+      <c r="AF135" s="10"/>
+      <c r="AG135" s="10"/>
+      <c r="AH135" s="10"/>
+      <c r="AI135" s="10"/>
+      <c r="AJ135" s="10"/>
+      <c r="AK135" s="9"/>
+      <c r="AL135" s="9"/>
+      <c r="AM135" s="9"/>
+      <c r="AN135" s="9"/>
+      <c r="AO135" s="9"/>
+      <c r="AP135" s="11"/>
+      <c r="AQ135" s="11"/>
+      <c r="AR135" s="11"/>
+      <c r="AS135" s="9"/>
+      <c r="AT135" s="9"/>
+      <c r="AU135" s="9"/>
+      <c r="AV135" s="9"/>
+      <c r="AW135" s="9"/>
+      <c r="AX135" s="9"/>
+      <c r="AY135" s="9"/>
+      <c r="AZ135" s="9"/>
+      <c r="BA135" s="9"/>
+      <c r="BB135" s="9"/>
+      <c r="BC135" s="9"/>
+      <c r="BD135" s="9"/>
+      <c r="BE135" s="9"/>
+      <c r="BF135" s="9"/>
+      <c r="BG135" s="12"/>
+      <c r="BH135" s="12"/>
+      <c r="BI135" s="12"/>
+      <c r="BJ135" s="12"/>
+      <c r="BK135" s="12"/>
+      <c r="BL135" s="12"/>
+      <c r="BM135" s="12"/>
+      <c r="BN135" s="12"/>
+      <c r="BO135" s="12"/>
+      <c r="BP135" s="12"/>
+      <c r="BQ135" s="12"/>
+      <c r="BR135" s="12"/>
+      <c r="BS135" s="12"/>
+      <c r="BT135" s="12"/>
+      <c r="BU135" s="12"/>
+      <c r="BV135" s="12"/>
+      <c r="BW135" s="12"/>
+      <c r="BX135" s="12"/>
+      <c r="BY135" s="12"/>
+      <c r="BZ135" s="12"/>
+      <c r="CA135" s="12"/>
+    </row>
+    <row r="136" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A136" s="8">
+        <v>124</v>
+      </c>
+      <c r="B136" s="8"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+      <c r="H136" s="9"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="9"/>
+      <c r="K136" s="9"/>
+      <c r="L136" s="9"/>
+      <c r="M136" s="9"/>
+      <c r="N136" s="9"/>
+      <c r="O136" s="9"/>
+      <c r="P136" s="9"/>
+      <c r="Q136" s="9"/>
+      <c r="R136" s="9"/>
+      <c r="S136" s="9"/>
+      <c r="T136" s="9"/>
+      <c r="U136" s="9"/>
+      <c r="V136" s="9"/>
+      <c r="W136" s="9"/>
+      <c r="X136" s="9"/>
+      <c r="Y136" s="9"/>
+      <c r="Z136" s="9"/>
+      <c r="AA136" s="9"/>
+      <c r="AB136" s="9"/>
+      <c r="AC136" s="9"/>
+      <c r="AD136" s="9"/>
+      <c r="AE136" s="9"/>
+      <c r="AF136" s="10"/>
+      <c r="AG136" s="10"/>
+      <c r="AH136" s="10"/>
+      <c r="AI136" s="10"/>
+      <c r="AJ136" s="10"/>
+      <c r="AK136" s="9"/>
+      <c r="AL136" s="9"/>
+      <c r="AM136" s="9"/>
+      <c r="AN136" s="9"/>
+      <c r="AO136" s="9"/>
+      <c r="AP136" s="11"/>
+      <c r="AQ136" s="11"/>
+      <c r="AR136" s="11"/>
+      <c r="AS136" s="9"/>
+      <c r="AT136" s="9"/>
+      <c r="AU136" s="9"/>
+      <c r="AV136" s="9"/>
+      <c r="AW136" s="9"/>
+      <c r="AX136" s="9"/>
+      <c r="AY136" s="9"/>
+      <c r="AZ136" s="9"/>
+      <c r="BA136" s="9"/>
+      <c r="BB136" s="9"/>
+      <c r="BC136" s="9"/>
+      <c r="BD136" s="9"/>
+      <c r="BE136" s="9"/>
+      <c r="BF136" s="9"/>
+      <c r="BG136" s="12"/>
+      <c r="BH136" s="12"/>
+      <c r="BI136" s="12"/>
+      <c r="BJ136" s="12"/>
+      <c r="BK136" s="12"/>
+      <c r="BL136" s="12"/>
+      <c r="BM136" s="12"/>
+      <c r="BN136" s="12"/>
+      <c r="BO136" s="12"/>
+      <c r="BP136" s="12"/>
+      <c r="BQ136" s="12"/>
+      <c r="BR136" s="12"/>
+      <c r="BS136" s="12"/>
+      <c r="BT136" s="12"/>
+      <c r="BU136" s="12"/>
+      <c r="BV136" s="12"/>
+      <c r="BW136" s="12"/>
+      <c r="BX136" s="12"/>
+      <c r="BY136" s="12"/>
+      <c r="BZ136" s="12"/>
+      <c r="CA136" s="12"/>
+    </row>
+    <row r="137" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A137" s="8">
+        <v>124</v>
+      </c>
+      <c r="B137" s="8"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+      <c r="H137" s="9"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="9"/>
+      <c r="K137" s="9"/>
+      <c r="L137" s="9"/>
+      <c r="M137" s="9"/>
+      <c r="N137" s="9"/>
+      <c r="O137" s="9"/>
+      <c r="P137" s="9"/>
+      <c r="Q137" s="9"/>
+      <c r="R137" s="9"/>
+      <c r="S137" s="9"/>
+      <c r="T137" s="9"/>
+      <c r="U137" s="9"/>
+      <c r="V137" s="9"/>
+      <c r="W137" s="9"/>
+      <c r="X137" s="9"/>
+      <c r="Y137" s="9"/>
+      <c r="Z137" s="9"/>
+      <c r="AA137" s="9"/>
+      <c r="AB137" s="9"/>
+      <c r="AC137" s="9"/>
+      <c r="AD137" s="9"/>
+      <c r="AE137" s="9"/>
+      <c r="AF137" s="10"/>
+      <c r="AG137" s="10"/>
+      <c r="AH137" s="10"/>
+      <c r="AI137" s="10"/>
+      <c r="AJ137" s="10"/>
+      <c r="AK137" s="9"/>
+      <c r="AL137" s="9"/>
+      <c r="AM137" s="9"/>
+      <c r="AN137" s="9"/>
+      <c r="AO137" s="9"/>
+      <c r="AP137" s="11"/>
+      <c r="AQ137" s="11"/>
+      <c r="AR137" s="11"/>
+      <c r="AS137" s="9"/>
+      <c r="AT137" s="9"/>
+      <c r="AU137" s="9"/>
+      <c r="AV137" s="9"/>
+      <c r="AW137" s="9"/>
+      <c r="AX137" s="9"/>
+      <c r="AY137" s="9"/>
+      <c r="AZ137" s="9"/>
+      <c r="BA137" s="9"/>
+      <c r="BB137" s="9"/>
+      <c r="BC137" s="9"/>
+      <c r="BD137" s="9"/>
+      <c r="BE137" s="9"/>
+      <c r="BF137" s="9"/>
+      <c r="BG137" s="12"/>
+      <c r="BH137" s="12"/>
+      <c r="BI137" s="12"/>
+      <c r="BJ137" s="12"/>
+      <c r="BK137" s="12"/>
+      <c r="BL137" s="12"/>
+      <c r="BM137" s="12"/>
+      <c r="BN137" s="12"/>
+      <c r="BO137" s="12"/>
+      <c r="BP137" s="12"/>
+      <c r="BQ137" s="12"/>
+      <c r="BR137" s="12"/>
+      <c r="BS137" s="12"/>
+      <c r="BT137" s="12"/>
+      <c r="BU137" s="12"/>
+      <c r="BV137" s="12"/>
+      <c r="BW137" s="12"/>
+      <c r="BX137" s="12"/>
+      <c r="BY137" s="12"/>
+      <c r="BZ137" s="12"/>
+      <c r="CA137" s="12"/>
+    </row>
+    <row r="138" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A138" s="8">
+        <v>124</v>
+      </c>
+      <c r="B138" s="8"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="9"/>
+      <c r="H138" s="9"/>
+      <c r="I138" s="9"/>
+      <c r="J138" s="9"/>
+      <c r="K138" s="9"/>
+      <c r="L138" s="9"/>
+      <c r="M138" s="9"/>
+      <c r="N138" s="9"/>
+      <c r="O138" s="9"/>
+      <c r="P138" s="9"/>
+      <c r="Q138" s="9"/>
+      <c r="R138" s="9"/>
+      <c r="S138" s="9"/>
+      <c r="T138" s="9"/>
+      <c r="U138" s="9"/>
+      <c r="V138" s="9"/>
+      <c r="W138" s="9"/>
+      <c r="X138" s="9"/>
+      <c r="Y138" s="9"/>
+      <c r="Z138" s="9"/>
+      <c r="AA138" s="9"/>
+      <c r="AB138" s="9"/>
+      <c r="AC138" s="9"/>
+      <c r="AD138" s="9"/>
+      <c r="AE138" s="9"/>
+      <c r="AF138" s="10"/>
+      <c r="AG138" s="10"/>
+      <c r="AH138" s="10"/>
+      <c r="AI138" s="10"/>
+      <c r="AJ138" s="10"/>
+      <c r="AK138" s="9"/>
+      <c r="AL138" s="9"/>
+      <c r="AM138" s="9"/>
+      <c r="AN138" s="9"/>
+      <c r="AO138" s="9"/>
+      <c r="AP138" s="11"/>
+      <c r="AQ138" s="11"/>
+      <c r="AR138" s="11"/>
+      <c r="AS138" s="9"/>
+      <c r="AT138" s="9"/>
+      <c r="AU138" s="9"/>
+      <c r="AV138" s="9"/>
+      <c r="AW138" s="9"/>
+      <c r="AX138" s="9"/>
+      <c r="AY138" s="9"/>
+      <c r="AZ138" s="9"/>
+      <c r="BA138" s="9"/>
+      <c r="BB138" s="9"/>
+      <c r="BC138" s="9"/>
+      <c r="BD138" s="9"/>
+      <c r="BE138" s="9"/>
+      <c r="BF138" s="9"/>
+      <c r="BG138" s="12"/>
+      <c r="BH138" s="12"/>
+      <c r="BI138" s="12"/>
+      <c r="BJ138" s="12"/>
+      <c r="BK138" s="12"/>
+      <c r="BL138" s="12"/>
+      <c r="BM138" s="12"/>
+      <c r="BN138" s="12"/>
+      <c r="BO138" s="12"/>
+      <c r="BP138" s="12"/>
+      <c r="BQ138" s="12"/>
+      <c r="BR138" s="12"/>
+      <c r="BS138" s="12"/>
+      <c r="BT138" s="12"/>
+      <c r="BU138" s="12"/>
+      <c r="BV138" s="12"/>
+      <c r="BW138" s="12"/>
+      <c r="BX138" s="12"/>
+      <c r="BY138" s="12"/>
+      <c r="BZ138" s="12"/>
+      <c r="CA138" s="12"/>
+    </row>
+    <row r="139" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A139" s="8">
+        <v>124</v>
+      </c>
+      <c r="B139" s="8"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
+      <c r="H139" s="9"/>
+      <c r="I139" s="9"/>
+      <c r="J139" s="9"/>
+      <c r="K139" s="9"/>
+      <c r="L139" s="9"/>
+      <c r="M139" s="9"/>
+      <c r="N139" s="9"/>
+      <c r="O139" s="9"/>
+      <c r="P139" s="9"/>
+      <c r="Q139" s="9"/>
+      <c r="R139" s="9"/>
+      <c r="S139" s="9"/>
+      <c r="T139" s="9"/>
+      <c r="U139" s="9"/>
+      <c r="V139" s="9"/>
+      <c r="W139" s="9"/>
+      <c r="X139" s="9"/>
+      <c r="Y139" s="9"/>
+      <c r="Z139" s="9"/>
+      <c r="AA139" s="9"/>
+      <c r="AB139" s="9"/>
+      <c r="AC139" s="9"/>
+      <c r="AD139" s="9"/>
+      <c r="AE139" s="9"/>
+      <c r="AF139" s="10"/>
+      <c r="AG139" s="10"/>
+      <c r="AH139" s="10"/>
+      <c r="AI139" s="10"/>
+      <c r="AJ139" s="10"/>
+      <c r="AK139" s="9"/>
+      <c r="AL139" s="9"/>
+      <c r="AM139" s="9"/>
+      <c r="AN139" s="9"/>
+      <c r="AO139" s="9"/>
+      <c r="AP139" s="11"/>
+      <c r="AQ139" s="11"/>
+      <c r="AR139" s="11"/>
+      <c r="AS139" s="9"/>
+      <c r="AT139" s="9"/>
+      <c r="AU139" s="9"/>
+      <c r="AV139" s="9"/>
+      <c r="AW139" s="9"/>
+      <c r="AX139" s="9"/>
+      <c r="AY139" s="9"/>
+      <c r="AZ139" s="9"/>
+      <c r="BA139" s="9"/>
+      <c r="BB139" s="9"/>
+      <c r="BC139" s="9"/>
+      <c r="BD139" s="9"/>
+      <c r="BE139" s="9"/>
+      <c r="BF139" s="9"/>
+      <c r="BG139" s="12"/>
+      <c r="BH139" s="12"/>
+      <c r="BI139" s="12"/>
+      <c r="BJ139" s="12"/>
+      <c r="BK139" s="12"/>
+      <c r="BL139" s="12"/>
+      <c r="BM139" s="12"/>
+      <c r="BN139" s="12"/>
+      <c r="BO139" s="12"/>
+      <c r="BP139" s="12"/>
+      <c r="BQ139" s="12"/>
+      <c r="BR139" s="12"/>
+      <c r="BS139" s="12"/>
+      <c r="BT139" s="12"/>
+      <c r="BU139" s="12"/>
+      <c r="BV139" s="12"/>
+      <c r="BW139" s="12"/>
+      <c r="BX139" s="12"/>
+      <c r="BY139" s="12"/>
+      <c r="BZ139" s="12"/>
+      <c r="CA139" s="12"/>
+    </row>
+    <row r="140" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A140" s="8">
+        <v>124</v>
+      </c>
+      <c r="B140" s="8"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="9"/>
+      <c r="J140" s="9"/>
+      <c r="K140" s="9"/>
+      <c r="L140" s="9"/>
+      <c r="M140" s="9"/>
+      <c r="N140" s="9"/>
+      <c r="O140" s="9"/>
+      <c r="P140" s="9"/>
+      <c r="Q140" s="9"/>
+      <c r="R140" s="9"/>
+      <c r="S140" s="9"/>
+      <c r="T140" s="9"/>
+      <c r="U140" s="9"/>
+      <c r="V140" s="9"/>
+      <c r="W140" s="9"/>
+      <c r="X140" s="9"/>
+      <c r="Y140" s="9"/>
+      <c r="Z140" s="9"/>
+      <c r="AA140" s="9"/>
+      <c r="AB140" s="9"/>
+      <c r="AC140" s="9"/>
+      <c r="AD140" s="9"/>
+      <c r="AE140" s="9"/>
+      <c r="AF140" s="10"/>
+      <c r="AG140" s="10"/>
+      <c r="AH140" s="10"/>
+      <c r="AI140" s="10"/>
+      <c r="AJ140" s="10"/>
+      <c r="AK140" s="9"/>
+      <c r="AL140" s="9"/>
+      <c r="AM140" s="9"/>
+      <c r="AN140" s="9"/>
+      <c r="AO140" s="9"/>
+      <c r="AP140" s="11"/>
+      <c r="AQ140" s="11"/>
+      <c r="AR140" s="11"/>
+      <c r="AS140" s="9"/>
+      <c r="AT140" s="9"/>
+      <c r="AU140" s="9"/>
+      <c r="AV140" s="9"/>
+      <c r="AW140" s="9"/>
+      <c r="AX140" s="9"/>
+      <c r="AY140" s="9"/>
+      <c r="AZ140" s="9"/>
+      <c r="BA140" s="9"/>
+      <c r="BB140" s="9"/>
+      <c r="BC140" s="9"/>
+      <c r="BD140" s="9"/>
+      <c r="BE140" s="9"/>
+      <c r="BF140" s="9"/>
+      <c r="BG140" s="12"/>
+      <c r="BH140" s="12"/>
+      <c r="BI140" s="12"/>
+      <c r="BJ140" s="12"/>
+      <c r="BK140" s="12"/>
+      <c r="BL140" s="12"/>
+      <c r="BM140" s="12"/>
+      <c r="BN140" s="12"/>
+      <c r="BO140" s="12"/>
+      <c r="BP140" s="12"/>
+      <c r="BQ140" s="12"/>
+      <c r="BR140" s="12"/>
+      <c r="BS140" s="12"/>
+      <c r="BT140" s="12"/>
+      <c r="BU140" s="12"/>
+      <c r="BV140" s="12"/>
+      <c r="BW140" s="12"/>
+      <c r="BX140" s="12"/>
+      <c r="BY140" s="12"/>
+      <c r="BZ140" s="12"/>
+      <c r="CA140" s="12"/>
+    </row>
+    <row r="141" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A141" s="8">
+        <v>124</v>
+      </c>
+      <c r="B141" s="8"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
+      <c r="I141" s="9"/>
+      <c r="J141" s="9"/>
+      <c r="K141" s="9"/>
+      <c r="L141" s="9"/>
+      <c r="M141" s="9"/>
+      <c r="N141" s="9"/>
+      <c r="O141" s="9"/>
+      <c r="P141" s="9"/>
+      <c r="Q141" s="9"/>
+      <c r="R141" s="9"/>
+      <c r="S141" s="9"/>
+      <c r="T141" s="9"/>
+      <c r="U141" s="9"/>
+      <c r="V141" s="9"/>
+      <c r="W141" s="9"/>
+      <c r="X141" s="9"/>
+      <c r="Y141" s="9"/>
+      <c r="Z141" s="9"/>
+      <c r="AA141" s="9"/>
+      <c r="AB141" s="9"/>
+      <c r="AC141" s="9"/>
+      <c r="AD141" s="9"/>
+      <c r="AE141" s="9"/>
+      <c r="AF141" s="10"/>
+      <c r="AG141" s="10"/>
+      <c r="AH141" s="10"/>
+      <c r="AI141" s="10"/>
+      <c r="AJ141" s="10"/>
+      <c r="AK141" s="9"/>
+      <c r="AL141" s="9"/>
+      <c r="AM141" s="9"/>
+      <c r="AN141" s="9"/>
+      <c r="AO141" s="9"/>
+      <c r="AP141" s="11"/>
+      <c r="AQ141" s="11"/>
+      <c r="AR141" s="11"/>
+      <c r="AS141" s="9"/>
+      <c r="AT141" s="9"/>
+      <c r="AU141" s="9"/>
+      <c r="AV141" s="9"/>
+      <c r="AW141" s="9"/>
+      <c r="AX141" s="9"/>
+      <c r="AY141" s="9"/>
+      <c r="AZ141" s="9"/>
+      <c r="BA141" s="9"/>
+      <c r="BB141" s="9"/>
+      <c r="BC141" s="9"/>
+      <c r="BD141" s="9"/>
+      <c r="BE141" s="9"/>
+      <c r="BF141" s="9"/>
+      <c r="BG141" s="12"/>
+      <c r="BH141" s="12"/>
+      <c r="BI141" s="12"/>
+      <c r="BJ141" s="12"/>
+      <c r="BK141" s="12"/>
+      <c r="BL141" s="12"/>
+      <c r="BM141" s="12"/>
+      <c r="BN141" s="12"/>
+      <c r="BO141" s="12"/>
+      <c r="BP141" s="12"/>
+      <c r="BQ141" s="12"/>
+      <c r="BR141" s="12"/>
+      <c r="BS141" s="12"/>
+      <c r="BT141" s="12"/>
+      <c r="BU141" s="12"/>
+      <c r="BV141" s="12"/>
+      <c r="BW141" s="12"/>
+      <c r="BX141" s="12"/>
+      <c r="BY141" s="12"/>
+      <c r="BZ141" s="12"/>
+      <c r="CA141" s="12"/>
+    </row>
+    <row r="142" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A142" s="8">
+        <v>124</v>
+      </c>
+      <c r="B142" s="8"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="9"/>
+      <c r="H142" s="9"/>
+      <c r="I142" s="9"/>
+      <c r="J142" s="9"/>
+      <c r="K142" s="9"/>
+      <c r="L142" s="9"/>
+      <c r="M142" s="9"/>
+      <c r="N142" s="9"/>
+      <c r="O142" s="9"/>
+      <c r="P142" s="9"/>
+      <c r="Q142" s="9"/>
+      <c r="R142" s="9"/>
+      <c r="S142" s="9"/>
+      <c r="T142" s="9"/>
+      <c r="U142" s="9"/>
+      <c r="V142" s="9"/>
+      <c r="W142" s="9"/>
+      <c r="X142" s="9"/>
+      <c r="Y142" s="9"/>
+      <c r="Z142" s="9"/>
+      <c r="AA142" s="9"/>
+      <c r="AB142" s="9"/>
+      <c r="AC142" s="9"/>
+      <c r="AD142" s="9"/>
+      <c r="AE142" s="9"/>
+      <c r="AF142" s="10"/>
+      <c r="AG142" s="10"/>
+      <c r="AH142" s="10"/>
+      <c r="AI142" s="10"/>
+      <c r="AJ142" s="10"/>
+      <c r="AK142" s="9"/>
+      <c r="AL142" s="9"/>
+      <c r="AM142" s="9"/>
+      <c r="AN142" s="9"/>
+      <c r="AO142" s="9"/>
+      <c r="AP142" s="11"/>
+      <c r="AQ142" s="11"/>
+      <c r="AR142" s="11"/>
+      <c r="AS142" s="9"/>
+      <c r="AT142" s="9"/>
+      <c r="AU142" s="9"/>
+      <c r="AV142" s="9"/>
+      <c r="AW142" s="9"/>
+      <c r="AX142" s="9"/>
+      <c r="AY142" s="9"/>
+      <c r="AZ142" s="9"/>
+      <c r="BA142" s="9"/>
+      <c r="BB142" s="9"/>
+      <c r="BC142" s="9"/>
+      <c r="BD142" s="9"/>
+      <c r="BE142" s="9"/>
+      <c r="BF142" s="9"/>
+      <c r="BG142" s="12"/>
+      <c r="BH142" s="12"/>
+      <c r="BI142" s="12"/>
+      <c r="BJ142" s="12"/>
+      <c r="BK142" s="12"/>
+      <c r="BL142" s="12"/>
+      <c r="BM142" s="12"/>
+      <c r="BN142" s="12"/>
+      <c r="BO142" s="12"/>
+      <c r="BP142" s="12"/>
+      <c r="BQ142" s="12"/>
+      <c r="BR142" s="12"/>
+      <c r="BS142" s="12"/>
+      <c r="BT142" s="12"/>
+      <c r="BU142" s="12"/>
+      <c r="BV142" s="12"/>
+      <c r="BW142" s="12"/>
+      <c r="BX142" s="12"/>
+      <c r="BY142" s="12"/>
+      <c r="BZ142" s="12"/>
+      <c r="CA142" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="856">
+  <mergeCells count="994">
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="D142:AE142"/>
+    <mergeCell ref="AF142:AJ142"/>
+    <mergeCell ref="AK142:AO142"/>
+    <mergeCell ref="AP142:AR142"/>
+    <mergeCell ref="AS142:BF142"/>
+    <mergeCell ref="BG142:CA142"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="D140:AE140"/>
+    <mergeCell ref="AF140:AJ140"/>
+    <mergeCell ref="AK140:AO140"/>
+    <mergeCell ref="AP140:AR140"/>
+    <mergeCell ref="AS140:BF140"/>
+    <mergeCell ref="BG140:CA140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="D141:AE141"/>
+    <mergeCell ref="AF141:AJ141"/>
+    <mergeCell ref="AK141:AO141"/>
+    <mergeCell ref="AP141:AR141"/>
+    <mergeCell ref="AS141:BF141"/>
+    <mergeCell ref="BG141:CA141"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="D138:AE138"/>
+    <mergeCell ref="AF138:AJ138"/>
+    <mergeCell ref="AK138:AO138"/>
+    <mergeCell ref="AP138:AR138"/>
+    <mergeCell ref="AS138:BF138"/>
+    <mergeCell ref="BG138:CA138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="D139:AE139"/>
+    <mergeCell ref="AF139:AJ139"/>
+    <mergeCell ref="AK139:AO139"/>
+    <mergeCell ref="AP139:AR139"/>
+    <mergeCell ref="AS139:BF139"/>
+    <mergeCell ref="BG139:CA139"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="D136:AE136"/>
+    <mergeCell ref="AF136:AJ136"/>
+    <mergeCell ref="AK136:AO136"/>
+    <mergeCell ref="AP136:AR136"/>
+    <mergeCell ref="AS136:BF136"/>
+    <mergeCell ref="BG136:CA136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="D137:AE137"/>
+    <mergeCell ref="AF137:AJ137"/>
+    <mergeCell ref="AK137:AO137"/>
+    <mergeCell ref="AP137:AR137"/>
+    <mergeCell ref="AS137:BF137"/>
+    <mergeCell ref="BG137:CA137"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="D134:AE134"/>
+    <mergeCell ref="AF134:AJ134"/>
+    <mergeCell ref="AK134:AO134"/>
+    <mergeCell ref="AP134:AR134"/>
+    <mergeCell ref="AS134:BF134"/>
+    <mergeCell ref="BG134:CA134"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="D135:AE135"/>
+    <mergeCell ref="AF135:AJ135"/>
+    <mergeCell ref="AK135:AO135"/>
+    <mergeCell ref="AP135:AR135"/>
+    <mergeCell ref="AS135:BF135"/>
+    <mergeCell ref="BG135:CA135"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="D132:AE132"/>
+    <mergeCell ref="AF132:AJ132"/>
+    <mergeCell ref="AK132:AO132"/>
+    <mergeCell ref="AP132:AR132"/>
+    <mergeCell ref="AS132:BF132"/>
+    <mergeCell ref="BG132:CA132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="D133:AE133"/>
+    <mergeCell ref="AF133:AJ133"/>
+    <mergeCell ref="AK133:AO133"/>
+    <mergeCell ref="AP133:AR133"/>
+    <mergeCell ref="AS133:BF133"/>
+    <mergeCell ref="BG133:CA133"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="D130:AE130"/>
+    <mergeCell ref="AF130:AJ130"/>
+    <mergeCell ref="AK130:AO130"/>
+    <mergeCell ref="AP130:AR130"/>
+    <mergeCell ref="AS130:BF130"/>
+    <mergeCell ref="BG130:CA130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="D131:AE131"/>
+    <mergeCell ref="AF131:AJ131"/>
+    <mergeCell ref="AK131:AO131"/>
+    <mergeCell ref="AP131:AR131"/>
+    <mergeCell ref="AS131:BF131"/>
+    <mergeCell ref="BG131:CA131"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="D128:AE128"/>
+    <mergeCell ref="AF128:AJ128"/>
+    <mergeCell ref="AK128:AO128"/>
+    <mergeCell ref="AP128:AR128"/>
+    <mergeCell ref="AS128:BF128"/>
+    <mergeCell ref="BG128:CA128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="D129:AE129"/>
+    <mergeCell ref="AF129:AJ129"/>
+    <mergeCell ref="AK129:AO129"/>
+    <mergeCell ref="AP129:AR129"/>
+    <mergeCell ref="AS129:BF129"/>
+    <mergeCell ref="BG129:CA129"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="D126:AE126"/>
+    <mergeCell ref="AF126:AJ126"/>
+    <mergeCell ref="AK126:AO126"/>
+    <mergeCell ref="AP126:AR126"/>
+    <mergeCell ref="AS126:BF126"/>
+    <mergeCell ref="BG126:CA126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="D127:AE127"/>
+    <mergeCell ref="AF127:AJ127"/>
+    <mergeCell ref="AK127:AO127"/>
+    <mergeCell ref="AP127:AR127"/>
+    <mergeCell ref="AS127:BF127"/>
+    <mergeCell ref="BG127:CA127"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="D124:AE124"/>
+    <mergeCell ref="AF124:AJ124"/>
+    <mergeCell ref="AK124:AO124"/>
+    <mergeCell ref="AP124:AR124"/>
+    <mergeCell ref="AS124:BF124"/>
+    <mergeCell ref="BG124:CA124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="D125:AE125"/>
+    <mergeCell ref="AF125:AJ125"/>
+    <mergeCell ref="AK125:AO125"/>
+    <mergeCell ref="AP125:AR125"/>
+    <mergeCell ref="AS125:BF125"/>
+    <mergeCell ref="BG125:CA125"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="BG121:CA121"/>
     <mergeCell ref="A122:B122"/>
     <mergeCell ref="D121:AE121"/>
     <mergeCell ref="AF121:AJ121"/>
@@ -12586,27 +14445,6 @@
     <mergeCell ref="AP121:AR121"/>
     <mergeCell ref="AS121:BF121"/>
     <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG121:CA121"/>
     <mergeCell ref="A118:B118"/>
     <mergeCell ref="D117:AE117"/>
     <mergeCell ref="AF117:AJ117"/>
@@ -12615,12 +14453,22 @@
     <mergeCell ref="AS117:BF117"/>
     <mergeCell ref="BG118:CA118"/>
     <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="D119:AE119"/>
     <mergeCell ref="D118:AE118"/>
     <mergeCell ref="AF118:AJ118"/>
     <mergeCell ref="AK118:AO118"/>
     <mergeCell ref="AP118:AR118"/>
     <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="BG119:CA119"/>
     <mergeCell ref="A116:B116"/>
     <mergeCell ref="D115:AE115"/>
     <mergeCell ref="AF115:AJ115"/>
@@ -13437,7 +15285,7 @@
     <mergeCell ref="BG72:CA72"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C123">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C142">
       <formula1>"!,?"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13456,7 +15304,7 @@
           <x14:formula1>
             <xm:f>Info!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>AK2:AO122</xm:sqref>
+          <xm:sqref>AK2:AO142</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -13465,7 +15313,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>AS2:BF122</xm:sqref>
+          <xm:sqref>AS2:BF142</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
báo cáo ngày 20/2/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="146">
   <si>
     <t>No.</t>
   </si>
@@ -433,13 +433,31 @@
     <t>19/2/2019</t>
   </si>
   <si>
-    <t>Trang tạo mới  -Thực hiện đồng bộ  -  delete data - Tạo câu lệnh sql để delete bảng server đích</t>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data - Tạo câu lệnh sql để delete bảng server đích</t>
   </si>
   <si>
-    <t>Trang tạo mới  -Thực hiện đồng bộ  -  delete data - Sửa lỗi chính tả khi thêm vào db đích</t>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  update data - Sửa lỗi chính tả khi thêm vào db đích</t>
   </si>
   <si>
-    <t>Trang tạo mới  -Thực hiện đồng bộ  -  delete data - Sửa lỗi back up dữ liệu khi sửa dữ liệu</t>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  update - Sửa lỗi back up dữ liệu khi sửa dữ liệu</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  delete - Gộp update và delete vào thành 1</t>
+  </si>
+  <si>
+    <t>20/2/2019</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  Sửa lỗi chữ khi lưu vào file csv không đọc được</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  Sửa lại đường dẫn lưu file import và backup</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  Khi gặp lỗi thì thực hiện xóa lịch sử đồng bộ và xóa file import hoặc backup đã lưu</t>
+  </si>
+  <si>
+    <t>Trang tạo mới  -Thực hiện đồng bộ  -  insertdata - Chỉ insert khi dữ liệu chưa có ở bảng đích</t>
   </si>
 </sst>
 </file>
@@ -711,11 +729,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,12 +754,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,7 +864,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1237,7 +1255,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1249,7 +1267,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D127" sqref="D127:AE127"/>
+      <selection pane="bottomLeft" activeCell="AP131" sqref="AP131:AR131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,99 +1282,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="24" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="23" t="s">
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="25" t="s">
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="23" t="s">
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="23"/>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
-      <c r="BF1" s="23"/>
-      <c r="BG1" s="26" t="s">
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="24"/>
+      <c r="BB1" s="24"/>
+      <c r="BC1" s="24"/>
+      <c r="BD1" s="24"/>
+      <c r="BE1" s="24"/>
+      <c r="BF1" s="24"/>
+      <c r="BG1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="26"/>
-      <c r="BI1" s="26"/>
-      <c r="BJ1" s="26"/>
-      <c r="BK1" s="26"/>
-      <c r="BL1" s="26"/>
-      <c r="BM1" s="26"/>
-      <c r="BN1" s="26"/>
-      <c r="BO1" s="26"/>
-      <c r="BP1" s="26"/>
-      <c r="BQ1" s="26"/>
-      <c r="BR1" s="26"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="26"/>
-      <c r="BU1" s="26"/>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="26"/>
-      <c r="BZ1" s="26"/>
-      <c r="CA1" s="26"/>
+      <c r="BH1" s="27"/>
+      <c r="BI1" s="27"/>
+      <c r="BJ1" s="27"/>
+      <c r="BK1" s="27"/>
+      <c r="BL1" s="27"/>
+      <c r="BM1" s="27"/>
+      <c r="BN1" s="27"/>
+      <c r="BO1" s="27"/>
+      <c r="BP1" s="27"/>
+      <c r="BQ1" s="27"/>
+      <c r="BR1" s="27"/>
+      <c r="BS1" s="27"/>
+      <c r="BT1" s="27"/>
+      <c r="BU1" s="27"/>
+      <c r="BV1" s="27"/>
+      <c r="BW1" s="27"/>
+      <c r="BX1" s="27"/>
+      <c r="BY1" s="27"/>
+      <c r="BZ1" s="27"/>
+      <c r="CA1" s="27"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
@@ -1364,92 +1382,92 @@
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="28" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="27" t="s">
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="29">
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="30">
         <v>1</v>
       </c>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AQ2" s="30"/>
+      <c r="AR2" s="30"/>
+      <c r="AS2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
-      <c r="AX2" s="27"/>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="27"/>
-      <c r="BG2" s="30"/>
-      <c r="BH2" s="30"/>
-      <c r="BI2" s="30"/>
-      <c r="BJ2" s="30"/>
-      <c r="BK2" s="30"/>
-      <c r="BL2" s="30"/>
-      <c r="BM2" s="30"/>
-      <c r="BN2" s="30"/>
-      <c r="BO2" s="30"/>
-      <c r="BP2" s="30"/>
-      <c r="BQ2" s="30"/>
-      <c r="BR2" s="30"/>
-      <c r="BS2" s="30"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="30"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="30"/>
-      <c r="BY2" s="30"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="30"/>
+      <c r="AT2" s="28"/>
+      <c r="AU2" s="28"/>
+      <c r="AV2" s="28"/>
+      <c r="AW2" s="28"/>
+      <c r="AX2" s="28"/>
+      <c r="AY2" s="28"/>
+      <c r="AZ2" s="28"/>
+      <c r="BA2" s="28"/>
+      <c r="BB2" s="28"/>
+      <c r="BC2" s="28"/>
+      <c r="BD2" s="28"/>
+      <c r="BE2" s="28"/>
+      <c r="BF2" s="28"/>
+      <c r="BG2" s="31"/>
+      <c r="BH2" s="31"/>
+      <c r="BI2" s="31"/>
+      <c r="BJ2" s="31"/>
+      <c r="BK2" s="31"/>
+      <c r="BL2" s="31"/>
+      <c r="BM2" s="31"/>
+      <c r="BN2" s="31"/>
+      <c r="BO2" s="31"/>
+      <c r="BP2" s="31"/>
+      <c r="BQ2" s="31"/>
+      <c r="BR2" s="31"/>
+      <c r="BS2" s="31"/>
+      <c r="BT2" s="31"/>
+      <c r="BU2" s="31"/>
+      <c r="BV2" s="31"/>
+      <c r="BW2" s="31"/>
+      <c r="BX2" s="31"/>
+      <c r="BY2" s="31"/>
+      <c r="BZ2" s="31"/>
+      <c r="CA2" s="31"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4170,43 +4188,43 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="19"/>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="19"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
-      <c r="AD32" s="19"/>
-      <c r="AE32" s="19"/>
-      <c r="AF32" s="20">
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
+      <c r="W32" s="32"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="32"/>
+      <c r="AA32" s="32"/>
+      <c r="AB32" s="32"/>
+      <c r="AC32" s="32"/>
+      <c r="AD32" s="32"/>
+      <c r="AE32" s="32"/>
+      <c r="AF32" s="33">
         <v>43293</v>
       </c>
-      <c r="AG32" s="20"/>
-      <c r="AH32" s="20"/>
-      <c r="AI32" s="20"/>
-      <c r="AJ32" s="20"/>
+      <c r="AG32" s="33"/>
+      <c r="AH32" s="33"/>
+      <c r="AI32" s="33"/>
+      <c r="AJ32" s="33"/>
       <c r="AK32" s="9" t="s">
         <v>16</v>
       </c>
@@ -4235,27 +4253,27 @@
       <c r="BD32" s="9"/>
       <c r="BE32" s="9"/>
       <c r="BF32" s="9"/>
-      <c r="BG32" s="21"/>
-      <c r="BH32" s="21"/>
-      <c r="BI32" s="21"/>
-      <c r="BJ32" s="21"/>
-      <c r="BK32" s="21"/>
-      <c r="BL32" s="21"/>
-      <c r="BM32" s="21"/>
-      <c r="BN32" s="21"/>
-      <c r="BO32" s="21"/>
-      <c r="BP32" s="21"/>
-      <c r="BQ32" s="21"/>
-      <c r="BR32" s="21"/>
-      <c r="BS32" s="21"/>
-      <c r="BT32" s="21"/>
-      <c r="BU32" s="21"/>
-      <c r="BV32" s="21"/>
-      <c r="BW32" s="21"/>
-      <c r="BX32" s="21"/>
-      <c r="BY32" s="21"/>
-      <c r="BZ32" s="21"/>
-      <c r="CA32" s="21"/>
+      <c r="BG32" s="34"/>
+      <c r="BH32" s="34"/>
+      <c r="BI32" s="34"/>
+      <c r="BJ32" s="34"/>
+      <c r="BK32" s="34"/>
+      <c r="BL32" s="34"/>
+      <c r="BM32" s="34"/>
+      <c r="BN32" s="34"/>
+      <c r="BO32" s="34"/>
+      <c r="BP32" s="34"/>
+      <c r="BQ32" s="34"/>
+      <c r="BR32" s="34"/>
+      <c r="BS32" s="34"/>
+      <c r="BT32" s="34"/>
+      <c r="BU32" s="34"/>
+      <c r="BV32" s="34"/>
+      <c r="BW32" s="34"/>
+      <c r="BX32" s="34"/>
+      <c r="BY32" s="34"/>
+      <c r="BZ32" s="34"/>
+      <c r="CA32" s="34"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
@@ -4307,27 +4325,27 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
-      <c r="AP33" s="17">
+      <c r="AP33" s="35">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="17"/>
-      <c r="AR33" s="17"/>
-      <c r="AS33" s="18" t="s">
+      <c r="AQ33" s="35"/>
+      <c r="AR33" s="35"/>
+      <c r="AS33" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="18"/>
-      <c r="AU33" s="18"/>
-      <c r="AV33" s="18"/>
-      <c r="AW33" s="18"/>
-      <c r="AX33" s="18"/>
-      <c r="AY33" s="18"/>
-      <c r="AZ33" s="18"/>
-      <c r="BA33" s="18"/>
-      <c r="BB33" s="18"/>
-      <c r="BC33" s="18"/>
-      <c r="BD33" s="18"/>
-      <c r="BE33" s="18"/>
-      <c r="BF33" s="18"/>
+      <c r="AT33" s="36"/>
+      <c r="AU33" s="36"/>
+      <c r="AV33" s="36"/>
+      <c r="AW33" s="36"/>
+      <c r="AX33" s="36"/>
+      <c r="AY33" s="36"/>
+      <c r="AZ33" s="36"/>
+      <c r="BA33" s="36"/>
+      <c r="BB33" s="36"/>
+      <c r="BC33" s="36"/>
+      <c r="BD33" s="36"/>
+      <c r="BE33" s="36"/>
+      <c r="BF33" s="36"/>
       <c r="BG33" s="12"/>
       <c r="BH33" s="12"/>
       <c r="BI33" s="12"/>
@@ -12271,13 +12289,13 @@
       <c r="AC119" s="15"/>
       <c r="AD119" s="15"/>
       <c r="AE119" s="16"/>
-      <c r="AF119" s="34" t="s">
+      <c r="AF119" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="AG119" s="35"/>
-      <c r="AH119" s="35"/>
-      <c r="AI119" s="35"/>
-      <c r="AJ119" s="36"/>
+      <c r="AG119" s="21"/>
+      <c r="AH119" s="21"/>
+      <c r="AI119" s="21"/>
+      <c r="AJ119" s="22"/>
       <c r="AK119" s="14" t="s">
         <v>16</v>
       </c>
@@ -12285,11 +12303,11 @@
       <c r="AM119" s="15"/>
       <c r="AN119" s="15"/>
       <c r="AO119" s="16"/>
-      <c r="AP119" s="31">
+      <c r="AP119" s="17">
         <v>1</v>
       </c>
-      <c r="AQ119" s="32"/>
-      <c r="AR119" s="33"/>
+      <c r="AQ119" s="18"/>
+      <c r="AR119" s="19"/>
       <c r="AS119" s="14" t="s">
         <v>8</v>
       </c>
@@ -12427,9 +12445,7 @@
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="5"/>
-      <c r="D121" s="9" t="s">
-        <v>137</v>
-      </c>
+      <c r="D121" s="9"/>
       <c r="E121" s="9"/>
       <c r="F121" s="9"/>
       <c r="G121" s="9"/>
@@ -12457,28 +12473,20 @@
       <c r="AC121" s="9"/>
       <c r="AD121" s="9"/>
       <c r="AE121" s="9"/>
-      <c r="AF121" s="10" t="s">
-        <v>136</v>
-      </c>
+      <c r="AF121" s="10"/>
       <c r="AG121" s="10"/>
       <c r="AH121" s="10"/>
       <c r="AI121" s="10"/>
       <c r="AJ121" s="10"/>
-      <c r="AK121" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="AK121" s="9"/>
       <c r="AL121" s="9"/>
       <c r="AM121" s="9"/>
       <c r="AN121" s="9"/>
       <c r="AO121" s="9"/>
-      <c r="AP121" s="11">
-        <v>1</v>
-      </c>
+      <c r="AP121" s="11"/>
       <c r="AQ121" s="11"/>
       <c r="AR121" s="11"/>
-      <c r="AS121" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="AS121" s="9"/>
       <c r="AT121" s="9"/>
       <c r="AU121" s="9"/>
       <c r="AV121" s="9"/>
@@ -12882,7 +12890,9 @@
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="5"/>
-      <c r="D126" s="9"/>
+      <c r="D126" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="E126" s="9"/>
       <c r="F126" s="9"/>
       <c r="G126" s="9"/>
@@ -12910,20 +12920,28 @@
       <c r="AC126" s="9"/>
       <c r="AD126" s="9"/>
       <c r="AE126" s="9"/>
-      <c r="AF126" s="10"/>
+      <c r="AF126" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="AG126" s="10"/>
       <c r="AH126" s="10"/>
       <c r="AI126" s="10"/>
       <c r="AJ126" s="10"/>
-      <c r="AK126" s="9"/>
+      <c r="AK126" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL126" s="9"/>
       <c r="AM126" s="9"/>
       <c r="AN126" s="9"/>
       <c r="AO126" s="9"/>
-      <c r="AP126" s="11"/>
+      <c r="AP126" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ126" s="11"/>
       <c r="AR126" s="11"/>
-      <c r="AS126" s="9"/>
+      <c r="AS126" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT126" s="9"/>
       <c r="AU126" s="9"/>
       <c r="AV126" s="9"/>
@@ -12965,7 +12983,9 @@
       </c>
       <c r="B127" s="8"/>
       <c r="C127" s="5"/>
-      <c r="D127" s="9"/>
+      <c r="D127" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="E127" s="9"/>
       <c r="F127" s="9"/>
       <c r="G127" s="9"/>
@@ -12993,20 +13013,28 @@
       <c r="AC127" s="9"/>
       <c r="AD127" s="9"/>
       <c r="AE127" s="9"/>
-      <c r="AF127" s="10"/>
+      <c r="AF127" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="AG127" s="10"/>
       <c r="AH127" s="10"/>
       <c r="AI127" s="10"/>
       <c r="AJ127" s="10"/>
-      <c r="AK127" s="9"/>
+      <c r="AK127" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL127" s="9"/>
       <c r="AM127" s="9"/>
       <c r="AN127" s="9"/>
       <c r="AO127" s="9"/>
-      <c r="AP127" s="11"/>
+      <c r="AP127" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ127" s="11"/>
       <c r="AR127" s="11"/>
-      <c r="AS127" s="9"/>
+      <c r="AS127" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT127" s="9"/>
       <c r="AU127" s="9"/>
       <c r="AV127" s="9"/>
@@ -13048,7 +13076,9 @@
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="5"/>
-      <c r="D128" s="9"/>
+      <c r="D128" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="E128" s="9"/>
       <c r="F128" s="9"/>
       <c r="G128" s="9"/>
@@ -13076,20 +13106,28 @@
       <c r="AC128" s="9"/>
       <c r="AD128" s="9"/>
       <c r="AE128" s="9"/>
-      <c r="AF128" s="10"/>
+      <c r="AF128" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="AG128" s="10"/>
       <c r="AH128" s="10"/>
       <c r="AI128" s="10"/>
       <c r="AJ128" s="10"/>
-      <c r="AK128" s="9"/>
+      <c r="AK128" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL128" s="9"/>
       <c r="AM128" s="9"/>
       <c r="AN128" s="9"/>
       <c r="AO128" s="9"/>
-      <c r="AP128" s="11"/>
+      <c r="AP128" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ128" s="11"/>
       <c r="AR128" s="11"/>
-      <c r="AS128" s="9"/>
+      <c r="AS128" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT128" s="9"/>
       <c r="AU128" s="9"/>
       <c r="AV128" s="9"/>
@@ -13131,7 +13169,9 @@
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="5"/>
-      <c r="D129" s="9"/>
+      <c r="D129" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="E129" s="9"/>
       <c r="F129" s="9"/>
       <c r="G129" s="9"/>
@@ -13159,20 +13199,28 @@
       <c r="AC129" s="9"/>
       <c r="AD129" s="9"/>
       <c r="AE129" s="9"/>
-      <c r="AF129" s="10"/>
+      <c r="AF129" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="AG129" s="10"/>
       <c r="AH129" s="10"/>
       <c r="AI129" s="10"/>
       <c r="AJ129" s="10"/>
-      <c r="AK129" s="9"/>
+      <c r="AK129" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL129" s="9"/>
       <c r="AM129" s="9"/>
       <c r="AN129" s="9"/>
       <c r="AO129" s="9"/>
-      <c r="AP129" s="11"/>
+      <c r="AP129" s="11">
+        <v>1</v>
+      </c>
       <c r="AQ129" s="11"/>
       <c r="AR129" s="11"/>
-      <c r="AS129" s="9"/>
+      <c r="AS129" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT129" s="9"/>
       <c r="AU129" s="9"/>
       <c r="AV129" s="9"/>
@@ -13214,7 +13262,9 @@
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="5"/>
-      <c r="D130" s="9"/>
+      <c r="D130" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="E130" s="9"/>
       <c r="F130" s="9"/>
       <c r="G130" s="9"/>
@@ -13242,20 +13292,28 @@
       <c r="AC130" s="9"/>
       <c r="AD130" s="9"/>
       <c r="AE130" s="9"/>
-      <c r="AF130" s="10"/>
+      <c r="AF130" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="AG130" s="10"/>
       <c r="AH130" s="10"/>
       <c r="AI130" s="10"/>
       <c r="AJ130" s="10"/>
-      <c r="AK130" s="9"/>
+      <c r="AK130" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="AL130" s="9"/>
       <c r="AM130" s="9"/>
       <c r="AN130" s="9"/>
       <c r="AO130" s="9"/>
-      <c r="AP130" s="11"/>
+      <c r="AP130" s="11">
+        <v>0.5</v>
+      </c>
       <c r="AQ130" s="11"/>
       <c r="AR130" s="11"/>
-      <c r="AS130" s="9"/>
+      <c r="AS130" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="AT130" s="9"/>
       <c r="AU130" s="9"/>
       <c r="AV130" s="9"/>
@@ -14289,162 +14347,820 @@
     </row>
   </sheetData>
   <mergeCells count="994">
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="D142:AE142"/>
-    <mergeCell ref="AF142:AJ142"/>
-    <mergeCell ref="AK142:AO142"/>
-    <mergeCell ref="AP142:AR142"/>
-    <mergeCell ref="AS142:BF142"/>
-    <mergeCell ref="BG142:CA142"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="D140:AE140"/>
-    <mergeCell ref="AF140:AJ140"/>
-    <mergeCell ref="AK140:AO140"/>
-    <mergeCell ref="AP140:AR140"/>
-    <mergeCell ref="AS140:BF140"/>
-    <mergeCell ref="BG140:CA140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="D141:AE141"/>
-    <mergeCell ref="AF141:AJ141"/>
-    <mergeCell ref="AK141:AO141"/>
-    <mergeCell ref="AP141:AR141"/>
-    <mergeCell ref="AS141:BF141"/>
-    <mergeCell ref="BG141:CA141"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="D138:AE138"/>
-    <mergeCell ref="AF138:AJ138"/>
-    <mergeCell ref="AK138:AO138"/>
-    <mergeCell ref="AP138:AR138"/>
-    <mergeCell ref="AS138:BF138"/>
-    <mergeCell ref="BG138:CA138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="D139:AE139"/>
-    <mergeCell ref="AF139:AJ139"/>
-    <mergeCell ref="AK139:AO139"/>
-    <mergeCell ref="AP139:AR139"/>
-    <mergeCell ref="AS139:BF139"/>
-    <mergeCell ref="BG139:CA139"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="D136:AE136"/>
-    <mergeCell ref="AF136:AJ136"/>
-    <mergeCell ref="AK136:AO136"/>
-    <mergeCell ref="AP136:AR136"/>
-    <mergeCell ref="AS136:BF136"/>
-    <mergeCell ref="BG136:CA136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="D137:AE137"/>
-    <mergeCell ref="AF137:AJ137"/>
-    <mergeCell ref="AK137:AO137"/>
-    <mergeCell ref="AP137:AR137"/>
-    <mergeCell ref="AS137:BF137"/>
-    <mergeCell ref="BG137:CA137"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="D134:AE134"/>
-    <mergeCell ref="AF134:AJ134"/>
-    <mergeCell ref="AK134:AO134"/>
-    <mergeCell ref="AP134:AR134"/>
-    <mergeCell ref="AS134:BF134"/>
-    <mergeCell ref="BG134:CA134"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="D135:AE135"/>
-    <mergeCell ref="AF135:AJ135"/>
-    <mergeCell ref="AK135:AO135"/>
-    <mergeCell ref="AP135:AR135"/>
-    <mergeCell ref="AS135:BF135"/>
-    <mergeCell ref="BG135:CA135"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="D132:AE132"/>
-    <mergeCell ref="AF132:AJ132"/>
-    <mergeCell ref="AK132:AO132"/>
-    <mergeCell ref="AP132:AR132"/>
-    <mergeCell ref="AS132:BF132"/>
-    <mergeCell ref="BG132:CA132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="D133:AE133"/>
-    <mergeCell ref="AF133:AJ133"/>
-    <mergeCell ref="AK133:AO133"/>
-    <mergeCell ref="AP133:AR133"/>
-    <mergeCell ref="AS133:BF133"/>
-    <mergeCell ref="BG133:CA133"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="D130:AE130"/>
-    <mergeCell ref="AF130:AJ130"/>
-    <mergeCell ref="AK130:AO130"/>
-    <mergeCell ref="AP130:AR130"/>
-    <mergeCell ref="AS130:BF130"/>
-    <mergeCell ref="BG130:CA130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="D131:AE131"/>
-    <mergeCell ref="AF131:AJ131"/>
-    <mergeCell ref="AK131:AO131"/>
-    <mergeCell ref="AP131:AR131"/>
-    <mergeCell ref="AS131:BF131"/>
-    <mergeCell ref="BG131:CA131"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="D128:AE128"/>
-    <mergeCell ref="AF128:AJ128"/>
-    <mergeCell ref="AK128:AO128"/>
-    <mergeCell ref="AP128:AR128"/>
-    <mergeCell ref="AS128:BF128"/>
-    <mergeCell ref="BG128:CA128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="D129:AE129"/>
-    <mergeCell ref="AF129:AJ129"/>
-    <mergeCell ref="AK129:AO129"/>
-    <mergeCell ref="AP129:AR129"/>
-    <mergeCell ref="AS129:BF129"/>
-    <mergeCell ref="BG129:CA129"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="D126:AE126"/>
-    <mergeCell ref="AF126:AJ126"/>
-    <mergeCell ref="AK126:AO126"/>
-    <mergeCell ref="AP126:AR126"/>
-    <mergeCell ref="AS126:BF126"/>
-    <mergeCell ref="BG126:CA126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="D127:AE127"/>
-    <mergeCell ref="AF127:AJ127"/>
-    <mergeCell ref="AK127:AO127"/>
-    <mergeCell ref="AP127:AR127"/>
-    <mergeCell ref="AS127:BF127"/>
-    <mergeCell ref="BG127:CA127"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="D124:AE124"/>
-    <mergeCell ref="AF124:AJ124"/>
-    <mergeCell ref="AK124:AO124"/>
-    <mergeCell ref="AP124:AR124"/>
-    <mergeCell ref="AS124:BF124"/>
-    <mergeCell ref="BG124:CA124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="D125:AE125"/>
-    <mergeCell ref="AF125:AJ125"/>
-    <mergeCell ref="AK125:AO125"/>
-    <mergeCell ref="AP125:AR125"/>
-    <mergeCell ref="AS125:BF125"/>
-    <mergeCell ref="BG125:CA125"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:AE70"/>
+    <mergeCell ref="AF70:AJ70"/>
+    <mergeCell ref="AK70:AO70"/>
+    <mergeCell ref="AP70:AR70"/>
+    <mergeCell ref="AS70:BF70"/>
+    <mergeCell ref="BG70:CA70"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AR1"/>
+    <mergeCell ref="AS1:BF1"/>
+    <mergeCell ref="BG1:CA1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:AE2"/>
+    <mergeCell ref="AF2:AJ2"/>
+    <mergeCell ref="AK2:AO2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AS2:BF2"/>
+    <mergeCell ref="BG2:CA2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG117:CA117"/>
     <mergeCell ref="A118:B118"/>
     <mergeCell ref="D117:AE117"/>
     <mergeCell ref="AF117:AJ117"/>
@@ -14469,820 +15185,162 @@
     <mergeCell ref="AK118:AO118"/>
     <mergeCell ref="AP118:AR118"/>
     <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:AE70"/>
-    <mergeCell ref="AF70:AJ70"/>
-    <mergeCell ref="AK70:AO70"/>
-    <mergeCell ref="AP70:AR70"/>
-    <mergeCell ref="AS70:BF70"/>
-    <mergeCell ref="BG70:CA70"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:AE1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AR1"/>
-    <mergeCell ref="AS1:BF1"/>
-    <mergeCell ref="BG1:CA1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:AE2"/>
-    <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AS2:BF2"/>
-    <mergeCell ref="BG2:CA2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:AE3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="D124:AE124"/>
+    <mergeCell ref="AF124:AJ124"/>
+    <mergeCell ref="AK124:AO124"/>
+    <mergeCell ref="AP124:AR124"/>
+    <mergeCell ref="AS124:BF124"/>
+    <mergeCell ref="BG124:CA124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="D125:AE125"/>
+    <mergeCell ref="AF125:AJ125"/>
+    <mergeCell ref="AK125:AO125"/>
+    <mergeCell ref="AP125:AR125"/>
+    <mergeCell ref="AS125:BF125"/>
+    <mergeCell ref="BG125:CA125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="D126:AE126"/>
+    <mergeCell ref="AF126:AJ126"/>
+    <mergeCell ref="AK126:AO126"/>
+    <mergeCell ref="AP126:AR126"/>
+    <mergeCell ref="AS126:BF126"/>
+    <mergeCell ref="BG126:CA126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="D127:AE127"/>
+    <mergeCell ref="AF127:AJ127"/>
+    <mergeCell ref="AK127:AO127"/>
+    <mergeCell ref="AP127:AR127"/>
+    <mergeCell ref="AS127:BF127"/>
+    <mergeCell ref="BG127:CA127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="D128:AE128"/>
+    <mergeCell ref="AF128:AJ128"/>
+    <mergeCell ref="AK128:AO128"/>
+    <mergeCell ref="AP128:AR128"/>
+    <mergeCell ref="AS128:BF128"/>
+    <mergeCell ref="BG128:CA128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="D129:AE129"/>
+    <mergeCell ref="AF129:AJ129"/>
+    <mergeCell ref="AK129:AO129"/>
+    <mergeCell ref="AP129:AR129"/>
+    <mergeCell ref="AS129:BF129"/>
+    <mergeCell ref="BG129:CA129"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="D130:AE130"/>
+    <mergeCell ref="AF130:AJ130"/>
+    <mergeCell ref="AK130:AO130"/>
+    <mergeCell ref="AP130:AR130"/>
+    <mergeCell ref="AS130:BF130"/>
+    <mergeCell ref="BG130:CA130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="D131:AE131"/>
+    <mergeCell ref="AF131:AJ131"/>
+    <mergeCell ref="AK131:AO131"/>
+    <mergeCell ref="AP131:AR131"/>
+    <mergeCell ref="AS131:BF131"/>
+    <mergeCell ref="BG131:CA131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="D132:AE132"/>
+    <mergeCell ref="AF132:AJ132"/>
+    <mergeCell ref="AK132:AO132"/>
+    <mergeCell ref="AP132:AR132"/>
+    <mergeCell ref="AS132:BF132"/>
+    <mergeCell ref="BG132:CA132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="D133:AE133"/>
+    <mergeCell ref="AF133:AJ133"/>
+    <mergeCell ref="AK133:AO133"/>
+    <mergeCell ref="AP133:AR133"/>
+    <mergeCell ref="AS133:BF133"/>
+    <mergeCell ref="BG133:CA133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="D134:AE134"/>
+    <mergeCell ref="AF134:AJ134"/>
+    <mergeCell ref="AK134:AO134"/>
+    <mergeCell ref="AP134:AR134"/>
+    <mergeCell ref="AS134:BF134"/>
+    <mergeCell ref="BG134:CA134"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="D135:AE135"/>
+    <mergeCell ref="AF135:AJ135"/>
+    <mergeCell ref="AK135:AO135"/>
+    <mergeCell ref="AP135:AR135"/>
+    <mergeCell ref="AS135:BF135"/>
+    <mergeCell ref="BG135:CA135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="D136:AE136"/>
+    <mergeCell ref="AF136:AJ136"/>
+    <mergeCell ref="AK136:AO136"/>
+    <mergeCell ref="AP136:AR136"/>
+    <mergeCell ref="AS136:BF136"/>
+    <mergeCell ref="BG136:CA136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="D137:AE137"/>
+    <mergeCell ref="AF137:AJ137"/>
+    <mergeCell ref="AK137:AO137"/>
+    <mergeCell ref="AP137:AR137"/>
+    <mergeCell ref="AS137:BF137"/>
+    <mergeCell ref="BG137:CA137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="D138:AE138"/>
+    <mergeCell ref="AF138:AJ138"/>
+    <mergeCell ref="AK138:AO138"/>
+    <mergeCell ref="AP138:AR138"/>
+    <mergeCell ref="AS138:BF138"/>
+    <mergeCell ref="BG138:CA138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="D139:AE139"/>
+    <mergeCell ref="AF139:AJ139"/>
+    <mergeCell ref="AK139:AO139"/>
+    <mergeCell ref="AP139:AR139"/>
+    <mergeCell ref="AS139:BF139"/>
+    <mergeCell ref="BG139:CA139"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="D142:AE142"/>
+    <mergeCell ref="AF142:AJ142"/>
+    <mergeCell ref="AK142:AO142"/>
+    <mergeCell ref="AP142:AR142"/>
+    <mergeCell ref="AS142:BF142"/>
+    <mergeCell ref="BG142:CA142"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="D140:AE140"/>
+    <mergeCell ref="AF140:AJ140"/>
+    <mergeCell ref="AK140:AO140"/>
+    <mergeCell ref="AP140:AR140"/>
+    <mergeCell ref="AS140:BF140"/>
+    <mergeCell ref="BG140:CA140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="D141:AE141"/>
+    <mergeCell ref="AF141:AJ141"/>
+    <mergeCell ref="AK141:AO141"/>
+    <mergeCell ref="AP141:AR141"/>
+    <mergeCell ref="AS141:BF141"/>
+    <mergeCell ref="BG141:CA141"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C142">

</xml_diff>

<commit_message>
báo cáo ngày 26/2/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="159">
   <si>
     <t>No.</t>
   </si>
@@ -486,6 +486,18 @@
   <si>
     <t>Thực hiện đồng bộ  -  Tìm cách sửa lỗi không gọi được service cần dùng</t>
   </si>
+  <si>
+    <t>26/2/2019</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa giao diện - Cho phép đồng bộ cùng database</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa giao diện - Chỉ marker với trường làm khóa phụ của bảng đích</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa giao diện - Bấm next tự sinh chuỗi cron ở step 1</t>
+  </si>
 </sst>
 </file>
 
@@ -796,16 +808,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -821,15 +831,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,7 +947,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1326,7 +1338,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1338,7 +1350,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP141" sqref="AP141:AR141"/>
+      <selection pane="bottomLeft" activeCell="AP144" sqref="AP144:AR144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,192 +1365,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="30" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="29" t="s">
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="31" t="s">
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="29" t="s">
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="29"/>
-      <c r="AU1" s="29"/>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="29"/>
-      <c r="AX1" s="29"/>
-      <c r="AY1" s="29"/>
-      <c r="AZ1" s="29"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="29"/>
-      <c r="BC1" s="29"/>
-      <c r="BD1" s="29"/>
-      <c r="BE1" s="29"/>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="32" t="s">
+      <c r="AT1" s="27"/>
+      <c r="AU1" s="27"/>
+      <c r="AV1" s="27"/>
+      <c r="AW1" s="27"/>
+      <c r="AX1" s="27"/>
+      <c r="AY1" s="27"/>
+      <c r="AZ1" s="27"/>
+      <c r="BA1" s="27"/>
+      <c r="BB1" s="27"/>
+      <c r="BC1" s="27"/>
+      <c r="BD1" s="27"/>
+      <c r="BE1" s="27"/>
+      <c r="BF1" s="27"/>
+      <c r="BG1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
-      <c r="BQ1" s="32"/>
-      <c r="BR1" s="32"/>
-      <c r="BS1" s="32"/>
-      <c r="BT1" s="32"/>
-      <c r="BU1" s="32"/>
-      <c r="BV1" s="32"/>
-      <c r="BW1" s="32"/>
-      <c r="BX1" s="32"/>
-      <c r="BY1" s="32"/>
-      <c r="BZ1" s="32"/>
-      <c r="CA1" s="32"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+      <c r="BN1" s="30"/>
+      <c r="BO1" s="30"/>
+      <c r="BP1" s="30"/>
+      <c r="BQ1" s="30"/>
+      <c r="BR1" s="30"/>
+      <c r="BS1" s="30"/>
+      <c r="BT1" s="30"/>
+      <c r="BU1" s="30"/>
+      <c r="BV1" s="30"/>
+      <c r="BW1" s="30"/>
+      <c r="BX1" s="30"/>
+      <c r="BY1" s="30"/>
+      <c r="BZ1" s="30"/>
+      <c r="CA1" s="30"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="34" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="33" t="s">
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="35">
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="34">
         <v>1</v>
       </c>
-      <c r="AQ2" s="35"/>
-      <c r="AR2" s="35"/>
-      <c r="AS2" s="33" t="s">
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="33"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="33"/>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="36"/>
-      <c r="BH2" s="36"/>
-      <c r="BI2" s="36"/>
-      <c r="BJ2" s="36"/>
-      <c r="BK2" s="36"/>
-      <c r="BL2" s="36"/>
-      <c r="BM2" s="36"/>
-      <c r="BN2" s="36"/>
-      <c r="BO2" s="36"/>
-      <c r="BP2" s="36"/>
-      <c r="BQ2" s="36"/>
-      <c r="BR2" s="36"/>
-      <c r="BS2" s="36"/>
-      <c r="BT2" s="36"/>
-      <c r="BU2" s="36"/>
-      <c r="BV2" s="36"/>
-      <c r="BW2" s="36"/>
-      <c r="BX2" s="36"/>
-      <c r="BY2" s="36"/>
-      <c r="BZ2" s="36"/>
-      <c r="CA2" s="36"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="32"/>
+      <c r="BG2" s="35"/>
+      <c r="BH2" s="35"/>
+      <c r="BI2" s="35"/>
+      <c r="BJ2" s="35"/>
+      <c r="BK2" s="35"/>
+      <c r="BL2" s="35"/>
+      <c r="BM2" s="35"/>
+      <c r="BN2" s="35"/>
+      <c r="BO2" s="35"/>
+      <c r="BP2" s="35"/>
+      <c r="BQ2" s="35"/>
+      <c r="BR2" s="35"/>
+      <c r="BS2" s="35"/>
+      <c r="BT2" s="35"/>
+      <c r="BU2" s="35"/>
+      <c r="BV2" s="35"/>
+      <c r="BW2" s="35"/>
+      <c r="BX2" s="35"/>
+      <c r="BY2" s="35"/>
+      <c r="BZ2" s="35"/>
+      <c r="CA2" s="35"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4259,43 +4271,43 @@
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="37"/>
-      <c r="T32" s="37"/>
-      <c r="U32" s="37"/>
-      <c r="V32" s="37"/>
-      <c r="W32" s="37"/>
-      <c r="X32" s="37"/>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="37"/>
-      <c r="AA32" s="37"/>
-      <c r="AB32" s="37"/>
-      <c r="AC32" s="37"/>
-      <c r="AD32" s="37"/>
-      <c r="AE32" s="37"/>
-      <c r="AF32" s="38">
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="21"/>
+      <c r="AA32" s="21"/>
+      <c r="AB32" s="21"/>
+      <c r="AC32" s="21"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="21"/>
+      <c r="AF32" s="22">
         <v>43293</v>
       </c>
-      <c r="AG32" s="38"/>
-      <c r="AH32" s="38"/>
-      <c r="AI32" s="38"/>
-      <c r="AJ32" s="38"/>
+      <c r="AG32" s="22"/>
+      <c r="AH32" s="22"/>
+      <c r="AI32" s="22"/>
+      <c r="AJ32" s="22"/>
       <c r="AK32" s="10" t="s">
         <v>16</v>
       </c>
@@ -4324,27 +4336,27 @@
       <c r="BD32" s="10"/>
       <c r="BE32" s="10"/>
       <c r="BF32" s="10"/>
-      <c r="BG32" s="39"/>
-      <c r="BH32" s="39"/>
-      <c r="BI32" s="39"/>
-      <c r="BJ32" s="39"/>
-      <c r="BK32" s="39"/>
-      <c r="BL32" s="39"/>
-      <c r="BM32" s="39"/>
-      <c r="BN32" s="39"/>
-      <c r="BO32" s="39"/>
-      <c r="BP32" s="39"/>
-      <c r="BQ32" s="39"/>
-      <c r="BR32" s="39"/>
-      <c r="BS32" s="39"/>
-      <c r="BT32" s="39"/>
-      <c r="BU32" s="39"/>
-      <c r="BV32" s="39"/>
-      <c r="BW32" s="39"/>
-      <c r="BX32" s="39"/>
-      <c r="BY32" s="39"/>
-      <c r="BZ32" s="39"/>
-      <c r="CA32" s="39"/>
+      <c r="BG32" s="23"/>
+      <c r="BH32" s="23"/>
+      <c r="BI32" s="23"/>
+      <c r="BJ32" s="23"/>
+      <c r="BK32" s="23"/>
+      <c r="BL32" s="23"/>
+      <c r="BM32" s="23"/>
+      <c r="BN32" s="23"/>
+      <c r="BO32" s="23"/>
+      <c r="BP32" s="23"/>
+      <c r="BQ32" s="23"/>
+      <c r="BR32" s="23"/>
+      <c r="BS32" s="23"/>
+      <c r="BT32" s="23"/>
+      <c r="BU32" s="23"/>
+      <c r="BV32" s="23"/>
+      <c r="BW32" s="23"/>
+      <c r="BX32" s="23"/>
+      <c r="BY32" s="23"/>
+      <c r="BZ32" s="23"/>
+      <c r="CA32" s="23"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
@@ -4396,27 +4408,27 @@
       <c r="AM33" s="10"/>
       <c r="AN33" s="10"/>
       <c r="AO33" s="10"/>
-      <c r="AP33" s="40">
+      <c r="AP33" s="24">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="40"/>
-      <c r="AR33" s="40"/>
-      <c r="AS33" s="41" t="s">
+      <c r="AQ33" s="24"/>
+      <c r="AR33" s="24"/>
+      <c r="AS33" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="41"/>
-      <c r="AU33" s="41"/>
-      <c r="AV33" s="41"/>
-      <c r="AW33" s="41"/>
-      <c r="AX33" s="41"/>
-      <c r="AY33" s="41"/>
-      <c r="AZ33" s="41"/>
-      <c r="BA33" s="41"/>
-      <c r="BB33" s="41"/>
-      <c r="BC33" s="41"/>
-      <c r="BD33" s="41"/>
-      <c r="BE33" s="41"/>
-      <c r="BF33" s="41"/>
+      <c r="AT33" s="25"/>
+      <c r="AU33" s="25"/>
+      <c r="AV33" s="25"/>
+      <c r="AW33" s="25"/>
+      <c r="AX33" s="25"/>
+      <c r="AY33" s="25"/>
+      <c r="AZ33" s="25"/>
+      <c r="BA33" s="25"/>
+      <c r="BB33" s="25"/>
+      <c r="BC33" s="25"/>
+      <c r="BD33" s="25"/>
+      <c r="BE33" s="25"/>
+      <c r="BF33" s="25"/>
       <c r="BG33" s="13"/>
       <c r="BH33" s="13"/>
       <c r="BI33" s="13"/>
@@ -4724,36 +4736,36 @@
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
-      <c r="Y37" s="20"/>
-      <c r="Z37" s="20"/>
-      <c r="AA37" s="20"/>
-      <c r="AB37" s="20"/>
-      <c r="AC37" s="20"/>
-      <c r="AD37" s="20"/>
-      <c r="AE37" s="21"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+      <c r="Y37" s="19"/>
+      <c r="Z37" s="19"/>
+      <c r="AA37" s="19"/>
+      <c r="AB37" s="19"/>
+      <c r="AC37" s="19"/>
+      <c r="AD37" s="19"/>
+      <c r="AE37" s="20"/>
       <c r="AF37" s="11">
         <v>43416</v>
       </c>
@@ -4817,36 +4829,36 @@
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
-      <c r="Y38" s="20"/>
-      <c r="Z38" s="20"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="20"/>
-      <c r="AC38" s="20"/>
-      <c r="AD38" s="20"/>
-      <c r="AE38" s="21"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19"/>
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="19"/>
+      <c r="AC38" s="19"/>
+      <c r="AD38" s="19"/>
+      <c r="AE38" s="20"/>
       <c r="AF38" s="11">
         <v>43446</v>
       </c>
@@ -5003,36 +5015,36 @@
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="20"/>
-      <c r="Q40" s="20"/>
-      <c r="R40" s="20"/>
-      <c r="S40" s="20"/>
-      <c r="T40" s="20"/>
-      <c r="U40" s="20"/>
-      <c r="V40" s="20"/>
-      <c r="W40" s="20"/>
-      <c r="X40" s="20"/>
-      <c r="Y40" s="20"/>
-      <c r="Z40" s="20"/>
-      <c r="AA40" s="20"/>
-      <c r="AB40" s="20"/>
-      <c r="AC40" s="20"/>
-      <c r="AD40" s="20"/>
-      <c r="AE40" s="21"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="19"/>
+      <c r="AA40" s="19"/>
+      <c r="AB40" s="19"/>
+      <c r="AC40" s="19"/>
+      <c r="AD40" s="19"/>
+      <c r="AE40" s="20"/>
       <c r="AF40" s="11">
         <v>43447</v>
       </c>
@@ -5189,36 +5201,36 @@
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
-      <c r="P42" s="20"/>
-      <c r="Q42" s="20"/>
-      <c r="R42" s="20"/>
-      <c r="S42" s="20"/>
-      <c r="T42" s="20"/>
-      <c r="U42" s="20"/>
-      <c r="V42" s="20"/>
-      <c r="W42" s="20"/>
-      <c r="X42" s="20"/>
-      <c r="Y42" s="20"/>
-      <c r="Z42" s="20"/>
-      <c r="AA42" s="20"/>
-      <c r="AB42" s="20"/>
-      <c r="AC42" s="20"/>
-      <c r="AD42" s="20"/>
-      <c r="AE42" s="21"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="19"/>
+      <c r="Z42" s="19"/>
+      <c r="AA42" s="19"/>
+      <c r="AB42" s="19"/>
+      <c r="AC42" s="19"/>
+      <c r="AD42" s="19"/>
+      <c r="AE42" s="20"/>
       <c r="AF42" s="11" t="s">
         <v>55</v>
       </c>
@@ -5282,36 +5294,36 @@
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20"/>
-      <c r="S43" s="20"/>
-      <c r="T43" s="20"/>
-      <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
-      <c r="W43" s="20"/>
-      <c r="X43" s="20"/>
-      <c r="Y43" s="20"/>
-      <c r="Z43" s="20"/>
-      <c r="AA43" s="20"/>
-      <c r="AB43" s="20"/>
-      <c r="AC43" s="20"/>
-      <c r="AD43" s="20"/>
-      <c r="AE43" s="21"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="19"/>
+      <c r="AD43" s="19"/>
+      <c r="AE43" s="20"/>
       <c r="AF43" s="11" t="s">
         <v>55</v>
       </c>
@@ -5375,36 +5387,36 @@
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="20"/>
-      <c r="O44" s="20"/>
-      <c r="P44" s="20"/>
-      <c r="Q44" s="20"/>
-      <c r="R44" s="20"/>
-      <c r="S44" s="20"/>
-      <c r="T44" s="20"/>
-      <c r="U44" s="20"/>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
-      <c r="X44" s="20"/>
-      <c r="Y44" s="20"/>
-      <c r="Z44" s="20"/>
-      <c r="AA44" s="20"/>
-      <c r="AB44" s="20"/>
-      <c r="AC44" s="20"/>
-      <c r="AD44" s="20"/>
-      <c r="AE44" s="21"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+      <c r="Y44" s="19"/>
+      <c r="Z44" s="19"/>
+      <c r="AA44" s="19"/>
+      <c r="AB44" s="19"/>
+      <c r="AC44" s="19"/>
+      <c r="AD44" s="19"/>
+      <c r="AE44" s="20"/>
       <c r="AF44" s="11" t="s">
         <v>58</v>
       </c>
@@ -12330,71 +12342,71 @@
       </c>
       <c r="B119" s="9"/>
       <c r="C119" s="5"/>
-      <c r="D119" s="19" t="s">
+      <c r="D119" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="E119" s="20"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="20"/>
-      <c r="H119" s="20"/>
-      <c r="I119" s="20"/>
-      <c r="J119" s="20"/>
-      <c r="K119" s="20"/>
-      <c r="L119" s="20"/>
-      <c r="M119" s="20"/>
-      <c r="N119" s="20"/>
-      <c r="O119" s="20"/>
-      <c r="P119" s="20"/>
-      <c r="Q119" s="20"/>
-      <c r="R119" s="20"/>
-      <c r="S119" s="20"/>
-      <c r="T119" s="20"/>
-      <c r="U119" s="20"/>
-      <c r="V119" s="20"/>
-      <c r="W119" s="20"/>
-      <c r="X119" s="20"/>
-      <c r="Y119" s="20"/>
-      <c r="Z119" s="20"/>
-      <c r="AA119" s="20"/>
-      <c r="AB119" s="20"/>
-      <c r="AC119" s="20"/>
-      <c r="AD119" s="20"/>
-      <c r="AE119" s="21"/>
-      <c r="AF119" s="25" t="s">
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="19"/>
+      <c r="H119" s="19"/>
+      <c r="I119" s="19"/>
+      <c r="J119" s="19"/>
+      <c r="K119" s="19"/>
+      <c r="L119" s="19"/>
+      <c r="M119" s="19"/>
+      <c r="N119" s="19"/>
+      <c r="O119" s="19"/>
+      <c r="P119" s="19"/>
+      <c r="Q119" s="19"/>
+      <c r="R119" s="19"/>
+      <c r="S119" s="19"/>
+      <c r="T119" s="19"/>
+      <c r="U119" s="19"/>
+      <c r="V119" s="19"/>
+      <c r="W119" s="19"/>
+      <c r="X119" s="19"/>
+      <c r="Y119" s="19"/>
+      <c r="Z119" s="19"/>
+      <c r="AA119" s="19"/>
+      <c r="AB119" s="19"/>
+      <c r="AC119" s="19"/>
+      <c r="AD119" s="19"/>
+      <c r="AE119" s="20"/>
+      <c r="AF119" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="AG119" s="26"/>
-      <c r="AH119" s="26"/>
-      <c r="AI119" s="26"/>
-      <c r="AJ119" s="27"/>
-      <c r="AK119" s="19" t="s">
+      <c r="AG119" s="40"/>
+      <c r="AH119" s="40"/>
+      <c r="AI119" s="40"/>
+      <c r="AJ119" s="41"/>
+      <c r="AK119" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="AL119" s="20"/>
-      <c r="AM119" s="20"/>
-      <c r="AN119" s="20"/>
-      <c r="AO119" s="21"/>
-      <c r="AP119" s="22">
+      <c r="AL119" s="19"/>
+      <c r="AM119" s="19"/>
+      <c r="AN119" s="19"/>
+      <c r="AO119" s="20"/>
+      <c r="AP119" s="36">
         <v>1</v>
       </c>
-      <c r="AQ119" s="23"/>
-      <c r="AR119" s="24"/>
-      <c r="AS119" s="19" t="s">
+      <c r="AQ119" s="37"/>
+      <c r="AR119" s="38"/>
+      <c r="AS119" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AT119" s="20"/>
-      <c r="AU119" s="20"/>
-      <c r="AV119" s="20"/>
-      <c r="AW119" s="20"/>
-      <c r="AX119" s="20"/>
-      <c r="AY119" s="20"/>
-      <c r="AZ119" s="20"/>
-      <c r="BA119" s="20"/>
-      <c r="BB119" s="20"/>
-      <c r="BC119" s="20"/>
-      <c r="BD119" s="20"/>
-      <c r="BE119" s="20"/>
-      <c r="BF119" s="21"/>
+      <c r="AT119" s="19"/>
+      <c r="AU119" s="19"/>
+      <c r="AV119" s="19"/>
+      <c r="AW119" s="19"/>
+      <c r="AX119" s="19"/>
+      <c r="AY119" s="19"/>
+      <c r="AZ119" s="19"/>
+      <c r="BA119" s="19"/>
+      <c r="BB119" s="19"/>
+      <c r="BC119" s="19"/>
+      <c r="BD119" s="19"/>
+      <c r="BE119" s="19"/>
+      <c r="BF119" s="20"/>
       <c r="BG119" s="13"/>
       <c r="BH119" s="13"/>
       <c r="BI119" s="13"/>
@@ -13690,10 +13702,10 @@
       <c r="CA133" s="13"/>
     </row>
     <row r="134" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A134" s="18">
+      <c r="A134" s="31">
         <v>133</v>
       </c>
-      <c r="B134" s="18"/>
+      <c r="B134" s="31"/>
       <c r="C134" s="5"/>
       <c r="D134" s="10" t="s">
         <v>148</v>
@@ -14419,7 +14431,9 @@
       </c>
       <c r="B142" s="17"/>
       <c r="C142" s="5"/>
-      <c r="D142" s="10"/>
+      <c r="D142" s="10" t="s">
+        <v>156</v>
+      </c>
       <c r="E142" s="10"/>
       <c r="F142" s="10"/>
       <c r="G142" s="10"/>
@@ -14447,20 +14461,28 @@
       <c r="AC142" s="10"/>
       <c r="AD142" s="10"/>
       <c r="AE142" s="10"/>
-      <c r="AF142" s="11"/>
+      <c r="AF142" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="AG142" s="11"/>
       <c r="AH142" s="11"/>
       <c r="AI142" s="11"/>
       <c r="AJ142" s="11"/>
-      <c r="AK142" s="10"/>
+      <c r="AK142" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="AL142" s="10"/>
       <c r="AM142" s="10"/>
       <c r="AN142" s="10"/>
       <c r="AO142" s="10"/>
-      <c r="AP142" s="12"/>
+      <c r="AP142" s="12">
+        <v>1</v>
+      </c>
       <c r="AQ142" s="12"/>
       <c r="AR142" s="12"/>
-      <c r="AS142" s="10"/>
+      <c r="AS142" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="AT142" s="10"/>
       <c r="AU142" s="10"/>
       <c r="AV142" s="10"/>
@@ -14502,7 +14524,9 @@
       </c>
       <c r="B143" s="9"/>
       <c r="C143" s="5"/>
-      <c r="D143" s="10"/>
+      <c r="D143" s="10" t="s">
+        <v>157</v>
+      </c>
       <c r="E143" s="10"/>
       <c r="F143" s="10"/>
       <c r="G143" s="10"/>
@@ -14530,20 +14554,28 @@
       <c r="AC143" s="10"/>
       <c r="AD143" s="10"/>
       <c r="AE143" s="10"/>
-      <c r="AF143" s="11"/>
+      <c r="AF143" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="AG143" s="11"/>
       <c r="AH143" s="11"/>
       <c r="AI143" s="11"/>
       <c r="AJ143" s="11"/>
-      <c r="AK143" s="10"/>
+      <c r="AK143" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="AL143" s="10"/>
       <c r="AM143" s="10"/>
       <c r="AN143" s="10"/>
       <c r="AO143" s="10"/>
-      <c r="AP143" s="12"/>
+      <c r="AP143" s="12">
+        <v>1</v>
+      </c>
       <c r="AQ143" s="12"/>
       <c r="AR143" s="12"/>
-      <c r="AS143" s="10"/>
+      <c r="AS143" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="AT143" s="10"/>
       <c r="AU143" s="10"/>
       <c r="AV143" s="10"/>
@@ -14585,7 +14617,9 @@
       </c>
       <c r="B144" s="9"/>
       <c r="C144" s="5"/>
-      <c r="D144" s="10"/>
+      <c r="D144" s="10" t="s">
+        <v>158</v>
+      </c>
       <c r="E144" s="10"/>
       <c r="F144" s="10"/>
       <c r="G144" s="10"/>
@@ -14613,20 +14647,28 @@
       <c r="AC144" s="10"/>
       <c r="AD144" s="10"/>
       <c r="AE144" s="10"/>
-      <c r="AF144" s="11"/>
+      <c r="AF144" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="AG144" s="11"/>
       <c r="AH144" s="11"/>
       <c r="AI144" s="11"/>
       <c r="AJ144" s="11"/>
-      <c r="AK144" s="10"/>
+      <c r="AK144" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="AL144" s="10"/>
       <c r="AM144" s="10"/>
       <c r="AN144" s="10"/>
       <c r="AO144" s="10"/>
-      <c r="AP144" s="12"/>
+      <c r="AP144" s="12">
+        <v>0.7</v>
+      </c>
       <c r="AQ144" s="12"/>
       <c r="AR144" s="12"/>
-      <c r="AS144" s="10"/>
+      <c r="AS144" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="AT144" s="10"/>
       <c r="AU144" s="10"/>
       <c r="AV144" s="10"/>
@@ -19312,6 +19354,1374 @@
     </row>
   </sheetData>
   <mergeCells count="1400">
+    <mergeCell ref="A199:B199"/>
+    <mergeCell ref="D199:AE199"/>
+    <mergeCell ref="AF199:AJ199"/>
+    <mergeCell ref="AK199:AO199"/>
+    <mergeCell ref="AP199:AR199"/>
+    <mergeCell ref="AS199:BF199"/>
+    <mergeCell ref="BG199:CA199"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="D200:AE200"/>
+    <mergeCell ref="AF200:AJ200"/>
+    <mergeCell ref="AK200:AO200"/>
+    <mergeCell ref="AP200:AR200"/>
+    <mergeCell ref="AS200:BF200"/>
+    <mergeCell ref="BG200:CA200"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="D197:AE197"/>
+    <mergeCell ref="AF197:AJ197"/>
+    <mergeCell ref="AK197:AO197"/>
+    <mergeCell ref="AP197:AR197"/>
+    <mergeCell ref="AS197:BF197"/>
+    <mergeCell ref="BG197:CA197"/>
+    <mergeCell ref="A198:B198"/>
+    <mergeCell ref="D198:AE198"/>
+    <mergeCell ref="AF198:AJ198"/>
+    <mergeCell ref="AK198:AO198"/>
+    <mergeCell ref="AP198:AR198"/>
+    <mergeCell ref="AS198:BF198"/>
+    <mergeCell ref="BG198:CA198"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="D195:AE195"/>
+    <mergeCell ref="AF195:AJ195"/>
+    <mergeCell ref="AK195:AO195"/>
+    <mergeCell ref="AP195:AR195"/>
+    <mergeCell ref="AS195:BF195"/>
+    <mergeCell ref="BG195:CA195"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="D196:AE196"/>
+    <mergeCell ref="AF196:AJ196"/>
+    <mergeCell ref="AK196:AO196"/>
+    <mergeCell ref="AP196:AR196"/>
+    <mergeCell ref="AS196:BF196"/>
+    <mergeCell ref="BG196:CA196"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="D193:AE193"/>
+    <mergeCell ref="AF193:AJ193"/>
+    <mergeCell ref="AK193:AO193"/>
+    <mergeCell ref="AP193:AR193"/>
+    <mergeCell ref="AS193:BF193"/>
+    <mergeCell ref="BG193:CA193"/>
+    <mergeCell ref="A194:B194"/>
+    <mergeCell ref="D194:AE194"/>
+    <mergeCell ref="AF194:AJ194"/>
+    <mergeCell ref="AK194:AO194"/>
+    <mergeCell ref="AP194:AR194"/>
+    <mergeCell ref="AS194:BF194"/>
+    <mergeCell ref="BG194:CA194"/>
+    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="D191:AE191"/>
+    <mergeCell ref="AF191:AJ191"/>
+    <mergeCell ref="AK191:AO191"/>
+    <mergeCell ref="AP191:AR191"/>
+    <mergeCell ref="AS191:BF191"/>
+    <mergeCell ref="BG191:CA191"/>
+    <mergeCell ref="A192:B192"/>
+    <mergeCell ref="D192:AE192"/>
+    <mergeCell ref="AF192:AJ192"/>
+    <mergeCell ref="AK192:AO192"/>
+    <mergeCell ref="AP192:AR192"/>
+    <mergeCell ref="AS192:BF192"/>
+    <mergeCell ref="BG192:CA192"/>
+    <mergeCell ref="A189:B189"/>
+    <mergeCell ref="D189:AE189"/>
+    <mergeCell ref="AF189:AJ189"/>
+    <mergeCell ref="AK189:AO189"/>
+    <mergeCell ref="AP189:AR189"/>
+    <mergeCell ref="AS189:BF189"/>
+    <mergeCell ref="BG189:CA189"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="D190:AE190"/>
+    <mergeCell ref="AF190:AJ190"/>
+    <mergeCell ref="AK190:AO190"/>
+    <mergeCell ref="AP190:AR190"/>
+    <mergeCell ref="AS190:BF190"/>
+    <mergeCell ref="BG190:CA190"/>
+    <mergeCell ref="AK187:AO187"/>
+    <mergeCell ref="AP187:AR187"/>
+    <mergeCell ref="AS187:BF187"/>
+    <mergeCell ref="BG187:CA187"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="D188:AE188"/>
+    <mergeCell ref="AF188:AJ188"/>
+    <mergeCell ref="AK188:AO188"/>
+    <mergeCell ref="AP188:AR188"/>
+    <mergeCell ref="AS188:BF188"/>
+    <mergeCell ref="BG188:CA188"/>
+    <mergeCell ref="A185:B185"/>
+    <mergeCell ref="D185:AE185"/>
+    <mergeCell ref="AF185:AJ185"/>
+    <mergeCell ref="AK185:AO185"/>
+    <mergeCell ref="AP185:AR185"/>
+    <mergeCell ref="AS185:BF185"/>
+    <mergeCell ref="BG185:CA185"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="D186:AE186"/>
+    <mergeCell ref="AF186:AJ186"/>
+    <mergeCell ref="AK186:AO186"/>
+    <mergeCell ref="AP186:AR186"/>
+    <mergeCell ref="AS186:BF186"/>
+    <mergeCell ref="BG186:CA186"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="D187:AE187"/>
+    <mergeCell ref="AF187:AJ187"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="D183:AE183"/>
+    <mergeCell ref="AF183:AJ183"/>
+    <mergeCell ref="AK183:AO183"/>
+    <mergeCell ref="AP183:AR183"/>
+    <mergeCell ref="AS183:BF183"/>
+    <mergeCell ref="BG183:CA183"/>
+    <mergeCell ref="A184:B184"/>
+    <mergeCell ref="D184:AE184"/>
+    <mergeCell ref="AF184:AJ184"/>
+    <mergeCell ref="AK184:AO184"/>
+    <mergeCell ref="AP184:AR184"/>
+    <mergeCell ref="AS184:BF184"/>
+    <mergeCell ref="BG184:CA184"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="D181:AE181"/>
+    <mergeCell ref="AF181:AJ181"/>
+    <mergeCell ref="AK181:AO181"/>
+    <mergeCell ref="AP181:AR181"/>
+    <mergeCell ref="AS181:BF181"/>
+    <mergeCell ref="BG181:CA181"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="D182:AE182"/>
+    <mergeCell ref="AF182:AJ182"/>
+    <mergeCell ref="AK182:AO182"/>
+    <mergeCell ref="AP182:AR182"/>
+    <mergeCell ref="AS182:BF182"/>
+    <mergeCell ref="BG182:CA182"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="D179:AE179"/>
+    <mergeCell ref="AF179:AJ179"/>
+    <mergeCell ref="AK179:AO179"/>
+    <mergeCell ref="AP179:AR179"/>
+    <mergeCell ref="AS179:BF179"/>
+    <mergeCell ref="BG179:CA179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="D180:AE180"/>
+    <mergeCell ref="AF180:AJ180"/>
+    <mergeCell ref="AK180:AO180"/>
+    <mergeCell ref="AP180:AR180"/>
+    <mergeCell ref="AS180:BF180"/>
+    <mergeCell ref="BG180:CA180"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="D177:AE177"/>
+    <mergeCell ref="AF177:AJ177"/>
+    <mergeCell ref="AK177:AO177"/>
+    <mergeCell ref="AP177:AR177"/>
+    <mergeCell ref="AS177:BF177"/>
+    <mergeCell ref="BG177:CA177"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="D178:AE178"/>
+    <mergeCell ref="AF178:AJ178"/>
+    <mergeCell ref="AK178:AO178"/>
+    <mergeCell ref="AP178:AR178"/>
+    <mergeCell ref="AS178:BF178"/>
+    <mergeCell ref="BG178:CA178"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="D175:AE175"/>
+    <mergeCell ref="AF175:AJ175"/>
+    <mergeCell ref="AK175:AO175"/>
+    <mergeCell ref="AP175:AR175"/>
+    <mergeCell ref="AS175:BF175"/>
+    <mergeCell ref="BG175:CA175"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="D176:AE176"/>
+    <mergeCell ref="AF176:AJ176"/>
+    <mergeCell ref="AK176:AO176"/>
+    <mergeCell ref="AP176:AR176"/>
+    <mergeCell ref="AS176:BF176"/>
+    <mergeCell ref="BG176:CA176"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="D173:AE173"/>
+    <mergeCell ref="AF173:AJ173"/>
+    <mergeCell ref="AK173:AO173"/>
+    <mergeCell ref="AP173:AR173"/>
+    <mergeCell ref="AS173:BF173"/>
+    <mergeCell ref="BG173:CA173"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="D174:AE174"/>
+    <mergeCell ref="AF174:AJ174"/>
+    <mergeCell ref="AK174:AO174"/>
+    <mergeCell ref="AP174:AR174"/>
+    <mergeCell ref="AS174:BF174"/>
+    <mergeCell ref="BG174:CA174"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="D171:AE171"/>
+    <mergeCell ref="AF171:AJ171"/>
+    <mergeCell ref="AK171:AO171"/>
+    <mergeCell ref="AP171:AR171"/>
+    <mergeCell ref="AS171:BF171"/>
+    <mergeCell ref="BG171:CA171"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="D172:AE172"/>
+    <mergeCell ref="AF172:AJ172"/>
+    <mergeCell ref="AK172:AO172"/>
+    <mergeCell ref="AP172:AR172"/>
+    <mergeCell ref="AS172:BF172"/>
+    <mergeCell ref="BG172:CA172"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="D169:AE169"/>
+    <mergeCell ref="AF169:AJ169"/>
+    <mergeCell ref="AK169:AO169"/>
+    <mergeCell ref="AP169:AR169"/>
+    <mergeCell ref="AS169:BF169"/>
+    <mergeCell ref="BG169:CA169"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="D170:AE170"/>
+    <mergeCell ref="AF170:AJ170"/>
+    <mergeCell ref="AK170:AO170"/>
+    <mergeCell ref="AP170:AR170"/>
+    <mergeCell ref="AS170:BF170"/>
+    <mergeCell ref="BG170:CA170"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="D167:AE167"/>
+    <mergeCell ref="AF167:AJ167"/>
+    <mergeCell ref="AK167:AO167"/>
+    <mergeCell ref="AP167:AR167"/>
+    <mergeCell ref="AS167:BF167"/>
+    <mergeCell ref="BG167:CA167"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="D168:AE168"/>
+    <mergeCell ref="AF168:AJ168"/>
+    <mergeCell ref="AK168:AO168"/>
+    <mergeCell ref="AP168:AR168"/>
+    <mergeCell ref="AS168:BF168"/>
+    <mergeCell ref="BG168:CA168"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="D165:AE165"/>
+    <mergeCell ref="AF165:AJ165"/>
+    <mergeCell ref="AK165:AO165"/>
+    <mergeCell ref="AP165:AR165"/>
+    <mergeCell ref="AS165:BF165"/>
+    <mergeCell ref="BG165:CA165"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="D166:AE166"/>
+    <mergeCell ref="AF166:AJ166"/>
+    <mergeCell ref="AK166:AO166"/>
+    <mergeCell ref="AP166:AR166"/>
+    <mergeCell ref="AS166:BF166"/>
+    <mergeCell ref="BG166:CA166"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="D163:AE163"/>
+    <mergeCell ref="AF163:AJ163"/>
+    <mergeCell ref="AK163:AO163"/>
+    <mergeCell ref="AP163:AR163"/>
+    <mergeCell ref="AS163:BF163"/>
+    <mergeCell ref="BG163:CA163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="D164:AE164"/>
+    <mergeCell ref="AF164:AJ164"/>
+    <mergeCell ref="AK164:AO164"/>
+    <mergeCell ref="AP164:AR164"/>
+    <mergeCell ref="AS164:BF164"/>
+    <mergeCell ref="BG164:CA164"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="D161:AE161"/>
+    <mergeCell ref="AF161:AJ161"/>
+    <mergeCell ref="AK161:AO161"/>
+    <mergeCell ref="AP161:AR161"/>
+    <mergeCell ref="AS161:BF161"/>
+    <mergeCell ref="BG161:CA161"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="D162:AE162"/>
+    <mergeCell ref="AF162:AJ162"/>
+    <mergeCell ref="AK162:AO162"/>
+    <mergeCell ref="AP162:AR162"/>
+    <mergeCell ref="AS162:BF162"/>
+    <mergeCell ref="BG162:CA162"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="D159:AE159"/>
+    <mergeCell ref="AF159:AJ159"/>
+    <mergeCell ref="AK159:AO159"/>
+    <mergeCell ref="AP159:AR159"/>
+    <mergeCell ref="AS159:BF159"/>
+    <mergeCell ref="BG159:CA159"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="D160:AE160"/>
+    <mergeCell ref="AF160:AJ160"/>
+    <mergeCell ref="AK160:AO160"/>
+    <mergeCell ref="AP160:AR160"/>
+    <mergeCell ref="AS160:BF160"/>
+    <mergeCell ref="BG160:CA160"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="D157:AE157"/>
+    <mergeCell ref="AF157:AJ157"/>
+    <mergeCell ref="AK157:AO157"/>
+    <mergeCell ref="AP157:AR157"/>
+    <mergeCell ref="AS157:BF157"/>
+    <mergeCell ref="BG157:CA157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="D158:AE158"/>
+    <mergeCell ref="AF158:AJ158"/>
+    <mergeCell ref="AK158:AO158"/>
+    <mergeCell ref="AP158:AR158"/>
+    <mergeCell ref="AS158:BF158"/>
+    <mergeCell ref="BG158:CA158"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="D155:AE155"/>
+    <mergeCell ref="AF155:AJ155"/>
+    <mergeCell ref="AK155:AO155"/>
+    <mergeCell ref="AP155:AR155"/>
+    <mergeCell ref="AS155:BF155"/>
+    <mergeCell ref="BG155:CA155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="D156:AE156"/>
+    <mergeCell ref="AF156:AJ156"/>
+    <mergeCell ref="AK156:AO156"/>
+    <mergeCell ref="AP156:AR156"/>
+    <mergeCell ref="AS156:BF156"/>
+    <mergeCell ref="BG156:CA156"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="D153:AE153"/>
+    <mergeCell ref="AF153:AJ153"/>
+    <mergeCell ref="AK153:AO153"/>
+    <mergeCell ref="AP153:AR153"/>
+    <mergeCell ref="AS153:BF153"/>
+    <mergeCell ref="BG153:CA153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="D154:AE154"/>
+    <mergeCell ref="AF154:AJ154"/>
+    <mergeCell ref="AK154:AO154"/>
+    <mergeCell ref="AP154:AR154"/>
+    <mergeCell ref="AS154:BF154"/>
+    <mergeCell ref="BG154:CA154"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="D151:AE151"/>
+    <mergeCell ref="AF151:AJ151"/>
+    <mergeCell ref="AK151:AO151"/>
+    <mergeCell ref="AP151:AR151"/>
+    <mergeCell ref="AS151:BF151"/>
+    <mergeCell ref="BG151:CA151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="D152:AE152"/>
+    <mergeCell ref="AF152:AJ152"/>
+    <mergeCell ref="AK152:AO152"/>
+    <mergeCell ref="AP152:AR152"/>
+    <mergeCell ref="AS152:BF152"/>
+    <mergeCell ref="BG152:CA152"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="D149:AE149"/>
+    <mergeCell ref="AF149:AJ149"/>
+    <mergeCell ref="AK149:AO149"/>
+    <mergeCell ref="AP149:AR149"/>
+    <mergeCell ref="AS149:BF149"/>
+    <mergeCell ref="BG149:CA149"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="D150:AE150"/>
+    <mergeCell ref="AF150:AJ150"/>
+    <mergeCell ref="AK150:AO150"/>
+    <mergeCell ref="AP150:AR150"/>
+    <mergeCell ref="AS150:BF150"/>
+    <mergeCell ref="BG150:CA150"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="D147:AE147"/>
+    <mergeCell ref="AF147:AJ147"/>
+    <mergeCell ref="AK147:AO147"/>
+    <mergeCell ref="AP147:AR147"/>
+    <mergeCell ref="AS147:BF147"/>
+    <mergeCell ref="BG147:CA147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="D148:AE148"/>
+    <mergeCell ref="AF148:AJ148"/>
+    <mergeCell ref="AK148:AO148"/>
+    <mergeCell ref="AP148:AR148"/>
+    <mergeCell ref="AS148:BF148"/>
+    <mergeCell ref="BG148:CA148"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="D145:AE145"/>
+    <mergeCell ref="AF145:AJ145"/>
+    <mergeCell ref="AK145:AO145"/>
+    <mergeCell ref="AP145:AR145"/>
+    <mergeCell ref="AS145:BF145"/>
+    <mergeCell ref="BG145:CA145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="D146:AE146"/>
+    <mergeCell ref="AF146:AJ146"/>
+    <mergeCell ref="AK146:AO146"/>
+    <mergeCell ref="AP146:AR146"/>
+    <mergeCell ref="AS146:BF146"/>
+    <mergeCell ref="BG146:CA146"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="D143:AE143"/>
+    <mergeCell ref="AF143:AJ143"/>
+    <mergeCell ref="AK143:AO143"/>
+    <mergeCell ref="AP143:AR143"/>
+    <mergeCell ref="AS143:BF143"/>
+    <mergeCell ref="BG143:CA143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="D144:AE144"/>
+    <mergeCell ref="AF144:AJ144"/>
+    <mergeCell ref="AK144:AO144"/>
+    <mergeCell ref="AP144:AR144"/>
+    <mergeCell ref="AS144:BF144"/>
+    <mergeCell ref="BG144:CA144"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="D142:AE142"/>
+    <mergeCell ref="AF142:AJ142"/>
+    <mergeCell ref="AK142:AO142"/>
+    <mergeCell ref="AP142:AR142"/>
+    <mergeCell ref="AS142:BF142"/>
+    <mergeCell ref="BG142:CA142"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="D140:AE140"/>
+    <mergeCell ref="AF140:AJ140"/>
+    <mergeCell ref="AK140:AO140"/>
+    <mergeCell ref="AP140:AR140"/>
+    <mergeCell ref="AS140:BF140"/>
+    <mergeCell ref="BG140:CA140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="D141:AE141"/>
+    <mergeCell ref="AF141:AJ141"/>
+    <mergeCell ref="AK141:AO141"/>
+    <mergeCell ref="AP141:AR141"/>
+    <mergeCell ref="AS141:BF141"/>
+    <mergeCell ref="BG141:CA141"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="D138:AE138"/>
+    <mergeCell ref="AF138:AJ138"/>
+    <mergeCell ref="AK138:AO138"/>
+    <mergeCell ref="AP138:AR138"/>
+    <mergeCell ref="AS138:BF138"/>
+    <mergeCell ref="BG138:CA138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="D139:AE139"/>
+    <mergeCell ref="AF139:AJ139"/>
+    <mergeCell ref="AK139:AO139"/>
+    <mergeCell ref="AP139:AR139"/>
+    <mergeCell ref="AS139:BF139"/>
+    <mergeCell ref="BG139:CA139"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="D136:AE136"/>
+    <mergeCell ref="AF136:AJ136"/>
+    <mergeCell ref="AK136:AO136"/>
+    <mergeCell ref="AP136:AR136"/>
+    <mergeCell ref="AS136:BF136"/>
+    <mergeCell ref="BG136:CA136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="D137:AE137"/>
+    <mergeCell ref="AF137:AJ137"/>
+    <mergeCell ref="AK137:AO137"/>
+    <mergeCell ref="AP137:AR137"/>
+    <mergeCell ref="AS137:BF137"/>
+    <mergeCell ref="BG137:CA137"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="D134:AE134"/>
+    <mergeCell ref="AF134:AJ134"/>
+    <mergeCell ref="AK134:AO134"/>
+    <mergeCell ref="AP134:AR134"/>
+    <mergeCell ref="AS134:BF134"/>
+    <mergeCell ref="BG134:CA134"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="D135:AE135"/>
+    <mergeCell ref="AF135:AJ135"/>
+    <mergeCell ref="AK135:AO135"/>
+    <mergeCell ref="AP135:AR135"/>
+    <mergeCell ref="AS135:BF135"/>
+    <mergeCell ref="BG135:CA135"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="D132:AE132"/>
+    <mergeCell ref="AF132:AJ132"/>
+    <mergeCell ref="AK132:AO132"/>
+    <mergeCell ref="AP132:AR132"/>
+    <mergeCell ref="AS132:BF132"/>
+    <mergeCell ref="BG132:CA132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="BG133:CA133"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="D130:AE130"/>
+    <mergeCell ref="AF130:AJ130"/>
+    <mergeCell ref="AK130:AO130"/>
+    <mergeCell ref="AP130:AR130"/>
+    <mergeCell ref="AS130:BF130"/>
+    <mergeCell ref="BG130:CA130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="D133:AE133"/>
+    <mergeCell ref="AF133:AJ133"/>
+    <mergeCell ref="AK133:AO133"/>
+    <mergeCell ref="AP133:AR133"/>
+    <mergeCell ref="AS133:BF133"/>
+    <mergeCell ref="BG131:CA131"/>
+    <mergeCell ref="D131:AE131"/>
+    <mergeCell ref="AF131:AJ131"/>
+    <mergeCell ref="AK131:AO131"/>
+    <mergeCell ref="AP131:AR131"/>
+    <mergeCell ref="AS131:BF131"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="D128:AE128"/>
+    <mergeCell ref="AF128:AJ128"/>
+    <mergeCell ref="AK128:AO128"/>
+    <mergeCell ref="AP128:AR128"/>
+    <mergeCell ref="AS128:BF128"/>
+    <mergeCell ref="BG128:CA128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="D129:AE129"/>
+    <mergeCell ref="AF129:AJ129"/>
+    <mergeCell ref="AK129:AO129"/>
+    <mergeCell ref="AP129:AR129"/>
+    <mergeCell ref="AS129:BF129"/>
+    <mergeCell ref="BG129:CA129"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="D126:AE126"/>
+    <mergeCell ref="AF126:AJ126"/>
+    <mergeCell ref="AK126:AO126"/>
+    <mergeCell ref="AP126:AR126"/>
+    <mergeCell ref="AS126:BF126"/>
+    <mergeCell ref="BG126:CA126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="D127:AE127"/>
+    <mergeCell ref="AF127:AJ127"/>
+    <mergeCell ref="AK127:AO127"/>
+    <mergeCell ref="AP127:AR127"/>
+    <mergeCell ref="AS127:BF127"/>
+    <mergeCell ref="BG127:CA127"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="D124:AE124"/>
+    <mergeCell ref="AF124:AJ124"/>
+    <mergeCell ref="AK124:AO124"/>
+    <mergeCell ref="AP124:AR124"/>
+    <mergeCell ref="AS124:BF124"/>
+    <mergeCell ref="BG124:CA124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="D125:AE125"/>
+    <mergeCell ref="AF125:AJ125"/>
+    <mergeCell ref="AK125:AO125"/>
+    <mergeCell ref="AP125:AR125"/>
+    <mergeCell ref="AS125:BF125"/>
+    <mergeCell ref="BG125:CA125"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="BG120:CA120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="BG121:CA121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="D121:AE121"/>
+    <mergeCell ref="AF121:AJ121"/>
+    <mergeCell ref="AK121:AO121"/>
+    <mergeCell ref="AP121:AR121"/>
+    <mergeCell ref="AS121:BF121"/>
+    <mergeCell ref="BG122:CA122"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D117:AE117"/>
+    <mergeCell ref="AF117:AJ117"/>
+    <mergeCell ref="AK117:AO117"/>
+    <mergeCell ref="AP117:AR117"/>
+    <mergeCell ref="AS117:BF117"/>
+    <mergeCell ref="BG118:CA118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="D120:AE120"/>
+    <mergeCell ref="AF120:AJ120"/>
+    <mergeCell ref="AK120:AO120"/>
+    <mergeCell ref="AP120:AR120"/>
+    <mergeCell ref="AS120:BF120"/>
+    <mergeCell ref="BG119:CA119"/>
+    <mergeCell ref="AS119:BF119"/>
+    <mergeCell ref="AP119:AR119"/>
+    <mergeCell ref="AK119:AO119"/>
+    <mergeCell ref="AF119:AJ119"/>
+    <mergeCell ref="D119:AE119"/>
+    <mergeCell ref="D118:AE118"/>
+    <mergeCell ref="AF118:AJ118"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG117:CA117"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:AE70"/>
+    <mergeCell ref="AF70:AJ70"/>
+    <mergeCell ref="AK70:AO70"/>
+    <mergeCell ref="AP70:AR70"/>
+    <mergeCell ref="AS70:BF70"/>
+    <mergeCell ref="BG70:CA70"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AR1"/>
+    <mergeCell ref="AS1:BF1"/>
+    <mergeCell ref="BG1:CA1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:AE2"/>
+    <mergeCell ref="AF2:AJ2"/>
+    <mergeCell ref="AK2:AO2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AS2:BF2"/>
+    <mergeCell ref="BG2:CA2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="D68:AE68"/>
     <mergeCell ref="AF68:AJ68"/>
@@ -19344,1374 +20754,6 @@
     <mergeCell ref="D72:AE72"/>
     <mergeCell ref="AF72:AJ72"/>
     <mergeCell ref="AK72:AO72"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:AE1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AR1"/>
-    <mergeCell ref="AS1:BF1"/>
-    <mergeCell ref="BG1:CA1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:AE2"/>
-    <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AS2:BF2"/>
-    <mergeCell ref="BG2:CA2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:AE3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:AE70"/>
-    <mergeCell ref="AF70:AJ70"/>
-    <mergeCell ref="AK70:AO70"/>
-    <mergeCell ref="AP70:AR70"/>
-    <mergeCell ref="AS70:BF70"/>
-    <mergeCell ref="BG70:CA70"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="BG120:CA120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="BG121:CA121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="D121:AE121"/>
-    <mergeCell ref="AF121:AJ121"/>
-    <mergeCell ref="AK121:AO121"/>
-    <mergeCell ref="AP121:AR121"/>
-    <mergeCell ref="AS121:BF121"/>
-    <mergeCell ref="BG122:CA122"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D117:AE117"/>
-    <mergeCell ref="AF117:AJ117"/>
-    <mergeCell ref="AK117:AO117"/>
-    <mergeCell ref="AP117:AR117"/>
-    <mergeCell ref="AS117:BF117"/>
-    <mergeCell ref="BG118:CA118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="D120:AE120"/>
-    <mergeCell ref="AF120:AJ120"/>
-    <mergeCell ref="AK120:AO120"/>
-    <mergeCell ref="AP120:AR120"/>
-    <mergeCell ref="AS120:BF120"/>
-    <mergeCell ref="BG119:CA119"/>
-    <mergeCell ref="AS119:BF119"/>
-    <mergeCell ref="AP119:AR119"/>
-    <mergeCell ref="AK119:AO119"/>
-    <mergeCell ref="AF119:AJ119"/>
-    <mergeCell ref="D119:AE119"/>
-    <mergeCell ref="D118:AE118"/>
-    <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="D124:AE124"/>
-    <mergeCell ref="AF124:AJ124"/>
-    <mergeCell ref="AK124:AO124"/>
-    <mergeCell ref="AP124:AR124"/>
-    <mergeCell ref="AS124:BF124"/>
-    <mergeCell ref="BG124:CA124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="D125:AE125"/>
-    <mergeCell ref="AF125:AJ125"/>
-    <mergeCell ref="AK125:AO125"/>
-    <mergeCell ref="AP125:AR125"/>
-    <mergeCell ref="AS125:BF125"/>
-    <mergeCell ref="BG125:CA125"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="D128:AE128"/>
-    <mergeCell ref="AF128:AJ128"/>
-    <mergeCell ref="AK128:AO128"/>
-    <mergeCell ref="AP128:AR128"/>
-    <mergeCell ref="AS128:BF128"/>
-    <mergeCell ref="BG128:CA128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="D129:AE129"/>
-    <mergeCell ref="AF129:AJ129"/>
-    <mergeCell ref="AK129:AO129"/>
-    <mergeCell ref="AP129:AR129"/>
-    <mergeCell ref="AS129:BF129"/>
-    <mergeCell ref="BG129:CA129"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="D126:AE126"/>
-    <mergeCell ref="AF126:AJ126"/>
-    <mergeCell ref="AK126:AO126"/>
-    <mergeCell ref="AP126:AR126"/>
-    <mergeCell ref="AS126:BF126"/>
-    <mergeCell ref="BG126:CA126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="D127:AE127"/>
-    <mergeCell ref="AF127:AJ127"/>
-    <mergeCell ref="AK127:AO127"/>
-    <mergeCell ref="AP127:AR127"/>
-    <mergeCell ref="AS127:BF127"/>
-    <mergeCell ref="BG127:CA127"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="D132:AE132"/>
-    <mergeCell ref="AF132:AJ132"/>
-    <mergeCell ref="AK132:AO132"/>
-    <mergeCell ref="AP132:AR132"/>
-    <mergeCell ref="AS132:BF132"/>
-    <mergeCell ref="BG132:CA132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="BG133:CA133"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="D130:AE130"/>
-    <mergeCell ref="AF130:AJ130"/>
-    <mergeCell ref="AK130:AO130"/>
-    <mergeCell ref="AP130:AR130"/>
-    <mergeCell ref="AS130:BF130"/>
-    <mergeCell ref="BG130:CA130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="D133:AE133"/>
-    <mergeCell ref="AF133:AJ133"/>
-    <mergeCell ref="AK133:AO133"/>
-    <mergeCell ref="AP133:AR133"/>
-    <mergeCell ref="AS133:BF133"/>
-    <mergeCell ref="BG131:CA131"/>
-    <mergeCell ref="D131:AE131"/>
-    <mergeCell ref="AF131:AJ131"/>
-    <mergeCell ref="AK131:AO131"/>
-    <mergeCell ref="AP131:AR131"/>
-    <mergeCell ref="AS131:BF131"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="D136:AE136"/>
-    <mergeCell ref="AF136:AJ136"/>
-    <mergeCell ref="AK136:AO136"/>
-    <mergeCell ref="AP136:AR136"/>
-    <mergeCell ref="AS136:BF136"/>
-    <mergeCell ref="BG136:CA136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="D137:AE137"/>
-    <mergeCell ref="AF137:AJ137"/>
-    <mergeCell ref="AK137:AO137"/>
-    <mergeCell ref="AP137:AR137"/>
-    <mergeCell ref="AS137:BF137"/>
-    <mergeCell ref="BG137:CA137"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="D134:AE134"/>
-    <mergeCell ref="AF134:AJ134"/>
-    <mergeCell ref="AK134:AO134"/>
-    <mergeCell ref="AP134:AR134"/>
-    <mergeCell ref="AS134:BF134"/>
-    <mergeCell ref="BG134:CA134"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="D135:AE135"/>
-    <mergeCell ref="AF135:AJ135"/>
-    <mergeCell ref="AK135:AO135"/>
-    <mergeCell ref="AP135:AR135"/>
-    <mergeCell ref="AS135:BF135"/>
-    <mergeCell ref="BG135:CA135"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="D140:AE140"/>
-    <mergeCell ref="AF140:AJ140"/>
-    <mergeCell ref="AK140:AO140"/>
-    <mergeCell ref="AP140:AR140"/>
-    <mergeCell ref="AS140:BF140"/>
-    <mergeCell ref="BG140:CA140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="D141:AE141"/>
-    <mergeCell ref="AF141:AJ141"/>
-    <mergeCell ref="AK141:AO141"/>
-    <mergeCell ref="AP141:AR141"/>
-    <mergeCell ref="AS141:BF141"/>
-    <mergeCell ref="BG141:CA141"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="D138:AE138"/>
-    <mergeCell ref="AF138:AJ138"/>
-    <mergeCell ref="AK138:AO138"/>
-    <mergeCell ref="AP138:AR138"/>
-    <mergeCell ref="AS138:BF138"/>
-    <mergeCell ref="BG138:CA138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="D139:AE139"/>
-    <mergeCell ref="AF139:AJ139"/>
-    <mergeCell ref="AK139:AO139"/>
-    <mergeCell ref="AP139:AR139"/>
-    <mergeCell ref="AS139:BF139"/>
-    <mergeCell ref="BG139:CA139"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="D143:AE143"/>
-    <mergeCell ref="AF143:AJ143"/>
-    <mergeCell ref="AK143:AO143"/>
-    <mergeCell ref="AP143:AR143"/>
-    <mergeCell ref="AS143:BF143"/>
-    <mergeCell ref="BG143:CA143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="D144:AE144"/>
-    <mergeCell ref="AF144:AJ144"/>
-    <mergeCell ref="AK144:AO144"/>
-    <mergeCell ref="AP144:AR144"/>
-    <mergeCell ref="AS144:BF144"/>
-    <mergeCell ref="BG144:CA144"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="D142:AE142"/>
-    <mergeCell ref="AF142:AJ142"/>
-    <mergeCell ref="AK142:AO142"/>
-    <mergeCell ref="AP142:AR142"/>
-    <mergeCell ref="AS142:BF142"/>
-    <mergeCell ref="BG142:CA142"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="D147:AE147"/>
-    <mergeCell ref="AF147:AJ147"/>
-    <mergeCell ref="AK147:AO147"/>
-    <mergeCell ref="AP147:AR147"/>
-    <mergeCell ref="AS147:BF147"/>
-    <mergeCell ref="BG147:CA147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="D148:AE148"/>
-    <mergeCell ref="AF148:AJ148"/>
-    <mergeCell ref="AK148:AO148"/>
-    <mergeCell ref="AP148:AR148"/>
-    <mergeCell ref="AS148:BF148"/>
-    <mergeCell ref="BG148:CA148"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="D145:AE145"/>
-    <mergeCell ref="AF145:AJ145"/>
-    <mergeCell ref="AK145:AO145"/>
-    <mergeCell ref="AP145:AR145"/>
-    <mergeCell ref="AS145:BF145"/>
-    <mergeCell ref="BG145:CA145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="D146:AE146"/>
-    <mergeCell ref="AF146:AJ146"/>
-    <mergeCell ref="AK146:AO146"/>
-    <mergeCell ref="AP146:AR146"/>
-    <mergeCell ref="AS146:BF146"/>
-    <mergeCell ref="BG146:CA146"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="D151:AE151"/>
-    <mergeCell ref="AF151:AJ151"/>
-    <mergeCell ref="AK151:AO151"/>
-    <mergeCell ref="AP151:AR151"/>
-    <mergeCell ref="AS151:BF151"/>
-    <mergeCell ref="BG151:CA151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="D152:AE152"/>
-    <mergeCell ref="AF152:AJ152"/>
-    <mergeCell ref="AK152:AO152"/>
-    <mergeCell ref="AP152:AR152"/>
-    <mergeCell ref="AS152:BF152"/>
-    <mergeCell ref="BG152:CA152"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="D149:AE149"/>
-    <mergeCell ref="AF149:AJ149"/>
-    <mergeCell ref="AK149:AO149"/>
-    <mergeCell ref="AP149:AR149"/>
-    <mergeCell ref="AS149:BF149"/>
-    <mergeCell ref="BG149:CA149"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="D150:AE150"/>
-    <mergeCell ref="AF150:AJ150"/>
-    <mergeCell ref="AK150:AO150"/>
-    <mergeCell ref="AP150:AR150"/>
-    <mergeCell ref="AS150:BF150"/>
-    <mergeCell ref="BG150:CA150"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="D155:AE155"/>
-    <mergeCell ref="AF155:AJ155"/>
-    <mergeCell ref="AK155:AO155"/>
-    <mergeCell ref="AP155:AR155"/>
-    <mergeCell ref="AS155:BF155"/>
-    <mergeCell ref="BG155:CA155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="D156:AE156"/>
-    <mergeCell ref="AF156:AJ156"/>
-    <mergeCell ref="AK156:AO156"/>
-    <mergeCell ref="AP156:AR156"/>
-    <mergeCell ref="AS156:BF156"/>
-    <mergeCell ref="BG156:CA156"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="D153:AE153"/>
-    <mergeCell ref="AF153:AJ153"/>
-    <mergeCell ref="AK153:AO153"/>
-    <mergeCell ref="AP153:AR153"/>
-    <mergeCell ref="AS153:BF153"/>
-    <mergeCell ref="BG153:CA153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="D154:AE154"/>
-    <mergeCell ref="AF154:AJ154"/>
-    <mergeCell ref="AK154:AO154"/>
-    <mergeCell ref="AP154:AR154"/>
-    <mergeCell ref="AS154:BF154"/>
-    <mergeCell ref="BG154:CA154"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="D159:AE159"/>
-    <mergeCell ref="AF159:AJ159"/>
-    <mergeCell ref="AK159:AO159"/>
-    <mergeCell ref="AP159:AR159"/>
-    <mergeCell ref="AS159:BF159"/>
-    <mergeCell ref="BG159:CA159"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="D160:AE160"/>
-    <mergeCell ref="AF160:AJ160"/>
-    <mergeCell ref="AK160:AO160"/>
-    <mergeCell ref="AP160:AR160"/>
-    <mergeCell ref="AS160:BF160"/>
-    <mergeCell ref="BG160:CA160"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="D157:AE157"/>
-    <mergeCell ref="AF157:AJ157"/>
-    <mergeCell ref="AK157:AO157"/>
-    <mergeCell ref="AP157:AR157"/>
-    <mergeCell ref="AS157:BF157"/>
-    <mergeCell ref="BG157:CA157"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="D158:AE158"/>
-    <mergeCell ref="AF158:AJ158"/>
-    <mergeCell ref="AK158:AO158"/>
-    <mergeCell ref="AP158:AR158"/>
-    <mergeCell ref="AS158:BF158"/>
-    <mergeCell ref="BG158:CA158"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="D163:AE163"/>
-    <mergeCell ref="AF163:AJ163"/>
-    <mergeCell ref="AK163:AO163"/>
-    <mergeCell ref="AP163:AR163"/>
-    <mergeCell ref="AS163:BF163"/>
-    <mergeCell ref="BG163:CA163"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="D164:AE164"/>
-    <mergeCell ref="AF164:AJ164"/>
-    <mergeCell ref="AK164:AO164"/>
-    <mergeCell ref="AP164:AR164"/>
-    <mergeCell ref="AS164:BF164"/>
-    <mergeCell ref="BG164:CA164"/>
-    <mergeCell ref="A161:B161"/>
-    <mergeCell ref="D161:AE161"/>
-    <mergeCell ref="AF161:AJ161"/>
-    <mergeCell ref="AK161:AO161"/>
-    <mergeCell ref="AP161:AR161"/>
-    <mergeCell ref="AS161:BF161"/>
-    <mergeCell ref="BG161:CA161"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="D162:AE162"/>
-    <mergeCell ref="AF162:AJ162"/>
-    <mergeCell ref="AK162:AO162"/>
-    <mergeCell ref="AP162:AR162"/>
-    <mergeCell ref="AS162:BF162"/>
-    <mergeCell ref="BG162:CA162"/>
-    <mergeCell ref="A167:B167"/>
-    <mergeCell ref="D167:AE167"/>
-    <mergeCell ref="AF167:AJ167"/>
-    <mergeCell ref="AK167:AO167"/>
-    <mergeCell ref="AP167:AR167"/>
-    <mergeCell ref="AS167:BF167"/>
-    <mergeCell ref="BG167:CA167"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="D168:AE168"/>
-    <mergeCell ref="AF168:AJ168"/>
-    <mergeCell ref="AK168:AO168"/>
-    <mergeCell ref="AP168:AR168"/>
-    <mergeCell ref="AS168:BF168"/>
-    <mergeCell ref="BG168:CA168"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="D165:AE165"/>
-    <mergeCell ref="AF165:AJ165"/>
-    <mergeCell ref="AK165:AO165"/>
-    <mergeCell ref="AP165:AR165"/>
-    <mergeCell ref="AS165:BF165"/>
-    <mergeCell ref="BG165:CA165"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="D166:AE166"/>
-    <mergeCell ref="AF166:AJ166"/>
-    <mergeCell ref="AK166:AO166"/>
-    <mergeCell ref="AP166:AR166"/>
-    <mergeCell ref="AS166:BF166"/>
-    <mergeCell ref="BG166:CA166"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="D171:AE171"/>
-    <mergeCell ref="AF171:AJ171"/>
-    <mergeCell ref="AK171:AO171"/>
-    <mergeCell ref="AP171:AR171"/>
-    <mergeCell ref="AS171:BF171"/>
-    <mergeCell ref="BG171:CA171"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="D172:AE172"/>
-    <mergeCell ref="AF172:AJ172"/>
-    <mergeCell ref="AK172:AO172"/>
-    <mergeCell ref="AP172:AR172"/>
-    <mergeCell ref="AS172:BF172"/>
-    <mergeCell ref="BG172:CA172"/>
-    <mergeCell ref="A169:B169"/>
-    <mergeCell ref="D169:AE169"/>
-    <mergeCell ref="AF169:AJ169"/>
-    <mergeCell ref="AK169:AO169"/>
-    <mergeCell ref="AP169:AR169"/>
-    <mergeCell ref="AS169:BF169"/>
-    <mergeCell ref="BG169:CA169"/>
-    <mergeCell ref="A170:B170"/>
-    <mergeCell ref="D170:AE170"/>
-    <mergeCell ref="AF170:AJ170"/>
-    <mergeCell ref="AK170:AO170"/>
-    <mergeCell ref="AP170:AR170"/>
-    <mergeCell ref="AS170:BF170"/>
-    <mergeCell ref="BG170:CA170"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="D175:AE175"/>
-    <mergeCell ref="AF175:AJ175"/>
-    <mergeCell ref="AK175:AO175"/>
-    <mergeCell ref="AP175:AR175"/>
-    <mergeCell ref="AS175:BF175"/>
-    <mergeCell ref="BG175:CA175"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="D176:AE176"/>
-    <mergeCell ref="AF176:AJ176"/>
-    <mergeCell ref="AK176:AO176"/>
-    <mergeCell ref="AP176:AR176"/>
-    <mergeCell ref="AS176:BF176"/>
-    <mergeCell ref="BG176:CA176"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="D173:AE173"/>
-    <mergeCell ref="AF173:AJ173"/>
-    <mergeCell ref="AK173:AO173"/>
-    <mergeCell ref="AP173:AR173"/>
-    <mergeCell ref="AS173:BF173"/>
-    <mergeCell ref="BG173:CA173"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="D174:AE174"/>
-    <mergeCell ref="AF174:AJ174"/>
-    <mergeCell ref="AK174:AO174"/>
-    <mergeCell ref="AP174:AR174"/>
-    <mergeCell ref="AS174:BF174"/>
-    <mergeCell ref="BG174:CA174"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="D179:AE179"/>
-    <mergeCell ref="AF179:AJ179"/>
-    <mergeCell ref="AK179:AO179"/>
-    <mergeCell ref="AP179:AR179"/>
-    <mergeCell ref="AS179:BF179"/>
-    <mergeCell ref="BG179:CA179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="D180:AE180"/>
-    <mergeCell ref="AF180:AJ180"/>
-    <mergeCell ref="AK180:AO180"/>
-    <mergeCell ref="AP180:AR180"/>
-    <mergeCell ref="AS180:BF180"/>
-    <mergeCell ref="BG180:CA180"/>
-    <mergeCell ref="A177:B177"/>
-    <mergeCell ref="D177:AE177"/>
-    <mergeCell ref="AF177:AJ177"/>
-    <mergeCell ref="AK177:AO177"/>
-    <mergeCell ref="AP177:AR177"/>
-    <mergeCell ref="AS177:BF177"/>
-    <mergeCell ref="BG177:CA177"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="D178:AE178"/>
-    <mergeCell ref="AF178:AJ178"/>
-    <mergeCell ref="AK178:AO178"/>
-    <mergeCell ref="AP178:AR178"/>
-    <mergeCell ref="AS178:BF178"/>
-    <mergeCell ref="BG178:CA178"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="D183:AE183"/>
-    <mergeCell ref="AF183:AJ183"/>
-    <mergeCell ref="AK183:AO183"/>
-    <mergeCell ref="AP183:AR183"/>
-    <mergeCell ref="AS183:BF183"/>
-    <mergeCell ref="BG183:CA183"/>
-    <mergeCell ref="A184:B184"/>
-    <mergeCell ref="D184:AE184"/>
-    <mergeCell ref="AF184:AJ184"/>
-    <mergeCell ref="AK184:AO184"/>
-    <mergeCell ref="AP184:AR184"/>
-    <mergeCell ref="AS184:BF184"/>
-    <mergeCell ref="BG184:CA184"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="D181:AE181"/>
-    <mergeCell ref="AF181:AJ181"/>
-    <mergeCell ref="AK181:AO181"/>
-    <mergeCell ref="AP181:AR181"/>
-    <mergeCell ref="AS181:BF181"/>
-    <mergeCell ref="BG181:CA181"/>
-    <mergeCell ref="A182:B182"/>
-    <mergeCell ref="D182:AE182"/>
-    <mergeCell ref="AF182:AJ182"/>
-    <mergeCell ref="AK182:AO182"/>
-    <mergeCell ref="AP182:AR182"/>
-    <mergeCell ref="AS182:BF182"/>
-    <mergeCell ref="BG182:CA182"/>
-    <mergeCell ref="AK187:AO187"/>
-    <mergeCell ref="AP187:AR187"/>
-    <mergeCell ref="AS187:BF187"/>
-    <mergeCell ref="BG187:CA187"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="D188:AE188"/>
-    <mergeCell ref="AF188:AJ188"/>
-    <mergeCell ref="AK188:AO188"/>
-    <mergeCell ref="AP188:AR188"/>
-    <mergeCell ref="AS188:BF188"/>
-    <mergeCell ref="BG188:CA188"/>
-    <mergeCell ref="A185:B185"/>
-    <mergeCell ref="D185:AE185"/>
-    <mergeCell ref="AF185:AJ185"/>
-    <mergeCell ref="AK185:AO185"/>
-    <mergeCell ref="AP185:AR185"/>
-    <mergeCell ref="AS185:BF185"/>
-    <mergeCell ref="BG185:CA185"/>
-    <mergeCell ref="A186:B186"/>
-    <mergeCell ref="D186:AE186"/>
-    <mergeCell ref="AF186:AJ186"/>
-    <mergeCell ref="AK186:AO186"/>
-    <mergeCell ref="AP186:AR186"/>
-    <mergeCell ref="AS186:BF186"/>
-    <mergeCell ref="BG186:CA186"/>
-    <mergeCell ref="A187:B187"/>
-    <mergeCell ref="D187:AE187"/>
-    <mergeCell ref="AF187:AJ187"/>
-    <mergeCell ref="A191:B191"/>
-    <mergeCell ref="D191:AE191"/>
-    <mergeCell ref="AF191:AJ191"/>
-    <mergeCell ref="AK191:AO191"/>
-    <mergeCell ref="AP191:AR191"/>
-    <mergeCell ref="AS191:BF191"/>
-    <mergeCell ref="BG191:CA191"/>
-    <mergeCell ref="A192:B192"/>
-    <mergeCell ref="D192:AE192"/>
-    <mergeCell ref="AF192:AJ192"/>
-    <mergeCell ref="AK192:AO192"/>
-    <mergeCell ref="AP192:AR192"/>
-    <mergeCell ref="AS192:BF192"/>
-    <mergeCell ref="BG192:CA192"/>
-    <mergeCell ref="A189:B189"/>
-    <mergeCell ref="D189:AE189"/>
-    <mergeCell ref="AF189:AJ189"/>
-    <mergeCell ref="AK189:AO189"/>
-    <mergeCell ref="AP189:AR189"/>
-    <mergeCell ref="AS189:BF189"/>
-    <mergeCell ref="BG189:CA189"/>
-    <mergeCell ref="A190:B190"/>
-    <mergeCell ref="D190:AE190"/>
-    <mergeCell ref="AF190:AJ190"/>
-    <mergeCell ref="AK190:AO190"/>
-    <mergeCell ref="AP190:AR190"/>
-    <mergeCell ref="AS190:BF190"/>
-    <mergeCell ref="BG190:CA190"/>
-    <mergeCell ref="A195:B195"/>
-    <mergeCell ref="D195:AE195"/>
-    <mergeCell ref="AF195:AJ195"/>
-    <mergeCell ref="AK195:AO195"/>
-    <mergeCell ref="AP195:AR195"/>
-    <mergeCell ref="AS195:BF195"/>
-    <mergeCell ref="BG195:CA195"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="D196:AE196"/>
-    <mergeCell ref="AF196:AJ196"/>
-    <mergeCell ref="AK196:AO196"/>
-    <mergeCell ref="AP196:AR196"/>
-    <mergeCell ref="AS196:BF196"/>
-    <mergeCell ref="BG196:CA196"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="D193:AE193"/>
-    <mergeCell ref="AF193:AJ193"/>
-    <mergeCell ref="AK193:AO193"/>
-    <mergeCell ref="AP193:AR193"/>
-    <mergeCell ref="AS193:BF193"/>
-    <mergeCell ref="BG193:CA193"/>
-    <mergeCell ref="A194:B194"/>
-    <mergeCell ref="D194:AE194"/>
-    <mergeCell ref="AF194:AJ194"/>
-    <mergeCell ref="AK194:AO194"/>
-    <mergeCell ref="AP194:AR194"/>
-    <mergeCell ref="AS194:BF194"/>
-    <mergeCell ref="BG194:CA194"/>
-    <mergeCell ref="A199:B199"/>
-    <mergeCell ref="D199:AE199"/>
-    <mergeCell ref="AF199:AJ199"/>
-    <mergeCell ref="AK199:AO199"/>
-    <mergeCell ref="AP199:AR199"/>
-    <mergeCell ref="AS199:BF199"/>
-    <mergeCell ref="BG199:CA199"/>
-    <mergeCell ref="A200:B200"/>
-    <mergeCell ref="D200:AE200"/>
-    <mergeCell ref="AF200:AJ200"/>
-    <mergeCell ref="AK200:AO200"/>
-    <mergeCell ref="AP200:AR200"/>
-    <mergeCell ref="AS200:BF200"/>
-    <mergeCell ref="BG200:CA200"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="D197:AE197"/>
-    <mergeCell ref="AF197:AJ197"/>
-    <mergeCell ref="AK197:AO197"/>
-    <mergeCell ref="AP197:AR197"/>
-    <mergeCell ref="AS197:BF197"/>
-    <mergeCell ref="BG197:CA197"/>
-    <mergeCell ref="A198:B198"/>
-    <mergeCell ref="D198:AE198"/>
-    <mergeCell ref="AF198:AJ198"/>
-    <mergeCell ref="AK198:AO198"/>
-    <mergeCell ref="AP198:AR198"/>
-    <mergeCell ref="AS198:BF198"/>
-    <mergeCell ref="BG198:CA198"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C200">

</xml_diff>

<commit_message>
báo cáo ngày 27/2/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="162">
   <si>
     <t>No.</t>
   </si>
@@ -498,6 +498,15 @@
   <si>
     <t>Chỉnh sửa giao diện - Bấm next tự sinh chuỗi cron ở step 1</t>
   </si>
+  <si>
+    <t>27/2/2019</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa giao diện - Map lại đường dẫn lưu backup và import</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa giao diện - Chỉnh sửa lại chuỗi cron đồng bộ</t>
+  </si>
 </sst>
 </file>
 
@@ -808,14 +817,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,17 +842,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,7 +956,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1338,7 +1347,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1349,8 +1358,8 @@
   <dimension ref="A1:CA200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP144" sqref="AP144:AR144"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D149" sqref="D149:AE149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,192 +1374,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="28" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="27" t="s">
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="29" t="s">
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="29"/>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="27" t="s">
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
-      <c r="BB1" s="27"/>
-      <c r="BC1" s="27"/>
-      <c r="BD1" s="27"/>
-      <c r="BE1" s="27"/>
-      <c r="BF1" s="27"/>
-      <c r="BG1" s="30" t="s">
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="29"/>
+      <c r="AV1" s="29"/>
+      <c r="AW1" s="29"/>
+      <c r="AX1" s="29"/>
+      <c r="AY1" s="29"/>
+      <c r="AZ1" s="29"/>
+      <c r="BA1" s="29"/>
+      <c r="BB1" s="29"/>
+      <c r="BC1" s="29"/>
+      <c r="BD1" s="29"/>
+      <c r="BE1" s="29"/>
+      <c r="BF1" s="29"/>
+      <c r="BG1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
-      <c r="BN1" s="30"/>
-      <c r="BO1" s="30"/>
-      <c r="BP1" s="30"/>
-      <c r="BQ1" s="30"/>
-      <c r="BR1" s="30"/>
-      <c r="BS1" s="30"/>
-      <c r="BT1" s="30"/>
-      <c r="BU1" s="30"/>
-      <c r="BV1" s="30"/>
-      <c r="BW1" s="30"/>
-      <c r="BX1" s="30"/>
-      <c r="BY1" s="30"/>
-      <c r="BZ1" s="30"/>
-      <c r="CA1" s="30"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
+      <c r="BQ1" s="32"/>
+      <c r="BR1" s="32"/>
+      <c r="BS1" s="32"/>
+      <c r="BT1" s="32"/>
+      <c r="BU1" s="32"/>
+      <c r="BV1" s="32"/>
+      <c r="BW1" s="32"/>
+      <c r="BX1" s="32"/>
+      <c r="BY1" s="32"/>
+      <c r="BZ1" s="32"/>
+      <c r="CA1" s="32"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="33" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="32" t="s">
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="34">
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="35">
         <v>1</v>
       </c>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="32" t="s">
+      <c r="AQ2" s="35"/>
+      <c r="AR2" s="35"/>
+      <c r="AS2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="32"/>
-      <c r="AX2" s="32"/>
-      <c r="AY2" s="32"/>
-      <c r="AZ2" s="32"/>
-      <c r="BA2" s="32"/>
-      <c r="BB2" s="32"/>
-      <c r="BC2" s="32"/>
-      <c r="BD2" s="32"/>
-      <c r="BE2" s="32"/>
-      <c r="BF2" s="32"/>
-      <c r="BG2" s="35"/>
-      <c r="BH2" s="35"/>
-      <c r="BI2" s="35"/>
-      <c r="BJ2" s="35"/>
-      <c r="BK2" s="35"/>
-      <c r="BL2" s="35"/>
-      <c r="BM2" s="35"/>
-      <c r="BN2" s="35"/>
-      <c r="BO2" s="35"/>
-      <c r="BP2" s="35"/>
-      <c r="BQ2" s="35"/>
-      <c r="BR2" s="35"/>
-      <c r="BS2" s="35"/>
-      <c r="BT2" s="35"/>
-      <c r="BU2" s="35"/>
-      <c r="BV2" s="35"/>
-      <c r="BW2" s="35"/>
-      <c r="BX2" s="35"/>
-      <c r="BY2" s="35"/>
-      <c r="BZ2" s="35"/>
-      <c r="CA2" s="35"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
+      <c r="AW2" s="33"/>
+      <c r="AX2" s="33"/>
+      <c r="AY2" s="33"/>
+      <c r="AZ2" s="33"/>
+      <c r="BA2" s="33"/>
+      <c r="BB2" s="33"/>
+      <c r="BC2" s="33"/>
+      <c r="BD2" s="33"/>
+      <c r="BE2" s="33"/>
+      <c r="BF2" s="33"/>
+      <c r="BG2" s="36"/>
+      <c r="BH2" s="36"/>
+      <c r="BI2" s="36"/>
+      <c r="BJ2" s="36"/>
+      <c r="BK2" s="36"/>
+      <c r="BL2" s="36"/>
+      <c r="BM2" s="36"/>
+      <c r="BN2" s="36"/>
+      <c r="BO2" s="36"/>
+      <c r="BP2" s="36"/>
+      <c r="BQ2" s="36"/>
+      <c r="BR2" s="36"/>
+      <c r="BS2" s="36"/>
+      <c r="BT2" s="36"/>
+      <c r="BU2" s="36"/>
+      <c r="BV2" s="36"/>
+      <c r="BW2" s="36"/>
+      <c r="BX2" s="36"/>
+      <c r="BY2" s="36"/>
+      <c r="BZ2" s="36"/>
+      <c r="CA2" s="36"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4271,43 +4280,43 @@
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="21"/>
-      <c r="V32" s="21"/>
-      <c r="W32" s="21"/>
-      <c r="X32" s="21"/>
-      <c r="Y32" s="21"/>
-      <c r="Z32" s="21"/>
-      <c r="AA32" s="21"/>
-      <c r="AB32" s="21"/>
-      <c r="AC32" s="21"/>
-      <c r="AD32" s="21"/>
-      <c r="AE32" s="21"/>
-      <c r="AF32" s="22">
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="37"/>
+      <c r="U32" s="37"/>
+      <c r="V32" s="37"/>
+      <c r="W32" s="37"/>
+      <c r="X32" s="37"/>
+      <c r="Y32" s="37"/>
+      <c r="Z32" s="37"/>
+      <c r="AA32" s="37"/>
+      <c r="AB32" s="37"/>
+      <c r="AC32" s="37"/>
+      <c r="AD32" s="37"/>
+      <c r="AE32" s="37"/>
+      <c r="AF32" s="38">
         <v>43293</v>
       </c>
-      <c r="AG32" s="22"/>
-      <c r="AH32" s="22"/>
-      <c r="AI32" s="22"/>
-      <c r="AJ32" s="22"/>
+      <c r="AG32" s="38"/>
+      <c r="AH32" s="38"/>
+      <c r="AI32" s="38"/>
+      <c r="AJ32" s="38"/>
       <c r="AK32" s="10" t="s">
         <v>16</v>
       </c>
@@ -4336,27 +4345,27 @@
       <c r="BD32" s="10"/>
       <c r="BE32" s="10"/>
       <c r="BF32" s="10"/>
-      <c r="BG32" s="23"/>
-      <c r="BH32" s="23"/>
-      <c r="BI32" s="23"/>
-      <c r="BJ32" s="23"/>
-      <c r="BK32" s="23"/>
-      <c r="BL32" s="23"/>
-      <c r="BM32" s="23"/>
-      <c r="BN32" s="23"/>
-      <c r="BO32" s="23"/>
-      <c r="BP32" s="23"/>
-      <c r="BQ32" s="23"/>
-      <c r="BR32" s="23"/>
-      <c r="BS32" s="23"/>
-      <c r="BT32" s="23"/>
-      <c r="BU32" s="23"/>
-      <c r="BV32" s="23"/>
-      <c r="BW32" s="23"/>
-      <c r="BX32" s="23"/>
-      <c r="BY32" s="23"/>
-      <c r="BZ32" s="23"/>
-      <c r="CA32" s="23"/>
+      <c r="BG32" s="39"/>
+      <c r="BH32" s="39"/>
+      <c r="BI32" s="39"/>
+      <c r="BJ32" s="39"/>
+      <c r="BK32" s="39"/>
+      <c r="BL32" s="39"/>
+      <c r="BM32" s="39"/>
+      <c r="BN32" s="39"/>
+      <c r="BO32" s="39"/>
+      <c r="BP32" s="39"/>
+      <c r="BQ32" s="39"/>
+      <c r="BR32" s="39"/>
+      <c r="BS32" s="39"/>
+      <c r="BT32" s="39"/>
+      <c r="BU32" s="39"/>
+      <c r="BV32" s="39"/>
+      <c r="BW32" s="39"/>
+      <c r="BX32" s="39"/>
+      <c r="BY32" s="39"/>
+      <c r="BZ32" s="39"/>
+      <c r="CA32" s="39"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
@@ -4408,27 +4417,27 @@
       <c r="AM33" s="10"/>
       <c r="AN33" s="10"/>
       <c r="AO33" s="10"/>
-      <c r="AP33" s="24">
+      <c r="AP33" s="40">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="24"/>
-      <c r="AR33" s="24"/>
-      <c r="AS33" s="25" t="s">
+      <c r="AQ33" s="40"/>
+      <c r="AR33" s="40"/>
+      <c r="AS33" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="25"/>
-      <c r="AU33" s="25"/>
-      <c r="AV33" s="25"/>
-      <c r="AW33" s="25"/>
-      <c r="AX33" s="25"/>
-      <c r="AY33" s="25"/>
-      <c r="AZ33" s="25"/>
-      <c r="BA33" s="25"/>
-      <c r="BB33" s="25"/>
-      <c r="BC33" s="25"/>
-      <c r="BD33" s="25"/>
-      <c r="BE33" s="25"/>
-      <c r="BF33" s="25"/>
+      <c r="AT33" s="41"/>
+      <c r="AU33" s="41"/>
+      <c r="AV33" s="41"/>
+      <c r="AW33" s="41"/>
+      <c r="AX33" s="41"/>
+      <c r="AY33" s="41"/>
+      <c r="AZ33" s="41"/>
+      <c r="BA33" s="41"/>
+      <c r="BB33" s="41"/>
+      <c r="BC33" s="41"/>
+      <c r="BD33" s="41"/>
+      <c r="BE33" s="41"/>
+      <c r="BF33" s="41"/>
       <c r="BG33" s="13"/>
       <c r="BH33" s="13"/>
       <c r="BI33" s="13"/>
@@ -4736,36 +4745,36 @@
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19"/>
-      <c r="Y37" s="19"/>
-      <c r="Z37" s="19"/>
-      <c r="AA37" s="19"/>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="19"/>
-      <c r="AD37" s="19"/>
-      <c r="AE37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="20"/>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="20"/>
+      <c r="AA37" s="20"/>
+      <c r="AB37" s="20"/>
+      <c r="AC37" s="20"/>
+      <c r="AD37" s="20"/>
+      <c r="AE37" s="21"/>
       <c r="AF37" s="11">
         <v>43416</v>
       </c>
@@ -4829,36 +4838,36 @@
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
-      <c r="Z38" s="19"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
-      <c r="AD38" s="19"/>
-      <c r="AE38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="20"/>
+      <c r="AE38" s="21"/>
       <c r="AF38" s="11">
         <v>43446</v>
       </c>
@@ -5015,36 +5024,36 @@
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
-      <c r="R40" s="19"/>
-      <c r="S40" s="19"/>
-      <c r="T40" s="19"/>
-      <c r="U40" s="19"/>
-      <c r="V40" s="19"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="19"/>
-      <c r="Y40" s="19"/>
-      <c r="Z40" s="19"/>
-      <c r="AA40" s="19"/>
-      <c r="AB40" s="19"/>
-      <c r="AC40" s="19"/>
-      <c r="AD40" s="19"/>
-      <c r="AE40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="20"/>
+      <c r="X40" s="20"/>
+      <c r="Y40" s="20"/>
+      <c r="Z40" s="20"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="20"/>
+      <c r="AC40" s="20"/>
+      <c r="AD40" s="20"/>
+      <c r="AE40" s="21"/>
       <c r="AF40" s="11">
         <v>43447</v>
       </c>
@@ -5201,36 +5210,36 @@
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
-      <c r="Y42" s="19"/>
-      <c r="Z42" s="19"/>
-      <c r="AA42" s="19"/>
-      <c r="AB42" s="19"/>
-      <c r="AC42" s="19"/>
-      <c r="AD42" s="19"/>
-      <c r="AE42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="20"/>
+      <c r="AA42" s="20"/>
+      <c r="AB42" s="20"/>
+      <c r="AC42" s="20"/>
+      <c r="AD42" s="20"/>
+      <c r="AE42" s="21"/>
       <c r="AF42" s="11" t="s">
         <v>55</v>
       </c>
@@ -5294,36 +5303,36 @@
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
-      <c r="S43" s="19"/>
-      <c r="T43" s="19"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="19"/>
-      <c r="Y43" s="19"/>
-      <c r="Z43" s="19"/>
-      <c r="AA43" s="19"/>
-      <c r="AB43" s="19"/>
-      <c r="AC43" s="19"/>
-      <c r="AD43" s="19"/>
-      <c r="AE43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="20"/>
+      <c r="X43" s="20"/>
+      <c r="Y43" s="20"/>
+      <c r="Z43" s="20"/>
+      <c r="AA43" s="20"/>
+      <c r="AB43" s="20"/>
+      <c r="AC43" s="20"/>
+      <c r="AD43" s="20"/>
+      <c r="AE43" s="21"/>
       <c r="AF43" s="11" t="s">
         <v>55</v>
       </c>
@@ -5387,36 +5396,36 @@
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="18" t="s">
+      <c r="D44" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-      <c r="Y44" s="19"/>
-      <c r="Z44" s="19"/>
-      <c r="AA44" s="19"/>
-      <c r="AB44" s="19"/>
-      <c r="AC44" s="19"/>
-      <c r="AD44" s="19"/>
-      <c r="AE44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="20"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="20"/>
+      <c r="AD44" s="20"/>
+      <c r="AE44" s="21"/>
       <c r="AF44" s="11" t="s">
         <v>58</v>
       </c>
@@ -12342,71 +12351,71 @@
       </c>
       <c r="B119" s="9"/>
       <c r="C119" s="5"/>
-      <c r="D119" s="18" t="s">
+      <c r="D119" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="E119" s="19"/>
-      <c r="F119" s="19"/>
-      <c r="G119" s="19"/>
-      <c r="H119" s="19"/>
-      <c r="I119" s="19"/>
-      <c r="J119" s="19"/>
-      <c r="K119" s="19"/>
-      <c r="L119" s="19"/>
-      <c r="M119" s="19"/>
-      <c r="N119" s="19"/>
-      <c r="O119" s="19"/>
-      <c r="P119" s="19"/>
-      <c r="Q119" s="19"/>
-      <c r="R119" s="19"/>
-      <c r="S119" s="19"/>
-      <c r="T119" s="19"/>
-      <c r="U119" s="19"/>
-      <c r="V119" s="19"/>
-      <c r="W119" s="19"/>
-      <c r="X119" s="19"/>
-      <c r="Y119" s="19"/>
-      <c r="Z119" s="19"/>
-      <c r="AA119" s="19"/>
-      <c r="AB119" s="19"/>
-      <c r="AC119" s="19"/>
-      <c r="AD119" s="19"/>
-      <c r="AE119" s="20"/>
-      <c r="AF119" s="39" t="s">
+      <c r="E119" s="20"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="20"/>
+      <c r="H119" s="20"/>
+      <c r="I119" s="20"/>
+      <c r="J119" s="20"/>
+      <c r="K119" s="20"/>
+      <c r="L119" s="20"/>
+      <c r="M119" s="20"/>
+      <c r="N119" s="20"/>
+      <c r="O119" s="20"/>
+      <c r="P119" s="20"/>
+      <c r="Q119" s="20"/>
+      <c r="R119" s="20"/>
+      <c r="S119" s="20"/>
+      <c r="T119" s="20"/>
+      <c r="U119" s="20"/>
+      <c r="V119" s="20"/>
+      <c r="W119" s="20"/>
+      <c r="X119" s="20"/>
+      <c r="Y119" s="20"/>
+      <c r="Z119" s="20"/>
+      <c r="AA119" s="20"/>
+      <c r="AB119" s="20"/>
+      <c r="AC119" s="20"/>
+      <c r="AD119" s="20"/>
+      <c r="AE119" s="21"/>
+      <c r="AF119" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="AG119" s="40"/>
-      <c r="AH119" s="40"/>
-      <c r="AI119" s="40"/>
-      <c r="AJ119" s="41"/>
-      <c r="AK119" s="18" t="s">
+      <c r="AG119" s="26"/>
+      <c r="AH119" s="26"/>
+      <c r="AI119" s="26"/>
+      <c r="AJ119" s="27"/>
+      <c r="AK119" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AL119" s="19"/>
-      <c r="AM119" s="19"/>
-      <c r="AN119" s="19"/>
-      <c r="AO119" s="20"/>
-      <c r="AP119" s="36">
+      <c r="AL119" s="20"/>
+      <c r="AM119" s="20"/>
+      <c r="AN119" s="20"/>
+      <c r="AO119" s="21"/>
+      <c r="AP119" s="22">
         <v>1</v>
       </c>
-      <c r="AQ119" s="37"/>
-      <c r="AR119" s="38"/>
-      <c r="AS119" s="18" t="s">
+      <c r="AQ119" s="23"/>
+      <c r="AR119" s="24"/>
+      <c r="AS119" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AT119" s="19"/>
-      <c r="AU119" s="19"/>
-      <c r="AV119" s="19"/>
-      <c r="AW119" s="19"/>
-      <c r="AX119" s="19"/>
-      <c r="AY119" s="19"/>
-      <c r="AZ119" s="19"/>
-      <c r="BA119" s="19"/>
-      <c r="BB119" s="19"/>
-      <c r="BC119" s="19"/>
-      <c r="BD119" s="19"/>
-      <c r="BE119" s="19"/>
-      <c r="BF119" s="20"/>
+      <c r="AT119" s="20"/>
+      <c r="AU119" s="20"/>
+      <c r="AV119" s="20"/>
+      <c r="AW119" s="20"/>
+      <c r="AX119" s="20"/>
+      <c r="AY119" s="20"/>
+      <c r="AZ119" s="20"/>
+      <c r="BA119" s="20"/>
+      <c r="BB119" s="20"/>
+      <c r="BC119" s="20"/>
+      <c r="BD119" s="20"/>
+      <c r="BE119" s="20"/>
+      <c r="BF119" s="21"/>
       <c r="BG119" s="13"/>
       <c r="BH119" s="13"/>
       <c r="BI119" s="13"/>
@@ -13702,10 +13711,10 @@
       <c r="CA133" s="13"/>
     </row>
     <row r="134" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A134" s="31">
+      <c r="A134" s="18">
         <v>133</v>
       </c>
-      <c r="B134" s="31"/>
+      <c r="B134" s="18"/>
       <c r="C134" s="5"/>
       <c r="D134" s="10" t="s">
         <v>148</v>
@@ -14710,61 +14719,61 @@
       </c>
       <c r="B145" s="15"/>
       <c r="C145" s="5"/>
-      <c r="D145" s="10"/>
-      <c r="E145" s="10"/>
-      <c r="F145" s="10"/>
-      <c r="G145" s="10"/>
-      <c r="H145" s="10"/>
-      <c r="I145" s="10"/>
-      <c r="J145" s="10"/>
-      <c r="K145" s="10"/>
-      <c r="L145" s="10"/>
-      <c r="M145" s="10"/>
-      <c r="N145" s="10"/>
-      <c r="O145" s="10"/>
-      <c r="P145" s="10"/>
-      <c r="Q145" s="10"/>
-      <c r="R145" s="10"/>
-      <c r="S145" s="10"/>
-      <c r="T145" s="10"/>
-      <c r="U145" s="10"/>
-      <c r="V145" s="10"/>
-      <c r="W145" s="10"/>
-      <c r="X145" s="10"/>
-      <c r="Y145" s="10"/>
-      <c r="Z145" s="10"/>
-      <c r="AA145" s="10"/>
-      <c r="AB145" s="10"/>
-      <c r="AC145" s="10"/>
-      <c r="AD145" s="10"/>
-      <c r="AE145" s="10"/>
-      <c r="AF145" s="11"/>
-      <c r="AG145" s="11"/>
-      <c r="AH145" s="11"/>
-      <c r="AI145" s="11"/>
-      <c r="AJ145" s="11"/>
-      <c r="AK145" s="10"/>
-      <c r="AL145" s="10"/>
-      <c r="AM145" s="10"/>
-      <c r="AN145" s="10"/>
-      <c r="AO145" s="10"/>
-      <c r="AP145" s="12"/>
-      <c r="AQ145" s="12"/>
-      <c r="AR145" s="12"/>
-      <c r="AS145" s="10"/>
-      <c r="AT145" s="10"/>
-      <c r="AU145" s="10"/>
-      <c r="AV145" s="10"/>
-      <c r="AW145" s="10"/>
-      <c r="AX145" s="10"/>
-      <c r="AY145" s="10"/>
-      <c r="AZ145" s="10"/>
-      <c r="BA145" s="10"/>
-      <c r="BB145" s="10"/>
-      <c r="BC145" s="10"/>
-      <c r="BD145" s="10"/>
-      <c r="BE145" s="10"/>
-      <c r="BF145" s="10"/>
+      <c r="D145" s="19"/>
+      <c r="E145" s="20"/>
+      <c r="F145" s="20"/>
+      <c r="G145" s="20"/>
+      <c r="H145" s="20"/>
+      <c r="I145" s="20"/>
+      <c r="J145" s="20"/>
+      <c r="K145" s="20"/>
+      <c r="L145" s="20"/>
+      <c r="M145" s="20"/>
+      <c r="N145" s="20"/>
+      <c r="O145" s="20"/>
+      <c r="P145" s="20"/>
+      <c r="Q145" s="20"/>
+      <c r="R145" s="20"/>
+      <c r="S145" s="20"/>
+      <c r="T145" s="20"/>
+      <c r="U145" s="20"/>
+      <c r="V145" s="20"/>
+      <c r="W145" s="20"/>
+      <c r="X145" s="20"/>
+      <c r="Y145" s="20"/>
+      <c r="Z145" s="20"/>
+      <c r="AA145" s="20"/>
+      <c r="AB145" s="20"/>
+      <c r="AC145" s="20"/>
+      <c r="AD145" s="20"/>
+      <c r="AE145" s="21"/>
+      <c r="AF145" s="25"/>
+      <c r="AG145" s="26"/>
+      <c r="AH145" s="26"/>
+      <c r="AI145" s="26"/>
+      <c r="AJ145" s="27"/>
+      <c r="AK145" s="19"/>
+      <c r="AL145" s="20"/>
+      <c r="AM145" s="20"/>
+      <c r="AN145" s="20"/>
+      <c r="AO145" s="21"/>
+      <c r="AP145" s="22"/>
+      <c r="AQ145" s="23"/>
+      <c r="AR145" s="24"/>
+      <c r="AS145" s="19"/>
+      <c r="AT145" s="20"/>
+      <c r="AU145" s="20"/>
+      <c r="AV145" s="20"/>
+      <c r="AW145" s="20"/>
+      <c r="AX145" s="20"/>
+      <c r="AY145" s="20"/>
+      <c r="AZ145" s="20"/>
+      <c r="BA145" s="20"/>
+      <c r="BB145" s="20"/>
+      <c r="BC145" s="20"/>
+      <c r="BD145" s="20"/>
+      <c r="BE145" s="20"/>
+      <c r="BF145" s="21"/>
       <c r="BG145" s="13"/>
       <c r="BH145" s="13"/>
       <c r="BI145" s="13"/>
@@ -14793,7 +14802,9 @@
       </c>
       <c r="B146" s="17"/>
       <c r="C146" s="5"/>
-      <c r="D146" s="10"/>
+      <c r="D146" s="10" t="s">
+        <v>158</v>
+      </c>
       <c r="E146" s="10"/>
       <c r="F146" s="10"/>
       <c r="G146" s="10"/>
@@ -14821,20 +14832,28 @@
       <c r="AC146" s="10"/>
       <c r="AD146" s="10"/>
       <c r="AE146" s="10"/>
-      <c r="AF146" s="11"/>
+      <c r="AF146" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="AG146" s="11"/>
       <c r="AH146" s="11"/>
       <c r="AI146" s="11"/>
       <c r="AJ146" s="11"/>
-      <c r="AK146" s="10"/>
+      <c r="AK146" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="AL146" s="10"/>
       <c r="AM146" s="10"/>
       <c r="AN146" s="10"/>
       <c r="AO146" s="10"/>
-      <c r="AP146" s="12"/>
+      <c r="AP146" s="12">
+        <v>1</v>
+      </c>
       <c r="AQ146" s="12"/>
       <c r="AR146" s="12"/>
-      <c r="AS146" s="10"/>
+      <c r="AS146" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="AT146" s="10"/>
       <c r="AU146" s="10"/>
       <c r="AV146" s="10"/>
@@ -14876,7 +14895,9 @@
       </c>
       <c r="B147" s="9"/>
       <c r="C147" s="5"/>
-      <c r="D147" s="10"/>
+      <c r="D147" s="10" t="s">
+        <v>160</v>
+      </c>
       <c r="E147" s="10"/>
       <c r="F147" s="10"/>
       <c r="G147" s="10"/>
@@ -14904,20 +14925,28 @@
       <c r="AC147" s="10"/>
       <c r="AD147" s="10"/>
       <c r="AE147" s="10"/>
-      <c r="AF147" s="11"/>
+      <c r="AF147" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="AG147" s="11"/>
       <c r="AH147" s="11"/>
       <c r="AI147" s="11"/>
       <c r="AJ147" s="11"/>
-      <c r="AK147" s="10"/>
+      <c r="AK147" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="AL147" s="10"/>
       <c r="AM147" s="10"/>
       <c r="AN147" s="10"/>
       <c r="AO147" s="10"/>
-      <c r="AP147" s="12"/>
+      <c r="AP147" s="12">
+        <v>1</v>
+      </c>
       <c r="AQ147" s="12"/>
       <c r="AR147" s="12"/>
-      <c r="AS147" s="10"/>
+      <c r="AS147" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="AT147" s="10"/>
       <c r="AU147" s="10"/>
       <c r="AV147" s="10"/>
@@ -14959,7 +14988,9 @@
       </c>
       <c r="B148" s="9"/>
       <c r="C148" s="5"/>
-      <c r="D148" s="10"/>
+      <c r="D148" s="10" t="s">
+        <v>161</v>
+      </c>
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
       <c r="G148" s="10"/>
@@ -14987,20 +15018,28 @@
       <c r="AC148" s="10"/>
       <c r="AD148" s="10"/>
       <c r="AE148" s="10"/>
-      <c r="AF148" s="11"/>
+      <c r="AF148" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="AG148" s="11"/>
       <c r="AH148" s="11"/>
       <c r="AI148" s="11"/>
       <c r="AJ148" s="11"/>
-      <c r="AK148" s="10"/>
+      <c r="AK148" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="AL148" s="10"/>
       <c r="AM148" s="10"/>
       <c r="AN148" s="10"/>
       <c r="AO148" s="10"/>
-      <c r="AP148" s="12"/>
+      <c r="AP148" s="12">
+        <v>1</v>
+      </c>
       <c r="AQ148" s="12"/>
       <c r="AR148" s="12"/>
-      <c r="AS148" s="10"/>
+      <c r="AS148" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="AT148" s="10"/>
       <c r="AU148" s="10"/>
       <c r="AV148" s="10"/>
@@ -19354,557 +19393,823 @@
     </row>
   </sheetData>
   <mergeCells count="1400">
-    <mergeCell ref="A199:B199"/>
-    <mergeCell ref="D199:AE199"/>
-    <mergeCell ref="AF199:AJ199"/>
-    <mergeCell ref="AK199:AO199"/>
-    <mergeCell ref="AP199:AR199"/>
-    <mergeCell ref="AS199:BF199"/>
-    <mergeCell ref="BG199:CA199"/>
-    <mergeCell ref="A200:B200"/>
-    <mergeCell ref="D200:AE200"/>
-    <mergeCell ref="AF200:AJ200"/>
-    <mergeCell ref="AK200:AO200"/>
-    <mergeCell ref="AP200:AR200"/>
-    <mergeCell ref="AS200:BF200"/>
-    <mergeCell ref="BG200:CA200"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="D197:AE197"/>
-    <mergeCell ref="AF197:AJ197"/>
-    <mergeCell ref="AK197:AO197"/>
-    <mergeCell ref="AP197:AR197"/>
-    <mergeCell ref="AS197:BF197"/>
-    <mergeCell ref="BG197:CA197"/>
-    <mergeCell ref="A198:B198"/>
-    <mergeCell ref="D198:AE198"/>
-    <mergeCell ref="AF198:AJ198"/>
-    <mergeCell ref="AK198:AO198"/>
-    <mergeCell ref="AP198:AR198"/>
-    <mergeCell ref="AS198:BF198"/>
-    <mergeCell ref="BG198:CA198"/>
-    <mergeCell ref="A195:B195"/>
-    <mergeCell ref="D195:AE195"/>
-    <mergeCell ref="AF195:AJ195"/>
-    <mergeCell ref="AK195:AO195"/>
-    <mergeCell ref="AP195:AR195"/>
-    <mergeCell ref="AS195:BF195"/>
-    <mergeCell ref="BG195:CA195"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="D196:AE196"/>
-    <mergeCell ref="AF196:AJ196"/>
-    <mergeCell ref="AK196:AO196"/>
-    <mergeCell ref="AP196:AR196"/>
-    <mergeCell ref="AS196:BF196"/>
-    <mergeCell ref="BG196:CA196"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="D193:AE193"/>
-    <mergeCell ref="AF193:AJ193"/>
-    <mergeCell ref="AK193:AO193"/>
-    <mergeCell ref="AP193:AR193"/>
-    <mergeCell ref="AS193:BF193"/>
-    <mergeCell ref="BG193:CA193"/>
-    <mergeCell ref="A194:B194"/>
-    <mergeCell ref="D194:AE194"/>
-    <mergeCell ref="AF194:AJ194"/>
-    <mergeCell ref="AK194:AO194"/>
-    <mergeCell ref="AP194:AR194"/>
-    <mergeCell ref="AS194:BF194"/>
-    <mergeCell ref="BG194:CA194"/>
-    <mergeCell ref="A191:B191"/>
-    <mergeCell ref="D191:AE191"/>
-    <mergeCell ref="AF191:AJ191"/>
-    <mergeCell ref="AK191:AO191"/>
-    <mergeCell ref="AP191:AR191"/>
-    <mergeCell ref="AS191:BF191"/>
-    <mergeCell ref="BG191:CA191"/>
-    <mergeCell ref="A192:B192"/>
-    <mergeCell ref="D192:AE192"/>
-    <mergeCell ref="AF192:AJ192"/>
-    <mergeCell ref="AK192:AO192"/>
-    <mergeCell ref="AP192:AR192"/>
-    <mergeCell ref="AS192:BF192"/>
-    <mergeCell ref="BG192:CA192"/>
-    <mergeCell ref="A189:B189"/>
-    <mergeCell ref="D189:AE189"/>
-    <mergeCell ref="AF189:AJ189"/>
-    <mergeCell ref="AK189:AO189"/>
-    <mergeCell ref="AP189:AR189"/>
-    <mergeCell ref="AS189:BF189"/>
-    <mergeCell ref="BG189:CA189"/>
-    <mergeCell ref="A190:B190"/>
-    <mergeCell ref="D190:AE190"/>
-    <mergeCell ref="AF190:AJ190"/>
-    <mergeCell ref="AK190:AO190"/>
-    <mergeCell ref="AP190:AR190"/>
-    <mergeCell ref="AS190:BF190"/>
-    <mergeCell ref="BG190:CA190"/>
-    <mergeCell ref="AK187:AO187"/>
-    <mergeCell ref="AP187:AR187"/>
-    <mergeCell ref="AS187:BF187"/>
-    <mergeCell ref="BG187:CA187"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="D188:AE188"/>
-    <mergeCell ref="AF188:AJ188"/>
-    <mergeCell ref="AK188:AO188"/>
-    <mergeCell ref="AP188:AR188"/>
-    <mergeCell ref="AS188:BF188"/>
-    <mergeCell ref="BG188:CA188"/>
-    <mergeCell ref="A185:B185"/>
-    <mergeCell ref="D185:AE185"/>
-    <mergeCell ref="AF185:AJ185"/>
-    <mergeCell ref="AK185:AO185"/>
-    <mergeCell ref="AP185:AR185"/>
-    <mergeCell ref="AS185:BF185"/>
-    <mergeCell ref="BG185:CA185"/>
-    <mergeCell ref="A186:B186"/>
-    <mergeCell ref="D186:AE186"/>
-    <mergeCell ref="AF186:AJ186"/>
-    <mergeCell ref="AK186:AO186"/>
-    <mergeCell ref="AP186:AR186"/>
-    <mergeCell ref="AS186:BF186"/>
-    <mergeCell ref="BG186:CA186"/>
-    <mergeCell ref="A187:B187"/>
-    <mergeCell ref="D187:AE187"/>
-    <mergeCell ref="AF187:AJ187"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="D183:AE183"/>
-    <mergeCell ref="AF183:AJ183"/>
-    <mergeCell ref="AK183:AO183"/>
-    <mergeCell ref="AP183:AR183"/>
-    <mergeCell ref="AS183:BF183"/>
-    <mergeCell ref="BG183:CA183"/>
-    <mergeCell ref="A184:B184"/>
-    <mergeCell ref="D184:AE184"/>
-    <mergeCell ref="AF184:AJ184"/>
-    <mergeCell ref="AK184:AO184"/>
-    <mergeCell ref="AP184:AR184"/>
-    <mergeCell ref="AS184:BF184"/>
-    <mergeCell ref="BG184:CA184"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="D181:AE181"/>
-    <mergeCell ref="AF181:AJ181"/>
-    <mergeCell ref="AK181:AO181"/>
-    <mergeCell ref="AP181:AR181"/>
-    <mergeCell ref="AS181:BF181"/>
-    <mergeCell ref="BG181:CA181"/>
-    <mergeCell ref="A182:B182"/>
-    <mergeCell ref="D182:AE182"/>
-    <mergeCell ref="AF182:AJ182"/>
-    <mergeCell ref="AK182:AO182"/>
-    <mergeCell ref="AP182:AR182"/>
-    <mergeCell ref="AS182:BF182"/>
-    <mergeCell ref="BG182:CA182"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="D179:AE179"/>
-    <mergeCell ref="AF179:AJ179"/>
-    <mergeCell ref="AK179:AO179"/>
-    <mergeCell ref="AP179:AR179"/>
-    <mergeCell ref="AS179:BF179"/>
-    <mergeCell ref="BG179:CA179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="D180:AE180"/>
-    <mergeCell ref="AF180:AJ180"/>
-    <mergeCell ref="AK180:AO180"/>
-    <mergeCell ref="AP180:AR180"/>
-    <mergeCell ref="AS180:BF180"/>
-    <mergeCell ref="BG180:CA180"/>
-    <mergeCell ref="A177:B177"/>
-    <mergeCell ref="D177:AE177"/>
-    <mergeCell ref="AF177:AJ177"/>
-    <mergeCell ref="AK177:AO177"/>
-    <mergeCell ref="AP177:AR177"/>
-    <mergeCell ref="AS177:BF177"/>
-    <mergeCell ref="BG177:CA177"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="D178:AE178"/>
-    <mergeCell ref="AF178:AJ178"/>
-    <mergeCell ref="AK178:AO178"/>
-    <mergeCell ref="AP178:AR178"/>
-    <mergeCell ref="AS178:BF178"/>
-    <mergeCell ref="BG178:CA178"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="D175:AE175"/>
-    <mergeCell ref="AF175:AJ175"/>
-    <mergeCell ref="AK175:AO175"/>
-    <mergeCell ref="AP175:AR175"/>
-    <mergeCell ref="AS175:BF175"/>
-    <mergeCell ref="BG175:CA175"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="D176:AE176"/>
-    <mergeCell ref="AF176:AJ176"/>
-    <mergeCell ref="AK176:AO176"/>
-    <mergeCell ref="AP176:AR176"/>
-    <mergeCell ref="AS176:BF176"/>
-    <mergeCell ref="BG176:CA176"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="D173:AE173"/>
-    <mergeCell ref="AF173:AJ173"/>
-    <mergeCell ref="AK173:AO173"/>
-    <mergeCell ref="AP173:AR173"/>
-    <mergeCell ref="AS173:BF173"/>
-    <mergeCell ref="BG173:CA173"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="D174:AE174"/>
-    <mergeCell ref="AF174:AJ174"/>
-    <mergeCell ref="AK174:AO174"/>
-    <mergeCell ref="AP174:AR174"/>
-    <mergeCell ref="AS174:BF174"/>
-    <mergeCell ref="BG174:CA174"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="D171:AE171"/>
-    <mergeCell ref="AF171:AJ171"/>
-    <mergeCell ref="AK171:AO171"/>
-    <mergeCell ref="AP171:AR171"/>
-    <mergeCell ref="AS171:BF171"/>
-    <mergeCell ref="BG171:CA171"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="D172:AE172"/>
-    <mergeCell ref="AF172:AJ172"/>
-    <mergeCell ref="AK172:AO172"/>
-    <mergeCell ref="AP172:AR172"/>
-    <mergeCell ref="AS172:BF172"/>
-    <mergeCell ref="BG172:CA172"/>
-    <mergeCell ref="A169:B169"/>
-    <mergeCell ref="D169:AE169"/>
-    <mergeCell ref="AF169:AJ169"/>
-    <mergeCell ref="AK169:AO169"/>
-    <mergeCell ref="AP169:AR169"/>
-    <mergeCell ref="AS169:BF169"/>
-    <mergeCell ref="BG169:CA169"/>
-    <mergeCell ref="A170:B170"/>
-    <mergeCell ref="D170:AE170"/>
-    <mergeCell ref="AF170:AJ170"/>
-    <mergeCell ref="AK170:AO170"/>
-    <mergeCell ref="AP170:AR170"/>
-    <mergeCell ref="AS170:BF170"/>
-    <mergeCell ref="BG170:CA170"/>
-    <mergeCell ref="A167:B167"/>
-    <mergeCell ref="D167:AE167"/>
-    <mergeCell ref="AF167:AJ167"/>
-    <mergeCell ref="AK167:AO167"/>
-    <mergeCell ref="AP167:AR167"/>
-    <mergeCell ref="AS167:BF167"/>
-    <mergeCell ref="BG167:CA167"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="D168:AE168"/>
-    <mergeCell ref="AF168:AJ168"/>
-    <mergeCell ref="AK168:AO168"/>
-    <mergeCell ref="AP168:AR168"/>
-    <mergeCell ref="AS168:BF168"/>
-    <mergeCell ref="BG168:CA168"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="D165:AE165"/>
-    <mergeCell ref="AF165:AJ165"/>
-    <mergeCell ref="AK165:AO165"/>
-    <mergeCell ref="AP165:AR165"/>
-    <mergeCell ref="AS165:BF165"/>
-    <mergeCell ref="BG165:CA165"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="D166:AE166"/>
-    <mergeCell ref="AF166:AJ166"/>
-    <mergeCell ref="AK166:AO166"/>
-    <mergeCell ref="AP166:AR166"/>
-    <mergeCell ref="AS166:BF166"/>
-    <mergeCell ref="BG166:CA166"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="D163:AE163"/>
-    <mergeCell ref="AF163:AJ163"/>
-    <mergeCell ref="AK163:AO163"/>
-    <mergeCell ref="AP163:AR163"/>
-    <mergeCell ref="AS163:BF163"/>
-    <mergeCell ref="BG163:CA163"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="D164:AE164"/>
-    <mergeCell ref="AF164:AJ164"/>
-    <mergeCell ref="AK164:AO164"/>
-    <mergeCell ref="AP164:AR164"/>
-    <mergeCell ref="AS164:BF164"/>
-    <mergeCell ref="BG164:CA164"/>
-    <mergeCell ref="A161:B161"/>
-    <mergeCell ref="D161:AE161"/>
-    <mergeCell ref="AF161:AJ161"/>
-    <mergeCell ref="AK161:AO161"/>
-    <mergeCell ref="AP161:AR161"/>
-    <mergeCell ref="AS161:BF161"/>
-    <mergeCell ref="BG161:CA161"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="D162:AE162"/>
-    <mergeCell ref="AF162:AJ162"/>
-    <mergeCell ref="AK162:AO162"/>
-    <mergeCell ref="AP162:AR162"/>
-    <mergeCell ref="AS162:BF162"/>
-    <mergeCell ref="BG162:CA162"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="D159:AE159"/>
-    <mergeCell ref="AF159:AJ159"/>
-    <mergeCell ref="AK159:AO159"/>
-    <mergeCell ref="AP159:AR159"/>
-    <mergeCell ref="AS159:BF159"/>
-    <mergeCell ref="BG159:CA159"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="D160:AE160"/>
-    <mergeCell ref="AF160:AJ160"/>
-    <mergeCell ref="AK160:AO160"/>
-    <mergeCell ref="AP160:AR160"/>
-    <mergeCell ref="AS160:BF160"/>
-    <mergeCell ref="BG160:CA160"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="D157:AE157"/>
-    <mergeCell ref="AF157:AJ157"/>
-    <mergeCell ref="AK157:AO157"/>
-    <mergeCell ref="AP157:AR157"/>
-    <mergeCell ref="AS157:BF157"/>
-    <mergeCell ref="BG157:CA157"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="D158:AE158"/>
-    <mergeCell ref="AF158:AJ158"/>
-    <mergeCell ref="AK158:AO158"/>
-    <mergeCell ref="AP158:AR158"/>
-    <mergeCell ref="AS158:BF158"/>
-    <mergeCell ref="BG158:CA158"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="D155:AE155"/>
-    <mergeCell ref="AF155:AJ155"/>
-    <mergeCell ref="AK155:AO155"/>
-    <mergeCell ref="AP155:AR155"/>
-    <mergeCell ref="AS155:BF155"/>
-    <mergeCell ref="BG155:CA155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="D156:AE156"/>
-    <mergeCell ref="AF156:AJ156"/>
-    <mergeCell ref="AK156:AO156"/>
-    <mergeCell ref="AP156:AR156"/>
-    <mergeCell ref="AS156:BF156"/>
-    <mergeCell ref="BG156:CA156"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="D153:AE153"/>
-    <mergeCell ref="AF153:AJ153"/>
-    <mergeCell ref="AK153:AO153"/>
-    <mergeCell ref="AP153:AR153"/>
-    <mergeCell ref="AS153:BF153"/>
-    <mergeCell ref="BG153:CA153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="D154:AE154"/>
-    <mergeCell ref="AF154:AJ154"/>
-    <mergeCell ref="AK154:AO154"/>
-    <mergeCell ref="AP154:AR154"/>
-    <mergeCell ref="AS154:BF154"/>
-    <mergeCell ref="BG154:CA154"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="D151:AE151"/>
-    <mergeCell ref="AF151:AJ151"/>
-    <mergeCell ref="AK151:AO151"/>
-    <mergeCell ref="AP151:AR151"/>
-    <mergeCell ref="AS151:BF151"/>
-    <mergeCell ref="BG151:CA151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="D152:AE152"/>
-    <mergeCell ref="AF152:AJ152"/>
-    <mergeCell ref="AK152:AO152"/>
-    <mergeCell ref="AP152:AR152"/>
-    <mergeCell ref="AS152:BF152"/>
-    <mergeCell ref="BG152:CA152"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="D149:AE149"/>
-    <mergeCell ref="AF149:AJ149"/>
-    <mergeCell ref="AK149:AO149"/>
-    <mergeCell ref="AP149:AR149"/>
-    <mergeCell ref="AS149:BF149"/>
-    <mergeCell ref="BG149:CA149"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="D150:AE150"/>
-    <mergeCell ref="AF150:AJ150"/>
-    <mergeCell ref="AK150:AO150"/>
-    <mergeCell ref="AP150:AR150"/>
-    <mergeCell ref="AS150:BF150"/>
-    <mergeCell ref="BG150:CA150"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="D147:AE147"/>
-    <mergeCell ref="AF147:AJ147"/>
-    <mergeCell ref="AK147:AO147"/>
-    <mergeCell ref="AP147:AR147"/>
-    <mergeCell ref="AS147:BF147"/>
-    <mergeCell ref="BG147:CA147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="D148:AE148"/>
-    <mergeCell ref="AF148:AJ148"/>
-    <mergeCell ref="AK148:AO148"/>
-    <mergeCell ref="AP148:AR148"/>
-    <mergeCell ref="AS148:BF148"/>
-    <mergeCell ref="BG148:CA148"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="D145:AE145"/>
-    <mergeCell ref="AF145:AJ145"/>
-    <mergeCell ref="AK145:AO145"/>
-    <mergeCell ref="AP145:AR145"/>
-    <mergeCell ref="AS145:BF145"/>
-    <mergeCell ref="BG145:CA145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="D146:AE146"/>
-    <mergeCell ref="AF146:AJ146"/>
-    <mergeCell ref="AK146:AO146"/>
-    <mergeCell ref="AP146:AR146"/>
-    <mergeCell ref="AS146:BF146"/>
-    <mergeCell ref="BG146:CA146"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="D143:AE143"/>
-    <mergeCell ref="AF143:AJ143"/>
-    <mergeCell ref="AK143:AO143"/>
-    <mergeCell ref="AP143:AR143"/>
-    <mergeCell ref="AS143:BF143"/>
-    <mergeCell ref="BG143:CA143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="D144:AE144"/>
-    <mergeCell ref="AF144:AJ144"/>
-    <mergeCell ref="AK144:AO144"/>
-    <mergeCell ref="AP144:AR144"/>
-    <mergeCell ref="AS144:BF144"/>
-    <mergeCell ref="BG144:CA144"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="D142:AE142"/>
-    <mergeCell ref="AF142:AJ142"/>
-    <mergeCell ref="AK142:AO142"/>
-    <mergeCell ref="AP142:AR142"/>
-    <mergeCell ref="AS142:BF142"/>
-    <mergeCell ref="BG142:CA142"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="D140:AE140"/>
-    <mergeCell ref="AF140:AJ140"/>
-    <mergeCell ref="AK140:AO140"/>
-    <mergeCell ref="AP140:AR140"/>
-    <mergeCell ref="AS140:BF140"/>
-    <mergeCell ref="BG140:CA140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="D141:AE141"/>
-    <mergeCell ref="AF141:AJ141"/>
-    <mergeCell ref="AK141:AO141"/>
-    <mergeCell ref="AP141:AR141"/>
-    <mergeCell ref="AS141:BF141"/>
-    <mergeCell ref="BG141:CA141"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="D138:AE138"/>
-    <mergeCell ref="AF138:AJ138"/>
-    <mergeCell ref="AK138:AO138"/>
-    <mergeCell ref="AP138:AR138"/>
-    <mergeCell ref="AS138:BF138"/>
-    <mergeCell ref="BG138:CA138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="D139:AE139"/>
-    <mergeCell ref="AF139:AJ139"/>
-    <mergeCell ref="AK139:AO139"/>
-    <mergeCell ref="AP139:AR139"/>
-    <mergeCell ref="AS139:BF139"/>
-    <mergeCell ref="BG139:CA139"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="D136:AE136"/>
-    <mergeCell ref="AF136:AJ136"/>
-    <mergeCell ref="AK136:AO136"/>
-    <mergeCell ref="AP136:AR136"/>
-    <mergeCell ref="AS136:BF136"/>
-    <mergeCell ref="BG136:CA136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="D137:AE137"/>
-    <mergeCell ref="AF137:AJ137"/>
-    <mergeCell ref="AK137:AO137"/>
-    <mergeCell ref="AP137:AR137"/>
-    <mergeCell ref="AS137:BF137"/>
-    <mergeCell ref="BG137:CA137"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="D134:AE134"/>
-    <mergeCell ref="AF134:AJ134"/>
-    <mergeCell ref="AK134:AO134"/>
-    <mergeCell ref="AP134:AR134"/>
-    <mergeCell ref="AS134:BF134"/>
-    <mergeCell ref="BG134:CA134"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="D135:AE135"/>
-    <mergeCell ref="AF135:AJ135"/>
-    <mergeCell ref="AK135:AO135"/>
-    <mergeCell ref="AP135:AR135"/>
-    <mergeCell ref="AS135:BF135"/>
-    <mergeCell ref="BG135:CA135"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="D132:AE132"/>
-    <mergeCell ref="AF132:AJ132"/>
-    <mergeCell ref="AK132:AO132"/>
-    <mergeCell ref="AP132:AR132"/>
-    <mergeCell ref="AS132:BF132"/>
-    <mergeCell ref="BG132:CA132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="BG133:CA133"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="D130:AE130"/>
-    <mergeCell ref="AF130:AJ130"/>
-    <mergeCell ref="AK130:AO130"/>
-    <mergeCell ref="AP130:AR130"/>
-    <mergeCell ref="AS130:BF130"/>
-    <mergeCell ref="BG130:CA130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="D133:AE133"/>
-    <mergeCell ref="AF133:AJ133"/>
-    <mergeCell ref="AK133:AO133"/>
-    <mergeCell ref="AP133:AR133"/>
-    <mergeCell ref="AS133:BF133"/>
-    <mergeCell ref="BG131:CA131"/>
-    <mergeCell ref="D131:AE131"/>
-    <mergeCell ref="AF131:AJ131"/>
-    <mergeCell ref="AK131:AO131"/>
-    <mergeCell ref="AP131:AR131"/>
-    <mergeCell ref="AS131:BF131"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="D128:AE128"/>
-    <mergeCell ref="AF128:AJ128"/>
-    <mergeCell ref="AK128:AO128"/>
-    <mergeCell ref="AP128:AR128"/>
-    <mergeCell ref="AS128:BF128"/>
-    <mergeCell ref="BG128:CA128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="D129:AE129"/>
-    <mergeCell ref="AF129:AJ129"/>
-    <mergeCell ref="AK129:AO129"/>
-    <mergeCell ref="AP129:AR129"/>
-    <mergeCell ref="AS129:BF129"/>
-    <mergeCell ref="BG129:CA129"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="D126:AE126"/>
-    <mergeCell ref="AF126:AJ126"/>
-    <mergeCell ref="AK126:AO126"/>
-    <mergeCell ref="AP126:AR126"/>
-    <mergeCell ref="AS126:BF126"/>
-    <mergeCell ref="BG126:CA126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="D127:AE127"/>
-    <mergeCell ref="AF127:AJ127"/>
-    <mergeCell ref="AK127:AO127"/>
-    <mergeCell ref="AP127:AR127"/>
-    <mergeCell ref="AS127:BF127"/>
-    <mergeCell ref="BG127:CA127"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="D124:AE124"/>
-    <mergeCell ref="AF124:AJ124"/>
-    <mergeCell ref="AK124:AO124"/>
-    <mergeCell ref="AP124:AR124"/>
-    <mergeCell ref="AS124:BF124"/>
-    <mergeCell ref="BG124:CA124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="D125:AE125"/>
-    <mergeCell ref="AF125:AJ125"/>
-    <mergeCell ref="AK125:AO125"/>
-    <mergeCell ref="AP125:AR125"/>
-    <mergeCell ref="AS125:BF125"/>
-    <mergeCell ref="BG125:CA125"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D122:AE122"/>
-    <mergeCell ref="AF122:AJ122"/>
-    <mergeCell ref="AK122:AO122"/>
-    <mergeCell ref="AP122:AR122"/>
-    <mergeCell ref="AS122:BF122"/>
-    <mergeCell ref="BG123:CA123"/>
-    <mergeCell ref="D123:AE123"/>
-    <mergeCell ref="AF123:AJ123"/>
-    <mergeCell ref="AK123:AO123"/>
-    <mergeCell ref="AP123:AR123"/>
-    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:AE68"/>
+    <mergeCell ref="AF68:AJ68"/>
+    <mergeCell ref="AK68:AO68"/>
+    <mergeCell ref="AP68:AR68"/>
+    <mergeCell ref="AS68:BF68"/>
+    <mergeCell ref="BG68:CA68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:AE69"/>
+    <mergeCell ref="AF69:AJ69"/>
+    <mergeCell ref="AK69:AO69"/>
+    <mergeCell ref="AP69:AR69"/>
+    <mergeCell ref="AS69:BF69"/>
+    <mergeCell ref="BG69:CA69"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:AE73"/>
+    <mergeCell ref="AF73:AJ73"/>
+    <mergeCell ref="AK73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:BF73"/>
+    <mergeCell ref="BG73:CA73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:AE71"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AK71:AO71"/>
+    <mergeCell ref="AP71:AR71"/>
+    <mergeCell ref="AS71:BF71"/>
+    <mergeCell ref="BG71:CA71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:AE65"/>
+    <mergeCell ref="AF65:AJ65"/>
+    <mergeCell ref="AK65:AO65"/>
+    <mergeCell ref="AP65:AR65"/>
+    <mergeCell ref="AS65:BF65"/>
+    <mergeCell ref="BG65:CA65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:AE66"/>
+    <mergeCell ref="AF66:AJ66"/>
+    <mergeCell ref="AK66:AO66"/>
+    <mergeCell ref="AP66:AR66"/>
+    <mergeCell ref="AS66:BF66"/>
+    <mergeCell ref="BG66:CA66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:AE67"/>
+    <mergeCell ref="AF67:AJ67"/>
+    <mergeCell ref="AK67:AO67"/>
+    <mergeCell ref="AP67:AR67"/>
+    <mergeCell ref="AS67:BF67"/>
+    <mergeCell ref="BG67:CA67"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:AE62"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AK62:AO62"/>
+    <mergeCell ref="AP62:AR62"/>
+    <mergeCell ref="AS62:BF62"/>
+    <mergeCell ref="BG62:CA62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:AE63"/>
+    <mergeCell ref="AF63:AJ63"/>
+    <mergeCell ref="AK63:AO63"/>
+    <mergeCell ref="AP63:AR63"/>
+    <mergeCell ref="AS63:BF63"/>
+    <mergeCell ref="BG63:CA63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:AE64"/>
+    <mergeCell ref="AF64:AJ64"/>
+    <mergeCell ref="AK64:AO64"/>
+    <mergeCell ref="AP64:AR64"/>
+    <mergeCell ref="AS64:BF64"/>
+    <mergeCell ref="BG64:CA64"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:AE58"/>
+    <mergeCell ref="AF58:AJ58"/>
+    <mergeCell ref="AK58:AO58"/>
+    <mergeCell ref="AP58:AR58"/>
+    <mergeCell ref="AS58:BF58"/>
+    <mergeCell ref="BG58:CA58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:AE61"/>
+    <mergeCell ref="AF61:AJ61"/>
+    <mergeCell ref="AK61:AO61"/>
+    <mergeCell ref="AP61:AR61"/>
+    <mergeCell ref="AS61:BF61"/>
+    <mergeCell ref="BG61:CA61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:AE59"/>
+    <mergeCell ref="AF59:AJ59"/>
+    <mergeCell ref="AK59:AO59"/>
+    <mergeCell ref="AP59:AR59"/>
+    <mergeCell ref="AS59:BF59"/>
+    <mergeCell ref="BG59:CA59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:AE60"/>
+    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AK60:AO60"/>
+    <mergeCell ref="AP60:AR60"/>
+    <mergeCell ref="AS60:BF60"/>
+    <mergeCell ref="BG60:CA60"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:AE55"/>
+    <mergeCell ref="AF55:AJ55"/>
+    <mergeCell ref="AK55:AO55"/>
+    <mergeCell ref="AP55:AR55"/>
+    <mergeCell ref="AS55:BF55"/>
+    <mergeCell ref="BG55:CA55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:AE56"/>
+    <mergeCell ref="AF56:AJ56"/>
+    <mergeCell ref="AK56:AO56"/>
+    <mergeCell ref="AP56:AR56"/>
+    <mergeCell ref="AS56:BF56"/>
+    <mergeCell ref="BG56:CA56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:AE57"/>
+    <mergeCell ref="AF57:AJ57"/>
+    <mergeCell ref="AK57:AO57"/>
+    <mergeCell ref="AP57:AR57"/>
+    <mergeCell ref="AS57:BF57"/>
+    <mergeCell ref="BG57:CA57"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:AE52"/>
+    <mergeCell ref="AF52:AJ52"/>
+    <mergeCell ref="AK52:AO52"/>
+    <mergeCell ref="AP52:AR52"/>
+    <mergeCell ref="AS52:BF52"/>
+    <mergeCell ref="BG52:CA52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:AE53"/>
+    <mergeCell ref="AF53:AJ53"/>
+    <mergeCell ref="AK53:AO53"/>
+    <mergeCell ref="AP53:AR53"/>
+    <mergeCell ref="AS53:BF53"/>
+    <mergeCell ref="BG53:CA53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:AE54"/>
+    <mergeCell ref="AF54:AJ54"/>
+    <mergeCell ref="AK54:AO54"/>
+    <mergeCell ref="AP54:AR54"/>
+    <mergeCell ref="AS54:BF54"/>
+    <mergeCell ref="BG54:CA54"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:AE49"/>
+    <mergeCell ref="AF49:AJ49"/>
+    <mergeCell ref="AK49:AO49"/>
+    <mergeCell ref="AP49:AR49"/>
+    <mergeCell ref="AS49:BF49"/>
+    <mergeCell ref="BG49:CA49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:AE50"/>
+    <mergeCell ref="AF50:AJ50"/>
+    <mergeCell ref="AK50:AO50"/>
+    <mergeCell ref="AP50:AR50"/>
+    <mergeCell ref="AS50:BF50"/>
+    <mergeCell ref="BG50:CA50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:AE51"/>
+    <mergeCell ref="AF51:AJ51"/>
+    <mergeCell ref="AK51:AO51"/>
+    <mergeCell ref="AP51:AR51"/>
+    <mergeCell ref="AS51:BF51"/>
+    <mergeCell ref="BG51:CA51"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:AE46"/>
+    <mergeCell ref="AF46:AJ46"/>
+    <mergeCell ref="AK46:AO46"/>
+    <mergeCell ref="AP46:AR46"/>
+    <mergeCell ref="AS46:BF46"/>
+    <mergeCell ref="BG46:CA46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:AE47"/>
+    <mergeCell ref="AF47:AJ47"/>
+    <mergeCell ref="AK47:AO47"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AS47:BF47"/>
+    <mergeCell ref="BG47:CA47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:AE48"/>
+    <mergeCell ref="AF48:AJ48"/>
+    <mergeCell ref="AK48:AO48"/>
+    <mergeCell ref="AP48:AR48"/>
+    <mergeCell ref="AS48:BF48"/>
+    <mergeCell ref="BG48:CA48"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:AE43"/>
+    <mergeCell ref="AF43:AJ43"/>
+    <mergeCell ref="AK43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:BF43"/>
+    <mergeCell ref="BG43:CA43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:AE44"/>
+    <mergeCell ref="AF44:AJ44"/>
+    <mergeCell ref="AK44:AO44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:BF44"/>
+    <mergeCell ref="BG44:CA44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:AE45"/>
+    <mergeCell ref="AF45:AJ45"/>
+    <mergeCell ref="AK45:AO45"/>
+    <mergeCell ref="AP45:AR45"/>
+    <mergeCell ref="AS45:BF45"/>
+    <mergeCell ref="BG45:CA45"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:AE40"/>
+    <mergeCell ref="AF40:AJ40"/>
+    <mergeCell ref="AK40:AO40"/>
+    <mergeCell ref="AP40:AR40"/>
+    <mergeCell ref="AS40:BF40"/>
+    <mergeCell ref="BG40:CA40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:AE41"/>
+    <mergeCell ref="AF41:AJ41"/>
+    <mergeCell ref="AK41:AO41"/>
+    <mergeCell ref="AP41:AR41"/>
+    <mergeCell ref="AS41:BF41"/>
+    <mergeCell ref="BG41:CA41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:AE42"/>
+    <mergeCell ref="AF42:AJ42"/>
+    <mergeCell ref="AK42:AO42"/>
+    <mergeCell ref="AP42:AR42"/>
+    <mergeCell ref="AS42:BF42"/>
+    <mergeCell ref="BG42:CA42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AR37"/>
+    <mergeCell ref="AS37:BF37"/>
+    <mergeCell ref="BG37:CA37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:AE38"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="AP38:AR38"/>
+    <mergeCell ref="AS38:BF38"/>
+    <mergeCell ref="BG38:CA38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:AE39"/>
+    <mergeCell ref="AF39:AJ39"/>
+    <mergeCell ref="AK39:AO39"/>
+    <mergeCell ref="AP39:AR39"/>
+    <mergeCell ref="AS39:BF39"/>
+    <mergeCell ref="BG39:CA39"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:AE34"/>
+    <mergeCell ref="AF34:AJ34"/>
+    <mergeCell ref="AK34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS34:BF34"/>
+    <mergeCell ref="BG34:CA34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:AE35"/>
+    <mergeCell ref="AF35:AJ35"/>
+    <mergeCell ref="AK35:AO35"/>
+    <mergeCell ref="AP35:AR35"/>
+    <mergeCell ref="AS35:BF35"/>
+    <mergeCell ref="BG35:CA35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:AE36"/>
+    <mergeCell ref="AF36:AJ36"/>
+    <mergeCell ref="AK36:AO36"/>
+    <mergeCell ref="AP36:AR36"/>
+    <mergeCell ref="AS36:BF36"/>
+    <mergeCell ref="BG36:CA36"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="AP31:AR31"/>
+    <mergeCell ref="AS31:BF31"/>
+    <mergeCell ref="BG31:CA31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="AP32:AR32"/>
+    <mergeCell ref="AS32:BF32"/>
+    <mergeCell ref="BG32:CA32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:AE33"/>
+    <mergeCell ref="AF33:AJ33"/>
+    <mergeCell ref="AK33:AO33"/>
+    <mergeCell ref="AP33:AR33"/>
+    <mergeCell ref="AS33:BF33"/>
+    <mergeCell ref="BG33:CA33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:AE28"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AK28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:BF28"/>
+    <mergeCell ref="BG28:CA28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="AP29:AR29"/>
+    <mergeCell ref="AS29:BF29"/>
+    <mergeCell ref="BG29:CA29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="AP30:AR30"/>
+    <mergeCell ref="AS30:BF30"/>
+    <mergeCell ref="BG30:CA30"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:AE25"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AK25:AO25"/>
+    <mergeCell ref="AP25:AR25"/>
+    <mergeCell ref="AS25:BF25"/>
+    <mergeCell ref="BG25:CA25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:AE26"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AK26:AO26"/>
+    <mergeCell ref="AP26:AR26"/>
+    <mergeCell ref="AS26:BF26"/>
+    <mergeCell ref="BG26:CA26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:AE27"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AK27:AO27"/>
+    <mergeCell ref="AP27:AR27"/>
+    <mergeCell ref="AS27:BF27"/>
+    <mergeCell ref="BG27:CA27"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:AE22"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AK22:AO22"/>
+    <mergeCell ref="AP22:AR22"/>
+    <mergeCell ref="AS22:BF22"/>
+    <mergeCell ref="BG22:CA22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:AE23"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AS23:BF23"/>
+    <mergeCell ref="BG23:CA23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AO24"/>
+    <mergeCell ref="AP24:AR24"/>
+    <mergeCell ref="AS24:BF24"/>
+    <mergeCell ref="BG24:CA24"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:AE19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AK19:AO19"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AS19:BF19"/>
+    <mergeCell ref="BG19:CA19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:AE20"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AK20:AO20"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AS20:BF20"/>
+    <mergeCell ref="BG20:CA20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:AE21"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AK21:AO21"/>
+    <mergeCell ref="AP21:AR21"/>
+    <mergeCell ref="AS21:BF21"/>
+    <mergeCell ref="BG21:CA21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:AE16"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AK16:AO16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AS16:BF16"/>
+    <mergeCell ref="BG16:CA16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:AE17"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AK17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AS17:BF17"/>
+    <mergeCell ref="BG17:CA17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:AE18"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AK18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AS18:BF18"/>
+    <mergeCell ref="BG18:CA18"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:AE13"/>
+    <mergeCell ref="AF13:AJ13"/>
+    <mergeCell ref="AK13:AO13"/>
+    <mergeCell ref="AP13:AR13"/>
+    <mergeCell ref="AS13:BF13"/>
+    <mergeCell ref="BG13:CA13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:AE14"/>
+    <mergeCell ref="AF14:AJ14"/>
+    <mergeCell ref="AK14:AO14"/>
+    <mergeCell ref="AP14:AR14"/>
+    <mergeCell ref="AS14:BF14"/>
+    <mergeCell ref="BG14:CA14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:AE15"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AK15:AO15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AS15:BF15"/>
+    <mergeCell ref="BG15:CA15"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:AE10"/>
+    <mergeCell ref="AF10:AJ10"/>
+    <mergeCell ref="AK10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:BF10"/>
+    <mergeCell ref="BG10:CA10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:AE11"/>
+    <mergeCell ref="AF11:AJ11"/>
+    <mergeCell ref="AK11:AO11"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:BF11"/>
+    <mergeCell ref="BG11:CA11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:AE12"/>
+    <mergeCell ref="AF12:AJ12"/>
+    <mergeCell ref="AK12:AO12"/>
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:BF12"/>
+    <mergeCell ref="BG12:CA12"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="AS7:BF7"/>
+    <mergeCell ref="BG7:CA7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:AE8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AS8:BF8"/>
+    <mergeCell ref="BG8:CA8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="AK9:AO9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AS9:BF9"/>
+    <mergeCell ref="BG9:CA9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="AK4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:BF4"/>
+    <mergeCell ref="BG4:CA4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:AE5"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AK5:AO5"/>
+    <mergeCell ref="AP5:AR5"/>
+    <mergeCell ref="AS5:BF5"/>
+    <mergeCell ref="BG5:CA5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="AK6:AO6"/>
+    <mergeCell ref="AP6:AR6"/>
+    <mergeCell ref="AS6:BF6"/>
+    <mergeCell ref="BG6:CA6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AR1"/>
+    <mergeCell ref="AS1:BF1"/>
+    <mergeCell ref="BG1:CA1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:AE2"/>
+    <mergeCell ref="AF2:AJ2"/>
+    <mergeCell ref="AK2:AO2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AS2:BF2"/>
+    <mergeCell ref="BG2:CA2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:CA3"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:AE74"/>
+    <mergeCell ref="AF74:AJ74"/>
+    <mergeCell ref="AK74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:BF74"/>
+    <mergeCell ref="BG74:CA74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:AE75"/>
+    <mergeCell ref="AF75:AJ75"/>
+    <mergeCell ref="AK75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:BF75"/>
+    <mergeCell ref="BG75:CA75"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:AE70"/>
+    <mergeCell ref="AF70:AJ70"/>
+    <mergeCell ref="AK70:AO70"/>
+    <mergeCell ref="AP70:AR70"/>
+    <mergeCell ref="AS70:BF70"/>
+    <mergeCell ref="BG70:CA70"/>
+    <mergeCell ref="AP72:AR72"/>
+    <mergeCell ref="AS72:BF72"/>
+    <mergeCell ref="BG72:CA72"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:AE78"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AK78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:BF78"/>
+    <mergeCell ref="BG78:CA78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:AE79"/>
+    <mergeCell ref="AF79:AJ79"/>
+    <mergeCell ref="AK79:AO79"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AS79:BF79"/>
+    <mergeCell ref="BG79:CA79"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:AE76"/>
+    <mergeCell ref="AF76:AJ76"/>
+    <mergeCell ref="AK76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:BF76"/>
+    <mergeCell ref="BG76:CA76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:AE77"/>
+    <mergeCell ref="AF77:AJ77"/>
+    <mergeCell ref="AK77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:BF77"/>
+    <mergeCell ref="BG77:CA77"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:AE82"/>
+    <mergeCell ref="AF82:AJ82"/>
+    <mergeCell ref="AK82:AO82"/>
+    <mergeCell ref="AP82:AR82"/>
+    <mergeCell ref="AS82:BF82"/>
+    <mergeCell ref="BG82:CA82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:AE83"/>
+    <mergeCell ref="AF83:AJ83"/>
+    <mergeCell ref="AK83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:BF83"/>
+    <mergeCell ref="BG83:CA83"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:AE80"/>
+    <mergeCell ref="AF80:AJ80"/>
+    <mergeCell ref="AK80:AO80"/>
+    <mergeCell ref="AP80:AR80"/>
+    <mergeCell ref="AS80:BF80"/>
+    <mergeCell ref="BG80:CA80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:AE81"/>
+    <mergeCell ref="AF81:AJ81"/>
+    <mergeCell ref="AK81:AO81"/>
+    <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AS81:BF81"/>
+    <mergeCell ref="BG81:CA81"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:AE86"/>
+    <mergeCell ref="AF86:AJ86"/>
+    <mergeCell ref="AK86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="AS86:BF86"/>
+    <mergeCell ref="BG86:CA86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:AE87"/>
+    <mergeCell ref="AF87:AJ87"/>
+    <mergeCell ref="AK87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:BF87"/>
+    <mergeCell ref="BG87:CA87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:AE84"/>
+    <mergeCell ref="AF84:AJ84"/>
+    <mergeCell ref="AK84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:BF84"/>
+    <mergeCell ref="BG84:CA84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:AE85"/>
+    <mergeCell ref="AF85:AJ85"/>
+    <mergeCell ref="AK85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:BF85"/>
+    <mergeCell ref="BG85:CA85"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:AE90"/>
+    <mergeCell ref="AF90:AJ90"/>
+    <mergeCell ref="AK90:AO90"/>
+    <mergeCell ref="AP90:AR90"/>
+    <mergeCell ref="AS90:BF90"/>
+    <mergeCell ref="BG90:CA90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:AE91"/>
+    <mergeCell ref="AF91:AJ91"/>
+    <mergeCell ref="AK91:AO91"/>
+    <mergeCell ref="AP91:AR91"/>
+    <mergeCell ref="AS91:BF91"/>
+    <mergeCell ref="BG91:CA91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D88:AE88"/>
+    <mergeCell ref="AF88:AJ88"/>
+    <mergeCell ref="AK88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:BF88"/>
+    <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D89:AE89"/>
+    <mergeCell ref="AF89:AJ89"/>
+    <mergeCell ref="AK89:AO89"/>
+    <mergeCell ref="AP89:AR89"/>
+    <mergeCell ref="AS89:BF89"/>
+    <mergeCell ref="BG89:CA89"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:AE94"/>
+    <mergeCell ref="AF94:AJ94"/>
+    <mergeCell ref="AK94:AO94"/>
+    <mergeCell ref="AP94:AR94"/>
+    <mergeCell ref="AS94:BF94"/>
+    <mergeCell ref="BG94:CA94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:AE95"/>
+    <mergeCell ref="AF95:AJ95"/>
+    <mergeCell ref="AK95:AO95"/>
+    <mergeCell ref="AP95:AR95"/>
+    <mergeCell ref="AS95:BF95"/>
+    <mergeCell ref="BG95:CA95"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:AE92"/>
+    <mergeCell ref="AF92:AJ92"/>
+    <mergeCell ref="AK92:AO92"/>
+    <mergeCell ref="AP92:AR92"/>
+    <mergeCell ref="AS92:BF92"/>
+    <mergeCell ref="BG92:CA92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:AE93"/>
+    <mergeCell ref="AF93:AJ93"/>
+    <mergeCell ref="AK93:AO93"/>
+    <mergeCell ref="AP93:AR93"/>
+    <mergeCell ref="AS93:BF93"/>
+    <mergeCell ref="BG93:CA93"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:AE98"/>
+    <mergeCell ref="AF98:AJ98"/>
+    <mergeCell ref="AK98:AO98"/>
+    <mergeCell ref="AP98:AR98"/>
+    <mergeCell ref="AS98:BF98"/>
+    <mergeCell ref="BG98:CA98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:AE99"/>
+    <mergeCell ref="AF99:AJ99"/>
+    <mergeCell ref="AK99:AO99"/>
+    <mergeCell ref="AP99:AR99"/>
+    <mergeCell ref="AS99:BF99"/>
+    <mergeCell ref="BG99:CA99"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:AE96"/>
+    <mergeCell ref="AF96:AJ96"/>
+    <mergeCell ref="AK96:AO96"/>
+    <mergeCell ref="AP96:AR96"/>
+    <mergeCell ref="AS96:BF96"/>
+    <mergeCell ref="BG96:CA96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:AE97"/>
+    <mergeCell ref="AF97:AJ97"/>
+    <mergeCell ref="AK97:AO97"/>
+    <mergeCell ref="AP97:AR97"/>
+    <mergeCell ref="AS97:BF97"/>
+    <mergeCell ref="BG97:CA97"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="BG102:CA102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D102:AE102"/>
+    <mergeCell ref="AF102:AJ102"/>
+    <mergeCell ref="AK102:AO102"/>
+    <mergeCell ref="AP102:AR102"/>
+    <mergeCell ref="AS102:BF102"/>
+    <mergeCell ref="BG103:CA103"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="AK100:AO100"/>
+    <mergeCell ref="AP100:AR100"/>
+    <mergeCell ref="AS100:BF100"/>
+    <mergeCell ref="BG100:CA100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="D101:AE101"/>
+    <mergeCell ref="AF101:AJ101"/>
+    <mergeCell ref="AK101:AO101"/>
+    <mergeCell ref="AP101:AR101"/>
+    <mergeCell ref="AS101:BF101"/>
+    <mergeCell ref="BG101:CA101"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D105:AE105"/>
+    <mergeCell ref="AF105:AJ105"/>
+    <mergeCell ref="AK105:AO105"/>
+    <mergeCell ref="AP105:AR105"/>
+    <mergeCell ref="AS105:BF105"/>
+    <mergeCell ref="BG106:CA106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D106:AE106"/>
+    <mergeCell ref="AF106:AJ106"/>
+    <mergeCell ref="AK106:AO106"/>
+    <mergeCell ref="AP106:AR106"/>
+    <mergeCell ref="AS106:BF106"/>
+    <mergeCell ref="BG107:CA107"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D103:AE103"/>
+    <mergeCell ref="AF103:AJ103"/>
+    <mergeCell ref="AK103:AO103"/>
+    <mergeCell ref="AP103:AR103"/>
+    <mergeCell ref="AS103:BF103"/>
+    <mergeCell ref="BG104:CA104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D104:AE104"/>
+    <mergeCell ref="AF104:AJ104"/>
+    <mergeCell ref="AK104:AO104"/>
+    <mergeCell ref="AP104:AR104"/>
+    <mergeCell ref="AS104:BF104"/>
+    <mergeCell ref="BG105:CA105"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D109:AE109"/>
+    <mergeCell ref="AF109:AJ109"/>
+    <mergeCell ref="AK109:AO109"/>
+    <mergeCell ref="AP109:AR109"/>
+    <mergeCell ref="AS109:BF109"/>
+    <mergeCell ref="BG110:CA110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D110:AE110"/>
+    <mergeCell ref="AF110:AJ110"/>
+    <mergeCell ref="AK110:AO110"/>
+    <mergeCell ref="AP110:AR110"/>
+    <mergeCell ref="AS110:BF110"/>
+    <mergeCell ref="BG111:CA111"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D107:AE107"/>
+    <mergeCell ref="AF107:AJ107"/>
+    <mergeCell ref="AK107:AO107"/>
+    <mergeCell ref="AP107:AR107"/>
+    <mergeCell ref="AS107:BF107"/>
+    <mergeCell ref="BG108:CA108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D108:AE108"/>
+    <mergeCell ref="AF108:AJ108"/>
+    <mergeCell ref="AK108:AO108"/>
+    <mergeCell ref="AP108:AR108"/>
+    <mergeCell ref="AS108:BF108"/>
+    <mergeCell ref="BG109:CA109"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="D113:AE113"/>
+    <mergeCell ref="AF113:AJ113"/>
+    <mergeCell ref="AK113:AO113"/>
+    <mergeCell ref="AP113:AR113"/>
+    <mergeCell ref="AS113:BF113"/>
+    <mergeCell ref="BG114:CA114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="D114:AE114"/>
+    <mergeCell ref="AF114:AJ114"/>
+    <mergeCell ref="AK114:AO114"/>
+    <mergeCell ref="AP114:AR114"/>
+    <mergeCell ref="AS114:BF114"/>
+    <mergeCell ref="BG115:CA115"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D111:AE111"/>
+    <mergeCell ref="AF111:AJ111"/>
+    <mergeCell ref="AK111:AO111"/>
+    <mergeCell ref="AP111:AR111"/>
+    <mergeCell ref="AS111:BF111"/>
+    <mergeCell ref="BG112:CA112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D112:AE112"/>
+    <mergeCell ref="AF112:AJ112"/>
+    <mergeCell ref="AK112:AO112"/>
+    <mergeCell ref="AP112:AR112"/>
+    <mergeCell ref="AS112:BF112"/>
+    <mergeCell ref="BG113:CA113"/>
+    <mergeCell ref="AK118:AO118"/>
+    <mergeCell ref="AP118:AR118"/>
+    <mergeCell ref="AS118:BF118"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="D115:AE115"/>
+    <mergeCell ref="AF115:AJ115"/>
+    <mergeCell ref="AK115:AO115"/>
+    <mergeCell ref="AP115:AR115"/>
+    <mergeCell ref="AS115:BF115"/>
+    <mergeCell ref="BG116:CA116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="D116:AE116"/>
+    <mergeCell ref="AF116:AJ116"/>
+    <mergeCell ref="AK116:AO116"/>
+    <mergeCell ref="AP116:AR116"/>
+    <mergeCell ref="AS116:BF116"/>
+    <mergeCell ref="BG117:CA117"/>
     <mergeCell ref="A120:B120"/>
     <mergeCell ref="BG120:CA120"/>
     <mergeCell ref="A121:B121"/>
@@ -19937,823 +20242,557 @@
     <mergeCell ref="D119:AE119"/>
     <mergeCell ref="D118:AE118"/>
     <mergeCell ref="AF118:AJ118"/>
-    <mergeCell ref="AK118:AO118"/>
-    <mergeCell ref="AP118:AR118"/>
-    <mergeCell ref="AS118:BF118"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="D115:AE115"/>
-    <mergeCell ref="AF115:AJ115"/>
-    <mergeCell ref="AK115:AO115"/>
-    <mergeCell ref="AP115:AR115"/>
-    <mergeCell ref="AS115:BF115"/>
-    <mergeCell ref="BG116:CA116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="D116:AE116"/>
-    <mergeCell ref="AF116:AJ116"/>
-    <mergeCell ref="AK116:AO116"/>
-    <mergeCell ref="AP116:AR116"/>
-    <mergeCell ref="AS116:BF116"/>
-    <mergeCell ref="BG117:CA117"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="D113:AE113"/>
-    <mergeCell ref="AF113:AJ113"/>
-    <mergeCell ref="AK113:AO113"/>
-    <mergeCell ref="AP113:AR113"/>
-    <mergeCell ref="AS113:BF113"/>
-    <mergeCell ref="BG114:CA114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="D114:AE114"/>
-    <mergeCell ref="AF114:AJ114"/>
-    <mergeCell ref="AK114:AO114"/>
-    <mergeCell ref="AP114:AR114"/>
-    <mergeCell ref="AS114:BF114"/>
-    <mergeCell ref="BG115:CA115"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D111:AE111"/>
-    <mergeCell ref="AF111:AJ111"/>
-    <mergeCell ref="AK111:AO111"/>
-    <mergeCell ref="AP111:AR111"/>
-    <mergeCell ref="AS111:BF111"/>
-    <mergeCell ref="BG112:CA112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D112:AE112"/>
-    <mergeCell ref="AF112:AJ112"/>
-    <mergeCell ref="AK112:AO112"/>
-    <mergeCell ref="AP112:AR112"/>
-    <mergeCell ref="AS112:BF112"/>
-    <mergeCell ref="BG113:CA113"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D109:AE109"/>
-    <mergeCell ref="AF109:AJ109"/>
-    <mergeCell ref="AK109:AO109"/>
-    <mergeCell ref="AP109:AR109"/>
-    <mergeCell ref="AS109:BF109"/>
-    <mergeCell ref="BG110:CA110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D110:AE110"/>
-    <mergeCell ref="AF110:AJ110"/>
-    <mergeCell ref="AK110:AO110"/>
-    <mergeCell ref="AP110:AR110"/>
-    <mergeCell ref="AS110:BF110"/>
-    <mergeCell ref="BG111:CA111"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D107:AE107"/>
-    <mergeCell ref="AF107:AJ107"/>
-    <mergeCell ref="AK107:AO107"/>
-    <mergeCell ref="AP107:AR107"/>
-    <mergeCell ref="AS107:BF107"/>
-    <mergeCell ref="BG108:CA108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D108:AE108"/>
-    <mergeCell ref="AF108:AJ108"/>
-    <mergeCell ref="AK108:AO108"/>
-    <mergeCell ref="AP108:AR108"/>
-    <mergeCell ref="AS108:BF108"/>
-    <mergeCell ref="BG109:CA109"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D105:AE105"/>
-    <mergeCell ref="AF105:AJ105"/>
-    <mergeCell ref="AK105:AO105"/>
-    <mergeCell ref="AP105:AR105"/>
-    <mergeCell ref="AS105:BF105"/>
-    <mergeCell ref="BG106:CA106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D106:AE106"/>
-    <mergeCell ref="AF106:AJ106"/>
-    <mergeCell ref="AK106:AO106"/>
-    <mergeCell ref="AP106:AR106"/>
-    <mergeCell ref="AS106:BF106"/>
-    <mergeCell ref="BG107:CA107"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D103:AE103"/>
-    <mergeCell ref="AF103:AJ103"/>
-    <mergeCell ref="AK103:AO103"/>
-    <mergeCell ref="AP103:AR103"/>
-    <mergeCell ref="AS103:BF103"/>
-    <mergeCell ref="BG104:CA104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D104:AE104"/>
-    <mergeCell ref="AF104:AJ104"/>
-    <mergeCell ref="AK104:AO104"/>
-    <mergeCell ref="AP104:AR104"/>
-    <mergeCell ref="AS104:BF104"/>
-    <mergeCell ref="BG105:CA105"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="BG102:CA102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D102:AE102"/>
-    <mergeCell ref="AF102:AJ102"/>
-    <mergeCell ref="AK102:AO102"/>
-    <mergeCell ref="AP102:AR102"/>
-    <mergeCell ref="AS102:BF102"/>
-    <mergeCell ref="BG103:CA103"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="AK100:AO100"/>
-    <mergeCell ref="AP100:AR100"/>
-    <mergeCell ref="AS100:BF100"/>
-    <mergeCell ref="BG100:CA100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="D101:AE101"/>
-    <mergeCell ref="AF101:AJ101"/>
-    <mergeCell ref="AK101:AO101"/>
-    <mergeCell ref="AP101:AR101"/>
-    <mergeCell ref="AS101:BF101"/>
-    <mergeCell ref="BG101:CA101"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:AE98"/>
-    <mergeCell ref="AF98:AJ98"/>
-    <mergeCell ref="AK98:AO98"/>
-    <mergeCell ref="AP98:AR98"/>
-    <mergeCell ref="AS98:BF98"/>
-    <mergeCell ref="BG98:CA98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="D99:AE99"/>
-    <mergeCell ref="AF99:AJ99"/>
-    <mergeCell ref="AK99:AO99"/>
-    <mergeCell ref="AP99:AR99"/>
-    <mergeCell ref="AS99:BF99"/>
-    <mergeCell ref="BG99:CA99"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:AE96"/>
-    <mergeCell ref="AF96:AJ96"/>
-    <mergeCell ref="AK96:AO96"/>
-    <mergeCell ref="AP96:AR96"/>
-    <mergeCell ref="AS96:BF96"/>
-    <mergeCell ref="BG96:CA96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:AE97"/>
-    <mergeCell ref="AF97:AJ97"/>
-    <mergeCell ref="AK97:AO97"/>
-    <mergeCell ref="AP97:AR97"/>
-    <mergeCell ref="AS97:BF97"/>
-    <mergeCell ref="BG97:CA97"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:AE94"/>
-    <mergeCell ref="AF94:AJ94"/>
-    <mergeCell ref="AK94:AO94"/>
-    <mergeCell ref="AP94:AR94"/>
-    <mergeCell ref="AS94:BF94"/>
-    <mergeCell ref="BG94:CA94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:AE95"/>
-    <mergeCell ref="AF95:AJ95"/>
-    <mergeCell ref="AK95:AO95"/>
-    <mergeCell ref="AP95:AR95"/>
-    <mergeCell ref="AS95:BF95"/>
-    <mergeCell ref="BG95:CA95"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:AE92"/>
-    <mergeCell ref="AF92:AJ92"/>
-    <mergeCell ref="AK92:AO92"/>
-    <mergeCell ref="AP92:AR92"/>
-    <mergeCell ref="AS92:BF92"/>
-    <mergeCell ref="BG92:CA92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:AE93"/>
-    <mergeCell ref="AF93:AJ93"/>
-    <mergeCell ref="AK93:AO93"/>
-    <mergeCell ref="AP93:AR93"/>
-    <mergeCell ref="AS93:BF93"/>
-    <mergeCell ref="BG93:CA93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:AE90"/>
-    <mergeCell ref="AF90:AJ90"/>
-    <mergeCell ref="AK90:AO90"/>
-    <mergeCell ref="AP90:AR90"/>
-    <mergeCell ref="AS90:BF90"/>
-    <mergeCell ref="BG90:CA90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:AE91"/>
-    <mergeCell ref="AF91:AJ91"/>
-    <mergeCell ref="AK91:AO91"/>
-    <mergeCell ref="AP91:AR91"/>
-    <mergeCell ref="AS91:BF91"/>
-    <mergeCell ref="BG91:CA91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D88:AE88"/>
-    <mergeCell ref="AF88:AJ88"/>
-    <mergeCell ref="AK88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:BF88"/>
-    <mergeCell ref="BG88:CA88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="D89:AE89"/>
-    <mergeCell ref="AF89:AJ89"/>
-    <mergeCell ref="AK89:AO89"/>
-    <mergeCell ref="AP89:AR89"/>
-    <mergeCell ref="AS89:BF89"/>
-    <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:AE86"/>
-    <mergeCell ref="AF86:AJ86"/>
-    <mergeCell ref="AK86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="AS86:BF86"/>
-    <mergeCell ref="BG86:CA86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:AE87"/>
-    <mergeCell ref="AF87:AJ87"/>
-    <mergeCell ref="AK87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:BF87"/>
-    <mergeCell ref="BG87:CA87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:AE84"/>
-    <mergeCell ref="AF84:AJ84"/>
-    <mergeCell ref="AK84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:BF84"/>
-    <mergeCell ref="BG84:CA84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:AE85"/>
-    <mergeCell ref="AF85:AJ85"/>
-    <mergeCell ref="AK85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:BF85"/>
-    <mergeCell ref="BG85:CA85"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:AE82"/>
-    <mergeCell ref="AF82:AJ82"/>
-    <mergeCell ref="AK82:AO82"/>
-    <mergeCell ref="AP82:AR82"/>
-    <mergeCell ref="AS82:BF82"/>
-    <mergeCell ref="BG82:CA82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:AE83"/>
-    <mergeCell ref="AF83:AJ83"/>
-    <mergeCell ref="AK83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:BF83"/>
-    <mergeCell ref="BG83:CA83"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:AE80"/>
-    <mergeCell ref="AF80:AJ80"/>
-    <mergeCell ref="AK80:AO80"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="AS80:BF80"/>
-    <mergeCell ref="BG80:CA80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:AE81"/>
-    <mergeCell ref="AF81:AJ81"/>
-    <mergeCell ref="AK81:AO81"/>
-    <mergeCell ref="AP81:AR81"/>
-    <mergeCell ref="AS81:BF81"/>
-    <mergeCell ref="BG81:CA81"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:AE78"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AK78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:BF78"/>
-    <mergeCell ref="BG78:CA78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:AE79"/>
-    <mergeCell ref="AF79:AJ79"/>
-    <mergeCell ref="AK79:AO79"/>
-    <mergeCell ref="AP79:AR79"/>
-    <mergeCell ref="AS79:BF79"/>
-    <mergeCell ref="BG79:CA79"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:AE76"/>
-    <mergeCell ref="AF76:AJ76"/>
-    <mergeCell ref="AK76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:BF76"/>
-    <mergeCell ref="BG76:CA76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:AE77"/>
-    <mergeCell ref="AF77:AJ77"/>
-    <mergeCell ref="AK77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:BF77"/>
-    <mergeCell ref="BG77:CA77"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:AE74"/>
-    <mergeCell ref="AF74:AJ74"/>
-    <mergeCell ref="AK74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:BF74"/>
-    <mergeCell ref="BG74:CA74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:AE75"/>
-    <mergeCell ref="AF75:AJ75"/>
-    <mergeCell ref="AK75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:BF75"/>
-    <mergeCell ref="BG75:CA75"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:AE70"/>
-    <mergeCell ref="AF70:AJ70"/>
-    <mergeCell ref="AK70:AO70"/>
-    <mergeCell ref="AP70:AR70"/>
-    <mergeCell ref="AS70:BF70"/>
-    <mergeCell ref="BG70:CA70"/>
-    <mergeCell ref="AP72:AR72"/>
-    <mergeCell ref="AS72:BF72"/>
-    <mergeCell ref="BG72:CA72"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:AE1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AR1"/>
-    <mergeCell ref="AS1:BF1"/>
-    <mergeCell ref="BG1:CA1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:AE2"/>
-    <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AS2:BF2"/>
-    <mergeCell ref="BG2:CA2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:AE3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:BF3"/>
-    <mergeCell ref="BG3:CA3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:BF4"/>
-    <mergeCell ref="BG4:CA4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:AE5"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AK5:AO5"/>
-    <mergeCell ref="AP5:AR5"/>
-    <mergeCell ref="AS5:BF5"/>
-    <mergeCell ref="BG5:CA5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="AK6:AO6"/>
-    <mergeCell ref="AP6:AR6"/>
-    <mergeCell ref="AS6:BF6"/>
-    <mergeCell ref="BG6:CA6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
-    <mergeCell ref="AS7:BF7"/>
-    <mergeCell ref="BG7:CA7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:AE8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AS8:BF8"/>
-    <mergeCell ref="BG8:CA8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:AE9"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="AK9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:BF9"/>
-    <mergeCell ref="BG9:CA9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:AE10"/>
-    <mergeCell ref="AF10:AJ10"/>
-    <mergeCell ref="AK10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:BF10"/>
-    <mergeCell ref="BG10:CA10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:AE11"/>
-    <mergeCell ref="AF11:AJ11"/>
-    <mergeCell ref="AK11:AO11"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:BF11"/>
-    <mergeCell ref="BG11:CA11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:AE12"/>
-    <mergeCell ref="AF12:AJ12"/>
-    <mergeCell ref="AK12:AO12"/>
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:BF12"/>
-    <mergeCell ref="BG12:CA12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:AE13"/>
-    <mergeCell ref="AF13:AJ13"/>
-    <mergeCell ref="AK13:AO13"/>
-    <mergeCell ref="AP13:AR13"/>
-    <mergeCell ref="AS13:BF13"/>
-    <mergeCell ref="BG13:CA13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:AE14"/>
-    <mergeCell ref="AF14:AJ14"/>
-    <mergeCell ref="AK14:AO14"/>
-    <mergeCell ref="AP14:AR14"/>
-    <mergeCell ref="AS14:BF14"/>
-    <mergeCell ref="BG14:CA14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:AE15"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AK15:AO15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AS15:BF15"/>
-    <mergeCell ref="BG15:CA15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:AE16"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AK16:AO16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AS16:BF16"/>
-    <mergeCell ref="BG16:CA16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:AE17"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AK17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AS17:BF17"/>
-    <mergeCell ref="BG17:CA17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:AE18"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AK18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AS18:BF18"/>
-    <mergeCell ref="BG18:CA18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:AE19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AK19:AO19"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AS19:BF19"/>
-    <mergeCell ref="BG19:CA19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:AE20"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AK20:AO20"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AS20:BF20"/>
-    <mergeCell ref="BG20:CA20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:AE21"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AK21:AO21"/>
-    <mergeCell ref="AP21:AR21"/>
-    <mergeCell ref="AS21:BF21"/>
-    <mergeCell ref="BG21:CA21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:AE22"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AK22:AO22"/>
-    <mergeCell ref="AP22:AR22"/>
-    <mergeCell ref="AS22:BF22"/>
-    <mergeCell ref="BG22:CA22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:AE23"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AS23:BF23"/>
-    <mergeCell ref="BG23:CA23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:AE24"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AK24:AO24"/>
-    <mergeCell ref="AP24:AR24"/>
-    <mergeCell ref="AS24:BF24"/>
-    <mergeCell ref="BG24:CA24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:AE25"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AK25:AO25"/>
-    <mergeCell ref="AP25:AR25"/>
-    <mergeCell ref="AS25:BF25"/>
-    <mergeCell ref="BG25:CA25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:AE26"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AK26:AO26"/>
-    <mergeCell ref="AP26:AR26"/>
-    <mergeCell ref="AS26:BF26"/>
-    <mergeCell ref="BG26:CA26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:AE27"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AK27:AO27"/>
-    <mergeCell ref="AP27:AR27"/>
-    <mergeCell ref="AS27:BF27"/>
-    <mergeCell ref="BG27:CA27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:AE28"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AK28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:BF28"/>
-    <mergeCell ref="BG28:CA28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
-    <mergeCell ref="AP29:AR29"/>
-    <mergeCell ref="AS29:BF29"/>
-    <mergeCell ref="BG29:CA29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="AP30:AR30"/>
-    <mergeCell ref="AS30:BF30"/>
-    <mergeCell ref="BG30:CA30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="AP31:AR31"/>
-    <mergeCell ref="AS31:BF31"/>
-    <mergeCell ref="BG31:CA31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="AP32:AR32"/>
-    <mergeCell ref="AS32:BF32"/>
-    <mergeCell ref="BG32:CA32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:AE33"/>
-    <mergeCell ref="AF33:AJ33"/>
-    <mergeCell ref="AK33:AO33"/>
-    <mergeCell ref="AP33:AR33"/>
-    <mergeCell ref="AS33:BF33"/>
-    <mergeCell ref="BG33:CA33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:AE34"/>
-    <mergeCell ref="AF34:AJ34"/>
-    <mergeCell ref="AK34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:BF34"/>
-    <mergeCell ref="BG34:CA34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:AE35"/>
-    <mergeCell ref="AF35:AJ35"/>
-    <mergeCell ref="AK35:AO35"/>
-    <mergeCell ref="AP35:AR35"/>
-    <mergeCell ref="AS35:BF35"/>
-    <mergeCell ref="BG35:CA35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:AE36"/>
-    <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="AK36:AO36"/>
-    <mergeCell ref="AP36:AR36"/>
-    <mergeCell ref="AS36:BF36"/>
-    <mergeCell ref="BG36:CA36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AR37"/>
-    <mergeCell ref="AS37:BF37"/>
-    <mergeCell ref="BG37:CA37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:AE38"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="AP38:AR38"/>
-    <mergeCell ref="AS38:BF38"/>
-    <mergeCell ref="BG38:CA38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:AE39"/>
-    <mergeCell ref="AF39:AJ39"/>
-    <mergeCell ref="AK39:AO39"/>
-    <mergeCell ref="AP39:AR39"/>
-    <mergeCell ref="AS39:BF39"/>
-    <mergeCell ref="BG39:CA39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:AE40"/>
-    <mergeCell ref="AF40:AJ40"/>
-    <mergeCell ref="AK40:AO40"/>
-    <mergeCell ref="AP40:AR40"/>
-    <mergeCell ref="AS40:BF40"/>
-    <mergeCell ref="BG40:CA40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:AE41"/>
-    <mergeCell ref="AF41:AJ41"/>
-    <mergeCell ref="AK41:AO41"/>
-    <mergeCell ref="AP41:AR41"/>
-    <mergeCell ref="AS41:BF41"/>
-    <mergeCell ref="BG41:CA41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:AE42"/>
-    <mergeCell ref="AF42:AJ42"/>
-    <mergeCell ref="AK42:AO42"/>
-    <mergeCell ref="AP42:AR42"/>
-    <mergeCell ref="AS42:BF42"/>
-    <mergeCell ref="BG42:CA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:AE43"/>
-    <mergeCell ref="AF43:AJ43"/>
-    <mergeCell ref="AK43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="AS43:BF43"/>
-    <mergeCell ref="BG43:CA43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:AE44"/>
-    <mergeCell ref="AF44:AJ44"/>
-    <mergeCell ref="AK44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AS44:BF44"/>
-    <mergeCell ref="BG44:CA44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:AE45"/>
-    <mergeCell ref="AF45:AJ45"/>
-    <mergeCell ref="AK45:AO45"/>
-    <mergeCell ref="AP45:AR45"/>
-    <mergeCell ref="AS45:BF45"/>
-    <mergeCell ref="BG45:CA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:AE46"/>
-    <mergeCell ref="AF46:AJ46"/>
-    <mergeCell ref="AK46:AO46"/>
-    <mergeCell ref="AP46:AR46"/>
-    <mergeCell ref="AS46:BF46"/>
-    <mergeCell ref="BG46:CA46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:AE47"/>
-    <mergeCell ref="AF47:AJ47"/>
-    <mergeCell ref="AK47:AO47"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AS47:BF47"/>
-    <mergeCell ref="BG47:CA47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:AE48"/>
-    <mergeCell ref="AF48:AJ48"/>
-    <mergeCell ref="AK48:AO48"/>
-    <mergeCell ref="AP48:AR48"/>
-    <mergeCell ref="AS48:BF48"/>
-    <mergeCell ref="BG48:CA48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:AE49"/>
-    <mergeCell ref="AF49:AJ49"/>
-    <mergeCell ref="AK49:AO49"/>
-    <mergeCell ref="AP49:AR49"/>
-    <mergeCell ref="AS49:BF49"/>
-    <mergeCell ref="BG49:CA49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:AE50"/>
-    <mergeCell ref="AF50:AJ50"/>
-    <mergeCell ref="AK50:AO50"/>
-    <mergeCell ref="AP50:AR50"/>
-    <mergeCell ref="AS50:BF50"/>
-    <mergeCell ref="BG50:CA50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:AE51"/>
-    <mergeCell ref="AF51:AJ51"/>
-    <mergeCell ref="AK51:AO51"/>
-    <mergeCell ref="AP51:AR51"/>
-    <mergeCell ref="AS51:BF51"/>
-    <mergeCell ref="BG51:CA51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:AE52"/>
-    <mergeCell ref="AF52:AJ52"/>
-    <mergeCell ref="AK52:AO52"/>
-    <mergeCell ref="AP52:AR52"/>
-    <mergeCell ref="AS52:BF52"/>
-    <mergeCell ref="BG52:CA52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:AE53"/>
-    <mergeCell ref="AF53:AJ53"/>
-    <mergeCell ref="AK53:AO53"/>
-    <mergeCell ref="AP53:AR53"/>
-    <mergeCell ref="AS53:BF53"/>
-    <mergeCell ref="BG53:CA53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:AE54"/>
-    <mergeCell ref="AF54:AJ54"/>
-    <mergeCell ref="AK54:AO54"/>
-    <mergeCell ref="AP54:AR54"/>
-    <mergeCell ref="AS54:BF54"/>
-    <mergeCell ref="BG54:CA54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:AE55"/>
-    <mergeCell ref="AF55:AJ55"/>
-    <mergeCell ref="AK55:AO55"/>
-    <mergeCell ref="AP55:AR55"/>
-    <mergeCell ref="AS55:BF55"/>
-    <mergeCell ref="BG55:CA55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:AE56"/>
-    <mergeCell ref="AF56:AJ56"/>
-    <mergeCell ref="AK56:AO56"/>
-    <mergeCell ref="AP56:AR56"/>
-    <mergeCell ref="AS56:BF56"/>
-    <mergeCell ref="BG56:CA56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:AE57"/>
-    <mergeCell ref="AF57:AJ57"/>
-    <mergeCell ref="AK57:AO57"/>
-    <mergeCell ref="AP57:AR57"/>
-    <mergeCell ref="AS57:BF57"/>
-    <mergeCell ref="BG57:CA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:AE58"/>
-    <mergeCell ref="AF58:AJ58"/>
-    <mergeCell ref="AK58:AO58"/>
-    <mergeCell ref="AP58:AR58"/>
-    <mergeCell ref="AS58:BF58"/>
-    <mergeCell ref="BG58:CA58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:AE61"/>
-    <mergeCell ref="AF61:AJ61"/>
-    <mergeCell ref="AK61:AO61"/>
-    <mergeCell ref="AP61:AR61"/>
-    <mergeCell ref="AS61:BF61"/>
-    <mergeCell ref="BG61:CA61"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:AE59"/>
-    <mergeCell ref="AF59:AJ59"/>
-    <mergeCell ref="AK59:AO59"/>
-    <mergeCell ref="AP59:AR59"/>
-    <mergeCell ref="AS59:BF59"/>
-    <mergeCell ref="BG59:CA59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:AE60"/>
-    <mergeCell ref="AF60:AJ60"/>
-    <mergeCell ref="AK60:AO60"/>
-    <mergeCell ref="AP60:AR60"/>
-    <mergeCell ref="AS60:BF60"/>
-    <mergeCell ref="BG60:CA60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:AE62"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AK62:AO62"/>
-    <mergeCell ref="AP62:AR62"/>
-    <mergeCell ref="AS62:BF62"/>
-    <mergeCell ref="BG62:CA62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:AE63"/>
-    <mergeCell ref="AF63:AJ63"/>
-    <mergeCell ref="AK63:AO63"/>
-    <mergeCell ref="AP63:AR63"/>
-    <mergeCell ref="AS63:BF63"/>
-    <mergeCell ref="BG63:CA63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:AE64"/>
-    <mergeCell ref="AF64:AJ64"/>
-    <mergeCell ref="AK64:AO64"/>
-    <mergeCell ref="AP64:AR64"/>
-    <mergeCell ref="AS64:BF64"/>
-    <mergeCell ref="BG64:CA64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:AE65"/>
-    <mergeCell ref="AF65:AJ65"/>
-    <mergeCell ref="AK65:AO65"/>
-    <mergeCell ref="AP65:AR65"/>
-    <mergeCell ref="AS65:BF65"/>
-    <mergeCell ref="BG65:CA65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:AE66"/>
-    <mergeCell ref="AF66:AJ66"/>
-    <mergeCell ref="AK66:AO66"/>
-    <mergeCell ref="AP66:AR66"/>
-    <mergeCell ref="AS66:BF66"/>
-    <mergeCell ref="BG66:CA66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:AE67"/>
-    <mergeCell ref="AF67:AJ67"/>
-    <mergeCell ref="AK67:AO67"/>
-    <mergeCell ref="AP67:AR67"/>
-    <mergeCell ref="AS67:BF67"/>
-    <mergeCell ref="BG67:CA67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:AE68"/>
-    <mergeCell ref="AF68:AJ68"/>
-    <mergeCell ref="AK68:AO68"/>
-    <mergeCell ref="AP68:AR68"/>
-    <mergeCell ref="AS68:BF68"/>
-    <mergeCell ref="BG68:CA68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:AE69"/>
-    <mergeCell ref="AF69:AJ69"/>
-    <mergeCell ref="AK69:AO69"/>
-    <mergeCell ref="AP69:AR69"/>
-    <mergeCell ref="AS69:BF69"/>
-    <mergeCell ref="BG69:CA69"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:AE73"/>
-    <mergeCell ref="AF73:AJ73"/>
-    <mergeCell ref="AK73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:BF73"/>
-    <mergeCell ref="BG73:CA73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:AE71"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AK71:AO71"/>
-    <mergeCell ref="AP71:AR71"/>
-    <mergeCell ref="AS71:BF71"/>
-    <mergeCell ref="BG71:CA71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="AK72:AO72"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="D124:AE124"/>
+    <mergeCell ref="AF124:AJ124"/>
+    <mergeCell ref="AK124:AO124"/>
+    <mergeCell ref="AP124:AR124"/>
+    <mergeCell ref="AS124:BF124"/>
+    <mergeCell ref="BG124:CA124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="D125:AE125"/>
+    <mergeCell ref="AF125:AJ125"/>
+    <mergeCell ref="AK125:AO125"/>
+    <mergeCell ref="AP125:AR125"/>
+    <mergeCell ref="AS125:BF125"/>
+    <mergeCell ref="BG125:CA125"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D122:AE122"/>
+    <mergeCell ref="AF122:AJ122"/>
+    <mergeCell ref="AK122:AO122"/>
+    <mergeCell ref="AP122:AR122"/>
+    <mergeCell ref="AS122:BF122"/>
+    <mergeCell ref="BG123:CA123"/>
+    <mergeCell ref="D123:AE123"/>
+    <mergeCell ref="AF123:AJ123"/>
+    <mergeCell ref="AK123:AO123"/>
+    <mergeCell ref="AP123:AR123"/>
+    <mergeCell ref="AS123:BF123"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="D128:AE128"/>
+    <mergeCell ref="AF128:AJ128"/>
+    <mergeCell ref="AK128:AO128"/>
+    <mergeCell ref="AP128:AR128"/>
+    <mergeCell ref="AS128:BF128"/>
+    <mergeCell ref="BG128:CA128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="D129:AE129"/>
+    <mergeCell ref="AF129:AJ129"/>
+    <mergeCell ref="AK129:AO129"/>
+    <mergeCell ref="AP129:AR129"/>
+    <mergeCell ref="AS129:BF129"/>
+    <mergeCell ref="BG129:CA129"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="D126:AE126"/>
+    <mergeCell ref="AF126:AJ126"/>
+    <mergeCell ref="AK126:AO126"/>
+    <mergeCell ref="AP126:AR126"/>
+    <mergeCell ref="AS126:BF126"/>
+    <mergeCell ref="BG126:CA126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="D127:AE127"/>
+    <mergeCell ref="AF127:AJ127"/>
+    <mergeCell ref="AK127:AO127"/>
+    <mergeCell ref="AP127:AR127"/>
+    <mergeCell ref="AS127:BF127"/>
+    <mergeCell ref="BG127:CA127"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="D132:AE132"/>
+    <mergeCell ref="AF132:AJ132"/>
+    <mergeCell ref="AK132:AO132"/>
+    <mergeCell ref="AP132:AR132"/>
+    <mergeCell ref="AS132:BF132"/>
+    <mergeCell ref="BG132:CA132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="BG133:CA133"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="D130:AE130"/>
+    <mergeCell ref="AF130:AJ130"/>
+    <mergeCell ref="AK130:AO130"/>
+    <mergeCell ref="AP130:AR130"/>
+    <mergeCell ref="AS130:BF130"/>
+    <mergeCell ref="BG130:CA130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="D133:AE133"/>
+    <mergeCell ref="AF133:AJ133"/>
+    <mergeCell ref="AK133:AO133"/>
+    <mergeCell ref="AP133:AR133"/>
+    <mergeCell ref="AS133:BF133"/>
+    <mergeCell ref="BG131:CA131"/>
+    <mergeCell ref="D131:AE131"/>
+    <mergeCell ref="AF131:AJ131"/>
+    <mergeCell ref="AK131:AO131"/>
+    <mergeCell ref="AP131:AR131"/>
+    <mergeCell ref="AS131:BF131"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="D136:AE136"/>
+    <mergeCell ref="AF136:AJ136"/>
+    <mergeCell ref="AK136:AO136"/>
+    <mergeCell ref="AP136:AR136"/>
+    <mergeCell ref="AS136:BF136"/>
+    <mergeCell ref="BG136:CA136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="D137:AE137"/>
+    <mergeCell ref="AF137:AJ137"/>
+    <mergeCell ref="AK137:AO137"/>
+    <mergeCell ref="AP137:AR137"/>
+    <mergeCell ref="AS137:BF137"/>
+    <mergeCell ref="BG137:CA137"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="D134:AE134"/>
+    <mergeCell ref="AF134:AJ134"/>
+    <mergeCell ref="AK134:AO134"/>
+    <mergeCell ref="AP134:AR134"/>
+    <mergeCell ref="AS134:BF134"/>
+    <mergeCell ref="BG134:CA134"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="D135:AE135"/>
+    <mergeCell ref="AF135:AJ135"/>
+    <mergeCell ref="AK135:AO135"/>
+    <mergeCell ref="AP135:AR135"/>
+    <mergeCell ref="AS135:BF135"/>
+    <mergeCell ref="BG135:CA135"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="D140:AE140"/>
+    <mergeCell ref="AF140:AJ140"/>
+    <mergeCell ref="AK140:AO140"/>
+    <mergeCell ref="AP140:AR140"/>
+    <mergeCell ref="AS140:BF140"/>
+    <mergeCell ref="BG140:CA140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="D141:AE141"/>
+    <mergeCell ref="AF141:AJ141"/>
+    <mergeCell ref="AK141:AO141"/>
+    <mergeCell ref="AP141:AR141"/>
+    <mergeCell ref="AS141:BF141"/>
+    <mergeCell ref="BG141:CA141"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="D138:AE138"/>
+    <mergeCell ref="AF138:AJ138"/>
+    <mergeCell ref="AK138:AO138"/>
+    <mergeCell ref="AP138:AR138"/>
+    <mergeCell ref="AS138:BF138"/>
+    <mergeCell ref="BG138:CA138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="D139:AE139"/>
+    <mergeCell ref="AF139:AJ139"/>
+    <mergeCell ref="AK139:AO139"/>
+    <mergeCell ref="AP139:AR139"/>
+    <mergeCell ref="AS139:BF139"/>
+    <mergeCell ref="BG139:CA139"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="D143:AE143"/>
+    <mergeCell ref="AF143:AJ143"/>
+    <mergeCell ref="AK143:AO143"/>
+    <mergeCell ref="AP143:AR143"/>
+    <mergeCell ref="AS143:BF143"/>
+    <mergeCell ref="BG143:CA143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="D144:AE144"/>
+    <mergeCell ref="AF144:AJ144"/>
+    <mergeCell ref="AK144:AO144"/>
+    <mergeCell ref="AP144:AR144"/>
+    <mergeCell ref="AS144:BF144"/>
+    <mergeCell ref="BG144:CA144"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="D142:AE142"/>
+    <mergeCell ref="AF142:AJ142"/>
+    <mergeCell ref="AK142:AO142"/>
+    <mergeCell ref="AP142:AR142"/>
+    <mergeCell ref="AS142:BF142"/>
+    <mergeCell ref="BG142:CA142"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="D147:AE147"/>
+    <mergeCell ref="AF147:AJ147"/>
+    <mergeCell ref="AK147:AO147"/>
+    <mergeCell ref="AP147:AR147"/>
+    <mergeCell ref="AS147:BF147"/>
+    <mergeCell ref="BG147:CA147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="D148:AE148"/>
+    <mergeCell ref="AF148:AJ148"/>
+    <mergeCell ref="AK148:AO148"/>
+    <mergeCell ref="AP148:AR148"/>
+    <mergeCell ref="AS148:BF148"/>
+    <mergeCell ref="BG148:CA148"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="D145:AE145"/>
+    <mergeCell ref="AF145:AJ145"/>
+    <mergeCell ref="AK145:AO145"/>
+    <mergeCell ref="AP145:AR145"/>
+    <mergeCell ref="AS145:BF145"/>
+    <mergeCell ref="BG145:CA145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="D146:AE146"/>
+    <mergeCell ref="AF146:AJ146"/>
+    <mergeCell ref="AK146:AO146"/>
+    <mergeCell ref="AP146:AR146"/>
+    <mergeCell ref="AS146:BF146"/>
+    <mergeCell ref="BG146:CA146"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="D151:AE151"/>
+    <mergeCell ref="AF151:AJ151"/>
+    <mergeCell ref="AK151:AO151"/>
+    <mergeCell ref="AP151:AR151"/>
+    <mergeCell ref="AS151:BF151"/>
+    <mergeCell ref="BG151:CA151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="D152:AE152"/>
+    <mergeCell ref="AF152:AJ152"/>
+    <mergeCell ref="AK152:AO152"/>
+    <mergeCell ref="AP152:AR152"/>
+    <mergeCell ref="AS152:BF152"/>
+    <mergeCell ref="BG152:CA152"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="D149:AE149"/>
+    <mergeCell ref="AF149:AJ149"/>
+    <mergeCell ref="AK149:AO149"/>
+    <mergeCell ref="AP149:AR149"/>
+    <mergeCell ref="AS149:BF149"/>
+    <mergeCell ref="BG149:CA149"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="D150:AE150"/>
+    <mergeCell ref="AF150:AJ150"/>
+    <mergeCell ref="AK150:AO150"/>
+    <mergeCell ref="AP150:AR150"/>
+    <mergeCell ref="AS150:BF150"/>
+    <mergeCell ref="BG150:CA150"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="D155:AE155"/>
+    <mergeCell ref="AF155:AJ155"/>
+    <mergeCell ref="AK155:AO155"/>
+    <mergeCell ref="AP155:AR155"/>
+    <mergeCell ref="AS155:BF155"/>
+    <mergeCell ref="BG155:CA155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="D156:AE156"/>
+    <mergeCell ref="AF156:AJ156"/>
+    <mergeCell ref="AK156:AO156"/>
+    <mergeCell ref="AP156:AR156"/>
+    <mergeCell ref="AS156:BF156"/>
+    <mergeCell ref="BG156:CA156"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="D153:AE153"/>
+    <mergeCell ref="AF153:AJ153"/>
+    <mergeCell ref="AK153:AO153"/>
+    <mergeCell ref="AP153:AR153"/>
+    <mergeCell ref="AS153:BF153"/>
+    <mergeCell ref="BG153:CA153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="D154:AE154"/>
+    <mergeCell ref="AF154:AJ154"/>
+    <mergeCell ref="AK154:AO154"/>
+    <mergeCell ref="AP154:AR154"/>
+    <mergeCell ref="AS154:BF154"/>
+    <mergeCell ref="BG154:CA154"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="D159:AE159"/>
+    <mergeCell ref="AF159:AJ159"/>
+    <mergeCell ref="AK159:AO159"/>
+    <mergeCell ref="AP159:AR159"/>
+    <mergeCell ref="AS159:BF159"/>
+    <mergeCell ref="BG159:CA159"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="D160:AE160"/>
+    <mergeCell ref="AF160:AJ160"/>
+    <mergeCell ref="AK160:AO160"/>
+    <mergeCell ref="AP160:AR160"/>
+    <mergeCell ref="AS160:BF160"/>
+    <mergeCell ref="BG160:CA160"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="D157:AE157"/>
+    <mergeCell ref="AF157:AJ157"/>
+    <mergeCell ref="AK157:AO157"/>
+    <mergeCell ref="AP157:AR157"/>
+    <mergeCell ref="AS157:BF157"/>
+    <mergeCell ref="BG157:CA157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="D158:AE158"/>
+    <mergeCell ref="AF158:AJ158"/>
+    <mergeCell ref="AK158:AO158"/>
+    <mergeCell ref="AP158:AR158"/>
+    <mergeCell ref="AS158:BF158"/>
+    <mergeCell ref="BG158:CA158"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="D163:AE163"/>
+    <mergeCell ref="AF163:AJ163"/>
+    <mergeCell ref="AK163:AO163"/>
+    <mergeCell ref="AP163:AR163"/>
+    <mergeCell ref="AS163:BF163"/>
+    <mergeCell ref="BG163:CA163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="D164:AE164"/>
+    <mergeCell ref="AF164:AJ164"/>
+    <mergeCell ref="AK164:AO164"/>
+    <mergeCell ref="AP164:AR164"/>
+    <mergeCell ref="AS164:BF164"/>
+    <mergeCell ref="BG164:CA164"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="D161:AE161"/>
+    <mergeCell ref="AF161:AJ161"/>
+    <mergeCell ref="AK161:AO161"/>
+    <mergeCell ref="AP161:AR161"/>
+    <mergeCell ref="AS161:BF161"/>
+    <mergeCell ref="BG161:CA161"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="D162:AE162"/>
+    <mergeCell ref="AF162:AJ162"/>
+    <mergeCell ref="AK162:AO162"/>
+    <mergeCell ref="AP162:AR162"/>
+    <mergeCell ref="AS162:BF162"/>
+    <mergeCell ref="BG162:CA162"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="D167:AE167"/>
+    <mergeCell ref="AF167:AJ167"/>
+    <mergeCell ref="AK167:AO167"/>
+    <mergeCell ref="AP167:AR167"/>
+    <mergeCell ref="AS167:BF167"/>
+    <mergeCell ref="BG167:CA167"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="D168:AE168"/>
+    <mergeCell ref="AF168:AJ168"/>
+    <mergeCell ref="AK168:AO168"/>
+    <mergeCell ref="AP168:AR168"/>
+    <mergeCell ref="AS168:BF168"/>
+    <mergeCell ref="BG168:CA168"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="D165:AE165"/>
+    <mergeCell ref="AF165:AJ165"/>
+    <mergeCell ref="AK165:AO165"/>
+    <mergeCell ref="AP165:AR165"/>
+    <mergeCell ref="AS165:BF165"/>
+    <mergeCell ref="BG165:CA165"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="D166:AE166"/>
+    <mergeCell ref="AF166:AJ166"/>
+    <mergeCell ref="AK166:AO166"/>
+    <mergeCell ref="AP166:AR166"/>
+    <mergeCell ref="AS166:BF166"/>
+    <mergeCell ref="BG166:CA166"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="D171:AE171"/>
+    <mergeCell ref="AF171:AJ171"/>
+    <mergeCell ref="AK171:AO171"/>
+    <mergeCell ref="AP171:AR171"/>
+    <mergeCell ref="AS171:BF171"/>
+    <mergeCell ref="BG171:CA171"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="D172:AE172"/>
+    <mergeCell ref="AF172:AJ172"/>
+    <mergeCell ref="AK172:AO172"/>
+    <mergeCell ref="AP172:AR172"/>
+    <mergeCell ref="AS172:BF172"/>
+    <mergeCell ref="BG172:CA172"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="D169:AE169"/>
+    <mergeCell ref="AF169:AJ169"/>
+    <mergeCell ref="AK169:AO169"/>
+    <mergeCell ref="AP169:AR169"/>
+    <mergeCell ref="AS169:BF169"/>
+    <mergeCell ref="BG169:CA169"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="D170:AE170"/>
+    <mergeCell ref="AF170:AJ170"/>
+    <mergeCell ref="AK170:AO170"/>
+    <mergeCell ref="AP170:AR170"/>
+    <mergeCell ref="AS170:BF170"/>
+    <mergeCell ref="BG170:CA170"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="D175:AE175"/>
+    <mergeCell ref="AF175:AJ175"/>
+    <mergeCell ref="AK175:AO175"/>
+    <mergeCell ref="AP175:AR175"/>
+    <mergeCell ref="AS175:BF175"/>
+    <mergeCell ref="BG175:CA175"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="D176:AE176"/>
+    <mergeCell ref="AF176:AJ176"/>
+    <mergeCell ref="AK176:AO176"/>
+    <mergeCell ref="AP176:AR176"/>
+    <mergeCell ref="AS176:BF176"/>
+    <mergeCell ref="BG176:CA176"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="D173:AE173"/>
+    <mergeCell ref="AF173:AJ173"/>
+    <mergeCell ref="AK173:AO173"/>
+    <mergeCell ref="AP173:AR173"/>
+    <mergeCell ref="AS173:BF173"/>
+    <mergeCell ref="BG173:CA173"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="D174:AE174"/>
+    <mergeCell ref="AF174:AJ174"/>
+    <mergeCell ref="AK174:AO174"/>
+    <mergeCell ref="AP174:AR174"/>
+    <mergeCell ref="AS174:BF174"/>
+    <mergeCell ref="BG174:CA174"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="D179:AE179"/>
+    <mergeCell ref="AF179:AJ179"/>
+    <mergeCell ref="AK179:AO179"/>
+    <mergeCell ref="AP179:AR179"/>
+    <mergeCell ref="AS179:BF179"/>
+    <mergeCell ref="BG179:CA179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="D180:AE180"/>
+    <mergeCell ref="AF180:AJ180"/>
+    <mergeCell ref="AK180:AO180"/>
+    <mergeCell ref="AP180:AR180"/>
+    <mergeCell ref="AS180:BF180"/>
+    <mergeCell ref="BG180:CA180"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="D177:AE177"/>
+    <mergeCell ref="AF177:AJ177"/>
+    <mergeCell ref="AK177:AO177"/>
+    <mergeCell ref="AP177:AR177"/>
+    <mergeCell ref="AS177:BF177"/>
+    <mergeCell ref="BG177:CA177"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="D178:AE178"/>
+    <mergeCell ref="AF178:AJ178"/>
+    <mergeCell ref="AK178:AO178"/>
+    <mergeCell ref="AP178:AR178"/>
+    <mergeCell ref="AS178:BF178"/>
+    <mergeCell ref="BG178:CA178"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="D183:AE183"/>
+    <mergeCell ref="AF183:AJ183"/>
+    <mergeCell ref="AK183:AO183"/>
+    <mergeCell ref="AP183:AR183"/>
+    <mergeCell ref="AS183:BF183"/>
+    <mergeCell ref="BG183:CA183"/>
+    <mergeCell ref="A184:B184"/>
+    <mergeCell ref="D184:AE184"/>
+    <mergeCell ref="AF184:AJ184"/>
+    <mergeCell ref="AK184:AO184"/>
+    <mergeCell ref="AP184:AR184"/>
+    <mergeCell ref="AS184:BF184"/>
+    <mergeCell ref="BG184:CA184"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="D181:AE181"/>
+    <mergeCell ref="AF181:AJ181"/>
+    <mergeCell ref="AK181:AO181"/>
+    <mergeCell ref="AP181:AR181"/>
+    <mergeCell ref="AS181:BF181"/>
+    <mergeCell ref="BG181:CA181"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="D182:AE182"/>
+    <mergeCell ref="AF182:AJ182"/>
+    <mergeCell ref="AK182:AO182"/>
+    <mergeCell ref="AP182:AR182"/>
+    <mergeCell ref="AS182:BF182"/>
+    <mergeCell ref="BG182:CA182"/>
+    <mergeCell ref="AK187:AO187"/>
+    <mergeCell ref="AP187:AR187"/>
+    <mergeCell ref="AS187:BF187"/>
+    <mergeCell ref="BG187:CA187"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="D188:AE188"/>
+    <mergeCell ref="AF188:AJ188"/>
+    <mergeCell ref="AK188:AO188"/>
+    <mergeCell ref="AP188:AR188"/>
+    <mergeCell ref="AS188:BF188"/>
+    <mergeCell ref="BG188:CA188"/>
+    <mergeCell ref="A185:B185"/>
+    <mergeCell ref="D185:AE185"/>
+    <mergeCell ref="AF185:AJ185"/>
+    <mergeCell ref="AK185:AO185"/>
+    <mergeCell ref="AP185:AR185"/>
+    <mergeCell ref="AS185:BF185"/>
+    <mergeCell ref="BG185:CA185"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="D186:AE186"/>
+    <mergeCell ref="AF186:AJ186"/>
+    <mergeCell ref="AK186:AO186"/>
+    <mergeCell ref="AP186:AR186"/>
+    <mergeCell ref="AS186:BF186"/>
+    <mergeCell ref="BG186:CA186"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="D187:AE187"/>
+    <mergeCell ref="AF187:AJ187"/>
+    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="D191:AE191"/>
+    <mergeCell ref="AF191:AJ191"/>
+    <mergeCell ref="AK191:AO191"/>
+    <mergeCell ref="AP191:AR191"/>
+    <mergeCell ref="AS191:BF191"/>
+    <mergeCell ref="BG191:CA191"/>
+    <mergeCell ref="A192:B192"/>
+    <mergeCell ref="D192:AE192"/>
+    <mergeCell ref="AF192:AJ192"/>
+    <mergeCell ref="AK192:AO192"/>
+    <mergeCell ref="AP192:AR192"/>
+    <mergeCell ref="AS192:BF192"/>
+    <mergeCell ref="BG192:CA192"/>
+    <mergeCell ref="A189:B189"/>
+    <mergeCell ref="D189:AE189"/>
+    <mergeCell ref="AF189:AJ189"/>
+    <mergeCell ref="AK189:AO189"/>
+    <mergeCell ref="AP189:AR189"/>
+    <mergeCell ref="AS189:BF189"/>
+    <mergeCell ref="BG189:CA189"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="D190:AE190"/>
+    <mergeCell ref="AF190:AJ190"/>
+    <mergeCell ref="AK190:AO190"/>
+    <mergeCell ref="AP190:AR190"/>
+    <mergeCell ref="AS190:BF190"/>
+    <mergeCell ref="BG190:CA190"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="D195:AE195"/>
+    <mergeCell ref="AF195:AJ195"/>
+    <mergeCell ref="AK195:AO195"/>
+    <mergeCell ref="AP195:AR195"/>
+    <mergeCell ref="AS195:BF195"/>
+    <mergeCell ref="BG195:CA195"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="D196:AE196"/>
+    <mergeCell ref="AF196:AJ196"/>
+    <mergeCell ref="AK196:AO196"/>
+    <mergeCell ref="AP196:AR196"/>
+    <mergeCell ref="AS196:BF196"/>
+    <mergeCell ref="BG196:CA196"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="D193:AE193"/>
+    <mergeCell ref="AF193:AJ193"/>
+    <mergeCell ref="AK193:AO193"/>
+    <mergeCell ref="AP193:AR193"/>
+    <mergeCell ref="AS193:BF193"/>
+    <mergeCell ref="BG193:CA193"/>
+    <mergeCell ref="A194:B194"/>
+    <mergeCell ref="D194:AE194"/>
+    <mergeCell ref="AF194:AJ194"/>
+    <mergeCell ref="AK194:AO194"/>
+    <mergeCell ref="AP194:AR194"/>
+    <mergeCell ref="AS194:BF194"/>
+    <mergeCell ref="BG194:CA194"/>
+    <mergeCell ref="A199:B199"/>
+    <mergeCell ref="D199:AE199"/>
+    <mergeCell ref="AF199:AJ199"/>
+    <mergeCell ref="AK199:AO199"/>
+    <mergeCell ref="AP199:AR199"/>
+    <mergeCell ref="AS199:BF199"/>
+    <mergeCell ref="BG199:CA199"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="D200:AE200"/>
+    <mergeCell ref="AF200:AJ200"/>
+    <mergeCell ref="AK200:AO200"/>
+    <mergeCell ref="AP200:AR200"/>
+    <mergeCell ref="AS200:BF200"/>
+    <mergeCell ref="BG200:CA200"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="D197:AE197"/>
+    <mergeCell ref="AF197:AJ197"/>
+    <mergeCell ref="AK197:AO197"/>
+    <mergeCell ref="AP197:AR197"/>
+    <mergeCell ref="AS197:BF197"/>
+    <mergeCell ref="BG197:CA197"/>
+    <mergeCell ref="A198:B198"/>
+    <mergeCell ref="D198:AE198"/>
+    <mergeCell ref="AF198:AJ198"/>
+    <mergeCell ref="AK198:AO198"/>
+    <mergeCell ref="AP198:AR198"/>
+    <mergeCell ref="AS198:BF198"/>
+    <mergeCell ref="BG198:CA198"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C4:C200">

</xml_diff>

<commit_message>
báo cáo ngày 28/02/2019
</commit_message>
<xml_diff>
--- a/DailyReport/Quan-DailyReport.xlsx
+++ b/DailyReport/Quan-DailyReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="165">
   <si>
     <t>No.</t>
   </si>
@@ -507,6 +507,15 @@
   <si>
     <t>Chỉnh sửa giao diện - Chỉnh sửa lại chuỗi cron đồng bộ</t>
   </si>
+  <si>
+    <t>28/2/2019</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa giao diện - Chỉnh sửa db (xóa bỏ và thay đổi các trường)</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa giao diện - Thay đổi giao diện job index</t>
+  </si>
 </sst>
 </file>
 
@@ -817,16 +826,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -842,15 +849,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,7 +965,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1347,7 +1356,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1359,7 +1368,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D149" sqref="D149:AE149"/>
+      <selection pane="bottomLeft" activeCell="D151" sqref="D151:BF151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,192 +1383,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="30" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="29" t="s">
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="31" t="s">
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="29" t="s">
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="29"/>
-      <c r="AU1" s="29"/>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="29"/>
-      <c r="AX1" s="29"/>
-      <c r="AY1" s="29"/>
-      <c r="AZ1" s="29"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="29"/>
-      <c r="BC1" s="29"/>
-      <c r="BD1" s="29"/>
-      <c r="BE1" s="29"/>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="32" t="s">
+      <c r="AT1" s="27"/>
+      <c r="AU1" s="27"/>
+      <c r="AV1" s="27"/>
+      <c r="AW1" s="27"/>
+      <c r="AX1" s="27"/>
+      <c r="AY1" s="27"/>
+      <c r="AZ1" s="27"/>
+      <c r="BA1" s="27"/>
+      <c r="BB1" s="27"/>
+      <c r="BC1" s="27"/>
+      <c r="BD1" s="27"/>
+      <c r="BE1" s="27"/>
+      <c r="BF1" s="27"/>
+      <c r="BG1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
-      <c r="BQ1" s="32"/>
-      <c r="BR1" s="32"/>
-      <c r="BS1" s="32"/>
-      <c r="BT1" s="32"/>
-      <c r="BU1" s="32"/>
-      <c r="BV1" s="32"/>
-      <c r="BW1" s="32"/>
-      <c r="BX1" s="32"/>
-      <c r="BY1" s="32"/>
-      <c r="BZ1" s="32"/>
-      <c r="CA1" s="32"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+      <c r="BN1" s="30"/>
+      <c r="BO1" s="30"/>
+      <c r="BP1" s="30"/>
+      <c r="BQ1" s="30"/>
+      <c r="BR1" s="30"/>
+      <c r="BS1" s="30"/>
+      <c r="BT1" s="30"/>
+      <c r="BU1" s="30"/>
+      <c r="BV1" s="30"/>
+      <c r="BW1" s="30"/>
+      <c r="BX1" s="30"/>
+      <c r="BY1" s="30"/>
+      <c r="BZ1" s="30"/>
+      <c r="CA1" s="30"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="34" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="33" t="s">
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="35">
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="34">
         <v>1</v>
       </c>
-      <c r="AQ2" s="35"/>
-      <c r="AR2" s="35"/>
-      <c r="AS2" s="33" t="s">
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="33"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="33"/>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="36"/>
-      <c r="BH2" s="36"/>
-      <c r="BI2" s="36"/>
-      <c r="BJ2" s="36"/>
-      <c r="BK2" s="36"/>
-      <c r="BL2" s="36"/>
-      <c r="BM2" s="36"/>
-      <c r="BN2" s="36"/>
-      <c r="BO2" s="36"/>
-      <c r="BP2" s="36"/>
-      <c r="BQ2" s="36"/>
-      <c r="BR2" s="36"/>
-      <c r="BS2" s="36"/>
-      <c r="BT2" s="36"/>
-      <c r="BU2" s="36"/>
-      <c r="BV2" s="36"/>
-      <c r="BW2" s="36"/>
-      <c r="BX2" s="36"/>
-      <c r="BY2" s="36"/>
-      <c r="BZ2" s="36"/>
-      <c r="CA2" s="36"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="32"/>
+      <c r="BG2" s="35"/>
+      <c r="BH2" s="35"/>
+      <c r="BI2" s="35"/>
+      <c r="BJ2" s="35"/>
+      <c r="BK2" s="35"/>
+      <c r="BL2" s="35"/>
+      <c r="BM2" s="35"/>
+      <c r="BN2" s="35"/>
+      <c r="BO2" s="35"/>
+      <c r="BP2" s="35"/>
+      <c r="BQ2" s="35"/>
+      <c r="BR2" s="35"/>
+      <c r="BS2" s="35"/>
+      <c r="BT2" s="35"/>
+      <c r="BU2" s="35"/>
+      <c r="BV2" s="35"/>
+      <c r="BW2" s="35"/>
+      <c r="BX2" s="35"/>
+      <c r="BY2" s="35"/>
+      <c r="BZ2" s="35"/>
+      <c r="CA2" s="35"/>
     </row>
     <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -4280,43 +4289,43 @@
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="37"/>
-      <c r="T32" s="37"/>
-      <c r="U32" s="37"/>
-      <c r="V32" s="37"/>
-      <c r="W32" s="37"/>
-      <c r="X32" s="37"/>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="37"/>
-      <c r="AA32" s="37"/>
-      <c r="AB32" s="37"/>
-      <c r="AC32" s="37"/>
-      <c r="AD32" s="37"/>
-      <c r="AE32" s="37"/>
-      <c r="AF32" s="38">
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="21"/>
+      <c r="AA32" s="21"/>
+      <c r="AB32" s="21"/>
+      <c r="AC32" s="21"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="21"/>
+      <c r="AF32" s="22">
         <v>43293</v>
       </c>
-      <c r="AG32" s="38"/>
-      <c r="AH32" s="38"/>
-      <c r="AI32" s="38"/>
-      <c r="AJ32" s="38"/>
+      <c r="AG32" s="22"/>
+      <c r="AH32" s="22"/>
+      <c r="AI32" s="22"/>
+      <c r="AJ32" s="22"/>
       <c r="AK32" s="10" t="s">
         <v>16</v>
       </c>
@@ -4345,27 +4354,27 @@
       <c r="BD32" s="10"/>
       <c r="BE32" s="10"/>
       <c r="BF32" s="10"/>
-      <c r="BG32" s="39"/>
-      <c r="BH32" s="39"/>
-      <c r="BI32" s="39"/>
-      <c r="BJ32" s="39"/>
-      <c r="BK32" s="39"/>
-      <c r="BL32" s="39"/>
-      <c r="BM32" s="39"/>
-      <c r="BN32" s="39"/>
-      <c r="BO32" s="39"/>
-      <c r="BP32" s="39"/>
-      <c r="BQ32" s="39"/>
-      <c r="BR32" s="39"/>
-      <c r="BS32" s="39"/>
-      <c r="BT32" s="39"/>
-      <c r="BU32" s="39"/>
-      <c r="BV32" s="39"/>
-      <c r="BW32" s="39"/>
-      <c r="BX32" s="39"/>
-      <c r="BY32" s="39"/>
-      <c r="BZ32" s="39"/>
-      <c r="CA32" s="39"/>
+      <c r="BG32" s="23"/>
+      <c r="BH32" s="23"/>
+      <c r="BI32" s="23"/>
+      <c r="BJ32" s="23"/>
+      <c r="BK32" s="23"/>
+      <c r="BL32" s="23"/>
+      <c r="BM32" s="23"/>
+      <c r="BN32" s="23"/>
+      <c r="BO32" s="23"/>
+      <c r="BP32" s="23"/>
+      <c r="BQ32" s="23"/>
+      <c r="BR32" s="23"/>
+      <c r="BS32" s="23"/>
+      <c r="BT32" s="23"/>
+      <c r="BU32" s="23"/>
+      <c r="BV32" s="23"/>
+      <c r="BW32" s="23"/>
+      <c r="BX32" s="23"/>
+      <c r="BY32" s="23"/>
+      <c r="BZ32" s="23"/>
+      <c r="CA32" s="23"/>
     </row>
     <row r="33" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
@@ -4417,27 +4426,27 @@
       <c r="AM33" s="10"/>
       <c r="AN33" s="10"/>
       <c r="AO33" s="10"/>
-      <c r="AP33" s="40">
+      <c r="AP33" s="24">
         <v>0.98</v>
       </c>
-      <c r="AQ33" s="40"/>
-      <c r="AR33" s="40"/>
-      <c r="AS33" s="41" t="s">
+      <c r="AQ33" s="24"/>
+      <c r="AR33" s="24"/>
+      <c r="AS33" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT33" s="41"/>
-      <c r="AU33" s="41"/>
-      <c r="AV33" s="41"/>
-      <c r="AW33" s="41"/>
-      <c r="AX33" s="41"/>
-      <c r="AY33" s="41"/>
-      <c r="AZ33" s="41"/>
-      <c r="BA33" s="41"/>
-      <c r="BB33" s="41"/>
-      <c r="BC33" s="41"/>
-      <c r="BD33" s="41"/>
-      <c r="BE33" s="41"/>
-      <c r="BF33" s="41"/>
+      <c r="AT33" s="25"/>
+      <c r="AU33" s="25"/>
+      <c r="AV33" s="25"/>
+      <c r="AW33" s="25"/>
+      <c r="AX33" s="25"/>
+      <c r="AY33" s="25"/>
+      <c r="AZ33" s="25"/>
+      <c r="BA33" s="25"/>
+      <c r="BB33" s="25"/>
+      <c r="BC33" s="25"/>
+      <c r="BD33" s="25"/>
+      <c r="BE33" s="25"/>
+      <c r="BF33" s="25"/>
       <c r="BG33" s="13"/>
       <c r="BH33" s="13"/>
       <c r="BI33" s="13"/>
@@ -4745,36 +4754,36 @@
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
-      <c r="Y37" s="20"/>
-      <c r="Z37" s="20"/>
-      <c r="AA37" s="20"/>
-      <c r="AB37" s="20"/>
-      <c r="AC37" s="20"/>
-      <c r="AD37" s="20"/>
-      <c r="AE37" s="21"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+      <c r="Y37" s="19"/>
+      <c r="Z37" s="19"/>
+      <c r="AA37" s="19"/>
+      <c r="AB37" s="19"/>
+      <c r="AC37" s="19"/>
+      <c r="AD37" s="19"/>
+      <c r="AE37" s="20"/>
       <c r="AF37" s="11">
         <v>43416</v>
       </c>
@@ -4838,36 +4847,36 @@
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
-      <c r="Y38" s="20"/>
-      <c r="Z38" s="20"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="20"/>
-      <c r="AC38" s="20"/>
-      <c r="AD38" s="20"/>
-      <c r="AE38" s="21"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19